<commit_message>
working cards work flow with problems
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3218" uniqueCount="2580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3240" uniqueCount="2599">
   <si>
     <t>Base Set</t>
   </si>
@@ -7772,6 +7772,63 @@
   </si>
   <si>
     <t>https://1.bp.blogspot.com/-fvpEHPG8_Wc/V7Y8Wuv0koI/AAAAAAABnhY/symLN0N71FwmhyzdOw2NrJs2neVjg2cNQCLcB/s1600/olympics-6-6-2.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-XSDcZ8WSzvY/V7cqfM8xjWI/AAAAAAAAdu0/_0OufMQ-SgURELpPdmDAgobzn9TAN_7BgCLcB/s1600/1970%2BTopps%2B%2523220%2BCarlton.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-C9iz7B67QC0/V7cqj-Q6rjI/AAAAAAAAdu4/jWRZIuFNnbgRZ9To-7hBHf9WBA1IP2IVQCLcB/s1600/1970%2BTopps%2B%2523605%2BWise.jpg</t>
+  </si>
+  <si>
+    <t>Jerry Koosman</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-y1R77DQJxYE/V8CX2zfLxpI/AAAAAAAAdx8/QdqDti79eI03UJY8x_Q5YFj-VUTOQ3qPwCLcB/s1600/1970%2BTopps%2B%2523610%2BKoosman.jpg</t>
+  </si>
+  <si>
+    <t>Frank Herrmann</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-nbOLB8Cak0s/V7c2QLmgwJI/AAAAAAAAdvY/07b0Dfh3wdQVbpwv3G8YYmtJcWyspQBvQCLcB/s1600/2016%2BChachi%2B%252357%2BHerrmann.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-CiRdx0OghdM/V7pNrjl6oxI/AAAAAAAAdwo/nwB5Qa5tYIs2BhAnEfATUCvt9CiDk3-lACLcB/s1600/2016%2BPhillies%2BTeam%2BIssue%2B%252316%2BHernandez.jpg</t>
+  </si>
+  <si>
+    <t>Tony Curry</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-hq_J13wlEg4/V7Hm_dwNUZI/AAAAAAAAIWk/ezOGy4KgLcIH_y_q0FE_Y84fuDTRY27dgCLcB/s1600/tony%2Bcurry.jpg</t>
+  </si>
+  <si>
+    <t>Chooch 2007 Topps</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-mC3KAHRqOMI/V8DIidQxcmI/AAAAAAAAdyk/BpJgPYA0P308Df6APO6veRygHp_Ew5t0QCLcB/s1600/2007%2BTopps%2BUpdate%2B%2523UH99%2BRuiz.jpg</t>
+  </si>
+  <si>
+    <t>Chooch 2008 Topps</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-MGQ6zHYCDow/V8DMcdZG4NI/AAAAAAAAdzE/PRCqSdcinDAmBLurg6MChNy_AQjM2D4bwCLcB/s1600/2008%2BTopps%2B%2523281%2BRuiz.jpg</t>
+  </si>
+  <si>
+    <t>Chooch 2009 Topps</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-ShJYa9iqlHw/V8DMcSThWeI/AAAAAAAAdy8/Gm81RZONoc42lK7lEXJXLMb_LF1H7hX5QCLcB/s1600/2009%2BTopps%2B%2523397%2BRuiz.jpg</t>
+  </si>
+  <si>
+    <t>Ryan Madsen 2004 Bazooka</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-AvVcQCgdF6M/V8DSvoonWMI/AAAAAAAAdzU/2LuClm5RPisUgxy5rc3Fsd8GY6Tk7tWzgCLcB/s1600/2004%2BBazooka%2B%2523259%2BMadson.jpg</t>
+  </si>
+  <si>
+    <t>A.J. Ellis 2014 Topps Heritage</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-9MBX49w7b_E/V8Cz4BReSsI/AAAAAAAAdyQ/qusG9Tyauv870NOtWP9HQW0Q1jSBEDnmwCLcB/s1600/2014%2BTopps%2BHeritage%2B%252322%2BEllis.jpg</t>
   </si>
 </sst>
 </file>
@@ -8139,10 +8196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B494"/>
+  <dimension ref="A1:B498"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A281" sqref="A281"/>
+      <selection activeCell="A285" sqref="A285:B285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8961,2671 +9018,2719 @@
         <v>2276</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>2451</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>2279</v>
-      </c>
-      <c r="B110" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>2280</v>
-      </c>
-      <c r="B111" t="s">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>2281</v>
-      </c>
-      <c r="B112" t="s">
-        <v>2458</v>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>2587</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>2589</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>2593</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>2595</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2596</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>2282</v>
-      </c>
-      <c r="B113" t="s">
-        <v>2457</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>2283</v>
+        <v>2279</v>
       </c>
       <c r="B114" t="s">
-        <v>2284</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>2285</v>
+        <v>2280</v>
       </c>
       <c r="B115" t="s">
-        <v>2286</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>2287</v>
+        <v>2281</v>
       </c>
       <c r="B116" t="s">
-        <v>2456</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>2288</v>
+        <v>2282</v>
       </c>
       <c r="B117" t="s">
-        <v>2289</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>2290</v>
+        <v>2283</v>
       </c>
       <c r="B118" t="s">
-        <v>2291</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>2292</v>
+        <v>2285</v>
       </c>
       <c r="B119" t="s">
-        <v>2293</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>2294</v>
+        <v>2287</v>
       </c>
       <c r="B120" t="s">
-        <v>2452</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>2295</v>
+        <v>2288</v>
       </c>
       <c r="B121" t="s">
-        <v>2453</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>2296</v>
+        <v>2290</v>
       </c>
       <c r="B122" t="s">
-        <v>2455</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="B123" t="s">
-        <v>2454</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>2298</v>
+        <v>2294</v>
       </c>
       <c r="B124" t="s">
-        <v>2299</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>2300</v>
+        <v>2295</v>
       </c>
       <c r="B125" t="s">
-        <v>2465</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>2301</v>
+        <v>2296</v>
       </c>
       <c r="B126" t="s">
-        <v>2466</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>2302</v>
+        <v>2297</v>
       </c>
       <c r="B127" t="s">
-        <v>2467</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>2303</v>
+        <v>2298</v>
       </c>
       <c r="B128" t="s">
-        <v>2468</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>2304</v>
+        <v>2300</v>
       </c>
       <c r="B129" t="s">
-        <v>2469</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>2305</v>
+        <v>2301</v>
       </c>
       <c r="B130" t="s">
-        <v>2470</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>2306</v>
+        <v>2302</v>
       </c>
       <c r="B131" t="s">
-        <v>2471</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>2307</v>
+        <v>2303</v>
       </c>
       <c r="B132" t="s">
-        <v>2472</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>2308</v>
+        <v>2304</v>
       </c>
       <c r="B133" t="s">
-        <v>2473</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>2309</v>
+        <v>2305</v>
       </c>
       <c r="B134" t="s">
-        <v>2474</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>2310</v>
+        <v>2306</v>
       </c>
       <c r="B135" t="s">
-        <v>2475</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>2311</v>
+        <v>2307</v>
       </c>
       <c r="B136" t="s">
-        <v>2476</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>2312</v>
+        <v>2308</v>
       </c>
       <c r="B137" t="s">
-        <v>2477</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>2313</v>
+        <v>2309</v>
       </c>
       <c r="B138" t="s">
-        <v>2478</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>2314</v>
+        <v>2310</v>
       </c>
       <c r="B139" t="s">
-        <v>2479</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>2315</v>
+        <v>2311</v>
       </c>
       <c r="B140" t="s">
-        <v>2480</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>2316</v>
+        <v>2312</v>
       </c>
       <c r="B141" t="s">
-        <v>2481</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>2317</v>
+        <v>2313</v>
       </c>
       <c r="B142" t="s">
-        <v>2482</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>2318</v>
+        <v>2314</v>
       </c>
       <c r="B143" t="s">
-        <v>2483</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>2319</v>
+        <v>2315</v>
       </c>
       <c r="B144" t="s">
-        <v>2464</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>2320</v>
+        <v>2316</v>
       </c>
       <c r="B145" t="s">
-        <v>2321</v>
+        <v>2481</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>2322</v>
+        <v>2317</v>
       </c>
       <c r="B146" t="s">
-        <v>2463</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>2323</v>
+        <v>2318</v>
       </c>
       <c r="B147" t="s">
-        <v>2462</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>2324</v>
+        <v>2319</v>
       </c>
       <c r="B148" t="s">
-        <v>2461</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>2327</v>
+        <v>2320</v>
       </c>
       <c r="B149" t="s">
-        <v>2328</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>2329</v>
+        <v>2322</v>
       </c>
       <c r="B150" t="s">
-        <v>2330</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>2331</v>
+        <v>2323</v>
       </c>
       <c r="B151" t="s">
-        <v>2332</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>2337</v>
+        <v>2324</v>
       </c>
       <c r="B152" t="s">
-        <v>2338</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>2345</v>
+        <v>2327</v>
       </c>
       <c r="B153" t="s">
-        <v>2346</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>2349</v>
+        <v>2329</v>
       </c>
       <c r="B154" t="s">
-        <v>2350</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>2351</v>
+        <v>2331</v>
       </c>
       <c r="B155" t="s">
-        <v>2352</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>2353</v>
+        <v>2337</v>
       </c>
       <c r="B156" t="s">
-        <v>2354</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>2355</v>
+        <v>2345</v>
       </c>
       <c r="B157" t="s">
-        <v>2356</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>2357</v>
+        <v>2349</v>
       </c>
       <c r="B158" t="s">
-        <v>2358</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>2363</v>
+        <v>2351</v>
       </c>
       <c r="B159" t="s">
-        <v>2364</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>2365</v>
+        <v>2353</v>
       </c>
       <c r="B160" t="s">
-        <v>2366</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>2367</v>
+        <v>2355</v>
       </c>
       <c r="B161" t="s">
-        <v>2368</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>2369</v>
+        <v>2357</v>
       </c>
       <c r="B162" t="s">
-        <v>2370</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>2371</v>
+        <v>2363</v>
       </c>
       <c r="B163" t="s">
-        <v>2372</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>2373</v>
+        <v>2365</v>
       </c>
       <c r="B164" t="s">
-        <v>2374</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>2375</v>
+        <v>2367</v>
       </c>
       <c r="B165" t="s">
-        <v>2376</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>2383</v>
+        <v>2369</v>
       </c>
       <c r="B166" t="s">
-        <v>2384</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>2385</v>
+        <v>2371</v>
       </c>
       <c r="B167" t="s">
-        <v>2386</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>2395</v>
+        <v>2373</v>
       </c>
       <c r="B168" t="s">
-        <v>2396</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>2403</v>
+        <v>2375</v>
       </c>
       <c r="B169" t="s">
-        <v>2404</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>2411</v>
+        <v>2383</v>
       </c>
       <c r="B170" t="s">
-        <v>2412</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>2415</v>
+        <v>2385</v>
       </c>
       <c r="B171" t="s">
-        <v>2416</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>2417</v>
+        <v>2395</v>
       </c>
       <c r="B172" t="s">
-        <v>2418</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>2419</v>
+        <v>2403</v>
       </c>
       <c r="B173" t="s">
-        <v>2420</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>2524</v>
+        <v>2411</v>
       </c>
       <c r="B174" t="s">
-        <v>2525</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>2520</v>
+        <v>2415</v>
       </c>
       <c r="B175" t="s">
-        <v>2521</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>2530</v>
+        <v>2417</v>
       </c>
       <c r="B176" t="s">
-        <v>2531</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>2532</v>
+        <v>2419</v>
       </c>
       <c r="B177" t="s">
-        <v>2533</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>2536</v>
+        <v>2524</v>
       </c>
       <c r="B178" t="s">
-        <v>2537</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>2546</v>
+        <v>2520</v>
       </c>
       <c r="B179" t="s">
-        <v>2547</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>2548</v>
+        <v>2530</v>
       </c>
       <c r="B180" t="s">
-        <v>2549</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>2550</v>
+        <v>2532</v>
       </c>
       <c r="B181" t="s">
-        <v>2551</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>2556</v>
+        <v>2536</v>
       </c>
       <c r="B182" t="s">
-        <v>2557</v>
+        <v>2537</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>2558</v>
+        <v>2546</v>
       </c>
       <c r="B183" t="s">
-        <v>2559</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>2564</v>
+        <v>2548</v>
       </c>
       <c r="B184" t="s">
-        <v>2565</v>
+        <v>2549</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>2550</v>
+      </c>
+      <c r="B185" t="s">
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B186" t="s">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>2558</v>
+      </c>
+      <c r="B187" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>2564</v>
+      </c>
+      <c r="B188" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>2572</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B189" t="s">
         <v>2573</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>2424</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>1552</v>
-      </c>
-      <c r="B208" t="s">
-        <v>1937</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>1524</v>
-      </c>
-      <c r="B209" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>293</v>
-      </c>
-      <c r="B210" t="s">
-        <v>1534</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>1537</v>
-      </c>
-      <c r="B211" t="s">
-        <v>1538</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>1541</v>
+        <v>1552</v>
       </c>
       <c r="B212" t="s">
-        <v>1539</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>1540</v>
+        <v>1524</v>
       </c>
       <c r="B213" t="s">
-        <v>1542</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>1548</v>
+        <v>293</v>
       </c>
       <c r="B214" t="s">
-        <v>1547</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>1569</v>
+        <v>1537</v>
       </c>
       <c r="B215" t="s">
-        <v>1570</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>1571</v>
+        <v>1541</v>
       </c>
       <c r="B216" t="s">
-        <v>1572</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>1811</v>
+        <v>1540</v>
       </c>
       <c r="B217" t="s">
-        <v>1812</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>1932</v>
+        <v>1548</v>
       </c>
       <c r="B218" t="s">
-        <v>1933</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>1934</v>
+        <v>1569</v>
       </c>
       <c r="B219" t="s">
-        <v>1935</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>1644</v>
+        <v>1571</v>
       </c>
       <c r="B220" t="s">
-        <v>1643</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>1648</v>
+        <v>1811</v>
       </c>
       <c r="B221" t="s">
-        <v>1649</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>1652</v>
+        <v>1932</v>
       </c>
       <c r="B222" t="s">
-        <v>1653</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>1650</v>
+        <v>1934</v>
       </c>
       <c r="B223" t="s">
-        <v>1651</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>1654</v>
+        <v>1644</v>
       </c>
       <c r="B224" t="s">
-        <v>1655</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>2036</v>
+        <v>1648</v>
       </c>
       <c r="B225" t="s">
-        <v>2037</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>2193</v>
+        <v>1652</v>
       </c>
       <c r="B226" t="s">
-        <v>2194</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>2205</v>
+        <v>1650</v>
       </c>
       <c r="B227" t="s">
-        <v>2206</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>2207</v>
+        <v>1654</v>
       </c>
       <c r="B228" t="s">
-        <v>2208</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>2209</v>
+        <v>2036</v>
       </c>
       <c r="B229" t="s">
-        <v>2210</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>2211</v>
+        <v>2193</v>
       </c>
       <c r="B230" t="s">
-        <v>2212</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>2219</v>
+        <v>2205</v>
       </c>
       <c r="B231" t="s">
-        <v>2220</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>2231</v>
+        <v>2207</v>
       </c>
       <c r="B232" t="s">
-        <v>2232</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>2239</v>
+        <v>2209</v>
       </c>
       <c r="B233" t="s">
-        <v>2240</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>2241</v>
+        <v>2211</v>
       </c>
       <c r="B234" t="s">
-        <v>2242</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>2257</v>
+        <v>2219</v>
       </c>
       <c r="B235" t="s">
-        <v>2258</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>2259</v>
+        <v>2231</v>
       </c>
       <c r="B236" t="s">
-        <v>2260</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>2261</v>
+        <v>2239</v>
       </c>
       <c r="B237" t="s">
-        <v>2262</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>2263</v>
+        <v>2241</v>
       </c>
       <c r="B238" t="s">
-        <v>2264</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>1548</v>
+        <v>2257</v>
       </c>
       <c r="B239" t="s">
-        <v>2265</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>2266</v>
+        <v>2259</v>
       </c>
       <c r="B240" t="s">
-        <v>2267</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>2269</v>
+        <v>2261</v>
       </c>
       <c r="B241" t="s">
-        <v>2270</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>2277</v>
+        <v>2263</v>
       </c>
       <c r="B242" t="s">
-        <v>2278</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>2377</v>
+        <v>1548</v>
       </c>
       <c r="B243" t="s">
-        <v>2378</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>2379</v>
+        <v>2266</v>
       </c>
       <c r="B244" t="s">
-        <v>2380</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>2381</v>
+        <v>2269</v>
       </c>
       <c r="B245" t="s">
-        <v>2382</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>2359</v>
+        <v>2277</v>
       </c>
       <c r="B246" t="s">
-        <v>2360</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>2361</v>
+        <v>2377</v>
       </c>
       <c r="B247" t="s">
-        <v>2362</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>2333</v>
+        <v>2379</v>
       </c>
       <c r="B248" t="s">
-        <v>2334</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>2335</v>
+        <v>2381</v>
       </c>
       <c r="B249" t="s">
-        <v>2336</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>2339</v>
+        <v>2359</v>
       </c>
       <c r="B250" t="s">
-        <v>2340</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>2341</v>
+        <v>2361</v>
       </c>
       <c r="B251" t="s">
-        <v>2342</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>2343</v>
+        <v>2333</v>
       </c>
       <c r="B252" t="s">
-        <v>2344</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>2347</v>
+        <v>2335</v>
       </c>
       <c r="B253" t="s">
-        <v>2348</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>2325</v>
+        <v>2339</v>
       </c>
       <c r="B254" t="s">
-        <v>2326</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>2387</v>
+        <v>2341</v>
       </c>
       <c r="B255" t="s">
-        <v>2388</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>2389</v>
+        <v>2343</v>
       </c>
       <c r="B256" t="s">
-        <v>2390</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>2393</v>
+        <v>2347</v>
       </c>
       <c r="B257" t="s">
-        <v>2394</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>2397</v>
+        <v>2325</v>
       </c>
       <c r="B258" t="s">
-        <v>2398</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>2399</v>
+        <v>2387</v>
       </c>
       <c r="B259" t="s">
-        <v>2400</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>2401</v>
+        <v>2389</v>
       </c>
       <c r="B260" t="s">
-        <v>2402</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>2405</v>
+        <v>2393</v>
       </c>
       <c r="B261" t="s">
-        <v>2406</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>2407</v>
+        <v>2397</v>
       </c>
       <c r="B262" t="s">
-        <v>2408</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>2413</v>
+        <v>2399</v>
       </c>
       <c r="B263" t="s">
-        <v>2414</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>1631</v>
+        <v>2401</v>
       </c>
       <c r="B264" t="s">
-        <v>2508</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>2522</v>
+        <v>2405</v>
       </c>
       <c r="B265" t="s">
-        <v>2523</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>2526</v>
+        <v>2407</v>
       </c>
       <c r="B266" t="s">
-        <v>2527</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>2528</v>
+        <v>2413</v>
       </c>
       <c r="B267" t="s">
-        <v>2529</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>2534</v>
+        <v>1631</v>
       </c>
       <c r="B268" t="s">
-        <v>2535</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>2538</v>
+        <v>2522</v>
       </c>
       <c r="B269" t="s">
-        <v>2539</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>2540</v>
+        <v>2526</v>
       </c>
       <c r="B270" t="s">
-        <v>2541</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>2542</v>
+        <v>2528</v>
       </c>
       <c r="B271" t="s">
-        <v>2543</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="B272" t="s">
-        <v>2545</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>2552</v>
+        <v>2538</v>
       </c>
       <c r="B273" t="s">
-        <v>2553</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>2554</v>
+        <v>2540</v>
       </c>
       <c r="B274" t="s">
-        <v>2555</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>2560</v>
+        <v>2542</v>
       </c>
       <c r="B275" t="s">
-        <v>2561</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>2562</v>
+        <v>2544</v>
       </c>
       <c r="B276" t="s">
-        <v>2563</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>2566</v>
+        <v>2552</v>
       </c>
       <c r="B277" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>2574</v>
+        <v>2554</v>
       </c>
       <c r="B278" t="s">
-        <v>2575</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>2576</v>
+        <v>2560</v>
       </c>
       <c r="B279" t="s">
-        <v>2577</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>2578</v>
+        <v>2562</v>
       </c>
       <c r="B280" t="s">
-        <v>2579</v>
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>2566</v>
+      </c>
+      <c r="B281" t="s">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>2574</v>
+      </c>
+      <c r="B282" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>2576</v>
+      </c>
+      <c r="B283" t="s">
+        <v>2577</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>2484</v>
+        <v>2578</v>
+      </c>
+      <c r="B284" t="s">
+        <v>2579</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>2391</v>
+        <v>2597</v>
       </c>
       <c r="B285" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>2409</v>
-      </c>
-      <c r="B286" t="s">
-        <v>2410</v>
+        <v>2598</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>2484</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>2426</v>
+        <v>2391</v>
+      </c>
+      <c r="B289" t="s">
+        <v>2392</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>1489</v>
+        <v>2409</v>
       </c>
       <c r="B290" t="s">
-        <v>1579</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>1581</v>
-      </c>
-      <c r="B291" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>1583</v>
-      </c>
-      <c r="B292" t="s">
-        <v>1582</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>1585</v>
-      </c>
-      <c r="B293" t="s">
-        <v>1584</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>1587</v>
+        <v>1489</v>
       </c>
       <c r="B294" t="s">
-        <v>1586</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>1589</v>
+        <v>1581</v>
       </c>
       <c r="B295" t="s">
-        <v>1588</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>1516</v>
+        <v>1583</v>
       </c>
       <c r="B296" t="s">
-        <v>1590</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>1592</v>
+        <v>1585</v>
       </c>
       <c r="B297" t="s">
-        <v>1591</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>1640</v>
+        <v>1587</v>
       </c>
       <c r="B298" t="s">
-        <v>1641</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
       <c r="B299" t="s">
-        <v>1593</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>1596</v>
+        <v>1516</v>
       </c>
       <c r="B300" t="s">
-        <v>1595</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>1598</v>
+        <v>1592</v>
       </c>
       <c r="B301" t="s">
-        <v>1597</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>1600</v>
+        <v>1640</v>
       </c>
       <c r="B302" t="s">
-        <v>1599</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>1601</v>
+        <v>1594</v>
       </c>
       <c r="B303" t="s">
-        <v>1602</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>1604</v>
+        <v>1596</v>
       </c>
       <c r="B304" t="s">
-        <v>1603</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>1605</v>
+        <v>1598</v>
       </c>
       <c r="B305" t="s">
-        <v>1606</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>1609</v>
+        <v>1600</v>
       </c>
       <c r="B306" t="s">
-        <v>1607</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>1608</v>
+        <v>1601</v>
       </c>
       <c r="B307" t="s">
-        <v>1610</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>1612</v>
+        <v>1604</v>
       </c>
       <c r="B308" t="s">
-        <v>1611</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>1422</v>
+        <v>1605</v>
       </c>
       <c r="B309" t="s">
-        <v>1613</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>1615</v>
+        <v>1609</v>
       </c>
       <c r="B310" t="s">
-        <v>1614</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>1617</v>
+        <v>1608</v>
       </c>
       <c r="B311" t="s">
-        <v>1616</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>1619</v>
+        <v>1612</v>
       </c>
       <c r="B312" t="s">
-        <v>1618</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>1621</v>
+        <v>1422</v>
       </c>
       <c r="B313" t="s">
-        <v>1620</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>1623</v>
+        <v>1615</v>
       </c>
       <c r="B314" t="s">
-        <v>1622</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>1625</v>
+        <v>1617</v>
       </c>
       <c r="B315" t="s">
-        <v>1624</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>1627</v>
+        <v>1619</v>
       </c>
       <c r="B316" t="s">
-        <v>1626</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>1629</v>
+        <v>1621</v>
       </c>
       <c r="B317" t="s">
-        <v>1628</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>1631</v>
+        <v>1623</v>
       </c>
       <c r="B318" t="s">
-        <v>1630</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>1634</v>
+        <v>1625</v>
       </c>
       <c r="B319" t="s">
-        <v>1632</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>1633</v>
+        <v>1627</v>
       </c>
       <c r="B320" t="s">
-        <v>1635</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>1636</v>
+        <v>1629</v>
       </c>
       <c r="B321" t="s">
-        <v>1638</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>1637</v>
+        <v>1631</v>
       </c>
       <c r="B322" t="s">
-        <v>1639</v>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1635</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>2509</v>
+        <v>1636</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1638</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>2510</v>
+        <v>1637</v>
       </c>
       <c r="B326" t="s">
-        <v>2511</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>2512</v>
-      </c>
-      <c r="B327" t="s">
-        <v>2513</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
-        <v>2514</v>
-      </c>
-      <c r="B328" t="s">
-        <v>2515</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>2516</v>
-      </c>
-      <c r="B329" t="s">
-        <v>2517</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
+        <v>2510</v>
+      </c>
+      <c r="B330" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B331" t="s">
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B332" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B333" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
         <v>2518</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B334" t="s">
         <v>2519</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>2428</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B344" t="s">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
-        <v>1422</v>
-      </c>
-      <c r="B345" t="s">
-        <v>1671</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
-        <v>1673</v>
-      </c>
-      <c r="B346" t="s">
-        <v>1672</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>1666</v>
-      </c>
-      <c r="B347" t="s">
-        <v>1674</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>1675</v>
+        <v>1554</v>
       </c>
       <c r="B348" t="s">
-        <v>1676</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>1678</v>
+        <v>1422</v>
       </c>
       <c r="B349" t="s">
-        <v>1677</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>1485</v>
+        <v>1673</v>
       </c>
       <c r="B350" t="s">
-        <v>1679</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>1594</v>
+        <v>1666</v>
       </c>
       <c r="B351" t="s">
-        <v>1680</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>1682</v>
+        <v>1675</v>
       </c>
       <c r="B352" t="s">
-        <v>1681</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>1683</v>
+        <v>1678</v>
       </c>
       <c r="B353" t="s">
-        <v>1684</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>1685</v>
+        <v>1485</v>
       </c>
       <c r="B354" t="s">
-        <v>1686</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>1687</v>
+        <v>1594</v>
       </c>
       <c r="B355" t="s">
-        <v>1688</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>1689</v>
+        <v>1682</v>
       </c>
       <c r="B356" t="s">
-        <v>1690</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>2185</v>
+        <v>1683</v>
       </c>
       <c r="B357" t="s">
-        <v>2186</v>
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1686</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>2429</v>
+        <v>1687</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1688</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1485</v>
+        <v>1689</v>
       </c>
       <c r="B360" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>1481</v>
+        <v>2185</v>
       </c>
       <c r="B361" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B362" t="s">
-        <v>1693</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B363" t="s">
-        <v>1695</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>1697</v>
+        <v>1485</v>
       </c>
       <c r="B364" t="s">
-        <v>1696</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>1673</v>
+        <v>1481</v>
       </c>
       <c r="B365" t="s">
-        <v>1698</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>1685</v>
+        <v>1555</v>
       </c>
       <c r="B366" t="s">
-        <v>1699</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>1675</v>
+        <v>1694</v>
       </c>
       <c r="B367" t="s">
-        <v>1700</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>1701</v>
+        <v>1697</v>
       </c>
       <c r="B368" t="s">
-        <v>1702</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>1194</v>
+        <v>1673</v>
       </c>
       <c r="B369" t="s">
-        <v>1703</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>1493</v>
+        <v>1685</v>
       </c>
       <c r="B370" t="s">
-        <v>1704</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>1422</v>
+        <v>1675</v>
       </c>
       <c r="B371" t="s">
-        <v>1705</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>1666</v>
+        <v>1701</v>
       </c>
       <c r="B372" t="s">
-        <v>1706</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>1554</v>
+        <v>1194</v>
       </c>
       <c r="B373" t="s">
-        <v>1707</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>1708</v>
+        <v>1493</v>
       </c>
       <c r="B374" t="s">
-        <v>1709</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>1711</v>
+        <v>1422</v>
       </c>
       <c r="B375" t="s">
-        <v>1710</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>1713</v>
+        <v>1666</v>
       </c>
       <c r="B376" t="s">
-        <v>1712</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>1715</v>
+        <v>1554</v>
       </c>
       <c r="B377" t="s">
-        <v>1714</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>1678</v>
+        <v>1708</v>
       </c>
       <c r="B378" t="s">
-        <v>1716</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>1717</v>
+        <v>1711</v>
       </c>
       <c r="B379" t="s">
-        <v>1718</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>1516</v>
+        <v>1713</v>
       </c>
       <c r="B380" t="s">
-        <v>1899</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>2187</v>
+        <v>1715</v>
       </c>
       <c r="B381" t="s">
-        <v>2188</v>
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B382" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B383" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B384" t="s">
+        <v>1899</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B386" t="s">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>1557</v>
-      </c>
-      <c r="B387" t="s">
-        <v>1721</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>1558</v>
-      </c>
-      <c r="B388" t="s">
-        <v>1722</v>
+        <v>2187</v>
+      </c>
+      <c r="B385" t="s">
+        <v>2188</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B389" t="s">
-        <v>1724</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>1725</v>
+        <v>1719</v>
       </c>
       <c r="B390" t="s">
-        <v>1726</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>1727</v>
+        <v>1557</v>
       </c>
       <c r="B391" t="s">
-        <v>1728</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>1730</v>
+        <v>1558</v>
       </c>
       <c r="B392" t="s">
-        <v>1729</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>1493</v>
+        <v>1723</v>
       </c>
       <c r="B393" t="s">
-        <v>1731</v>
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1726</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>2431</v>
+        <v>1727</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1728</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="B396" t="s">
-        <v>1763</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>1733</v>
+        <v>1493</v>
       </c>
       <c r="B397" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" t="s">
-        <v>1517</v>
-      </c>
-      <c r="B398" t="s">
-        <v>1765</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B399" t="s">
-        <v>1766</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B400" t="s">
-        <v>1767</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>1737</v>
+        <v>1733</v>
       </c>
       <c r="B401" t="s">
-        <v>1736</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>1701</v>
+        <v>1517</v>
       </c>
       <c r="B402" t="s">
-        <v>1781</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>1738</v>
+        <v>1734</v>
       </c>
       <c r="B403" t="s">
-        <v>1739</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>1740</v>
+        <v>1735</v>
       </c>
       <c r="B404" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>1741</v>
+        <v>1737</v>
       </c>
       <c r="B405" t="s">
-        <v>1769</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>1742</v>
+        <v>1701</v>
       </c>
       <c r="B406" t="s">
-        <v>1743</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>1744</v>
+        <v>1738</v>
       </c>
       <c r="B407" t="s">
-        <v>1770</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>1493</v>
+        <v>1740</v>
       </c>
       <c r="B408" t="s">
-        <v>1745</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>1723</v>
+        <v>1741</v>
       </c>
       <c r="B409" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>1746</v>
+        <v>1742</v>
       </c>
       <c r="B410" t="s">
-        <v>1772</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>1194</v>
+        <v>1744</v>
       </c>
       <c r="B411" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>1748</v>
+        <v>1493</v>
       </c>
       <c r="B412" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>1730</v>
+        <v>1723</v>
       </c>
       <c r="B413" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="B414" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>1751</v>
+        <v>1194</v>
       </c>
       <c r="B415" t="s">
-        <v>1750</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>1727</v>
+        <v>1748</v>
       </c>
       <c r="B416" t="s">
-        <v>1776</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>1558</v>
+        <v>1730</v>
       </c>
       <c r="B417" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="B418" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
       <c r="B419" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>1755</v>
+        <v>1727</v>
       </c>
       <c r="B420" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>1757</v>
+        <v>1558</v>
       </c>
       <c r="B421" t="s">
-        <v>1756</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>1759</v>
+        <v>1752</v>
       </c>
       <c r="B422" t="s">
-        <v>1758</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>1760</v>
+        <v>1754</v>
       </c>
       <c r="B423" t="s">
-        <v>1780</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>1762</v>
+        <v>1755</v>
       </c>
       <c r="B424" t="s">
-        <v>1761</v>
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B425" t="s">
+        <v>1756</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>2432</v>
+        <v>1759</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1758</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>1796</v>
+        <v>1760</v>
       </c>
       <c r="B427" t="s">
-        <v>1797</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>1798</v>
+        <v>1762</v>
       </c>
       <c r="B428" t="s">
-        <v>1799</v>
-      </c>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A429" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B429" t="s">
-        <v>1904</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B430" t="s">
-        <v>1905</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>1567</v>
+        <v>1796</v>
       </c>
       <c r="B431" t="s">
-        <v>1907</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>1194</v>
+        <v>1798</v>
       </c>
       <c r="B432" t="s">
-        <v>1908</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>1909</v>
+        <v>1723</v>
       </c>
       <c r="B433" t="s">
-        <v>1910</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>1911</v>
+        <v>1906</v>
       </c>
       <c r="B434" t="s">
-        <v>1912</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>1914</v>
+        <v>1567</v>
       </c>
       <c r="B435" t="s">
-        <v>1913</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>1915</v>
+        <v>1194</v>
       </c>
       <c r="B436" t="s">
-        <v>1916</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>1752</v>
+        <v>1909</v>
       </c>
       <c r="B437" t="s">
-        <v>1917</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>1919</v>
+        <v>1911</v>
       </c>
       <c r="B438" t="s">
-        <v>1918</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>1485</v>
+        <v>1914</v>
       </c>
       <c r="B439" t="s">
-        <v>1920</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>1921</v>
+        <v>1915</v>
       </c>
       <c r="B440" t="s">
-        <v>1922</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>1923</v>
+        <v>1752</v>
       </c>
       <c r="B441" t="s">
-        <v>1924</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>1925</v>
+        <v>1919</v>
       </c>
       <c r="B442" t="s">
-        <v>1926</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>1927</v>
+        <v>1485</v>
       </c>
       <c r="B443" t="s">
-        <v>1928</v>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1922</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>2433</v>
+        <v>1923</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1924</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>1195</v>
+        <v>1925</v>
       </c>
       <c r="B446" t="s">
-        <v>1938</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>1940</v>
+        <v>1927</v>
       </c>
       <c r="B447" t="s">
-        <v>1939</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B448" t="s">
-        <v>1941</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B449" t="s">
-        <v>1942</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>1442</v>
+        <v>1195</v>
       </c>
       <c r="B450" t="s">
-        <v>1943</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>1264</v>
+        <v>1940</v>
       </c>
       <c r="B451" t="s">
-        <v>1944</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>286</v>
+        <v>1237</v>
       </c>
       <c r="B452" t="s">
-        <v>1945</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>1221</v>
+        <v>1270</v>
       </c>
       <c r="B453" t="s">
-        <v>1946</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>1272</v>
+        <v>1442</v>
       </c>
       <c r="B454" t="s">
-        <v>1947</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>1215</v>
+        <v>1264</v>
       </c>
       <c r="B455" t="s">
-        <v>1948</v>
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>286</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1945</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>2434</v>
+        <v>1221</v>
+      </c>
+      <c r="B457" t="s">
+        <v>1946</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>1949</v>
+        <v>1272</v>
       </c>
       <c r="B458" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>1790</v>
+        <v>1215</v>
       </c>
       <c r="B459" t="s">
-        <v>1951</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A460" t="s">
-        <v>1953</v>
-      </c>
-      <c r="B460" t="s">
-        <v>1952</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>1955</v>
-      </c>
-      <c r="B461" t="s">
-        <v>1954</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>1957</v>
+        <v>1949</v>
       </c>
       <c r="B462" t="s">
-        <v>1956</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>1959</v>
+        <v>1790</v>
       </c>
       <c r="B463" t="s">
-        <v>1958</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>1960</v>
+        <v>1953</v>
       </c>
       <c r="B464" t="s">
-        <v>1961</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>1963</v>
+        <v>1955</v>
       </c>
       <c r="B465" t="s">
-        <v>1962</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>1436</v>
+        <v>1957</v>
       </c>
       <c r="B466" t="s">
-        <v>1964</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>1968</v>
+        <v>1959</v>
       </c>
       <c r="B467" t="s">
-        <v>1965</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>1967</v>
+        <v>1960</v>
       </c>
       <c r="B468" t="s">
-        <v>1966</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>1970</v>
+        <v>1963</v>
       </c>
       <c r="B469" t="s">
-        <v>1969</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1612</v>
+        <v>1436</v>
       </c>
       <c r="B470" t="s">
-        <v>1971</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
       <c r="B471" t="s">
-        <v>1972</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>1975</v>
+        <v>1967</v>
       </c>
       <c r="B472" t="s">
-        <v>1974</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>1333</v>
+        <v>1970</v>
       </c>
       <c r="B473" t="s">
-        <v>1976</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>1977</v>
+        <v>1612</v>
       </c>
       <c r="B474" t="s">
-        <v>1978</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>1980</v>
+        <v>1973</v>
       </c>
       <c r="B475" t="s">
-        <v>1979</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>1982</v>
+        <v>1975</v>
       </c>
       <c r="B476" t="s">
-        <v>1981</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>1984</v>
+        <v>1333</v>
       </c>
       <c r="B477" t="s">
-        <v>1983</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>1986</v>
+        <v>1977</v>
       </c>
       <c r="B478" t="s">
-        <v>1985</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>1987</v>
+        <v>1980</v>
       </c>
       <c r="B479" t="s">
-        <v>1988</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>1990</v>
+        <v>1982</v>
       </c>
       <c r="B480" t="s">
-        <v>1989</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>1992</v>
+        <v>1984</v>
       </c>
       <c r="B481" t="s">
-        <v>1991</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1994</v>
+        <v>1986</v>
       </c>
       <c r="B482" t="s">
-        <v>1993</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>1321</v>
+        <v>1987</v>
       </c>
       <c r="B483" t="s">
-        <v>1995</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>1997</v>
+        <v>1990</v>
       </c>
       <c r="B484" t="s">
-        <v>1996</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>1537</v>
+        <v>1992</v>
       </c>
       <c r="B485" t="s">
-        <v>1998</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>1999</v>
+        <v>1994</v>
       </c>
       <c r="B486" t="s">
-        <v>2000</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>2002</v>
+        <v>1321</v>
       </c>
       <c r="B487" t="s">
-        <v>2001</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>2004</v>
+        <v>1997</v>
       </c>
       <c r="B488" t="s">
-        <v>2003</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>2006</v>
+        <v>1537</v>
       </c>
       <c r="B489" t="s">
-        <v>2005</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>2007</v>
+        <v>1999</v>
       </c>
       <c r="B490" t="s">
-        <v>2008</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="B491" t="s">
-        <v>2009</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="B492" t="s">
-        <v>2011</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="B493" t="s">
-        <v>2013</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B494" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B495" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B496" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B497" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
         <v>2016</v>
       </c>
-      <c r="B494" t="s">
+      <c r="B498" t="s">
         <v>2015</v>
       </c>
     </row>
@@ -15069,10 +15174,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD63"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15251,6 +15356,14 @@
         <v>2491</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2581</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>1480</v>
@@ -15542,6 +15655,22 @@
       </c>
       <c r="B63" t="s">
         <v>2492</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2583</v>
       </c>
     </row>
   </sheetData>
@@ -15551,10 +15680,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:B49"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15934,6 +16063,14 @@
       </c>
       <c r="B49" t="s">
         <v>2507</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2586</v>
       </c>
     </row>
   </sheetData>
@@ -16842,8 +16979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:B46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17215,6 +17352,14 @@
       </c>
       <c r="B46" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2585</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Chachi and Bunt cleanup
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="2705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="2711">
   <si>
     <t>Base Set</t>
   </si>
@@ -8147,6 +8147,24 @@
   </si>
   <si>
     <t>http://3.bp.blogspot.com/-vmQbmFm1uCE/V-AgzOioh-I/AAAAAAAAmx0/fwhJzWNoHowXKReunSY0oFwvQLcZHRN9gCK4B/s1600/Bowman%2B2006%2BzzBDP%2BValdez.jpg</t>
+  </si>
+  <si>
+    <t>1970 Rookie Stars (Lis, Reid)</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-6MHEQWrCllk/V-A0i6hGUkI/AAAAAAAAeB8/4OgAdimYpwMpwKUxQyzX2FL6ElS7IoQcwCLcB/s1600/1970%2BTopps%2B%252356%2BLis%2B%2526%2BReid.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-_27tz5hvEBI/V-ABT5MZspI/AAAAAAAAeBs/SpSm7wXBw98VPv2x_Fu7BEwvTJ_O0uvrQCLcB/s1600/2016%2BTopps%2BPro%2BDebut%2B%252342%2BAppel.jpg</t>
+  </si>
+  <si>
+    <t>Mark Appel 2016 Topps Pro Debut</t>
+  </si>
+  <si>
+    <t>Charlie Morton 2016 Topps (diff from Bunt)</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-K3TuTF1Hhwc/V-ABTod0VtI/AAAAAAAAeBg/eUTE0Gan7pwdqyDrXcqTFZjXBbjaCkEPACLcB/s1600/2016%2BTopps%2BPhillies%2B%2523PP-17%2BMorton.jpg</t>
   </si>
 </sst>
 </file>
@@ -8516,8 +8534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B529"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175:XFD175"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9408,6 +9426,14 @@
         <v>2589</v>
       </c>
     </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>2709</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2710</v>
+      </c>
+    </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>2444</v>
@@ -10864,6 +10890,14 @@
       </c>
       <c r="B301" t="s">
         <v>2704</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>2708</v>
+      </c>
+      <c r="B302" t="s">
+        <v>2707</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -15915,8 +15949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16133,6 +16167,14 @@
       </c>
       <c r="B27" t="s">
         <v>2691</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2705</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2706</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -17782,7 +17824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A146" sqref="A146:XFD146"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Talk to rails for tech books - categories
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="14" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="2711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="2712">
   <si>
     <t>Base Set</t>
   </si>
@@ -8165,6 +8165,9 @@
   </si>
   <si>
     <t>https://1.bp.blogspot.com/-K3TuTF1Hhwc/V-ABTod0VtI/AAAAAAAAeBg/eUTE0Gan7pwdqyDrXcqTFZjXBbjaCkEPACLcB/s1600/2016%2BTopps%2BPhillies%2B%2523PP-17%2BMorton.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-dIqtyRjwwcQ/V-Prrp6HhsI/AAAAAAAAeDk/cWLCRbIKB2cUwZnl27R_ebcR9KQ9BWgBgCLcB/s1600/2016%2BPhillies%2BTeam%2BIssue%2B2%2B%252312%2BMorandini%2B%2528Auto%2529.jpg</t>
   </si>
 </sst>
 </file>
@@ -8534,7 +8537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B529"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
@@ -16525,10 +16528,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16916,6 +16919,14 @@
       </c>
       <c r="B50" t="s">
         <v>2634</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Google books query working
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="2770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="2778">
   <si>
     <t>Base Set</t>
   </si>
@@ -8342,6 +8342,30 @@
   </si>
   <si>
     <t>Ben Zobrist</t>
+  </si>
+  <si>
+    <t>Bartolo Colon</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-not0KMcuNt4/V-q-JXKEs4I/AAAAAAAAf_k/6IBCcraCKLMzsDQWbxlNf3xlgKgOwghmgCEw/s1600/colon.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-CvTQidEFp6c/V-nDH_o6KvI/AAAAAAAAeHk/xt9wZRf-i_EMBdASglL8uyphKfXXP3lUwCLcB/s1600/1970%2BTopps%2B%2523546%2BReed.jpg</t>
+  </si>
+  <si>
+    <t>Ron Reed</t>
+  </si>
+  <si>
+    <t>1981 Home Run Leaders</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-ieJ8Y3w_h2c/V-r-hJVXPoI/AAAAAAABoeQ/r5E1OHrLCeYgUMGk34x54h3KY_kHWEZgACLcB/s1600/mustache-1.jpg</t>
+  </si>
+  <si>
+    <t>1971 Tony Perez</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-wfLNlVbejNs/V-s61ODW47I/AAAAAAABoe4/EjURzoXqIRgKhRAyKCw9YnGx58ta2TrWgCLcB/s1600/mustache-1-1.jpg</t>
   </si>
 </sst>
 </file>
@@ -15978,10 +16002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16669,6 +16693,14 @@
         <v>2736</v>
       </c>
     </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>2773</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2772</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16676,10 +16708,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B542"/>
+  <dimension ref="A1:B546"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="B320" sqref="B320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16893,6 +16925,14 @@
         <v>2768</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2771</v>
+      </c>
+    </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2416</v>
@@ -17698,3076 +17738,3092 @@
         <v>2749</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>2444</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>2274</v>
-      </c>
-      <c r="B132" t="s">
-        <v>2452</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>2275</v>
-      </c>
-      <c r="B133" t="s">
-        <v>2453</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>2276</v>
-      </c>
-      <c r="B134" t="s">
-        <v>2451</v>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>2774</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2775</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>2277</v>
-      </c>
-      <c r="B135" t="s">
-        <v>2450</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>2278</v>
+        <v>2274</v>
       </c>
       <c r="B136" t="s">
-        <v>2279</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>2280</v>
+        <v>2275</v>
       </c>
       <c r="B137" t="s">
-        <v>2281</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>2282</v>
+        <v>2276</v>
       </c>
       <c r="B138" t="s">
-        <v>2449</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>2283</v>
+        <v>2277</v>
       </c>
       <c r="B139" t="s">
-        <v>2284</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>2285</v>
+        <v>2278</v>
       </c>
       <c r="B140" t="s">
-        <v>2286</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>2287</v>
+        <v>2280</v>
       </c>
       <c r="B141" t="s">
-        <v>2288</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>2289</v>
+        <v>2282</v>
       </c>
       <c r="B142" t="s">
-        <v>2445</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>2290</v>
+        <v>2283</v>
       </c>
       <c r="B143" t="s">
-        <v>2446</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>2291</v>
+        <v>2285</v>
       </c>
       <c r="B144" t="s">
-        <v>2448</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>2292</v>
+        <v>2287</v>
       </c>
       <c r="B145" t="s">
-        <v>2447</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>2293</v>
+        <v>2289</v>
       </c>
       <c r="B146" t="s">
-        <v>2294</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>2295</v>
+        <v>2290</v>
       </c>
       <c r="B147" t="s">
-        <v>2458</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>2296</v>
+        <v>2291</v>
       </c>
       <c r="B148" t="s">
-        <v>2459</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="B149" t="s">
-        <v>2460</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>2298</v>
+        <v>2293</v>
       </c>
       <c r="B150" t="s">
-        <v>2461</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>2299</v>
+        <v>2295</v>
       </c>
       <c r="B151" t="s">
-        <v>2462</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>2300</v>
+        <v>2296</v>
       </c>
       <c r="B152" t="s">
-        <v>2463</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>2301</v>
+        <v>2297</v>
       </c>
       <c r="B153" t="s">
-        <v>2464</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>2302</v>
+        <v>2298</v>
       </c>
       <c r="B154" t="s">
-        <v>2465</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>2303</v>
+        <v>2299</v>
       </c>
       <c r="B155" t="s">
-        <v>2466</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>2304</v>
+        <v>2300</v>
       </c>
       <c r="B156" t="s">
-        <v>2467</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>2305</v>
+        <v>2301</v>
       </c>
       <c r="B157" t="s">
-        <v>2468</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>2306</v>
+        <v>2302</v>
       </c>
       <c r="B158" t="s">
-        <v>2469</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>2307</v>
+        <v>2303</v>
       </c>
       <c r="B159" t="s">
-        <v>2470</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>2308</v>
+        <v>2304</v>
       </c>
       <c r="B160" t="s">
-        <v>2471</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>2309</v>
+        <v>2305</v>
       </c>
       <c r="B161" t="s">
-        <v>2472</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>2310</v>
+        <v>2306</v>
       </c>
       <c r="B162" t="s">
-        <v>2473</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>2311</v>
+        <v>2307</v>
       </c>
       <c r="B163" t="s">
-        <v>2474</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>2312</v>
+        <v>2308</v>
       </c>
       <c r="B164" t="s">
-        <v>2475</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>2313</v>
+        <v>2309</v>
       </c>
       <c r="B165" t="s">
-        <v>2476</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>2314</v>
+        <v>2310</v>
       </c>
       <c r="B166" t="s">
-        <v>2457</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>2315</v>
+        <v>2311</v>
       </c>
       <c r="B167" t="s">
-        <v>2316</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>2317</v>
+        <v>2312</v>
       </c>
       <c r="B168" t="s">
-        <v>2456</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>2318</v>
+        <v>2313</v>
       </c>
       <c r="B169" t="s">
-        <v>2455</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>2319</v>
+        <v>2314</v>
       </c>
       <c r="B170" t="s">
-        <v>2454</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>2322</v>
+        <v>2315</v>
       </c>
       <c r="B171" t="s">
-        <v>2323</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>2324</v>
+        <v>2317</v>
       </c>
       <c r="B172" t="s">
-        <v>2325</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>2326</v>
+        <v>2318</v>
       </c>
       <c r="B173" t="s">
-        <v>2327</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>2332</v>
+        <v>2319</v>
       </c>
       <c r="B174" t="s">
-        <v>2333</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>2340</v>
+        <v>2322</v>
       </c>
       <c r="B175" t="s">
-        <v>2341</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>2344</v>
+        <v>2324</v>
       </c>
       <c r="B176" t="s">
-        <v>2345</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>2346</v>
+        <v>2326</v>
       </c>
       <c r="B177" t="s">
-        <v>2347</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>2348</v>
+        <v>2332</v>
       </c>
       <c r="B178" t="s">
-        <v>2349</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>2350</v>
+        <v>2340</v>
       </c>
       <c r="B179" t="s">
-        <v>2351</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>2352</v>
+        <v>2344</v>
       </c>
       <c r="B180" t="s">
-        <v>2353</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>2358</v>
+        <v>2346</v>
       </c>
       <c r="B181" t="s">
-        <v>2359</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>2360</v>
+        <v>2348</v>
       </c>
       <c r="B182" t="s">
-        <v>2361</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>2362</v>
+        <v>2350</v>
       </c>
       <c r="B183" t="s">
-        <v>2363</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>2364</v>
+        <v>2352</v>
       </c>
       <c r="B184" t="s">
-        <v>2365</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>2366</v>
+        <v>2358</v>
       </c>
       <c r="B185" t="s">
-        <v>2367</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>2368</v>
+        <v>2360</v>
       </c>
       <c r="B186" t="s">
-        <v>2369</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>2370</v>
+        <v>2362</v>
       </c>
       <c r="B187" t="s">
-        <v>2371</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>2378</v>
+        <v>2364</v>
       </c>
       <c r="B188" t="s">
-        <v>2379</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>2388</v>
+        <v>2366</v>
       </c>
       <c r="B189" t="s">
-        <v>2389</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>2396</v>
+        <v>2368</v>
       </c>
       <c r="B190" t="s">
-        <v>2397</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>2404</v>
+        <v>2370</v>
       </c>
       <c r="B191" t="s">
-        <v>2405</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>2408</v>
+        <v>2378</v>
       </c>
       <c r="B192" t="s">
-        <v>2409</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>2410</v>
+        <v>2388</v>
       </c>
       <c r="B193" t="s">
-        <v>2411</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>2412</v>
+        <v>2396</v>
       </c>
       <c r="B194" t="s">
-        <v>2413</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>2517</v>
+        <v>2404</v>
       </c>
       <c r="B195" t="s">
-        <v>2518</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>2513</v>
+        <v>2408</v>
       </c>
       <c r="B196" t="s">
-        <v>2514</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>2523</v>
+        <v>2410</v>
       </c>
       <c r="B197" t="s">
-        <v>2524</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>2525</v>
+        <v>2412</v>
       </c>
       <c r="B198" t="s">
-        <v>2526</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>2529</v>
+        <v>2517</v>
       </c>
       <c r="B199" t="s">
-        <v>2530</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>2539</v>
+        <v>2513</v>
       </c>
       <c r="B200" t="s">
-        <v>2540</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>2541</v>
+        <v>2523</v>
       </c>
       <c r="B201" t="s">
-        <v>2542</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>2543</v>
+        <v>2525</v>
       </c>
       <c r="B202" t="s">
-        <v>2544</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>2549</v>
+        <v>2529</v>
       </c>
       <c r="B203" t="s">
-        <v>2550</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>2551</v>
+        <v>2539</v>
       </c>
       <c r="B204" t="s">
-        <v>2552</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>2557</v>
+        <v>2541</v>
       </c>
       <c r="B205" t="s">
-        <v>2558</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>2565</v>
+        <v>2543</v>
       </c>
       <c r="B206" t="s">
-        <v>2566</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>2600</v>
+        <v>2549</v>
       </c>
       <c r="B207" t="s">
-        <v>2599</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>2602</v>
+        <v>2551</v>
       </c>
       <c r="B208" t="s">
-        <v>2603</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>2604</v>
+        <v>2557</v>
       </c>
       <c r="B209" t="s">
-        <v>2605</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>2635</v>
+        <v>2565</v>
       </c>
       <c r="B210" t="s">
-        <v>2636</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>2637</v>
+        <v>2600</v>
       </c>
       <c r="B211" t="s">
-        <v>2638</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>2640</v>
+        <v>2602</v>
       </c>
       <c r="B212" t="s">
-        <v>2639</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>2641</v>
+        <v>2604</v>
       </c>
       <c r="B213" t="s">
-        <v>2644</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>2642</v>
+        <v>2635</v>
       </c>
       <c r="B214" t="s">
-        <v>2645</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>2643</v>
+        <v>2637</v>
       </c>
       <c r="B215" t="s">
-        <v>2646</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>2647</v>
+        <v>2640</v>
       </c>
       <c r="B216" t="s">
-        <v>2648</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>2649</v>
+        <v>2641</v>
       </c>
       <c r="B217" t="s">
-        <v>2650</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>2655</v>
+        <v>2642</v>
       </c>
       <c r="B218" t="s">
-        <v>2656</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>2659</v>
+        <v>2643</v>
       </c>
       <c r="B219" t="s">
-        <v>2660</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>2665</v>
+        <v>2647</v>
       </c>
       <c r="B220" t="s">
-        <v>2666</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>2667</v>
+        <v>2649</v>
       </c>
       <c r="B221" t="s">
-        <v>2668</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>2669</v>
+        <v>2655</v>
       </c>
       <c r="B222" t="s">
-        <v>2670</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>2674</v>
+        <v>2659</v>
       </c>
       <c r="B223" t="s">
-        <v>2675</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>2678</v>
+        <v>2665</v>
       </c>
       <c r="B224" t="s">
-        <v>2679</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>2687</v>
+        <v>2667</v>
       </c>
       <c r="B225" t="s">
-        <v>2688</v>
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B226" t="s">
+        <v>2670</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>2417</v>
+        <v>2674</v>
+      </c>
+      <c r="B227" t="s">
+        <v>2675</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>1548</v>
+        <v>2678</v>
       </c>
       <c r="B228" t="s">
-        <v>1933</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>1520</v>
+        <v>2687</v>
       </c>
       <c r="B229" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>289</v>
-      </c>
-      <c r="B230" t="s">
-        <v>1530</v>
+        <v>2688</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B231" t="s">
-        <v>1534</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>1537</v>
+        <v>1548</v>
       </c>
       <c r="B232" t="s">
-        <v>1535</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>1536</v>
+        <v>1520</v>
       </c>
       <c r="B233" t="s">
-        <v>1538</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>1544</v>
+        <v>289</v>
       </c>
       <c r="B234" t="s">
-        <v>1543</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>1565</v>
+        <v>1533</v>
       </c>
       <c r="B235" t="s">
-        <v>1566</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>1567</v>
+        <v>1537</v>
       </c>
       <c r="B236" t="s">
-        <v>1568</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>1807</v>
+        <v>1536</v>
       </c>
       <c r="B237" t="s">
-        <v>1808</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>1928</v>
+        <v>1544</v>
       </c>
       <c r="B238" t="s">
-        <v>1929</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>1930</v>
+        <v>1565</v>
       </c>
       <c r="B239" t="s">
-        <v>1931</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>1640</v>
+        <v>1567</v>
       </c>
       <c r="B240" t="s">
-        <v>1639</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>1644</v>
+        <v>1807</v>
       </c>
       <c r="B241" t="s">
-        <v>1645</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>1648</v>
+        <v>1928</v>
       </c>
       <c r="B242" t="s">
-        <v>1649</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>1646</v>
+        <v>1930</v>
       </c>
       <c r="B243" t="s">
-        <v>1647</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>1650</v>
+        <v>1640</v>
       </c>
       <c r="B244" t="s">
-        <v>1651</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>2031</v>
+        <v>1644</v>
       </c>
       <c r="B245" t="s">
-        <v>2032</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>2188</v>
+        <v>1648</v>
       </c>
       <c r="B246" t="s">
-        <v>2189</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>2200</v>
+        <v>1646</v>
       </c>
       <c r="B247" t="s">
-        <v>2201</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>2202</v>
+        <v>1650</v>
       </c>
       <c r="B248" t="s">
-        <v>2203</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>2204</v>
+        <v>2031</v>
       </c>
       <c r="B249" t="s">
-        <v>2205</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>2206</v>
+        <v>2188</v>
       </c>
       <c r="B250" t="s">
-        <v>2207</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>2214</v>
+        <v>2200</v>
       </c>
       <c r="B251" t="s">
-        <v>2215</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>2226</v>
+        <v>2202</v>
       </c>
       <c r="B252" t="s">
-        <v>2227</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>2234</v>
+        <v>2204</v>
       </c>
       <c r="B253" t="s">
-        <v>2235</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>2236</v>
+        <v>2206</v>
       </c>
       <c r="B254" t="s">
-        <v>2237</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>2252</v>
+        <v>2214</v>
       </c>
       <c r="B255" t="s">
-        <v>2253</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>2254</v>
+        <v>2226</v>
       </c>
       <c r="B256" t="s">
-        <v>2255</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>2256</v>
+        <v>2234</v>
       </c>
       <c r="B257" t="s">
-        <v>2257</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>2258</v>
+        <v>2236</v>
       </c>
       <c r="B258" t="s">
-        <v>2259</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>1544</v>
+        <v>2252</v>
       </c>
       <c r="B259" t="s">
-        <v>2260</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>2261</v>
+        <v>2254</v>
       </c>
       <c r="B260" t="s">
-        <v>2262</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>2264</v>
+        <v>2256</v>
       </c>
       <c r="B261" t="s">
-        <v>2265</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>2272</v>
+        <v>2258</v>
       </c>
       <c r="B262" t="s">
-        <v>2273</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>2372</v>
+        <v>1544</v>
       </c>
       <c r="B263" t="s">
-        <v>2373</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>2374</v>
+        <v>2261</v>
       </c>
       <c r="B264" t="s">
-        <v>2375</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>2376</v>
+        <v>2264</v>
       </c>
       <c r="B265" t="s">
-        <v>2377</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>2354</v>
+        <v>2272</v>
       </c>
       <c r="B266" t="s">
-        <v>2355</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>2356</v>
+        <v>2372</v>
       </c>
       <c r="B267" t="s">
-        <v>2357</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>2328</v>
+        <v>2374</v>
       </c>
       <c r="B268" t="s">
-        <v>2329</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>2330</v>
+        <v>2376</v>
       </c>
       <c r="B269" t="s">
-        <v>2331</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>2334</v>
+        <v>2354</v>
       </c>
       <c r="B270" t="s">
-        <v>2335</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>2336</v>
+        <v>2356</v>
       </c>
       <c r="B271" t="s">
-        <v>2337</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>2338</v>
+        <v>2328</v>
       </c>
       <c r="B272" t="s">
-        <v>2339</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>2342</v>
+        <v>2330</v>
       </c>
       <c r="B273" t="s">
-        <v>2343</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>2320</v>
+        <v>2334</v>
       </c>
       <c r="B274" t="s">
-        <v>2321</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>2380</v>
+        <v>2336</v>
       </c>
       <c r="B275" t="s">
-        <v>2381</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>2382</v>
+        <v>2338</v>
       </c>
       <c r="B276" t="s">
-        <v>2383</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>2386</v>
+        <v>2342</v>
       </c>
       <c r="B277" t="s">
-        <v>2387</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>2390</v>
+        <v>2320</v>
       </c>
       <c r="B278" t="s">
-        <v>2391</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>2392</v>
+        <v>2380</v>
       </c>
       <c r="B279" t="s">
-        <v>2393</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>2394</v>
+        <v>2382</v>
       </c>
       <c r="B280" t="s">
-        <v>2395</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>2398</v>
+        <v>2386</v>
       </c>
       <c r="B281" t="s">
-        <v>2399</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>2400</v>
+        <v>2390</v>
       </c>
       <c r="B282" t="s">
-        <v>2401</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>2406</v>
+        <v>2392</v>
       </c>
       <c r="B283" t="s">
-        <v>2407</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>1627</v>
+        <v>2394</v>
       </c>
       <c r="B284" t="s">
-        <v>2501</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>2515</v>
+        <v>2398</v>
       </c>
       <c r="B285" t="s">
-        <v>2516</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>2519</v>
+        <v>2400</v>
       </c>
       <c r="B286" t="s">
-        <v>2520</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>2521</v>
+        <v>2406</v>
       </c>
       <c r="B287" t="s">
-        <v>2522</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>2527</v>
+        <v>1627</v>
       </c>
       <c r="B288" t="s">
-        <v>2528</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>2531</v>
+        <v>2515</v>
       </c>
       <c r="B289" t="s">
-        <v>2532</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>2533</v>
+        <v>2519</v>
       </c>
       <c r="B290" t="s">
-        <v>2534</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>2535</v>
+        <v>2521</v>
       </c>
       <c r="B291" t="s">
-        <v>2536</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>2537</v>
+        <v>2527</v>
       </c>
       <c r="B292" t="s">
-        <v>2538</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>2545</v>
+        <v>2531</v>
       </c>
       <c r="B293" t="s">
-        <v>2546</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>2547</v>
+        <v>2533</v>
       </c>
       <c r="B294" t="s">
-        <v>2548</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>2553</v>
+        <v>2535</v>
       </c>
       <c r="B295" t="s">
-        <v>2554</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>2555</v>
+        <v>2537</v>
       </c>
       <c r="B296" t="s">
-        <v>2556</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>2559</v>
+        <v>2545</v>
       </c>
       <c r="B297" t="s">
-        <v>2560</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>2567</v>
+        <v>2547</v>
       </c>
       <c r="B298" t="s">
-        <v>2568</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>2569</v>
+        <v>2553</v>
       </c>
       <c r="B299" t="s">
-        <v>2570</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>2571</v>
+        <v>2555</v>
       </c>
       <c r="B300" t="s">
-        <v>2572</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>2593</v>
+        <v>2559</v>
       </c>
       <c r="B301" t="s">
-        <v>2591</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>2590</v>
+        <v>2567</v>
       </c>
       <c r="B302" t="s">
-        <v>2592</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>2606</v>
+        <v>2569</v>
       </c>
       <c r="B303" t="s">
-        <v>2607</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>2608</v>
+        <v>2571</v>
       </c>
       <c r="B304" t="s">
-        <v>2609</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>2610</v>
+        <v>2593</v>
       </c>
       <c r="B305" t="s">
-        <v>2611</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>2624</v>
+        <v>2590</v>
       </c>
       <c r="B306" t="s">
-        <v>2625</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>2628</v>
+        <v>2606</v>
       </c>
       <c r="B307" t="s">
-        <v>2629</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>2681</v>
+        <v>2608</v>
       </c>
       <c r="B308" t="s">
-        <v>2680</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>1418</v>
+        <v>2610</v>
       </c>
       <c r="B309" t="s">
-        <v>2682</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>2683</v>
+        <v>2624</v>
       </c>
       <c r="B310" t="s">
-        <v>2684</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>2685</v>
+        <v>2628</v>
       </c>
       <c r="B311" t="s">
-        <v>2686</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>2690</v>
+        <v>2681</v>
       </c>
       <c r="B312" t="s">
-        <v>2689</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>2701</v>
+        <v>1418</v>
       </c>
       <c r="B313" t="s">
-        <v>2702</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>2703</v>
+        <v>2683</v>
       </c>
       <c r="B314" t="s">
-        <v>2704</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>2708</v>
+        <v>2685</v>
       </c>
       <c r="B315" t="s">
-        <v>2707</v>
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B316" t="s">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>2701</v>
+      </c>
+      <c r="B317" t="s">
+        <v>2702</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>2477</v>
+        <v>2703</v>
+      </c>
+      <c r="B318" t="s">
+        <v>2704</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>2384</v>
+        <v>2708</v>
       </c>
       <c r="B319" t="s">
-        <v>2385</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>2402</v>
+        <v>2776</v>
       </c>
       <c r="B320" t="s">
-        <v>2403</v>
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>2477</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>2419</v>
+        <v>2384</v>
+      </c>
+      <c r="B323" t="s">
+        <v>2385</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>1485</v>
+        <v>2402</v>
       </c>
       <c r="B324" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>1577</v>
-      </c>
-      <c r="B325" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>1579</v>
-      </c>
-      <c r="B326" t="s">
-        <v>1578</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>1581</v>
-      </c>
-      <c r="B327" t="s">
-        <v>1580</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>1583</v>
+        <v>1485</v>
       </c>
       <c r="B328" t="s">
-        <v>1582</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>1585</v>
+        <v>1577</v>
       </c>
       <c r="B329" t="s">
-        <v>1584</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>1512</v>
+        <v>1579</v>
       </c>
       <c r="B330" t="s">
-        <v>1586</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>1588</v>
+        <v>1581</v>
       </c>
       <c r="B331" t="s">
-        <v>1587</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>1636</v>
+        <v>1583</v>
       </c>
       <c r="B332" t="s">
-        <v>1637</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>1590</v>
+        <v>1585</v>
       </c>
       <c r="B333" t="s">
-        <v>1589</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>1592</v>
+        <v>1512</v>
       </c>
       <c r="B334" t="s">
-        <v>1591</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>1594</v>
+        <v>1588</v>
       </c>
       <c r="B335" t="s">
-        <v>1593</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>1596</v>
+        <v>1636</v>
       </c>
       <c r="B336" t="s">
-        <v>1595</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>1597</v>
+        <v>1590</v>
       </c>
       <c r="B337" t="s">
-        <v>1598</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>1600</v>
+        <v>1592</v>
       </c>
       <c r="B338" t="s">
-        <v>1599</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>1601</v>
+        <v>1594</v>
       </c>
       <c r="B339" t="s">
-        <v>1602</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>1605</v>
+        <v>1596</v>
       </c>
       <c r="B340" t="s">
-        <v>1603</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>1604</v>
+        <v>1597</v>
       </c>
       <c r="B341" t="s">
-        <v>1606</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>1608</v>
+        <v>1600</v>
       </c>
       <c r="B342" t="s">
-        <v>1607</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>1418</v>
+        <v>1601</v>
       </c>
       <c r="B343" t="s">
-        <v>1609</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>1611</v>
+        <v>1605</v>
       </c>
       <c r="B344" t="s">
-        <v>1610</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>1613</v>
+        <v>1604</v>
       </c>
       <c r="B345" t="s">
-        <v>1612</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>1615</v>
+        <v>1608</v>
       </c>
       <c r="B346" t="s">
-        <v>1614</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>1617</v>
+        <v>1418</v>
       </c>
       <c r="B347" t="s">
-        <v>1616</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>1619</v>
+        <v>1611</v>
       </c>
       <c r="B348" t="s">
-        <v>1618</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>1621</v>
+        <v>1613</v>
       </c>
       <c r="B349" t="s">
-        <v>1620</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>1623</v>
+        <v>1615</v>
       </c>
       <c r="B350" t="s">
-        <v>1622</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>1625</v>
+        <v>1617</v>
       </c>
       <c r="B351" t="s">
-        <v>1624</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>1627</v>
+        <v>1619</v>
       </c>
       <c r="B352" t="s">
-        <v>1626</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>1630</v>
+        <v>1621</v>
       </c>
       <c r="B353" t="s">
-        <v>1628</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>1629</v>
+        <v>1623</v>
       </c>
       <c r="B354" t="s">
-        <v>1631</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>1632</v>
+        <v>1625</v>
       </c>
       <c r="B355" t="s">
-        <v>1634</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>1633</v>
+        <v>1627</v>
       </c>
       <c r="B356" t="s">
-        <v>1635</v>
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B357" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1631</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>2502</v>
+        <v>1632</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1634</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>2503</v>
+        <v>1633</v>
       </c>
       <c r="B360" t="s">
-        <v>2504</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>2505</v>
-      </c>
-      <c r="B361" t="s">
-        <v>2506</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>2507</v>
-      </c>
-      <c r="B362" t="s">
-        <v>2508</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>2509</v>
-      </c>
-      <c r="B363" t="s">
-        <v>2510</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>2511</v>
+        <v>2503</v>
       </c>
       <c r="B364" t="s">
-        <v>2512</v>
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B365" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>2507</v>
+      </c>
+      <c r="B366" t="s">
+        <v>2508</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>2612</v>
+        <v>2509</v>
+      </c>
+      <c r="B367" t="s">
+        <v>2510</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>1485</v>
+        <v>2511</v>
       </c>
       <c r="B368" t="s">
-        <v>2613</v>
-      </c>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
-        <v>2614</v>
-      </c>
-      <c r="B369" t="s">
-        <v>2615</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
-        <v>1619</v>
-      </c>
-      <c r="B370" t="s">
-        <v>2616</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>1596</v>
-      </c>
-      <c r="B371" t="s">
-        <v>2617</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>1632</v>
+        <v>1485</v>
       </c>
       <c r="B372" t="s">
-        <v>2618</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>1180</v>
+        <v>2614</v>
       </c>
       <c r="B373" t="s">
-        <v>2619</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>1249</v>
+        <v>1619</v>
       </c>
       <c r="B374" t="s">
-        <v>2622</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>1627</v>
+        <v>1596</v>
       </c>
       <c r="B375" t="s">
-        <v>2623</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>2627</v>
+        <v>1632</v>
       </c>
       <c r="B376" t="s">
-        <v>2626</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>1623</v>
+        <v>1180</v>
       </c>
       <c r="B377" t="s">
-        <v>2630</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>1590</v>
+        <v>1249</v>
       </c>
       <c r="B378" t="s">
-        <v>2631</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="B379" t="s">
-        <v>2632</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
+        <v>2627</v>
+      </c>
+      <c r="B380" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B381" t="s">
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B382" t="s">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B383" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
         <v>1579</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B384" t="s">
         <v>2633</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
-        <v>2421</v>
-      </c>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
-        <v>1550</v>
-      </c>
-      <c r="B386" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>1418</v>
-      </c>
-      <c r="B387" t="s">
-        <v>1667</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>1669</v>
-      </c>
-      <c r="B388" t="s">
-        <v>1668</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>1662</v>
-      </c>
-      <c r="B389" t="s">
-        <v>1670</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>1671</v>
+        <v>1550</v>
       </c>
       <c r="B390" t="s">
-        <v>1672</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>1674</v>
+        <v>1418</v>
       </c>
       <c r="B391" t="s">
-        <v>1673</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>1481</v>
+        <v>1669</v>
       </c>
       <c r="B392" t="s">
-        <v>1675</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>1590</v>
+        <v>1662</v>
       </c>
       <c r="B393" t="s">
-        <v>1676</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>1678</v>
+        <v>1671</v>
       </c>
       <c r="B394" t="s">
-        <v>1677</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>1679</v>
+        <v>1674</v>
       </c>
       <c r="B395" t="s">
-        <v>1680</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>1681</v>
+        <v>1481</v>
       </c>
       <c r="B396" t="s">
-        <v>1682</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>1683</v>
+        <v>1590</v>
       </c>
       <c r="B397" t="s">
-        <v>1684</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>1685</v>
+        <v>1678</v>
       </c>
       <c r="B398" t="s">
-        <v>1686</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>2180</v>
+        <v>1679</v>
       </c>
       <c r="B399" t="s">
-        <v>2181</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>2621</v>
+        <v>1681</v>
       </c>
       <c r="B400" t="s">
-        <v>2620</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>1713</v>
+        <v>1683</v>
       </c>
       <c r="B401" t="s">
-        <v>2651</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B402" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B403" t="s">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>2621</v>
+      </c>
+      <c r="B404" t="s">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B405" t="s">
+        <v>2651</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
         <v>1623</v>
       </c>
-      <c r="B402" t="s">
+      <c r="B406" t="s">
         <v>2692</v>
-      </c>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" t="s">
-        <v>2422</v>
-      </c>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
-        <v>1481</v>
-      </c>
-      <c r="B408" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>1477</v>
-      </c>
-      <c r="B409" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
-        <v>1551</v>
-      </c>
-      <c r="B410" t="s">
-        <v>1689</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>1690</v>
-      </c>
-      <c r="B411" t="s">
-        <v>1691</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>1693</v>
+        <v>1481</v>
       </c>
       <c r="B412" t="s">
-        <v>1692</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>1669</v>
+        <v>1477</v>
       </c>
       <c r="B413" t="s">
-        <v>1694</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>1681</v>
+        <v>1551</v>
       </c>
       <c r="B414" t="s">
-        <v>1695</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>1671</v>
+        <v>1690</v>
       </c>
       <c r="B415" t="s">
-        <v>1696</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>1697</v>
+        <v>1693</v>
       </c>
       <c r="B416" t="s">
-        <v>1698</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>1190</v>
+        <v>1669</v>
       </c>
       <c r="B417" t="s">
-        <v>1699</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>1489</v>
+        <v>1681</v>
       </c>
       <c r="B418" t="s">
-        <v>1700</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>1418</v>
+        <v>1671</v>
       </c>
       <c r="B419" t="s">
-        <v>1701</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>1662</v>
+        <v>1697</v>
       </c>
       <c r="B420" t="s">
-        <v>1702</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>1550</v>
+        <v>1190</v>
       </c>
       <c r="B421" t="s">
-        <v>1703</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>1704</v>
+        <v>1489</v>
       </c>
       <c r="B422" t="s">
-        <v>1705</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>1707</v>
+        <v>1418</v>
       </c>
       <c r="B423" t="s">
-        <v>1706</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>1709</v>
+        <v>1662</v>
       </c>
       <c r="B424" t="s">
-        <v>1708</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>1711</v>
+        <v>1550</v>
       </c>
       <c r="B425" t="s">
-        <v>1710</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>1674</v>
+        <v>1704</v>
       </c>
       <c r="B426" t="s">
-        <v>1712</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>1713</v>
+        <v>1707</v>
       </c>
       <c r="B427" t="s">
-        <v>1714</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>1512</v>
+        <v>1709</v>
       </c>
       <c r="B428" t="s">
-        <v>1895</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>2182</v>
+        <v>1711</v>
       </c>
       <c r="B429" t="s">
-        <v>2183</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>1729</v>
+        <v>1674</v>
       </c>
       <c r="B430" t="s">
-        <v>2671</v>
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1895</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>2423</v>
+        <v>2182</v>
+      </c>
+      <c r="B433" t="s">
+        <v>2183</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>1715</v>
+        <v>1729</v>
       </c>
       <c r="B434" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" t="s">
-        <v>1553</v>
-      </c>
-      <c r="B435" t="s">
-        <v>1717</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B436" t="s">
-        <v>1718</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B437" t="s">
-        <v>1720</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>1721</v>
+        <v>1715</v>
       </c>
       <c r="B438" t="s">
-        <v>1722</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>1723</v>
+        <v>1553</v>
       </c>
       <c r="B439" t="s">
-        <v>1724</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>1726</v>
+        <v>1554</v>
       </c>
       <c r="B440" t="s">
-        <v>1725</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>1489</v>
+        <v>1719</v>
       </c>
       <c r="B441" t="s">
-        <v>1727</v>
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1722</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>2424</v>
+        <v>1723</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1724</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="B444" t="s">
-        <v>1759</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>1729</v>
+        <v>1489</v>
       </c>
       <c r="B445" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" t="s">
-        <v>1513</v>
-      </c>
-      <c r="B446" t="s">
-        <v>1761</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>1730</v>
-      </c>
-      <c r="B447" t="s">
-        <v>1762</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="B448" t="s">
-        <v>1763</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>1733</v>
+        <v>1729</v>
       </c>
       <c r="B449" t="s">
-        <v>1732</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>1697</v>
+        <v>1513</v>
       </c>
       <c r="B450" t="s">
-        <v>1777</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>1734</v>
+        <v>1730</v>
       </c>
       <c r="B451" t="s">
-        <v>1735</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>1736</v>
+        <v>1731</v>
       </c>
       <c r="B452" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>1737</v>
+        <v>1733</v>
       </c>
       <c r="B453" t="s">
-        <v>1765</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>1738</v>
+        <v>1697</v>
       </c>
       <c r="B454" t="s">
-        <v>1739</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>1740</v>
+        <v>1734</v>
       </c>
       <c r="B455" t="s">
-        <v>1766</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>1489</v>
+        <v>1736</v>
       </c>
       <c r="B456" t="s">
-        <v>1741</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>1719</v>
+        <v>1737</v>
       </c>
       <c r="B457" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>1742</v>
+        <v>1738</v>
       </c>
       <c r="B458" t="s">
-        <v>1768</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>1190</v>
+        <v>1740</v>
       </c>
       <c r="B459" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>1744</v>
+        <v>1489</v>
       </c>
       <c r="B460" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>1726</v>
+        <v>1719</v>
       </c>
       <c r="B461" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="B462" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>1747</v>
+        <v>1190</v>
       </c>
       <c r="B463" t="s">
-        <v>1746</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>1723</v>
+        <v>1744</v>
       </c>
       <c r="B464" t="s">
-        <v>1772</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>1554</v>
+        <v>1726</v>
       </c>
       <c r="B465" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="B466" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="B467" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>1751</v>
+        <v>1723</v>
       </c>
       <c r="B468" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>1753</v>
+        <v>1554</v>
       </c>
       <c r="B469" t="s">
-        <v>1752</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1755</v>
+        <v>1748</v>
       </c>
       <c r="B470" t="s">
-        <v>1754</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>1756</v>
+        <v>1750</v>
       </c>
       <c r="B471" t="s">
-        <v>1776</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>1758</v>
+        <v>1751</v>
       </c>
       <c r="B472" t="s">
-        <v>1757</v>
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B473" t="s">
+        <v>1752</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>2425</v>
+        <v>1755</v>
+      </c>
+      <c r="B474" t="s">
+        <v>1754</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>1792</v>
+        <v>1756</v>
       </c>
       <c r="B475" t="s">
-        <v>1793</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>1794</v>
+        <v>1758</v>
       </c>
       <c r="B476" t="s">
-        <v>1795</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A477" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B477" t="s">
-        <v>1900</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>1902</v>
-      </c>
-      <c r="B478" t="s">
-        <v>1901</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>1563</v>
+        <v>1792</v>
       </c>
       <c r="B479" t="s">
-        <v>1903</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>1190</v>
+        <v>1794</v>
       </c>
       <c r="B480" t="s">
-        <v>1904</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>1905</v>
+        <v>1719</v>
       </c>
       <c r="B481" t="s">
-        <v>1906</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1907</v>
+        <v>1902</v>
       </c>
       <c r="B482" t="s">
-        <v>1908</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>1910</v>
+        <v>1563</v>
       </c>
       <c r="B483" t="s">
-        <v>1909</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>1911</v>
+        <v>1190</v>
       </c>
       <c r="B484" t="s">
-        <v>1912</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>1748</v>
+        <v>1905</v>
       </c>
       <c r="B485" t="s">
-        <v>1913</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>1915</v>
+        <v>1907</v>
       </c>
       <c r="B486" t="s">
-        <v>1914</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>1481</v>
+        <v>1910</v>
       </c>
       <c r="B487" t="s">
-        <v>1916</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>1917</v>
+        <v>1911</v>
       </c>
       <c r="B488" t="s">
-        <v>1918</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>1919</v>
+        <v>1748</v>
       </c>
       <c r="B489" t="s">
-        <v>1920</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>1921</v>
+        <v>1915</v>
       </c>
       <c r="B490" t="s">
-        <v>1922</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>1923</v>
+        <v>1481</v>
       </c>
       <c r="B491" t="s">
-        <v>1924</v>
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B492" t="s">
+        <v>1918</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>2426</v>
+        <v>1919</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1920</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>1191</v>
+        <v>1921</v>
       </c>
       <c r="B494" t="s">
-        <v>1934</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>1936</v>
+        <v>1923</v>
       </c>
       <c r="B495" t="s">
-        <v>1935</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B496" t="s">
-        <v>1937</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>1266</v>
-      </c>
-      <c r="B497" t="s">
-        <v>1938</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>1438</v>
+        <v>1191</v>
       </c>
       <c r="B498" t="s">
-        <v>1939</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>1260</v>
+        <v>1936</v>
       </c>
       <c r="B499" t="s">
-        <v>1940</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>282</v>
+        <v>1233</v>
       </c>
       <c r="B500" t="s">
-        <v>1941</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>1217</v>
+        <v>1266</v>
       </c>
       <c r="B501" t="s">
-        <v>1942</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1268</v>
+        <v>1438</v>
       </c>
       <c r="B502" t="s">
-        <v>1943</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1211</v>
+        <v>1260</v>
       </c>
       <c r="B503" t="s">
-        <v>1944</v>
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>282</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1941</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>2427</v>
+        <v>1217</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1942</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>1945</v>
+        <v>1268</v>
       </c>
       <c r="B506" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>1786</v>
+        <v>1211</v>
       </c>
       <c r="B507" t="s">
-        <v>1947</v>
-      </c>
-    </row>
-    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A508" t="s">
-        <v>1949</v>
-      </c>
-      <c r="B508" t="s">
-        <v>1948</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>1951</v>
-      </c>
-      <c r="B509" t="s">
-        <v>1950</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>1953</v>
+        <v>1945</v>
       </c>
       <c r="B510" t="s">
-        <v>1952</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1955</v>
+        <v>1786</v>
       </c>
       <c r="B511" t="s">
-        <v>1954</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>1956</v>
+        <v>1949</v>
       </c>
       <c r="B512" t="s">
-        <v>1957</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>1959</v>
+        <v>1951</v>
       </c>
       <c r="B513" t="s">
-        <v>1958</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>1432</v>
+        <v>1953</v>
       </c>
       <c r="B514" t="s">
-        <v>1960</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>1964</v>
+        <v>1955</v>
       </c>
       <c r="B515" t="s">
-        <v>1961</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>1963</v>
+        <v>1956</v>
       </c>
       <c r="B516" t="s">
-        <v>1962</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>1966</v>
+        <v>1959</v>
       </c>
       <c r="B517" t="s">
-        <v>1965</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>1608</v>
+        <v>1432</v>
       </c>
       <c r="B518" t="s">
-        <v>1967</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1969</v>
+        <v>1964</v>
       </c>
       <c r="B519" t="s">
-        <v>1968</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1971</v>
+        <v>1963</v>
       </c>
       <c r="B520" t="s">
-        <v>1970</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1329</v>
+        <v>1966</v>
       </c>
       <c r="B521" t="s">
-        <v>1972</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1973</v>
+        <v>1608</v>
       </c>
       <c r="B522" t="s">
-        <v>1974</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1976</v>
+        <v>1969</v>
       </c>
       <c r="B523" t="s">
-        <v>1975</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1978</v>
+        <v>1971</v>
       </c>
       <c r="B524" t="s">
-        <v>1977</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1980</v>
+        <v>1329</v>
       </c>
       <c r="B525" t="s">
-        <v>1979</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1982</v>
+        <v>1973</v>
       </c>
       <c r="B526" t="s">
-        <v>1981</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1983</v>
+        <v>1976</v>
       </c>
       <c r="B527" t="s">
-        <v>1984</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1986</v>
+        <v>1978</v>
       </c>
       <c r="B528" t="s">
-        <v>1985</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1988</v>
+        <v>1980</v>
       </c>
       <c r="B529" t="s">
-        <v>1987</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1990</v>
+        <v>1982</v>
       </c>
       <c r="B530" t="s">
-        <v>1989</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1317</v>
+        <v>1983</v>
       </c>
       <c r="B531" t="s">
-        <v>1991</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1993</v>
+        <v>1986</v>
       </c>
       <c r="B532" t="s">
-        <v>1992</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1533</v>
+        <v>1988</v>
       </c>
       <c r="B533" t="s">
-        <v>1994</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="B534" t="s">
-        <v>1996</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1998</v>
+        <v>1317</v>
       </c>
       <c r="B535" t="s">
-        <v>1997</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>2000</v>
+        <v>1993</v>
       </c>
       <c r="B536" t="s">
-        <v>1999</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>2002</v>
+        <v>1533</v>
       </c>
       <c r="B537" t="s">
-        <v>2001</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>2003</v>
+        <v>1995</v>
       </c>
       <c r="B538" t="s">
-        <v>2004</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>2006</v>
+        <v>1998</v>
       </c>
       <c r="B539" t="s">
-        <v>2005</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="B540" t="s">
-        <v>2007</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="B541" t="s">
-        <v>2009</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B542" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B543" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B544" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B545" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
         <v>2012</v>
       </c>
-      <c r="B542" t="s">
+      <c r="B546" t="s">
         <v>2011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Proxy doc_mgr calls in server
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3659" uniqueCount="2980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3675" uniqueCount="2999">
   <si>
     <t>Base Set</t>
   </si>
@@ -8972,6 +8972,63 @@
   </si>
   <si>
     <t>https://4.bp.blogspot.com/-1c0HZf76lF0/WAa1uyy88BI/AAAAAAAARpw/2zLlEOeYuJkQODf9d6CZE3aCqNiAw9ajgCLcB/s1600/img490%2B-%2BCopy%2B%25284%2529.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-tV2YRYPjBdI/WAdyOH9wM8I/AAAAAAAAebY/7N8K6YNZvWQkK2-bfNkXQ-kW4SR2dAf0ACLcB/s1600/2016%2BChachi%2B%252368%2BERA%2BLeaders%2B-%2BEickhoff%2B%2526%2BHellickson.jpg</t>
+  </si>
+  <si>
+    <t>Matt Wieters</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-RH42DSY4Bsc/WAf5bVmNvmI/AAAAAAABo-g/wpUDUiNaPrIJfcIOM5C43vAcQV_eXfpGwCLcB/s1600/Wieters.jpg</t>
+  </si>
+  <si>
+    <t>1927 New York Yankees</t>
+  </si>
+  <si>
+    <t>http://www.sportscollectorsdaily.com/wp-content/uploads/2016/10/1927-Yankees-1024x815.jpg</t>
+  </si>
+  <si>
+    <t>Braves - Murphy, Mattheews</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-78gt1TTOYJk/WAed9dZ1XdI/AAAAAAAAQSc/1NtqU_h1gAgsgsJBXoDJlqx1HydQvSO8gCLcB/s1600/MARK%2BHOYLE%2B001.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-3sDVf-Tg74A/VqY0oOzUCfI/AAAAAAAA5Dg/wkiwNBYKHgw6N409ldaRcfmU4TaIGeLsgCPcB/s1600/20160125_093035.jpg</t>
+  </si>
+  <si>
+    <t>Odubbel Herrera All Star</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-svCq7RRjB54/WAowt6OpaqI/AAAAAAAAgSw/s4qcYVy8JIo0u7Jn4cF0LJT7wv8e8TE4gCEw/s1600/herrera.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-nbumESbs3kM/WAe-bmyPi9I/AAAAAAAAecA/0vw0qdU2x4UCg3rr_gKYGV7FeGhHIwRzgCLcB/s1600/2016%2BChachi%2B%252369%2BPitching%2BLeaders%2B-%2BHellickson%252C%2BEickhoff%252C%2BVelaseuz.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-hBt_ZkTlzoo/WAuVL1mYNYI/AAAAAAAAecw/7CmjHXEkv2Aehp6Uqi29Oiphw8-V4ghSwCLcB/s1600/2016%2BChachi%2B%252370%2BStrikeout%2BLeaders%2B-%2BEickhoff%252C%2BHellickson%252C%2BVelasquez.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-LIcdB6BOQ5Y/WAuasYRpd8I/AAAAAAAAedQ/bAN26tzvxUMBbyyAlU058q89FfAMqkDrACLcB/s1600/2016%2BChachi%2B%252371%2BLeading%2BFiremen%2B-%2BGomez%252C%2BNeris%252C%2BMariot.jpg</t>
+  </si>
+  <si>
+    <t>https://blowoutbuzz.files.wordpress.com/2016/10/2016-panini-black-friday-durant.jpg</t>
+  </si>
+  <si>
+    <t>Kevin Durant Black Friday</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-l7-NrtX5nlg/WAvYfBI-CDI/AAAAAAAAQVU/gKEm8oyhvlAHM0U_v1RsfM3E25_OjPzqACEw/s1600/WACKY%2B064%2B5.jpg</t>
+  </si>
+  <si>
+    <t>Mitch Williams Fleer Ultra</t>
+  </si>
+  <si>
+    <t>Pete Rose 69 Deckle Edge</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/--8O5h8tgiKw/WAqRoIlolDI/AAAAAAAAQUQ/xhtgioV2pwcIPY7b-qvBM1TV9Gp-adHdQCLcB/s1600/JAX%2BODDBALLS%2B001%2B2.jpg</t>
   </si>
 </sst>
 </file>
@@ -9341,10 +9398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <pane ySplit="4800" topLeftCell="A33"/>
-      <selection activeCell="B71" sqref="B71"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78:XFD82"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9923,7 +9978,7 @@
         <v>2826</v>
       </c>
       <c r="B72" t="s">
-        <v>2399</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -9931,7 +9986,7 @@
         <v>2827</v>
       </c>
       <c r="B73" t="s">
-        <v>2399</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -9939,7 +9994,7 @@
         <v>2828</v>
       </c>
       <c r="B74" t="s">
-        <v>2399</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -9947,7 +10002,7 @@
         <v>2829</v>
       </c>
       <c r="B75" t="s">
-        <v>2399</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -17448,10 +17503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B653"/>
+  <dimension ref="A1:B655"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="B395" sqref="B395"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="B313" sqref="B313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17777,6 +17832,14 @@
         <v>2952</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2981</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2982</v>
+      </c>
+    </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2386</v>
@@ -18614,6 +18677,14 @@
         <v>2794</v>
       </c>
     </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>2988</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2989</v>
+      </c>
+    </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>2414</v>
@@ -19395,6 +19466,14 @@
         <v>2977</v>
       </c>
     </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B252" t="s">
+        <v>2995</v>
+      </c>
+    </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>2387</v>
@@ -19858,2442 +19937,2482 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>2491</v>
+        <v>2997</v>
       </c>
       <c r="B313" t="s">
-        <v>2492</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>2497</v>
+        <v>2491</v>
       </c>
       <c r="B314" t="s">
-        <v>2498</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>2501</v>
+        <v>2497</v>
       </c>
       <c r="B315" t="s">
-        <v>2502</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="B316" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
       <c r="B317" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="B318" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>2515</v>
+        <v>2507</v>
       </c>
       <c r="B319" t="s">
-        <v>2516</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="B320" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>2523</v>
+        <v>2517</v>
       </c>
       <c r="B321" t="s">
-        <v>2524</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="B322" t="s">
-        <v>2526</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>2529</v>
+        <v>2525</v>
       </c>
       <c r="B323" t="s">
-        <v>2530</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>2537</v>
+        <v>2529</v>
       </c>
       <c r="B324" t="s">
-        <v>2538</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="B325" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="B326" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>2563</v>
+        <v>2541</v>
       </c>
       <c r="B327" t="s">
-        <v>2561</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>2560</v>
+        <v>2563</v>
       </c>
       <c r="B328" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>2576</v>
+        <v>2560</v>
       </c>
       <c r="B329" t="s">
-        <v>2577</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="B330" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="B331" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>2594</v>
+        <v>2580</v>
       </c>
       <c r="B332" t="s">
-        <v>2595</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>2598</v>
+        <v>2594</v>
       </c>
       <c r="B333" t="s">
-        <v>2599</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>2651</v>
+        <v>2598</v>
       </c>
       <c r="B334" t="s">
-        <v>2650</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>1388</v>
+        <v>2651</v>
       </c>
       <c r="B335" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>2653</v>
+        <v>1388</v>
       </c>
       <c r="B336" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="B337" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>2660</v>
+        <v>2655</v>
       </c>
       <c r="B338" t="s">
-        <v>2659</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>2671</v>
+        <v>2660</v>
       </c>
       <c r="B339" t="s">
-        <v>2672</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
       <c r="B340" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>2678</v>
+        <v>2673</v>
       </c>
       <c r="B341" t="s">
-        <v>2677</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>2746</v>
+        <v>2678</v>
       </c>
       <c r="B342" t="s">
-        <v>2747</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>2771</v>
+        <v>2746</v>
       </c>
       <c r="B343" t="s">
-        <v>2772</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>2799</v>
+        <v>2771</v>
       </c>
       <c r="B344" t="s">
-        <v>2800</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>2802</v>
+        <v>2799</v>
       </c>
       <c r="B345" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>2814</v>
+        <v>2802</v>
       </c>
       <c r="B346" t="s">
-        <v>2815</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>2855</v>
+        <v>2814</v>
       </c>
       <c r="B347" t="s">
-        <v>2856</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="B348" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="B349" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>2863</v>
+        <v>2859</v>
       </c>
       <c r="B350" t="s">
-        <v>2864</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="B351" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>2870</v>
+        <v>2865</v>
       </c>
       <c r="B352" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>2901</v>
+        <v>2870</v>
       </c>
       <c r="B353" t="s">
-        <v>2902</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>2904</v>
+        <v>2901</v>
       </c>
       <c r="B354" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="B355" t="s">
-        <v>2906</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="B356" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="B357" t="s">
-        <v>2911</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="B358" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>2914</v>
+        <v>2910</v>
       </c>
       <c r="B359" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="B360" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>2919</v>
+        <v>2915</v>
       </c>
       <c r="B361" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>2918</v>
+        <v>2919</v>
       </c>
       <c r="B362" t="s">
-        <v>2922</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="B363" t="s">
-        <v>2920</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>1889</v>
+        <v>2921</v>
       </c>
       <c r="B364" t="s">
-        <v>2923</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>2925</v>
+        <v>1889</v>
       </c>
       <c r="B365" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="B366" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="B367" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
       <c r="B368" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="B369" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="B370" t="s">
-        <v>2935</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="B371" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>2939</v>
+        <v>2936</v>
       </c>
       <c r="B372" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="B373" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="B374" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="B375" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="B376" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="B377" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>2953</v>
+        <v>2949</v>
       </c>
       <c r="B378" t="s">
-        <v>2954</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="B379" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="B380" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>2019</v>
+        <v>2957</v>
       </c>
       <c r="B381" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>2036</v>
+        <v>2019</v>
       </c>
       <c r="B382" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>2970</v>
+        <v>2036</v>
       </c>
       <c r="B383" t="s">
-        <v>2971</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>2972</v>
+        <v>2970</v>
       </c>
       <c r="B384" t="s">
-        <v>2973</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
+        <v>2972</v>
+      </c>
+      <c r="B385" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
         <v>2975</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B386" t="s">
         <v>2974</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
-        <v>2447</v>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>2983</v>
+      </c>
+      <c r="B387" t="s">
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>2985</v>
+      </c>
+      <c r="B388" t="s">
+        <v>2986</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>2354</v>
-      </c>
-      <c r="B392" t="s">
-        <v>2355</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>2372</v>
+        <v>2354</v>
       </c>
       <c r="B393" t="s">
-        <v>2373</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>2965</v>
+        <v>2372</v>
       </c>
       <c r="B394" t="s">
-        <v>2964</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
+        <v>2994</v>
+      </c>
+      <c r="B395" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B396" t="s">
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
         <v>2978</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B397" t="s">
         <v>2979</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" t="s">
-        <v>2809</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" t="s">
-        <v>2810</v>
-      </c>
-      <c r="B402" t="s">
-        <v>2811</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>2812</v>
-      </c>
-      <c r="B403" t="s">
-        <v>2813</v>
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B404" t="s">
+        <v>2811</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>2867</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B406" t="s">
-        <v>2868</v>
+        <v>2812</v>
+      </c>
+      <c r="B405" t="s">
+        <v>2813</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>2118</v>
-      </c>
-      <c r="B407" t="s">
-        <v>2117</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>1543</v>
+        <v>1982</v>
       </c>
       <c r="B408" t="s">
-        <v>1544</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>1578</v>
+        <v>2118</v>
       </c>
       <c r="B409" t="s">
-        <v>2871</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>1972</v>
+        <v>1543</v>
       </c>
       <c r="B410" t="s">
-        <v>2872</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>1936</v>
+        <v>1578</v>
       </c>
       <c r="B411" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>2875</v>
+        <v>1972</v>
       </c>
       <c r="B412" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>2877</v>
+        <v>1936</v>
       </c>
       <c r="B413" t="s">
-        <v>2876</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>1593</v>
+        <v>2875</v>
       </c>
       <c r="B414" t="s">
-        <v>2878</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>2880</v>
+        <v>2877</v>
       </c>
       <c r="B415" t="s">
-        <v>2879</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>2882</v>
+        <v>1593</v>
       </c>
       <c r="B416" t="s">
-        <v>2881</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>1402</v>
+        <v>2880</v>
       </c>
       <c r="B417" t="s">
-        <v>2883</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>2885</v>
+        <v>2882</v>
       </c>
       <c r="B418" t="s">
-        <v>2884</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>2887</v>
+        <v>1402</v>
       </c>
       <c r="B419" t="s">
-        <v>2886</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>2888</v>
+        <v>2885</v>
       </c>
       <c r="B420" t="s">
-        <v>2889</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>1460</v>
+        <v>2887</v>
       </c>
       <c r="B421" t="s">
-        <v>2890</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>2028</v>
+        <v>2888</v>
       </c>
       <c r="B422" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>1299</v>
+        <v>1460</v>
       </c>
       <c r="B423" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>2893</v>
+        <v>2028</v>
       </c>
       <c r="B424" t="s">
-        <v>2894</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>1965</v>
+        <v>1299</v>
       </c>
       <c r="B425" t="s">
-        <v>2895</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>2896</v>
+        <v>2893</v>
       </c>
       <c r="B426" t="s">
-        <v>2897</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>2545</v>
+        <v>1965</v>
       </c>
       <c r="B427" t="s">
-        <v>2898</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>2899</v>
+        <v>2896</v>
       </c>
       <c r="B428" t="s">
-        <v>2900</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>1597</v>
+        <v>2545</v>
       </c>
       <c r="B429" t="s">
-        <v>2471</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B430" t="s">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B431" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
         <v>2170</v>
       </c>
-      <c r="B430" t="s">
+      <c r="B432" t="s">
         <v>2171</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B434" t="s">
-        <v>1545</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>1547</v>
-      </c>
-      <c r="B435" t="s">
-        <v>1546</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>1549</v>
+        <v>1455</v>
       </c>
       <c r="B436" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>1551</v>
+        <v>1547</v>
       </c>
       <c r="B437" t="s">
-        <v>1550</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>1553</v>
+        <v>1549</v>
       </c>
       <c r="B438" t="s">
-        <v>1552</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="B439" t="s">
-        <v>1554</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>1482</v>
+        <v>1553</v>
       </c>
       <c r="B440" t="s">
-        <v>1556</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="B441" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>1606</v>
+        <v>1482</v>
       </c>
       <c r="B442" t="s">
-        <v>1607</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="B443" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>1562</v>
+        <v>1606</v>
       </c>
       <c r="B444" t="s">
-        <v>1561</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="B445" t="s">
-        <v>1563</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>1566</v>
+        <v>1562</v>
       </c>
       <c r="B446" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="B447" t="s">
-        <v>1568</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>1570</v>
+        <v>1566</v>
       </c>
       <c r="B448" t="s">
-        <v>1569</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>1571</v>
+        <v>1567</v>
       </c>
       <c r="B449" t="s">
-        <v>1572</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>1575</v>
+        <v>1570</v>
       </c>
       <c r="B450" t="s">
-        <v>1573</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="B451" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="B452" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>1388</v>
+        <v>1574</v>
       </c>
       <c r="B453" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="B454" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>1583</v>
+        <v>1388</v>
       </c>
       <c r="B455" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
       <c r="B456" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="B457" t="s">
-        <v>1586</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="B458" t="s">
-        <v>1588</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="B459" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="B460" t="s">
-        <v>1592</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="B461" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="B462" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="B463" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="B464" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="B465" t="s">
-        <v>1604</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B467" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
         <v>1603</v>
       </c>
-      <c r="B466" t="s">
+      <c r="B468" t="s">
         <v>1605</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A469" t="s">
-        <v>2472</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A470" t="s">
-        <v>2473</v>
-      </c>
-      <c r="B470" t="s">
-        <v>2474</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>2475</v>
-      </c>
-      <c r="B471" t="s">
-        <v>2476</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>2477</v>
+        <v>2473</v>
       </c>
       <c r="B472" t="s">
-        <v>2478</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>2479</v>
+        <v>2475</v>
       </c>
       <c r="B473" t="s">
-        <v>2480</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
+        <v>2477</v>
+      </c>
+      <c r="B474" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B475" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
         <v>2481</v>
       </c>
-      <c r="B474" t="s">
+      <c r="B476" t="s">
         <v>2482</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A477" t="s">
-        <v>2582</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A478" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B478" t="s">
-        <v>2583</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>2584</v>
-      </c>
-      <c r="B479" t="s">
-        <v>2585</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>1589</v>
+        <v>1455</v>
       </c>
       <c r="B480" t="s">
-        <v>2586</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>1566</v>
+        <v>2584</v>
       </c>
       <c r="B481" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B482" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>1150</v>
+        <v>1566</v>
       </c>
       <c r="B483" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>1219</v>
+        <v>1602</v>
       </c>
       <c r="B484" t="s">
-        <v>2592</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>1597</v>
+        <v>1150</v>
       </c>
       <c r="B485" t="s">
-        <v>2593</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>2597</v>
+        <v>1219</v>
       </c>
       <c r="B486" t="s">
-        <v>2596</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>1593</v>
+        <v>1597</v>
       </c>
       <c r="B487" t="s">
-        <v>2600</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>1560</v>
+        <v>2597</v>
       </c>
       <c r="B488" t="s">
-        <v>2601</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="B489" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B490" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B491" t="s">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
         <v>1549</v>
       </c>
-      <c r="B490" t="s">
+      <c r="B492" t="s">
         <v>2603</v>
       </c>
     </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B496" t="s">
-        <v>1636</v>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B493" t="s">
+        <v>2987</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>1388</v>
-      </c>
-      <c r="B497" t="s">
-        <v>1637</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>1639</v>
+        <v>1520</v>
       </c>
       <c r="B498" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>1632</v>
+        <v>1388</v>
       </c>
       <c r="B499" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="B500" t="s">
-        <v>1642</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>1644</v>
+        <v>1632</v>
       </c>
       <c r="B501" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1451</v>
+        <v>1641</v>
       </c>
       <c r="B502" t="s">
-        <v>1645</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1560</v>
+        <v>1644</v>
       </c>
       <c r="B503" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>1648</v>
+        <v>1451</v>
       </c>
       <c r="B504" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>1649</v>
+        <v>1560</v>
       </c>
       <c r="B505" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="B506" t="s">
-        <v>1652</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>1653</v>
+        <v>1649</v>
       </c>
       <c r="B507" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>1655</v>
+        <v>1651</v>
       </c>
       <c r="B508" t="s">
-        <v>1656</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>2150</v>
+        <v>1653</v>
       </c>
       <c r="B509" t="s">
-        <v>2151</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>2591</v>
+        <v>1655</v>
       </c>
       <c r="B510" t="s">
-        <v>2590</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1683</v>
+        <v>2150</v>
       </c>
       <c r="B511" t="s">
-        <v>2621</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B512" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B513" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
         <v>1593</v>
       </c>
-      <c r="B512" t="s">
+      <c r="B514" t="s">
         <v>2662</v>
-      </c>
-    </row>
-    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A517" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A518" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B518" t="s">
-        <v>1657</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1447</v>
-      </c>
-      <c r="B519" t="s">
-        <v>1658</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1521</v>
+        <v>1451</v>
       </c>
       <c r="B520" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1660</v>
+        <v>1447</v>
       </c>
       <c r="B521" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1663</v>
+        <v>1521</v>
       </c>
       <c r="B522" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1639</v>
+        <v>1660</v>
       </c>
       <c r="B523" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1651</v>
+        <v>1663</v>
       </c>
       <c r="B524" t="s">
-        <v>1665</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="B525" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1667</v>
+        <v>1651</v>
       </c>
       <c r="B526" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1160</v>
+        <v>1641</v>
       </c>
       <c r="B527" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1459</v>
+        <v>1667</v>
       </c>
       <c r="B528" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1388</v>
+        <v>1160</v>
       </c>
       <c r="B529" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1632</v>
+        <v>1459</v>
       </c>
       <c r="B530" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1520</v>
+        <v>1388</v>
       </c>
       <c r="B531" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1674</v>
+        <v>1632</v>
       </c>
       <c r="B532" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1677</v>
+        <v>1520</v>
       </c>
       <c r="B533" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1679</v>
+        <v>1674</v>
       </c>
       <c r="B534" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="B535" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>1644</v>
+        <v>1679</v>
       </c>
       <c r="B536" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="B537" t="s">
-        <v>1684</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1482</v>
+        <v>1644</v>
       </c>
       <c r="B538" t="s">
-        <v>1865</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>2152</v>
+        <v>1683</v>
       </c>
       <c r="B539" t="s">
-        <v>2153</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B540" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B541" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
         <v>1699</v>
       </c>
-      <c r="B540" t="s">
+      <c r="B542" t="s">
         <v>2641</v>
-      </c>
-    </row>
-    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A543" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A544" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B544" t="s">
-        <v>1686</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B545" t="s">
-        <v>1687</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1524</v>
+        <v>1685</v>
       </c>
       <c r="B546" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1689</v>
+        <v>1523</v>
       </c>
       <c r="B547" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>1691</v>
+        <v>1524</v>
       </c>
       <c r="B548" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="B549" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1696</v>
+        <v>1691</v>
       </c>
       <c r="B550" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>1459</v>
+        <v>1693</v>
       </c>
       <c r="B551" t="s">
-        <v>1697</v>
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B552" t="s">
+        <v>1695</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A554" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B554" t="s">
-        <v>1729</v>
+        <v>1459</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1697</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B555" t="s">
-        <v>1730</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>1483</v>
+        <v>1698</v>
       </c>
       <c r="B556" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B557" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>1701</v>
+        <v>1483</v>
       </c>
       <c r="B558" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>1703</v>
+        <v>1700</v>
       </c>
       <c r="B559" t="s">
-        <v>1702</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>1667</v>
+        <v>1701</v>
       </c>
       <c r="B560" t="s">
-        <v>1747</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B561" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>1706</v>
+        <v>1667</v>
       </c>
       <c r="B562" t="s">
-        <v>1734</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="B563" t="s">
-        <v>1735</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="B564" t="s">
-        <v>1709</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>1710</v>
+        <v>1707</v>
       </c>
       <c r="B565" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>1459</v>
+        <v>1708</v>
       </c>
       <c r="B566" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>1689</v>
+        <v>1710</v>
       </c>
       <c r="B567" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1712</v>
+        <v>1459</v>
       </c>
       <c r="B568" t="s">
-        <v>1738</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>1160</v>
+        <v>1689</v>
       </c>
       <c r="B569" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="B570" t="s">
-        <v>1713</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>1696</v>
+        <v>1160</v>
       </c>
       <c r="B571" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B572" t="s">
-        <v>1741</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1717</v>
+        <v>1696</v>
       </c>
       <c r="B573" t="s">
-        <v>1716</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1693</v>
+        <v>1715</v>
       </c>
       <c r="B574" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1524</v>
+        <v>1717</v>
       </c>
       <c r="B575" t="s">
-        <v>1743</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1718</v>
+        <v>1693</v>
       </c>
       <c r="B576" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>1720</v>
+        <v>1524</v>
       </c>
       <c r="B577" t="s">
-        <v>1719</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="B578" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="B579" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>1725</v>
+        <v>1721</v>
       </c>
       <c r="B580" t="s">
-        <v>1724</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="B581" t="s">
-        <v>1746</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
       <c r="B582" t="s">
-        <v>1727</v>
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1746</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B585" t="s">
-        <v>1763</v>
+        <v>1728</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1727</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1764</v>
-      </c>
-      <c r="B586" t="s">
-        <v>1765</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1689</v>
+        <v>1762</v>
       </c>
       <c r="B587" t="s">
-        <v>1870</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1872</v>
+        <v>1764</v>
       </c>
       <c r="B588" t="s">
-        <v>1871</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1533</v>
+        <v>1689</v>
       </c>
       <c r="B589" t="s">
-        <v>1873</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1160</v>
+        <v>1872</v>
       </c>
       <c r="B590" t="s">
-        <v>1874</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1875</v>
+        <v>1533</v>
       </c>
       <c r="B591" t="s">
-        <v>1876</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1877</v>
+        <v>1160</v>
       </c>
       <c r="B592" t="s">
-        <v>1878</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1880</v>
+        <v>1875</v>
       </c>
       <c r="B593" t="s">
-        <v>1879</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1881</v>
+        <v>1877</v>
       </c>
       <c r="B594" t="s">
-        <v>1882</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1718</v>
+        <v>1880</v>
       </c>
       <c r="B595" t="s">
-        <v>1883</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>1885</v>
+        <v>1881</v>
       </c>
       <c r="B596" t="s">
-        <v>1884</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>1451</v>
+        <v>1718</v>
       </c>
       <c r="B597" t="s">
-        <v>1886</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="B598" t="s">
-        <v>1888</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1889</v>
+        <v>1451</v>
       </c>
       <c r="B599" t="s">
-        <v>1890</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>1891</v>
+        <v>1887</v>
       </c>
       <c r="B600" t="s">
-        <v>1892</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>1893</v>
+        <v>1889</v>
       </c>
       <c r="B601" t="s">
-        <v>1894</v>
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B602" t="s">
+        <v>1892</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A604" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B604" t="s">
-        <v>1904</v>
+        <v>1893</v>
+      </c>
+      <c r="B603" t="s">
+        <v>1894</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B605" t="s">
-        <v>1905</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1203</v>
+        <v>1161</v>
       </c>
       <c r="B606" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>1236</v>
+        <v>1906</v>
       </c>
       <c r="B607" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>1408</v>
+        <v>1203</v>
       </c>
       <c r="B608" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
       <c r="B609" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>252</v>
+        <v>1408</v>
       </c>
       <c r="B610" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>1187</v>
+        <v>1230</v>
       </c>
       <c r="B611" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>1238</v>
+        <v>252</v>
       </c>
       <c r="B612" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>1181</v>
+        <v>1187</v>
       </c>
       <c r="B613" t="s">
-        <v>1914</v>
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B614" t="s">
+        <v>1913</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A616" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B616" t="s">
-        <v>1916</v>
+        <v>1181</v>
+      </c>
+      <c r="B615" t="s">
+        <v>1914</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B617" t="s">
-        <v>1917</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1919</v>
+        <v>1915</v>
       </c>
       <c r="B618" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1921</v>
+        <v>1756</v>
       </c>
       <c r="B619" t="s">
-        <v>1920</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1923</v>
+        <v>1919</v>
       </c>
       <c r="B620" t="s">
-        <v>1922</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>1925</v>
+        <v>1921</v>
       </c>
       <c r="B621" t="s">
-        <v>1924</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1926</v>
+        <v>1923</v>
       </c>
       <c r="B622" t="s">
-        <v>1927</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1929</v>
+        <v>1925</v>
       </c>
       <c r="B623" t="s">
-        <v>1928</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1402</v>
+        <v>1926</v>
       </c>
       <c r="B624" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>1934</v>
+        <v>1929</v>
       </c>
       <c r="B625" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1933</v>
+        <v>1402</v>
       </c>
       <c r="B626" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="B627" t="s">
-        <v>1935</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1578</v>
+        <v>1933</v>
       </c>
       <c r="B628" t="s">
-        <v>1937</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="B629" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1941</v>
+        <v>1578</v>
       </c>
       <c r="B630" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>1299</v>
+        <v>1939</v>
       </c>
       <c r="B631" t="s">
-        <v>1942</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="B632" t="s">
-        <v>1944</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>1946</v>
+        <v>1299</v>
       </c>
       <c r="B633" t="s">
-        <v>1945</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>1948</v>
+        <v>1943</v>
       </c>
       <c r="B634" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>1950</v>
+        <v>1946</v>
       </c>
       <c r="B635" t="s">
-        <v>1949</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1952</v>
+        <v>1948</v>
       </c>
       <c r="B636" t="s">
-        <v>1951</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="B637" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>1956</v>
+        <v>1952</v>
       </c>
       <c r="B638" t="s">
-        <v>1955</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>1958</v>
+        <v>1953</v>
       </c>
       <c r="B639" t="s">
-        <v>1957</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>1960</v>
+        <v>1956</v>
       </c>
       <c r="B640" t="s">
-        <v>1959</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>1287</v>
+        <v>1958</v>
       </c>
       <c r="B641" t="s">
-        <v>1961</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="B642" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1503</v>
+        <v>1287</v>
       </c>
       <c r="B643" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="B644" t="s">
-        <v>1966</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1968</v>
+        <v>1503</v>
       </c>
       <c r="B645" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1970</v>
+        <v>1965</v>
       </c>
       <c r="B646" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>1972</v>
+        <v>1968</v>
       </c>
       <c r="B647" t="s">
-        <v>1971</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="B648" t="s">
-        <v>1974</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="B649" t="s">
-        <v>1975</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1978</v>
+        <v>1973</v>
       </c>
       <c r="B650" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="B651" t="s">
-        <v>1979</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="B652" t="s">
-        <v>1981</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B653" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B654" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
         <v>2962</v>
       </c>
-      <c r="B653" t="s">
+      <c r="B655" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chachi and bunt updates
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695"/>
   </bookViews>
   <sheets>
-    <sheet name="2016" sheetId="1" r:id="rId1"/>
-    <sheet name="1970" sheetId="13" r:id="rId2"/>
-    <sheet name="2017" sheetId="21" r:id="rId3"/>
+    <sheet name="2017" sheetId="21" r:id="rId1"/>
+    <sheet name="2016" sheetId="1" r:id="rId2"/>
+    <sheet name="1970" sheetId="13" r:id="rId3"/>
     <sheet name="Misc" sheetId="14" r:id="rId4"/>
     <sheet name="2005" sheetId="3" r:id="rId5"/>
     <sheet name="2006" sheetId="4" r:id="rId6"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3814" uniqueCount="3112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3875" uniqueCount="3143">
   <si>
     <t>Base Set</t>
   </si>
@@ -9369,6 +9369,99 @@
   </si>
   <si>
     <t>https://shlabotnikreport.files.wordpress.com/2016/11/2016-tsr-expansion40-1-carlos-ruiz.jpg?w=216&amp;h=300</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-wej1BybCOpI/V-_8z4U1s_I/AAAAAAAAeQk/c5D4X0uYNggb_8lyJ-qRW_Flh5l0oqcTgCLcB/s1600/Herrera.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-Zc8a8dLz6cI/V-_8zRWjG-I/AAAAAAAAeQQ/Je6SRf-EZ_89lglDnlxWuKnJKEABIy6AwCLcB/s1600/Altherr.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-umWxQJHDwcM/V-_8zYAAzNI/AAAAAAAAeQU/mcW3Ne9RB1wyXnLRjxuMPIsArvFEMThhwCLcB/s1600/Franco.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-YG7X9hItuY8/V-_8zpiOfdI/AAAAAAAAeQY/S9U9M01L-RUgJtEv4XZS27cl7ABkgeSIACLcB/s1600/Galvis.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-qFozyhBmkzc/V-_8zjYQQmI/AAAAAAAAeQg/xXr_zgQ3OsYSwfvSe50M9TX3p1O9SSvcQCLcB/s1600/Hernandez%2BC.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-txw4DT-5m5w/V-_8zzr1-wI/AAAAAAAAeQo/deBqMOfO6KwQ-IIfvwoTwKwe6ZVgbFHrQCLcB/s1600/Joseph.jpg</t>
+  </si>
+  <si>
+    <t>Jared Eichoff</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-h5sYX6YU-Dk/V-_8zeJvozI/AAAAAAAAeQM/IVdR03M1h9I9UlNbnjN_6nNGi5FrXwu3QCLcB/s1600/Eickhoff.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-KXpulpcYHZw/V-_80Nn34dI/AAAAAAAAeQs/xD4A9ui763cdtQo8389aFs0hL09P1v42QCLcB/s1600/Nola.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-hab4_lEAl5s/V-_80dDDGTI/AAAAAAAAeQ4/2T6dGiOnVqA5tQfG08YHXPB_Gk9xYLksQCLcB/s1600/Velasquez.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-wXbHGBrRqNs/V-_80F2SiII/AAAAAAAAeQ0/rwa_j7U8KsolAft4Mh-yYC95WRGv_fhbACLcB/s1600/Thompson.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-BJ_88jHr1mE/V-_98ORJkUI/AAAAAAAAeRA/WNDzOsNleI4d5OMYpqEBbEY9FPyhw3-TACLcB/s1600/Rupp.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-3YrjNQAsgys/V_AD0n8cdMI/AAAAAAAAeRU/l2JBa4YMmlwrQtNFyLkniqG27wizKlPcQCLcB/s1600/Alfaro.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-laVjlONrMsM/V_AEcM4P3uI/AAAAAAAAeRw/DPhtWQ2M8yIN3q1LTMSkXTpeR42lri_YgCLcB/s1600/Asche.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-3PBOzg3RA04/V_AD0_Wy-nI/AAAAAAAAeRg/GuDY7mMRwEgdWzgRoGfiVoKphGFWHu9hACLcB/s1600/Goeddel.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-O3aQZLpdQZE/V-_80DFHyYI/AAAAAAAAeQw/GgugWbMsK4Q1eVisZrdrn2ET_sxbMTq5gCLcB/s1600/Quinn.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-HLgNnuiFpsU/V_AGC9fVehI/AAAAAAAAeSI/4Yxr1R2G0GMweXhmPbZiyq87QXPxC2M5ACLcB/s1600/Araujo.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-QeOaULZ8I90/V_AGC1AfuHI/AAAAAAAAeSE/DUsEi-3tLtQ5DGMUh8ulbkU8MmF9mOXSACLcB/s1600/Asher.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-Mzt_lvk6Ml4/V_AGC4vacYI/AAAAAAAAeSM/sXLaIPYljNck2XgjaUGFfsVjpctYUv7sQCLcB/s1600/Buchanan.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-O-hA49I8bcU/V_AGDFSABwI/AAAAAAAAeSQ/WGNxYDaRZokCqyJ8BLuqM0SWcE9urwZKwCLcB/s1600/Cordero.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-jTmCj0Px_u0/V_AGDcdnPQI/AAAAAAAAeSU/x9v67fJ5gRgDUvrdAI_FwiNoESo-n2uNACLcB/s1600/Eflin.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-urGNP8QrdsU/V_AGDStHmTI/AAAAAAAAeSY/t-dzxdgyDXg0AYpo373qLkRdMjS61JwRwCLcB/s1600/Garcia.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-AcYeDOHUAqQ/V_AGDTyAapI/AAAAAAAAeSc/W01x_DTccMcttca9NOYzOsdL5QwiSTVLwCLcB/s1600/Gomez.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-LSb8b0_zsU8/V_AGDsaWmlI/AAAAAAAAeSg/uKtR7xOr-Zk8bhxf70HMjeikcuFYmZe4gCLcB/s1600/Gonzalez.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-oPdxfSm7RsA/V_AGEDYGw3I/AAAAAAAAeS0/LyxLD21_ot0xf_-PdNEBhztGdry0zMhGwCLcB/s1600/Klein.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-xtmOQplwPb0/V_AGELIjHDI/AAAAAAAAeS4/Tq0VBQ4P5_kOZ0CU4SS_4Q0jt4uZ7vrZgCLcB/s1600/Mariot.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-4bvZc1bQrbA/V_AGEHqPZMI/AAAAAAAAeS8/fNx8WjodI1QDPN7DLOK1lHMPCb0Sy5jsQCLcB/s1600/Morgan.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-u80_aR_5674/V_AGEjiodgI/AAAAAAAAeTM/nzK5ztcpaKsfdKe91sfCKYmApqVuQKTJACLcB/s1600/Neris.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-tpPhX5judOM/V_AGEobkIiI/AAAAAAAAeTI/ow_ZiG1Aje043FYLtp8GvKREpuW9UT7cwCLcB/s1600/Ramos.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-9KAK774lYSY/V_AGEhA2jfI/AAAAAAAAeTQ/j6qD0fTL6SUo6uHeFlTJelDZuvNVkm8CACLcB/s1600/Rodriguez.jpg</t>
+  </si>
+  <si>
+    <t>2017 Chachi</t>
   </si>
 </sst>
 </file>
@@ -9736,16 +9829,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="154.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -9756,1199 +9848,283 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2398</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1859</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>3112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>3113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>3114</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>2044</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>3118</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>3120</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>3036</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>2458</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>3122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>3124</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>2646</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>3128</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>2837</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>2060</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>2462</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1440</v>
+        <v>2460</v>
       </c>
       <c r="B28" t="s">
-        <v>1441</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1442</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>1443</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>1444</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>2063</v>
       </c>
       <c r="B31" t="s">
-        <v>1515</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>209</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1517</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>2044</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>2046</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2047</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>2048</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2049</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>2060</v>
-      </c>
-      <c r="B37" t="s">
-        <v>2061</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" t="s">
-        <v>2062</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>2063</v>
-      </c>
       <c r="B39" t="s">
-        <v>2064</v>
+        <v>3103</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2065</v>
+        <v>3104</v>
       </c>
       <c r="B40" t="s">
-        <v>2066</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2067</v>
+        <v>3107</v>
       </c>
       <c r="B41" t="s">
-        <v>2068</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" t="s">
-        <v>2069</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>2458</v>
-      </c>
-      <c r="B43" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>2460</v>
-      </c>
-      <c r="B44" t="s">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>2462</v>
-      </c>
-      <c r="B45" t="s">
-        <v>2463</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>130</v>
-      </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2547</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>2548</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>2567</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s">
-        <v>2568</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" t="s">
-        <v>2571</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>136</v>
-      </c>
-      <c r="B50" t="s">
-        <v>2624</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>2627</v>
-      </c>
-      <c r="B51" t="s">
-        <v>2628</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>146</v>
-      </c>
-      <c r="B52" t="s">
-        <v>2634</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>2646</v>
-      </c>
-      <c r="B53" t="s">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>215</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1895</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>201</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1902</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>203</v>
-      </c>
-      <c r="B56" t="s">
-        <v>2817</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>2821</v>
-      </c>
-      <c r="B57" t="s">
-        <v>2818</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>204</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>2822</v>
-      </c>
-      <c r="B60" t="s">
-        <v>2043</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1400</v>
-      </c>
-      <c r="B61" t="s">
-        <v>2820</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>2464</v>
-      </c>
-      <c r="B62" t="s">
-        <v>2465</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>2533</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>2534</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1861</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>2456</v>
-      </c>
-      <c r="B65" t="s">
-        <v>2457</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>2531</v>
-      </c>
-      <c r="B66" t="s">
-        <v>2532</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>2803</v>
-      </c>
-      <c r="B67" t="s">
-        <v>2804</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>2720</v>
-      </c>
-      <c r="B68" t="s">
-        <v>2721</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>2823</v>
-      </c>
-      <c r="B69" t="s">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>2824</v>
-      </c>
-      <c r="B70" t="s">
-        <v>2951</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>2825</v>
-      </c>
-      <c r="B71" t="s">
-        <v>2963</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>2826</v>
-      </c>
-      <c r="B72" t="s">
-        <v>2980</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>2827</v>
-      </c>
-      <c r="B73" t="s">
-        <v>2990</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>2828</v>
-      </c>
-      <c r="B74" t="s">
-        <v>2991</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>2829</v>
-      </c>
-      <c r="B75" t="s">
-        <v>2992</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>1147</v>
-      </c>
-      <c r="B76" t="s">
-        <v>2770</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>2058</v>
-      </c>
-      <c r="B79" t="s">
-        <v>2059</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>139</v>
-      </c>
-      <c r="B80" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>2830</v>
-      </c>
-      <c r="B81" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>2831</v>
-      </c>
-      <c r="B82" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>2050</v>
-      </c>
-      <c r="B83" t="s">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>2052</v>
-      </c>
-      <c r="B84" t="s">
-        <v>2053</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>2054</v>
-      </c>
-      <c r="B85" t="s">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>2056</v>
-      </c>
-      <c r="B86" t="s">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>2832</v>
-      </c>
-      <c r="B87" t="s">
-        <v>2841</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>2833</v>
-      </c>
-      <c r="B88" t="s">
-        <v>2842</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>2834</v>
-      </c>
-      <c r="B89" t="s">
-        <v>2843</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>2835</v>
-      </c>
-      <c r="B90" t="s">
-        <v>2844</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>2836</v>
-      </c>
-      <c r="B91" t="s">
-        <v>2845</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>140</v>
-      </c>
-      <c r="B92" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>2837</v>
-      </c>
-      <c r="B93" t="s">
-        <v>2846</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>149</v>
-      </c>
-      <c r="B94" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>150</v>
-      </c>
-      <c r="B95" t="s">
-        <v>2847</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>2838</v>
-      </c>
-      <c r="B96" t="s">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>2839</v>
-      </c>
-      <c r="B97" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>207</v>
-      </c>
-      <c r="B98" t="s">
-        <v>2850</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>2611</v>
-      </c>
-      <c r="B99" t="s">
-        <v>2851</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>2840</v>
-      </c>
-      <c r="B100" t="s">
-        <v>2852</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>132</v>
-      </c>
-      <c r="B101" t="s">
-        <v>2853</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>2612</v>
-      </c>
-      <c r="B102" t="s">
-        <v>2854</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>2816</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>27</v>
-      </c>
-      <c r="B106" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>28</v>
-      </c>
-      <c r="B107" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>29</v>
-      </c>
-      <c r="B108" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>30</v>
-      </c>
-      <c r="B109" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>31</v>
-      </c>
-      <c r="B110" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>32</v>
-      </c>
-      <c r="B111" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>33</v>
-      </c>
-      <c r="B112" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>35</v>
-      </c>
-      <c r="B117" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>36</v>
-      </c>
-      <c r="B118" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>37</v>
-      </c>
-      <c r="B119" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>38</v>
-      </c>
-      <c r="B120" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>39</v>
-      </c>
-      <c r="B121" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>40</v>
-      </c>
-      <c r="B122" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>41</v>
-      </c>
-      <c r="B123" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>42</v>
-      </c>
-      <c r="B124" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>43</v>
-      </c>
-      <c r="B125" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>44</v>
-      </c>
-      <c r="B126" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>45</v>
-      </c>
-      <c r="B127" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>46</v>
-      </c>
-      <c r="B128" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>47</v>
-      </c>
-      <c r="B129" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>48</v>
-      </c>
-      <c r="B130" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>49</v>
-      </c>
-      <c r="B131" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>50</v>
-      </c>
-      <c r="B132" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>51</v>
-      </c>
-      <c r="B133" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>52</v>
-      </c>
-      <c r="B134" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>53</v>
-      </c>
-      <c r="B135" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>54</v>
-      </c>
-      <c r="B136" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>55</v>
-      </c>
-      <c r="B137" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>56</v>
-      </c>
-      <c r="B138" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>2819</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>58</v>
-      </c>
-      <c r="B140" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>59</v>
-      </c>
-      <c r="B141" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>60</v>
-      </c>
-      <c r="B142" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>61</v>
-      </c>
-      <c r="B143" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>62</v>
-      </c>
-      <c r="B144" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>63</v>
-      </c>
-      <c r="B145" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>64</v>
-      </c>
-      <c r="B146" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>65</v>
-      </c>
-      <c r="B147" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>66</v>
-      </c>
-      <c r="B148" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>67</v>
-      </c>
-      <c r="B149" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>86</v>
-      </c>
-      <c r="B152" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>87</v>
-      </c>
-      <c r="B153" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>88</v>
-      </c>
-      <c r="B154" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>89</v>
-      </c>
-      <c r="B155" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>90</v>
-      </c>
-      <c r="B156" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>91</v>
-      </c>
-      <c r="B157" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>2466</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>2044</v>
-      </c>
-      <c r="B164" t="s">
-        <v>2467</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>8</v>
-      </c>
-      <c r="B165" t="s">
-        <v>2790</v>
+        <v>3109</v>
       </c>
     </row>
   </sheetData>
@@ -17856,16 +17032,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="154.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17877,762 +17053,1198 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2411</v>
+      <c r="A2" s="1" t="s">
+        <v>2398</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1859</v>
+      </c>
       <c r="B3" t="s">
-        <v>1445</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1766</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2707</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1677</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2687</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1447</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>1449</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1451</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>1453</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1455</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1458</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1459</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>1461</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1464</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>1465</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1482</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>1481</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1518</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>1528</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1519</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>1529</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1520</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>1530</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1521</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>1531</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1866</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>1867</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1648</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>2003</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2004</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>2005</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1639</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>2006</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1641</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>2007</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1632</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>2008</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1644</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>2009</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2016</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>2017</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2453</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>2454</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1712</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>2544</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1663</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>2566</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1699</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>2622</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1691</v>
+        <v>1440</v>
       </c>
       <c r="B28" t="s">
-        <v>2631</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1667</v>
+        <v>1442</v>
       </c>
       <c r="B29" t="s">
-        <v>2661</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2675</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>2676</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2683</v>
+        <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>2684</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2700</v>
+        <v>144</v>
       </c>
       <c r="B32" t="s">
-        <v>2701</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>2702</v>
+        <v>209</v>
       </c>
       <c r="B33" t="s">
-        <v>2703</v>
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2045</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2046</v>
+      </c>
       <c r="B35" t="s">
-        <v>1446</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1558</v>
+        <v>2048</v>
       </c>
       <c r="B36" t="s">
-        <v>2018</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>2019</v>
+        <v>2060</v>
       </c>
       <c r="B37" t="s">
-        <v>2020</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1161</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
-        <v>2021</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2022</v>
+        <v>2063</v>
       </c>
       <c r="B39" t="s">
-        <v>2023</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2024</v>
+        <v>2065</v>
       </c>
       <c r="B40" t="s">
-        <v>2025</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2026</v>
+        <v>2067</v>
       </c>
       <c r="B41" t="s">
-        <v>2027</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1448</v>
+        <v>131</v>
       </c>
       <c r="B42" t="s">
-        <v>1450</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1452</v>
+        <v>2458</v>
       </c>
       <c r="B43" t="s">
-        <v>1454</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1456</v>
+        <v>2460</v>
       </c>
       <c r="B44" t="s">
-        <v>1457</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1460</v>
+        <v>2462</v>
       </c>
       <c r="B45" t="s">
-        <v>1462</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1463</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>1466</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1483</v>
+        <v>2547</v>
       </c>
       <c r="B47" t="s">
-        <v>1484</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1522</v>
+        <v>2567</v>
       </c>
       <c r="B48" t="s">
-        <v>1525</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1523</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>1526</v>
+        <v>2571</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1524</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>1527</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1533</v>
+        <v>2627</v>
       </c>
       <c r="B51" t="s">
-        <v>1534</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1771</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>1773</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1772</v>
+        <v>2646</v>
       </c>
       <c r="B53" t="s">
-        <v>1774</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1714</v>
+        <v>215</v>
       </c>
       <c r="B54" t="s">
-        <v>1848</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1845</v>
+        <v>201</v>
       </c>
       <c r="B55" t="s">
-        <v>1849</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1846</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
-        <v>1850</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1847</v>
+        <v>2821</v>
       </c>
       <c r="B57" t="s">
-        <v>1851</v>
+        <v>2818</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>2010</v>
+        <v>204</v>
       </c>
       <c r="B58" t="s">
-        <v>2011</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2012</v>
+        <v>1541</v>
       </c>
       <c r="B59" t="s">
-        <v>2013</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2014</v>
+        <v>2822</v>
       </c>
       <c r="B60" t="s">
-        <v>2015</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2028</v>
+        <v>1400</v>
       </c>
       <c r="B61" t="s">
-        <v>2029</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>2030</v>
+        <v>2464</v>
       </c>
       <c r="B62" t="s">
-        <v>2031</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2032</v>
+        <v>2533</v>
       </c>
       <c r="B63" t="s">
-        <v>2033</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>2034</v>
+        <v>2534</v>
       </c>
       <c r="B64" t="s">
-        <v>2035</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>2036</v>
+        <v>2456</v>
       </c>
       <c r="B65" t="s">
-        <v>2037</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>2038</v>
+        <v>2531</v>
       </c>
       <c r="B66" t="s">
-        <v>2039</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>2040</v>
+        <v>2803</v>
       </c>
       <c r="B67" t="s">
-        <v>2041</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1725</v>
+        <v>2720</v>
       </c>
       <c r="B68" t="s">
-        <v>2448</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>2449</v>
+        <v>2823</v>
       </c>
       <c r="B69" t="s">
-        <v>2450</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2451</v>
+        <v>2824</v>
       </c>
       <c r="B70" t="s">
-        <v>2452</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1581</v>
+        <v>2825</v>
       </c>
       <c r="B71" t="s">
-        <v>2455</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1593</v>
+        <v>2826</v>
       </c>
       <c r="B72" t="s">
-        <v>2543</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>2545</v>
+        <v>2827</v>
       </c>
       <c r="B73" t="s">
-        <v>2546</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>2564</v>
+        <v>2828</v>
       </c>
       <c r="B74" t="s">
-        <v>2565</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>1718</v>
+        <v>2829</v>
       </c>
       <c r="B75" t="s">
-        <v>2623</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>2632</v>
+        <v>1147</v>
       </c>
       <c r="B76" t="s">
-        <v>2633</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>2642</v>
-      </c>
-      <c r="B77" t="s">
-        <v>2643</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>2685</v>
-      </c>
       <c r="B78" t="s">
-        <v>2686</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>2688</v>
+        <v>2058</v>
       </c>
       <c r="B79" t="s">
-        <v>2689</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>2690</v>
+        <v>139</v>
       </c>
       <c r="B80" t="s">
-        <v>2691</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>2693</v>
+        <v>2830</v>
       </c>
       <c r="B81" t="s">
-        <v>2692</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>1595</v>
+        <v>2831</v>
       </c>
       <c r="B82" t="s">
-        <v>2694</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>2597</v>
+        <v>2050</v>
       </c>
       <c r="B83" t="s">
-        <v>2695</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>2697</v>
+        <v>2052</v>
       </c>
       <c r="B84" t="s">
-        <v>2696</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>2698</v>
+        <v>2054</v>
       </c>
       <c r="B85" t="s">
-        <v>2699</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>2705</v>
+        <v>2056</v>
       </c>
       <c r="B86" t="s">
-        <v>2704</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>1620</v>
+        <v>2832</v>
       </c>
       <c r="B87" t="s">
-        <v>2706</v>
+        <v>2841</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>2743</v>
+        <v>2833</v>
       </c>
       <c r="B88" t="s">
-        <v>2742</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1571</v>
+        <v>2834</v>
       </c>
       <c r="B89" t="s">
-        <v>2773</v>
+        <v>2843</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>2775</v>
+        <v>2835</v>
       </c>
       <c r="B90" t="s">
-        <v>2774</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>2777</v>
+        <v>2836</v>
       </c>
       <c r="B91" t="s">
-        <v>2776</v>
+        <v>2845</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1585</v>
+        <v>140</v>
       </c>
       <c r="B92" t="s">
-        <v>2778</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>2779</v>
+        <v>2837</v>
       </c>
       <c r="B93" t="s">
-        <v>2780</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>2781</v>
+        <v>149</v>
       </c>
       <c r="B94" t="s">
-        <v>2782</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>2783</v>
+        <v>150</v>
       </c>
       <c r="B95" t="s">
-        <v>2784</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1696</v>
+        <v>2838</v>
       </c>
       <c r="B96" t="s">
-        <v>2785</v>
+        <v>2848</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>2786</v>
+        <v>2839</v>
       </c>
       <c r="B97" t="s">
-        <v>2787</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>2788</v>
+        <v>207</v>
       </c>
       <c r="B98" t="s">
-        <v>2789</v>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>2611</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>2840</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>132</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>2612</v>
+      </c>
+      <c r="B102" t="s">
+        <v>2854</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>27</v>
+      </c>
+      <c r="B106" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>32</v>
+      </c>
+      <c r="B111" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>33</v>
+      </c>
+      <c r="B112" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>35</v>
+      </c>
+      <c r="B117" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>36</v>
+      </c>
+      <c r="B118" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>37</v>
+      </c>
+      <c r="B119" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>39</v>
+      </c>
+      <c r="B121" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>40</v>
+      </c>
+      <c r="B122" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>41</v>
+      </c>
+      <c r="B123" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>42</v>
+      </c>
+      <c r="B124" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>43</v>
+      </c>
+      <c r="B125" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>44</v>
+      </c>
+      <c r="B126" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>45</v>
+      </c>
+      <c r="B127" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>46</v>
+      </c>
+      <c r="B128" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>47</v>
+      </c>
+      <c r="B129" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>48</v>
+      </c>
+      <c r="B130" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>49</v>
+      </c>
+      <c r="B131" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>50</v>
+      </c>
+      <c r="B132" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>51</v>
+      </c>
+      <c r="B133" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>52</v>
+      </c>
+      <c r="B134" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>53</v>
+      </c>
+      <c r="B135" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>54</v>
+      </c>
+      <c r="B136" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>55</v>
+      </c>
+      <c r="B137" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>56</v>
+      </c>
+      <c r="B138" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>58</v>
+      </c>
+      <c r="B140" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>59</v>
+      </c>
+      <c r="B141" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>60</v>
+      </c>
+      <c r="B142" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>61</v>
+      </c>
+      <c r="B143" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>62</v>
+      </c>
+      <c r="B144" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>63</v>
+      </c>
+      <c r="B145" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>64</v>
+      </c>
+      <c r="B146" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>65</v>
+      </c>
+      <c r="B147" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>66</v>
+      </c>
+      <c r="B148" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>67</v>
+      </c>
+      <c r="B149" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>86</v>
+      </c>
+      <c r="B152" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>87</v>
+      </c>
+      <c r="B153" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>88</v>
+      </c>
+      <c r="B154" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>89</v>
+      </c>
+      <c r="B155" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>90</v>
+      </c>
+      <c r="B156" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>91</v>
+      </c>
+      <c r="B157" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B164" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165" t="s">
+        <v>2790</v>
       </c>
     </row>
   </sheetData>
@@ -18766,62 +18378,783 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B13"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1438</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2017</v>
+      <c r="A2" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1445</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1766</v>
+      </c>
       <c r="B4" t="s">
-        <v>3103</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3104</v>
+        <v>1677</v>
       </c>
       <c r="B5" t="s">
-        <v>3105</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3107</v>
+        <v>1447</v>
       </c>
       <c r="B6" t="s">
-        <v>3106</v>
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1465</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1482</v>
+      </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>1518</v>
       </c>
       <c r="B12" t="s">
-        <v>3108</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>1519</v>
       </c>
       <c r="B13" t="s">
-        <v>3109</v>
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2675</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2700</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2702</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2019</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>2038</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>2449</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>2451</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B71" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>2564</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>2688</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>2693</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2692</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>2597</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>2705</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>2743</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2774</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>2777</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2782</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2789</v>
       </c>
     </row>
   </sheetData>
@@ -18833,7 +19166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+    <sheetView topLeftCell="A271" workbookViewId="0">
       <selection activeCell="B289" sqref="B289"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More chachi and bunt spreadsheet updates
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="21" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3875" uniqueCount="3143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3889" uniqueCount="3154">
   <si>
     <t>Base Set</t>
   </si>
@@ -9462,6 +9462,39 @@
   </si>
   <si>
     <t>2017 Chachi</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-qbSjKZNE-Es/WCzr7wlFUrI/AAAAAAAAlIk/ToGbZMoBnVQA8NF92u6K-T4Xf3vxTrkTQCLcB/s1600/imh992.jpg</t>
+  </si>
+  <si>
+    <t>Pat Neshek 2011 Topps Padres</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-pNke_dxqUeA/WCzr8YPv5GI/AAAAAAAAlIw/9AG4Q_sBAfUiqIBGwF90zgB5PwcV2fySwCLcB/s1600/imh994.jpg</t>
+  </si>
+  <si>
+    <t>Anthony Rizzo 2011 Finest</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-tSVsiozwNTA/WCzr8tzaV-I/AAAAAAAAlI4/TDplSZOZOe8xlRqBaI2JffwREJ58Gi8_gCLcB/s1600/imh995.jpg</t>
+  </si>
+  <si>
+    <t>Tadahito Iguchi 2008 Topps Heritage</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-hgRHvoGDQaM/WC5KVcNFtMI/AAAAAAABpwc/YsYl0_MZ2QMn26CnAgFKCQBrmEEdq1xxwCLcB/s1600/hhn-1%253D1.jpg</t>
+  </si>
+  <si>
+    <t>Enrique Hernandez</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-Nqia8ccHhxM/WC8AlEepu7I/AAAAAAAAes8/AaLvgKxp3F4oSMWtk_wKwA3r3gWXYk_uwCLcB/s1600/2017%2BChachi%2BDepartures%2B%25234%2BMorton.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-4rreGmUhQBw/WC8AlAJHNiI/AAAAAAAAes4/5ssQJAvj6J4SE5ksxAsbDRUuO2dFfdi6wCLcB/s1600/2017%2BChachi%2BDepartures%2B%25231%2BSchuster.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-Ebx0MoFkEqY/WC6DyZMCNVI/AAAAAAABpww/R3BsPS6xe5MEXuVz8LI2S-kndFHsXxfQACLcB/s1600/Wise%2B71T.jpg</t>
   </si>
 </sst>
 </file>
@@ -9829,10 +9862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10125,6 +10158,22 @@
       </c>
       <c r="B48" t="s">
         <v>3109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>2627</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3152</v>
       </c>
     </row>
   </sheetData>
@@ -19164,10 +19213,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B721"/>
+  <dimension ref="A1:B728"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView tabSelected="1" topLeftCell="A586" workbookViewId="0">
+      <selection activeCell="B616" sqref="B616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19541,6 +19590,14 @@
         <v>3047</v>
       </c>
     </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3150</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3149</v>
+      </c>
+    </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>2386</v>
@@ -22721,1876 +22778,1908 @@
         <v>3049</v>
       </c>
     </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>3144</v>
+      </c>
+      <c r="B457" t="s">
+        <v>3143</v>
+      </c>
+    </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>2447</v>
+        <v>3146</v>
+      </c>
+      <c r="B458" t="s">
+        <v>3145</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B459" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
         <v>2354</v>
       </c>
-      <c r="B459" t="s">
+      <c r="B466" t="s">
         <v>2355</v>
       </c>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A460" t="s">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
         <v>2372</v>
       </c>
-      <c r="B460" t="s">
+      <c r="B467" t="s">
         <v>2373</v>
       </c>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A461" t="s">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
         <v>2994</v>
       </c>
-      <c r="B461" t="s">
+      <c r="B468" t="s">
         <v>2993</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A462" t="s">
-        <v>2965</v>
-      </c>
-      <c r="B462" t="s">
-        <v>2964</v>
-      </c>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A463" t="s">
-        <v>2978</v>
-      </c>
-      <c r="B463" t="s">
-        <v>2979</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>2809</v>
+        <v>2965</v>
+      </c>
+      <c r="B469" t="s">
+        <v>2964</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>2810</v>
+        <v>2978</v>
       </c>
       <c r="B470" t="s">
-        <v>2811</v>
-      </c>
-    </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>2812</v>
-      </c>
-      <c r="B471" t="s">
-        <v>2813</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A473" t="s">
-        <v>2867</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A474" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B474" t="s">
-        <v>2868</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A475" t="s">
-        <v>2118</v>
-      </c>
-      <c r="B475" t="s">
-        <v>2117</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>1543</v>
-      </c>
-      <c r="B476" t="s">
-        <v>1544</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>1578</v>
+        <v>2810</v>
       </c>
       <c r="B477" t="s">
-        <v>2871</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>1972</v>
+        <v>2812</v>
       </c>
       <c r="B478" t="s">
-        <v>2872</v>
-      </c>
-    </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A479" t="s">
-        <v>1936</v>
-      </c>
-      <c r="B479" t="s">
-        <v>2873</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>2875</v>
-      </c>
-      <c r="B480" t="s">
-        <v>2874</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>2877</v>
+        <v>1982</v>
       </c>
       <c r="B481" t="s">
-        <v>2876</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1593</v>
+        <v>2118</v>
       </c>
       <c r="B482" t="s">
-        <v>2878</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>2880</v>
+        <v>1543</v>
       </c>
       <c r="B483" t="s">
-        <v>2879</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>2882</v>
+        <v>1578</v>
       </c>
       <c r="B484" t="s">
-        <v>2881</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>1402</v>
+        <v>1972</v>
       </c>
       <c r="B485" t="s">
-        <v>2883</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>2885</v>
+        <v>1936</v>
       </c>
       <c r="B486" t="s">
-        <v>2884</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>2887</v>
+        <v>2875</v>
       </c>
       <c r="B487" t="s">
-        <v>2886</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>2888</v>
+        <v>2877</v>
       </c>
       <c r="B488" t="s">
-        <v>2889</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B489" t="s">
-        <v>2890</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>2028</v>
+        <v>2880</v>
       </c>
       <c r="B490" t="s">
-        <v>2891</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>1299</v>
+        <v>2882</v>
       </c>
       <c r="B491" t="s">
-        <v>2892</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>2893</v>
+        <v>1402</v>
       </c>
       <c r="B492" t="s">
-        <v>2894</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>1965</v>
+        <v>2885</v>
       </c>
       <c r="B493" t="s">
-        <v>2895</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>2896</v>
+        <v>2887</v>
       </c>
       <c r="B494" t="s">
-        <v>2897</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>2545</v>
+        <v>2888</v>
       </c>
       <c r="B495" t="s">
-        <v>2898</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>2899</v>
+        <v>1460</v>
       </c>
       <c r="B496" t="s">
-        <v>2900</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>1597</v>
+        <v>2028</v>
       </c>
       <c r="B497" t="s">
-        <v>2471</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>2170</v>
+        <v>1299</v>
       </c>
       <c r="B498" t="s">
-        <v>2171</v>
+        <v>2892</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B499" t="s">
+        <v>2894</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B500" t="s">
+        <v>2895</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>2389</v>
+        <v>2896</v>
+      </c>
+      <c r="B501" t="s">
+        <v>2897</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1455</v>
+        <v>2545</v>
       </c>
       <c r="B502" t="s">
-        <v>1545</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1547</v>
+        <v>2899</v>
       </c>
       <c r="B503" t="s">
-        <v>1546</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>1549</v>
+        <v>1597</v>
       </c>
       <c r="B504" t="s">
-        <v>1548</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>1551</v>
+        <v>2170</v>
       </c>
       <c r="B505" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A506" t="s">
-        <v>1553</v>
-      </c>
-      <c r="B506" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A507" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B507" t="s">
-        <v>1554</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>1482</v>
-      </c>
-      <c r="B508" t="s">
-        <v>1556</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>1558</v>
+        <v>1455</v>
       </c>
       <c r="B509" t="s">
-        <v>1557</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>1606</v>
+        <v>1547</v>
       </c>
       <c r="B510" t="s">
-        <v>1607</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1560</v>
+        <v>1549</v>
       </c>
       <c r="B511" t="s">
-        <v>1559</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>1562</v>
+        <v>1551</v>
       </c>
       <c r="B512" t="s">
-        <v>1561</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>1564</v>
+        <v>1553</v>
       </c>
       <c r="B513" t="s">
-        <v>1563</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>1566</v>
+        <v>1555</v>
       </c>
       <c r="B514" t="s">
-        <v>1565</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>1567</v>
+        <v>1482</v>
       </c>
       <c r="B515" t="s">
-        <v>1568</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>1570</v>
+        <v>1558</v>
       </c>
       <c r="B516" t="s">
-        <v>1569</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>1571</v>
+        <v>1606</v>
       </c>
       <c r="B517" t="s">
-        <v>1572</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>1575</v>
+        <v>1560</v>
       </c>
       <c r="B518" t="s">
-        <v>1573</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1574</v>
+        <v>1562</v>
       </c>
       <c r="B519" t="s">
-        <v>1576</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1578</v>
+        <v>1564</v>
       </c>
       <c r="B520" t="s">
-        <v>1577</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1388</v>
+        <v>1566</v>
       </c>
       <c r="B521" t="s">
-        <v>1579</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1581</v>
+        <v>1567</v>
       </c>
       <c r="B522" t="s">
-        <v>1580</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1583</v>
+        <v>1570</v>
       </c>
       <c r="B523" t="s">
-        <v>1582</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1585</v>
+        <v>1571</v>
       </c>
       <c r="B524" t="s">
-        <v>1584</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1587</v>
+        <v>1575</v>
       </c>
       <c r="B525" t="s">
-        <v>1586</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1589</v>
+        <v>1574</v>
       </c>
       <c r="B526" t="s">
-        <v>1588</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1591</v>
+        <v>1578</v>
       </c>
       <c r="B527" t="s">
-        <v>1590</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1593</v>
+        <v>1388</v>
       </c>
       <c r="B528" t="s">
-        <v>1592</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1595</v>
+        <v>1581</v>
       </c>
       <c r="B529" t="s">
-        <v>1594</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1597</v>
+        <v>1583</v>
       </c>
       <c r="B530" t="s">
-        <v>1596</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1600</v>
+        <v>1585</v>
       </c>
       <c r="B531" t="s">
-        <v>1598</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1599</v>
+        <v>1587</v>
       </c>
       <c r="B532" t="s">
-        <v>1601</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B533" t="s">
-        <v>1604</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1603</v>
+        <v>1591</v>
       </c>
       <c r="B534" t="s">
-        <v>1605</v>
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B535" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B536" t="s">
+        <v>1594</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>2472</v>
+        <v>1597</v>
+      </c>
+      <c r="B537" t="s">
+        <v>1596</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>2473</v>
+        <v>1600</v>
       </c>
       <c r="B538" t="s">
-        <v>2474</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>2475</v>
+        <v>1599</v>
       </c>
       <c r="B539" t="s">
-        <v>2476</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>2477</v>
+        <v>1602</v>
       </c>
       <c r="B540" t="s">
-        <v>2478</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>2479</v>
+        <v>1603</v>
       </c>
       <c r="B541" t="s">
-        <v>2480</v>
-      </c>
-    </row>
-    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A542" t="s">
-        <v>2481</v>
-      </c>
-      <c r="B542" t="s">
-        <v>2482</v>
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>2472</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>2582</v>
+        <v>2473</v>
+      </c>
+      <c r="B545" t="s">
+        <v>2474</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1455</v>
+        <v>2475</v>
       </c>
       <c r="B546" t="s">
-        <v>2583</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>2584</v>
+        <v>2477</v>
       </c>
       <c r="B547" t="s">
-        <v>2585</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>1589</v>
+        <v>2479</v>
       </c>
       <c r="B548" t="s">
-        <v>2586</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1566</v>
+        <v>2481</v>
       </c>
       <c r="B549" t="s">
-        <v>2587</v>
-      </c>
-    </row>
-    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A550" t="s">
-        <v>1602</v>
-      </c>
-      <c r="B550" t="s">
-        <v>2588</v>
-      </c>
-    </row>
-    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A551" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B551" t="s">
-        <v>2589</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B552" t="s">
-        <v>2592</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>1597</v>
+        <v>1455</v>
       </c>
       <c r="B553" t="s">
-        <v>2593</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>2597</v>
+        <v>2584</v>
       </c>
       <c r="B554" t="s">
-        <v>2596</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="B555" t="s">
-        <v>2600</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>1560</v>
+        <v>1566</v>
       </c>
       <c r="B556" t="s">
-        <v>2601</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>1595</v>
+        <v>1602</v>
       </c>
       <c r="B557" t="s">
-        <v>2602</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>1549</v>
+        <v>1150</v>
       </c>
       <c r="B558" t="s">
-        <v>2603</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>1388</v>
+        <v>1219</v>
       </c>
       <c r="B559" t="s">
-        <v>2987</v>
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B560" t="s">
+        <v>2593</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>2597</v>
+      </c>
+      <c r="B561" t="s">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B562" t="s">
+        <v>2600</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>2391</v>
+        <v>1560</v>
+      </c>
+      <c r="B563" t="s">
+        <v>2601</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>1520</v>
+        <v>1595</v>
       </c>
       <c r="B564" t="s">
-        <v>1636</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>1388</v>
+        <v>1549</v>
       </c>
       <c r="B565" t="s">
-        <v>1637</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>1639</v>
+        <v>1388</v>
       </c>
       <c r="B566" t="s">
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="567" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B567" t="s">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="568" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A568" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B568" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A569" t="s">
-        <v>1644</v>
-      </c>
-      <c r="B569" t="s">
-        <v>1643</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B570" t="s">
-        <v>1645</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>1560</v>
+        <v>1520</v>
       </c>
       <c r="B571" t="s">
-        <v>1646</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>1648</v>
+        <v>1388</v>
       </c>
       <c r="B572" t="s">
-        <v>1647</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1649</v>
+        <v>1639</v>
       </c>
       <c r="B573" t="s">
-        <v>1650</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1651</v>
+        <v>1632</v>
       </c>
       <c r="B574" t="s">
-        <v>1652</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1653</v>
+        <v>1641</v>
       </c>
       <c r="B575" t="s">
-        <v>1654</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1655</v>
+        <v>1644</v>
       </c>
       <c r="B576" t="s">
-        <v>1656</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>2150</v>
+        <v>1451</v>
       </c>
       <c r="B577" t="s">
-        <v>2151</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>2591</v>
+        <v>1560</v>
       </c>
       <c r="B578" t="s">
-        <v>2590</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1683</v>
+        <v>1648</v>
       </c>
       <c r="B579" t="s">
-        <v>2621</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>1593</v>
+        <v>1649</v>
       </c>
       <c r="B580" t="s">
-        <v>2662</v>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B582" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B584" t="s">
+        <v>2151</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>2392</v>
+        <v>2591</v>
+      </c>
+      <c r="B585" t="s">
+        <v>2590</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1451</v>
+        <v>1683</v>
       </c>
       <c r="B586" t="s">
-        <v>1657</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1447</v>
+        <v>1593</v>
       </c>
       <c r="B587" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="588" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A588" t="s">
-        <v>1521</v>
-      </c>
-      <c r="B588" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B589" t="s">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="590" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A590" t="s">
-        <v>1663</v>
-      </c>
-      <c r="B590" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="591" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A591" t="s">
-        <v>1639</v>
-      </c>
-      <c r="B591" t="s">
-        <v>1664</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1651</v>
-      </c>
-      <c r="B592" t="s">
-        <v>1665</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1641</v>
+        <v>1451</v>
       </c>
       <c r="B593" t="s">
-        <v>1666</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1667</v>
+        <v>1447</v>
       </c>
       <c r="B594" t="s">
-        <v>1668</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1160</v>
+        <v>1521</v>
       </c>
       <c r="B595" t="s">
-        <v>1669</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>1459</v>
+        <v>1660</v>
       </c>
       <c r="B596" t="s">
-        <v>1670</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>1388</v>
+        <v>1663</v>
       </c>
       <c r="B597" t="s">
-        <v>1671</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1632</v>
+        <v>1639</v>
       </c>
       <c r="B598" t="s">
-        <v>1672</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1520</v>
+        <v>1651</v>
       </c>
       <c r="B599" t="s">
-        <v>1673</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>1674</v>
+        <v>1641</v>
       </c>
       <c r="B600" t="s">
-        <v>1675</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>1677</v>
+        <v>1667</v>
       </c>
       <c r="B601" t="s">
-        <v>1676</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>1679</v>
+        <v>1160</v>
       </c>
       <c r="B602" t="s">
-        <v>1678</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1681</v>
+        <v>1459</v>
       </c>
       <c r="B603" t="s">
-        <v>1680</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1644</v>
+        <v>1388</v>
       </c>
       <c r="B604" t="s">
-        <v>1682</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1683</v>
+        <v>1632</v>
       </c>
       <c r="B605" t="s">
-        <v>1684</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1482</v>
+        <v>1520</v>
       </c>
       <c r="B606" t="s">
-        <v>1865</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>2152</v>
+        <v>1674</v>
       </c>
       <c r="B607" t="s">
-        <v>2153</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>1699</v>
+        <v>1677</v>
       </c>
       <c r="B608" t="s">
-        <v>2641</v>
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B609" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B610" t="s">
+        <v>1680</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>2393</v>
+        <v>1644</v>
+      </c>
+      <c r="B611" t="s">
+        <v>1682</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="B612" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>1523</v>
+        <v>1482</v>
       </c>
       <c r="B613" t="s">
-        <v>1687</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>1524</v>
+        <v>2152</v>
       </c>
       <c r="B614" t="s">
-        <v>1688</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>1689</v>
+        <v>1699</v>
       </c>
       <c r="B615" t="s">
-        <v>1690</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1691</v>
+        <v>1712</v>
       </c>
       <c r="B616" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A617" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B617" t="s">
-        <v>1694</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1696</v>
-      </c>
-      <c r="B618" t="s">
-        <v>1695</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1459</v>
+        <v>1685</v>
       </c>
       <c r="B619" t="s">
-        <v>1697</v>
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B620" t="s">
+        <v>1687</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>2394</v>
+        <v>1524</v>
+      </c>
+      <c r="B621" t="s">
+        <v>1688</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1698</v>
+        <v>1689</v>
       </c>
       <c r="B622" t="s">
-        <v>1729</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1699</v>
+        <v>1691</v>
       </c>
       <c r="B623" t="s">
-        <v>1730</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1483</v>
+        <v>1693</v>
       </c>
       <c r="B624" t="s">
-        <v>1731</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="B625" t="s">
-        <v>1732</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1701</v>
+        <v>1459</v>
       </c>
       <c r="B626" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A627" t="s">
-        <v>1703</v>
-      </c>
-      <c r="B627" t="s">
-        <v>1702</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1667</v>
-      </c>
-      <c r="B628" t="s">
-        <v>1747</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>1704</v>
+        <v>1698</v>
       </c>
       <c r="B629" t="s">
-        <v>1705</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1706</v>
+        <v>1699</v>
       </c>
       <c r="B630" t="s">
-        <v>1734</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>1707</v>
+        <v>1483</v>
       </c>
       <c r="B631" t="s">
-        <v>1735</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>1708</v>
+        <v>1700</v>
       </c>
       <c r="B632" t="s">
-        <v>1709</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>1710</v>
+        <v>1701</v>
       </c>
       <c r="B633" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>1459</v>
+        <v>1703</v>
       </c>
       <c r="B634" t="s">
-        <v>1711</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>1689</v>
+        <v>1667</v>
       </c>
       <c r="B635" t="s">
-        <v>1737</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1712</v>
+        <v>1704</v>
       </c>
       <c r="B636" t="s">
-        <v>1738</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1160</v>
+        <v>1706</v>
       </c>
       <c r="B637" t="s">
-        <v>1739</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>1714</v>
+        <v>1707</v>
       </c>
       <c r="B638" t="s">
-        <v>1713</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>1696</v>
+        <v>1708</v>
       </c>
       <c r="B639" t="s">
-        <v>1740</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="B640" t="s">
-        <v>1741</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>1717</v>
+        <v>1459</v>
       </c>
       <c r="B641" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="B642" t="s">
-        <v>1742</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1524</v>
+        <v>1712</v>
       </c>
       <c r="B643" t="s">
-        <v>1743</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1718</v>
+        <v>1160</v>
       </c>
       <c r="B644" t="s">
-        <v>1744</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1720</v>
+        <v>1714</v>
       </c>
       <c r="B645" t="s">
-        <v>1719</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1721</v>
+        <v>1696</v>
       </c>
       <c r="B646" t="s">
-        <v>1745</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>1723</v>
+        <v>1715</v>
       </c>
       <c r="B647" t="s">
-        <v>1722</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1725</v>
+        <v>1717</v>
       </c>
       <c r="B648" t="s">
-        <v>1724</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1726</v>
+        <v>1693</v>
       </c>
       <c r="B649" t="s">
-        <v>1746</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1728</v>
+        <v>1524</v>
       </c>
       <c r="B650" t="s">
-        <v>1727</v>
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B651" t="s">
+        <v>1744</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>2395</v>
+        <v>1720</v>
+      </c>
+      <c r="B652" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1762</v>
+        <v>1721</v>
       </c>
       <c r="B653" t="s">
-        <v>1763</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>1764</v>
+        <v>1723</v>
       </c>
       <c r="B654" t="s">
-        <v>1765</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1689</v>
+        <v>1725</v>
       </c>
       <c r="B655" t="s">
-        <v>1870</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>1872</v>
+        <v>1726</v>
       </c>
       <c r="B656" t="s">
-        <v>1871</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>1533</v>
+        <v>1728</v>
       </c>
       <c r="B657" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A658" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B658" t="s">
-        <v>1874</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1875</v>
-      </c>
-      <c r="B659" t="s">
-        <v>1876</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1877</v>
+        <v>1762</v>
       </c>
       <c r="B660" t="s">
-        <v>1878</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1880</v>
+        <v>1764</v>
       </c>
       <c r="B661" t="s">
-        <v>1879</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1881</v>
+        <v>1689</v>
       </c>
       <c r="B662" t="s">
-        <v>1882</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1718</v>
+        <v>1872</v>
       </c>
       <c r="B663" t="s">
-        <v>1883</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1885</v>
+        <v>1533</v>
       </c>
       <c r="B664" t="s">
-        <v>1884</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1451</v>
+        <v>1160</v>
       </c>
       <c r="B665" t="s">
-        <v>1886</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1887</v>
+        <v>1875</v>
       </c>
       <c r="B666" t="s">
-        <v>1888</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1889</v>
+        <v>1877</v>
       </c>
       <c r="B667" t="s">
-        <v>1890</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1891</v>
+        <v>1880</v>
       </c>
       <c r="B668" t="s">
-        <v>1892</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1893</v>
+        <v>1881</v>
       </c>
       <c r="B669" t="s">
-        <v>1894</v>
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B670" t="s">
+        <v>1883</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>2396</v>
+        <v>1885</v>
+      </c>
+      <c r="B671" t="s">
+        <v>1884</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1161</v>
+        <v>1451</v>
       </c>
       <c r="B672" t="s">
-        <v>1904</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1906</v>
+        <v>1887</v>
       </c>
       <c r="B673" t="s">
-        <v>1905</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1203</v>
+        <v>1889</v>
       </c>
       <c r="B674" t="s">
-        <v>1907</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1236</v>
+        <v>1891</v>
       </c>
       <c r="B675" t="s">
-        <v>1908</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1408</v>
+        <v>1893</v>
       </c>
       <c r="B676" t="s">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A677" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B677" t="s">
-        <v>1910</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>252</v>
-      </c>
-      <c r="B678" t="s">
-        <v>1911</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1187</v>
+        <v>1161</v>
       </c>
       <c r="B679" t="s">
-        <v>1912</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1238</v>
+        <v>1906</v>
       </c>
       <c r="B680" t="s">
-        <v>1913</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1181</v>
+        <v>1203</v>
       </c>
       <c r="B681" t="s">
-        <v>1914</v>
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B682" t="s">
+        <v>1908</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>2397</v>
+        <v>1408</v>
+      </c>
+      <c r="B683" t="s">
+        <v>1909</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1915</v>
+        <v>1230</v>
       </c>
       <c r="B684" t="s">
-        <v>1916</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1756</v>
+        <v>252</v>
       </c>
       <c r="B685" t="s">
-        <v>1917</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>1919</v>
+        <v>1187</v>
       </c>
       <c r="B686" t="s">
-        <v>1918</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>1921</v>
+        <v>1238</v>
       </c>
       <c r="B687" t="s">
-        <v>1920</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>1923</v>
+        <v>1181</v>
       </c>
       <c r="B688" t="s">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A689" t="s">
-        <v>1925</v>
-      </c>
-      <c r="B689" t="s">
-        <v>1924</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1926</v>
-      </c>
-      <c r="B690" t="s">
-        <v>1927</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>1929</v>
+        <v>1915</v>
       </c>
       <c r="B691" t="s">
-        <v>1928</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1402</v>
+        <v>1756</v>
       </c>
       <c r="B692" t="s">
-        <v>1930</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1934</v>
+        <v>1919</v>
       </c>
       <c r="B693" t="s">
-        <v>1931</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1933</v>
+        <v>1921</v>
       </c>
       <c r="B694" t="s">
-        <v>1932</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1936</v>
+        <v>1923</v>
       </c>
       <c r="B695" t="s">
-        <v>1935</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1578</v>
+        <v>1925</v>
       </c>
       <c r="B696" t="s">
-        <v>1937</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1939</v>
+        <v>1926</v>
       </c>
       <c r="B697" t="s">
-        <v>1938</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1941</v>
+        <v>1929</v>
       </c>
       <c r="B698" t="s">
-        <v>1940</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1299</v>
+        <v>1402</v>
       </c>
       <c r="B699" t="s">
-        <v>1942</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1943</v>
+        <v>1934</v>
       </c>
       <c r="B700" t="s">
-        <v>1944</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1946</v>
+        <v>1933</v>
       </c>
       <c r="B701" t="s">
-        <v>1945</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1948</v>
+        <v>1936</v>
       </c>
       <c r="B702" t="s">
-        <v>1947</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1950</v>
+        <v>1578</v>
       </c>
       <c r="B703" t="s">
-        <v>1949</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1952</v>
+        <v>1939</v>
       </c>
       <c r="B704" t="s">
-        <v>1951</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1953</v>
+        <v>1941</v>
       </c>
       <c r="B705" t="s">
-        <v>1954</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1956</v>
+        <v>1299</v>
       </c>
       <c r="B706" t="s">
-        <v>1955</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1958</v>
+        <v>1943</v>
       </c>
       <c r="B707" t="s">
-        <v>1957</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>1960</v>
+        <v>1946</v>
       </c>
       <c r="B708" t="s">
-        <v>1959</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>1287</v>
+        <v>1948</v>
       </c>
       <c r="B709" t="s">
-        <v>1961</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1963</v>
+        <v>1950</v>
       </c>
       <c r="B710" t="s">
-        <v>1962</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1503</v>
+        <v>1952</v>
       </c>
       <c r="B711" t="s">
-        <v>1964</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1965</v>
+        <v>1953</v>
       </c>
       <c r="B712" t="s">
-        <v>1966</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1968</v>
+        <v>1956</v>
       </c>
       <c r="B713" t="s">
-        <v>1967</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1970</v>
+        <v>1958</v>
       </c>
       <c r="B714" t="s">
-        <v>1969</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1972</v>
+        <v>1960</v>
       </c>
       <c r="B715" t="s">
-        <v>1971</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1973</v>
+        <v>1287</v>
       </c>
       <c r="B716" t="s">
-        <v>1974</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1976</v>
+        <v>1963</v>
       </c>
       <c r="B717" t="s">
-        <v>1975</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1978</v>
+        <v>1503</v>
       </c>
       <c r="B718" t="s">
-        <v>1977</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1980</v>
+        <v>1965</v>
       </c>
       <c r="B719" t="s">
-        <v>1979</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1982</v>
+        <v>1968</v>
       </c>
       <c r="B720" t="s">
-        <v>1981</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B722" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B723" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B724" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B726" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" t="s">
         <v>2962</v>
       </c>
-      <c r="B721" t="s">
+      <c r="B728" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add backup to loadstage
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4068" uniqueCount="3296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4076" uniqueCount="3304">
   <si>
     <t>Base Set</t>
   </si>
@@ -9921,6 +9921,30 @@
   </si>
   <si>
     <t>https://4.bp.blogspot.com/-PtoVqjy6KsI/WD3f-fTDB4I/AAAAAAAAg2I/QOJ9r7B7wQ4AzqbPyeOG5gCy6_oJD5MUQCEw/s1600/bobbyjones.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-mLzRlCUSlGw/WEX1dj8elBI/AAAAAAAAlQc/1HfbeJVR_AA77hOKd87yTagZJdiMopmNwCLcB/s1600/imk085.jpg</t>
+  </si>
+  <si>
+    <t>Kenny Lofton Parachute</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-6EBYkQgLYGs/WEX1i3DG2eI/AAAAAAAAlQw/j2FAz634dZ4OtqizpJy0Lf5etvlFJYn6wCLcB/s1600/imk086.jpg</t>
+  </si>
+  <si>
+    <t>Kenny Lofton - PS Stolen Bases</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-dPIwYicOKwc/WEX1iFvOJKI/AAAAAAAAlQg/c_hMChvwwck2Oa1S-96x44ZzqJbThxk1wCLcB/s1600/imk087.jpg</t>
+  </si>
+  <si>
+    <t>Kenny Lofton - 2008 Topps</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-AOze5qm-VG4/WEX1itrNMJI/AAAAAAAAlQo/NFDbFG5KbyMsBVjDkZlJXd5lJSEUghUpwCLcB/s1600/imk090.jpg</t>
+  </si>
+  <si>
+    <t>Kenny Lofton - Upper Deck</t>
   </si>
 </sst>
 </file>
@@ -20298,10 +20322,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B742"/>
+  <dimension ref="A1:B745"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
-      <selection activeCell="B477" sqref="B477"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="A471" sqref="A471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23919,1916 +23943,1948 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>2447</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A472" t="s">
-        <v>2354</v>
-      </c>
-      <c r="B472" t="s">
-        <v>2355</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A473" t="s">
-        <v>2372</v>
-      </c>
-      <c r="B473" t="s">
-        <v>2373</v>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B467" t="s">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>3299</v>
+      </c>
+      <c r="B468" t="s">
+        <v>3298</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>3301</v>
+      </c>
+      <c r="B469" t="s">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>3303</v>
+      </c>
+      <c r="B470" t="s">
+        <v>3302</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>2994</v>
-      </c>
-      <c r="B474" t="s">
-        <v>2993</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>2965</v>
+        <v>2354</v>
       </c>
       <c r="B475" t="s">
-        <v>2964</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>2978</v>
+        <v>2372</v>
       </c>
       <c r="B476" t="s">
-        <v>2979</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
+        <v>2994</v>
+      </c>
+      <c r="B477" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B478" t="s">
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>2978</v>
+      </c>
+      <c r="B479" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
         <v>3294</v>
       </c>
-      <c r="B477" t="s">
+      <c r="B480" t="s">
         <v>3295</v>
       </c>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A482" t="s">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
         <v>2809</v>
-      </c>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A483" t="s">
-        <v>2810</v>
-      </c>
-      <c r="B483" t="s">
-        <v>2811</v>
-      </c>
-    </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A484" t="s">
-        <v>2812</v>
-      </c>
-      <c r="B484" t="s">
-        <v>2813</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>2867</v>
+        <v>2810</v>
+      </c>
+      <c r="B486" t="s">
+        <v>2811</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>1982</v>
+        <v>2812</v>
       </c>
       <c r="B487" t="s">
-        <v>2868</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A488" t="s">
-        <v>2118</v>
-      </c>
-      <c r="B488" t="s">
-        <v>2117</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>1543</v>
-      </c>
-      <c r="B489" t="s">
-        <v>1544</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>1578</v>
+        <v>1982</v>
       </c>
       <c r="B490" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>1972</v>
+        <v>2118</v>
       </c>
       <c r="B491" t="s">
-        <v>2872</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>1936</v>
+        <v>1543</v>
       </c>
       <c r="B492" t="s">
-        <v>2873</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>2875</v>
+        <v>1578</v>
       </c>
       <c r="B493" t="s">
-        <v>2874</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>2877</v>
+        <v>1972</v>
       </c>
       <c r="B494" t="s">
-        <v>2876</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>1593</v>
+        <v>1936</v>
       </c>
       <c r="B495" t="s">
-        <v>2878</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>2880</v>
+        <v>2875</v>
       </c>
       <c r="B496" t="s">
-        <v>2879</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>2882</v>
+        <v>2877</v>
       </c>
       <c r="B497" t="s">
-        <v>2881</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>1402</v>
+        <v>1593</v>
       </c>
       <c r="B498" t="s">
-        <v>2883</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>2885</v>
+        <v>2880</v>
       </c>
       <c r="B499" t="s">
-        <v>2884</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>2887</v>
+        <v>2882</v>
       </c>
       <c r="B500" t="s">
-        <v>2886</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>2888</v>
+        <v>1402</v>
       </c>
       <c r="B501" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1460</v>
+        <v>2885</v>
       </c>
       <c r="B502" t="s">
-        <v>2890</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>2028</v>
+        <v>2887</v>
       </c>
       <c r="B503" t="s">
-        <v>2891</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>1299</v>
+        <v>2888</v>
       </c>
       <c r="B504" t="s">
-        <v>2892</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>2893</v>
+        <v>1460</v>
       </c>
       <c r="B505" t="s">
-        <v>2894</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>1965</v>
+        <v>2028</v>
       </c>
       <c r="B506" t="s">
-        <v>2895</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>2896</v>
+        <v>1299</v>
       </c>
       <c r="B507" t="s">
-        <v>2897</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>2545</v>
+        <v>2893</v>
       </c>
       <c r="B508" t="s">
-        <v>2898</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>2899</v>
+        <v>1965</v>
       </c>
       <c r="B509" t="s">
-        <v>2900</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>1597</v>
+        <v>2896</v>
       </c>
       <c r="B510" t="s">
-        <v>2471</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>2170</v>
+        <v>2545</v>
       </c>
       <c r="B511" t="s">
-        <v>2171</v>
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B512" t="s">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B513" t="s">
+        <v>2471</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A515" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B515" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A516" t="s">
-        <v>1547</v>
-      </c>
-      <c r="B516" t="s">
-        <v>1546</v>
+        <v>2170</v>
+      </c>
+      <c r="B514" t="s">
+        <v>2171</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B517" t="s">
-        <v>1548</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>1551</v>
+        <v>1455</v>
       </c>
       <c r="B518" t="s">
-        <v>1550</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1553</v>
+        <v>1547</v>
       </c>
       <c r="B519" t="s">
-        <v>1552</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1555</v>
+        <v>1549</v>
       </c>
       <c r="B520" t="s">
-        <v>1554</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1482</v>
+        <v>1551</v>
       </c>
       <c r="B521" t="s">
-        <v>1556</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="B522" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1606</v>
+        <v>1555</v>
       </c>
       <c r="B523" t="s">
-        <v>1607</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1560</v>
+        <v>1482</v>
       </c>
       <c r="B524" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1562</v>
+        <v>1558</v>
       </c>
       <c r="B525" t="s">
-        <v>1561</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1564</v>
+        <v>1606</v>
       </c>
       <c r="B526" t="s">
-        <v>1563</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1566</v>
+        <v>1560</v>
       </c>
       <c r="B527" t="s">
-        <v>1565</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
       <c r="B528" t="s">
-        <v>1568</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1570</v>
+        <v>1564</v>
       </c>
       <c r="B529" t="s">
-        <v>1569</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
       <c r="B530" t="s">
-        <v>1572</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1575</v>
+        <v>1567</v>
       </c>
       <c r="B531" t="s">
-        <v>1573</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1574</v>
+        <v>1570</v>
       </c>
       <c r="B532" t="s">
-        <v>1576</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1578</v>
+        <v>1571</v>
       </c>
       <c r="B533" t="s">
-        <v>1577</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1388</v>
+        <v>1575</v>
       </c>
       <c r="B534" t="s">
-        <v>1579</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1581</v>
+        <v>1574</v>
       </c>
       <c r="B535" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="B536" t="s">
-        <v>1582</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1585</v>
+        <v>1388</v>
       </c>
       <c r="B537" t="s">
-        <v>1584</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1587</v>
+        <v>1581</v>
       </c>
       <c r="B538" t="s">
-        <v>1586</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>1589</v>
+        <v>1583</v>
       </c>
       <c r="B539" t="s">
-        <v>1588</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>1591</v>
+        <v>1585</v>
       </c>
       <c r="B540" t="s">
-        <v>1590</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>1593</v>
+        <v>1587</v>
       </c>
       <c r="B541" t="s">
-        <v>1592</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>1595</v>
+        <v>1589</v>
       </c>
       <c r="B542" t="s">
-        <v>1594</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>1597</v>
+        <v>1591</v>
       </c>
       <c r="B543" t="s">
-        <v>1596</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>1600</v>
+        <v>1593</v>
       </c>
       <c r="B544" t="s">
-        <v>1598</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="B545" t="s">
-        <v>1601</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1602</v>
+        <v>1597</v>
       </c>
       <c r="B546" t="s">
-        <v>1604</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="B547" t="s">
-        <v>1605</v>
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B549" t="s">
+        <v>1604</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>2472</v>
-      </c>
-    </row>
-    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A551" t="s">
-        <v>2473</v>
-      </c>
-      <c r="B551" t="s">
-        <v>2474</v>
-      </c>
-    </row>
-    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A552" t="s">
-        <v>2475</v>
-      </c>
-      <c r="B552" t="s">
-        <v>2476</v>
+        <v>1603</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1605</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>2477</v>
-      </c>
-      <c r="B553" t="s">
-        <v>2478</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>2479</v>
+        <v>2473</v>
       </c>
       <c r="B554" t="s">
-        <v>2480</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>2481</v>
+        <v>2475</v>
       </c>
       <c r="B555" t="s">
-        <v>2482</v>
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>2477</v>
+      </c>
+      <c r="B556" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B557" t="s">
+        <v>2480</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>2582</v>
-      </c>
-    </row>
-    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A559" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B559" t="s">
-        <v>2583</v>
-      </c>
-    </row>
-    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A560" t="s">
-        <v>2584</v>
-      </c>
-      <c r="B560" t="s">
-        <v>2585</v>
+        <v>2481</v>
+      </c>
+      <c r="B558" t="s">
+        <v>2482</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B561" t="s">
-        <v>2586</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>1566</v>
+        <v>1455</v>
       </c>
       <c r="B562" t="s">
-        <v>2587</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>1602</v>
+        <v>2584</v>
       </c>
       <c r="B563" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>1150</v>
+        <v>1589</v>
       </c>
       <c r="B564" t="s">
-        <v>2589</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>1219</v>
+        <v>1566</v>
       </c>
       <c r="B565" t="s">
-        <v>2592</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>1597</v>
+        <v>1602</v>
       </c>
       <c r="B566" t="s">
-        <v>2593</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>2597</v>
+        <v>1150</v>
       </c>
       <c r="B567" t="s">
-        <v>2596</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1593</v>
+        <v>1219</v>
       </c>
       <c r="B568" t="s">
-        <v>2600</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>1560</v>
+        <v>1597</v>
       </c>
       <c r="B569" t="s">
-        <v>2601</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>1595</v>
+        <v>2597</v>
       </c>
       <c r="B570" t="s">
-        <v>2602</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>1549</v>
+        <v>1593</v>
       </c>
       <c r="B571" t="s">
-        <v>2603</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B572" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B573" t="s">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B574" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
         <v>1388</v>
       </c>
-      <c r="B572" t="s">
+      <c r="B575" t="s">
         <v>2987</v>
-      </c>
-    </row>
-    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A576" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A577" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B577" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A578" t="s">
-        <v>1388</v>
-      </c>
-      <c r="B578" t="s">
-        <v>1637</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1639</v>
-      </c>
-      <c r="B579" t="s">
-        <v>1638</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>1632</v>
+        <v>1520</v>
       </c>
       <c r="B580" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1641</v>
+        <v>1388</v>
       </c>
       <c r="B581" t="s">
-        <v>1642</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1644</v>
+        <v>1639</v>
       </c>
       <c r="B582" t="s">
-        <v>1643</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1451</v>
+        <v>1632</v>
       </c>
       <c r="B583" t="s">
-        <v>1645</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>1560</v>
+        <v>1641</v>
       </c>
       <c r="B584" t="s">
-        <v>1646</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="B585" t="s">
-        <v>1647</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1649</v>
+        <v>1451</v>
       </c>
       <c r="B586" t="s">
-        <v>1650</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1651</v>
+        <v>1560</v>
       </c>
       <c r="B587" t="s">
-        <v>1652</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1653</v>
+        <v>1648</v>
       </c>
       <c r="B588" t="s">
-        <v>1654</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1655</v>
+        <v>1649</v>
       </c>
       <c r="B589" t="s">
-        <v>1656</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>2150</v>
+        <v>1651</v>
       </c>
       <c r="B590" t="s">
-        <v>2151</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>2591</v>
+        <v>1653</v>
       </c>
       <c r="B591" t="s">
-        <v>2590</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>3286</v>
+        <v>1655</v>
       </c>
       <c r="B592" t="s">
-        <v>3287</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1683</v>
+        <v>2150</v>
       </c>
       <c r="B593" t="s">
-        <v>2621</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1593</v>
+        <v>2591</v>
       </c>
       <c r="B594" t="s">
-        <v>2662</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
+        <v>3286</v>
+      </c>
+      <c r="B595" t="s">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B596" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B597" t="s">
+        <v>2662</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
         <v>2016</v>
       </c>
-      <c r="B595" t="s">
+      <c r="B598" t="s">
         <v>3285</v>
-      </c>
-    </row>
-    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A599" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A600" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B600" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A601" t="s">
-        <v>1447</v>
-      </c>
-      <c r="B601" t="s">
-        <v>1658</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>1521</v>
-      </c>
-      <c r="B602" t="s">
-        <v>1659</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1660</v>
+        <v>1451</v>
       </c>
       <c r="B603" t="s">
-        <v>1661</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1663</v>
+        <v>1447</v>
       </c>
       <c r="B604" t="s">
-        <v>1662</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1639</v>
+        <v>1521</v>
       </c>
       <c r="B605" t="s">
-        <v>1664</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1651</v>
+        <v>1660</v>
       </c>
       <c r="B606" t="s">
-        <v>1665</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>1641</v>
+        <v>1663</v>
       </c>
       <c r="B607" t="s">
-        <v>1666</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>1667</v>
+        <v>1639</v>
       </c>
       <c r="B608" t="s">
-        <v>1668</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>1160</v>
+        <v>1651</v>
       </c>
       <c r="B609" t="s">
-        <v>1669</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>1459</v>
+        <v>1641</v>
       </c>
       <c r="B610" t="s">
-        <v>1670</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>1388</v>
+        <v>1667</v>
       </c>
       <c r="B611" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>1632</v>
+        <v>1160</v>
       </c>
       <c r="B612" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>1520</v>
+        <v>1459</v>
       </c>
       <c r="B613" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>1674</v>
+        <v>1388</v>
       </c>
       <c r="B614" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>1677</v>
+        <v>1632</v>
       </c>
       <c r="B615" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1679</v>
+        <v>1520</v>
       </c>
       <c r="B616" t="s">
-        <v>1678</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1681</v>
+        <v>1674</v>
       </c>
       <c r="B617" t="s">
-        <v>1680</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1644</v>
+        <v>1677</v>
       </c>
       <c r="B618" t="s">
-        <v>1682</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
       <c r="B619" t="s">
-        <v>1684</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1482</v>
+        <v>1681</v>
       </c>
       <c r="B620" t="s">
-        <v>1865</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>2152</v>
+        <v>1644</v>
       </c>
       <c r="B621" t="s">
-        <v>2153</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1699</v>
+        <v>1683</v>
       </c>
       <c r="B622" t="s">
-        <v>2641</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1712</v>
+        <v>1482</v>
       </c>
       <c r="B623" t="s">
-        <v>3152</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B624" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B625" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B626" t="s">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
         <v>3289</v>
       </c>
-      <c r="B624" t="s">
+      <c r="B627" t="s">
         <v>3288</v>
-      </c>
-    </row>
-    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A632" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B633" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A634" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B634" t="s">
-        <v>1687</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>1524</v>
-      </c>
-      <c r="B635" t="s">
-        <v>1688</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="B636" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1691</v>
+        <v>1523</v>
       </c>
       <c r="B637" t="s">
-        <v>1692</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>1693</v>
+        <v>1524</v>
       </c>
       <c r="B638" t="s">
-        <v>1694</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>1696</v>
+        <v>1689</v>
       </c>
       <c r="B639" t="s">
-        <v>1695</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>1459</v>
+        <v>1691</v>
       </c>
       <c r="B640" t="s">
-        <v>1697</v>
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B641" t="s">
+        <v>1694</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>2394</v>
+        <v>1696</v>
+      </c>
+      <c r="B642" t="s">
+        <v>1695</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1698</v>
+        <v>1459</v>
       </c>
       <c r="B643" t="s">
-        <v>1729</v>
-      </c>
-    </row>
-    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A644" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B644" t="s">
-        <v>1730</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B645" t="s">
-        <v>1731</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="B646" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="B647" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1703</v>
+        <v>1483</v>
       </c>
       <c r="B648" t="s">
-        <v>1702</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1667</v>
+        <v>1700</v>
       </c>
       <c r="B649" t="s">
-        <v>1747</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="B650" t="s">
-        <v>1705</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="B651" t="s">
-        <v>1734</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1707</v>
+        <v>1667</v>
       </c>
       <c r="B652" t="s">
-        <v>1735</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="B653" t="s">
-        <v>1709</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>1710</v>
+        <v>1706</v>
       </c>
       <c r="B654" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1459</v>
+        <v>1707</v>
       </c>
       <c r="B655" t="s">
-        <v>1711</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>1689</v>
+        <v>1708</v>
       </c>
       <c r="B656" t="s">
-        <v>1737</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="B657" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>1160</v>
+        <v>1459</v>
       </c>
       <c r="B658" t="s">
-        <v>1739</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1714</v>
+        <v>1689</v>
       </c>
       <c r="B659" t="s">
-        <v>1713</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1696</v>
+        <v>1712</v>
       </c>
       <c r="B660" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1715</v>
+        <v>1160</v>
       </c>
       <c r="B661" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="B662" t="s">
-        <v>1716</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1693</v>
+        <v>1696</v>
       </c>
       <c r="B663" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1524</v>
+        <v>1715</v>
       </c>
       <c r="B664" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B665" t="s">
-        <v>1744</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1720</v>
+        <v>1693</v>
       </c>
       <c r="B666" t="s">
-        <v>1719</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1721</v>
+        <v>1524</v>
       </c>
       <c r="B667" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1723</v>
+        <v>1718</v>
       </c>
       <c r="B668" t="s">
-        <v>1722</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1725</v>
+        <v>1720</v>
       </c>
       <c r="B669" t="s">
-        <v>1724</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1726</v>
+        <v>1721</v>
       </c>
       <c r="B670" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1728</v>
+        <v>1723</v>
       </c>
       <c r="B671" t="s">
-        <v>1727</v>
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A672" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B672" t="s">
+        <v>1724</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>2395</v>
+        <v>1726</v>
+      </c>
+      <c r="B673" t="s">
+        <v>1746</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1762</v>
+        <v>1728</v>
       </c>
       <c r="B674" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A675" t="s">
-        <v>1764</v>
-      </c>
-      <c r="B675" t="s">
-        <v>1765</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B676" t="s">
-        <v>1870</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1872</v>
+        <v>1762</v>
       </c>
       <c r="B677" t="s">
-        <v>1871</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>1533</v>
+        <v>1764</v>
       </c>
       <c r="B678" t="s">
-        <v>1873</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1160</v>
+        <v>1689</v>
       </c>
       <c r="B679" t="s">
-        <v>1874</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1875</v>
+        <v>1872</v>
       </c>
       <c r="B680" t="s">
-        <v>1876</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1877</v>
+        <v>1533</v>
       </c>
       <c r="B681" t="s">
-        <v>1878</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1880</v>
+        <v>1160</v>
       </c>
       <c r="B682" t="s">
-        <v>1879</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>1881</v>
+        <v>1875</v>
       </c>
       <c r="B683" t="s">
-        <v>1882</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1718</v>
+        <v>1877</v>
       </c>
       <c r="B684" t="s">
-        <v>1883</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1885</v>
+        <v>1880</v>
       </c>
       <c r="B685" t="s">
-        <v>1884</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>1451</v>
+        <v>1881</v>
       </c>
       <c r="B686" t="s">
-        <v>1886</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>1887</v>
+        <v>1718</v>
       </c>
       <c r="B687" t="s">
-        <v>1888</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>1889</v>
+        <v>1885</v>
       </c>
       <c r="B688" t="s">
-        <v>1890</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>1891</v>
+        <v>1451</v>
       </c>
       <c r="B689" t="s">
-        <v>1892</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1893</v>
+        <v>1887</v>
       </c>
       <c r="B690" t="s">
-        <v>1894</v>
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B691" t="s">
+        <v>1890</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>2396</v>
+        <v>1891</v>
+      </c>
+      <c r="B692" t="s">
+        <v>1892</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1161</v>
+        <v>1893</v>
       </c>
       <c r="B693" t="s">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A694" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B694" t="s">
-        <v>1905</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B695" t="s">
-        <v>1907</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1236</v>
+        <v>1161</v>
       </c>
       <c r="B696" t="s">
-        <v>1908</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1408</v>
+        <v>1906</v>
       </c>
       <c r="B697" t="s">
-        <v>1909</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1230</v>
+        <v>1203</v>
       </c>
       <c r="B698" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>252</v>
+        <v>1236</v>
       </c>
       <c r="B699" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1187</v>
+        <v>1408</v>
       </c>
       <c r="B700" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1238</v>
+        <v>1230</v>
       </c>
       <c r="B701" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1181</v>
+        <v>252</v>
       </c>
       <c r="B702" t="s">
-        <v>1914</v>
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B703" t="s">
+        <v>1912</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>2397</v>
+        <v>1238</v>
+      </c>
+      <c r="B704" t="s">
+        <v>1913</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1915</v>
+        <v>1181</v>
       </c>
       <c r="B705" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A706" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B706" t="s">
-        <v>1917</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1919</v>
-      </c>
-      <c r="B707" t="s">
-        <v>1918</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>1921</v>
+        <v>1915</v>
       </c>
       <c r="B708" t="s">
-        <v>1920</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>1923</v>
+        <v>1756</v>
       </c>
       <c r="B709" t="s">
-        <v>1922</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1925</v>
+        <v>1919</v>
       </c>
       <c r="B710" t="s">
-        <v>1924</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1926</v>
+        <v>1921</v>
       </c>
       <c r="B711" t="s">
-        <v>1927</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1929</v>
+        <v>1923</v>
       </c>
       <c r="B712" t="s">
-        <v>1928</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1402</v>
+        <v>1925</v>
       </c>
       <c r="B713" t="s">
-        <v>1930</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1934</v>
+        <v>1926</v>
       </c>
       <c r="B714" t="s">
-        <v>1931</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1933</v>
+        <v>1929</v>
       </c>
       <c r="B715" t="s">
-        <v>1932</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1936</v>
+        <v>1402</v>
       </c>
       <c r="B716" t="s">
-        <v>1935</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1578</v>
+        <v>1934</v>
       </c>
       <c r="B717" t="s">
-        <v>1937</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1939</v>
+        <v>1933</v>
       </c>
       <c r="B718" t="s">
-        <v>1938</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="B719" t="s">
-        <v>1940</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1299</v>
+        <v>1578</v>
       </c>
       <c r="B720" t="s">
-        <v>1942</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1943</v>
+        <v>1939</v>
       </c>
       <c r="B721" t="s">
-        <v>1944</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1946</v>
+        <v>1941</v>
       </c>
       <c r="B722" t="s">
-        <v>1945</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1948</v>
+        <v>1299</v>
       </c>
       <c r="B723" t="s">
-        <v>1947</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1950</v>
+        <v>1943</v>
       </c>
       <c r="B724" t="s">
-        <v>1949</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="B725" t="s">
-        <v>1951</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1953</v>
+        <v>1948</v>
       </c>
       <c r="B726" t="s">
-        <v>1954</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1956</v>
+        <v>1950</v>
       </c>
       <c r="B727" t="s">
-        <v>1955</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1958</v>
+        <v>1952</v>
       </c>
       <c r="B728" t="s">
-        <v>1957</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1960</v>
+        <v>1953</v>
       </c>
       <c r="B729" t="s">
-        <v>1959</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1287</v>
+        <v>1956</v>
       </c>
       <c r="B730" t="s">
-        <v>1961</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1963</v>
+        <v>1958</v>
       </c>
       <c r="B731" t="s">
-        <v>1962</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1503</v>
+        <v>1960</v>
       </c>
       <c r="B732" t="s">
-        <v>1964</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1965</v>
+        <v>1287</v>
       </c>
       <c r="B733" t="s">
-        <v>1966</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1968</v>
+        <v>1963</v>
       </c>
       <c r="B734" t="s">
-        <v>1967</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1970</v>
+        <v>1503</v>
       </c>
       <c r="B735" t="s">
-        <v>1969</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1972</v>
+        <v>1965</v>
       </c>
       <c r="B736" t="s">
-        <v>1971</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
       <c r="B737" t="s">
-        <v>1974</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1976</v>
+        <v>1970</v>
       </c>
       <c r="B738" t="s">
-        <v>1975</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1978</v>
+        <v>1972</v>
       </c>
       <c r="B739" t="s">
-        <v>1977</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1980</v>
+        <v>1973</v>
       </c>
       <c r="B740" t="s">
-        <v>1979</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1982</v>
+        <v>1976</v>
       </c>
       <c r="B741" t="s">
-        <v>1981</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B742" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B743" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B744" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
         <v>2962</v>
       </c>
-      <c r="B742" t="s">
+      <c r="B745" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All one doc to be staged
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4096" uniqueCount="3322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4098" uniqueCount="3324">
   <si>
     <t>Base Set</t>
   </si>
@@ -9999,6 +9999,12 @@
   </si>
   <si>
     <t>Roger Freed</t>
+  </si>
+  <si>
+    <t>Mickey Moniak 2017 Topps Pro Debut</t>
+  </si>
+  <si>
+    <t>https://blowoutbuzz.files.wordpress.com/2016/12/2017-topps-pro-debut-moniak-auto.jpg</t>
   </si>
 </sst>
 </file>
@@ -20416,10 +20422,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B747"/>
+  <dimension ref="A1:B748"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A571" workbookViewId="0">
-      <selection activeCell="O588" sqref="O588"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="B324" sqref="B324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22938,3087 +22944,3095 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B324" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
         <v>3303</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B325" t="s">
         <v>3302</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
-        <v>2387</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>1518</v>
-      </c>
-      <c r="B330" t="s">
-        <v>1903</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>1490</v>
+        <v>1518</v>
       </c>
       <c r="B331" t="s">
-        <v>1491</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>259</v>
+        <v>1490</v>
       </c>
       <c r="B332" t="s">
-        <v>1500</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>1503</v>
+        <v>259</v>
       </c>
       <c r="B333" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>1507</v>
+        <v>1503</v>
       </c>
       <c r="B334" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="B335" t="s">
-        <v>1508</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>1514</v>
+        <v>1506</v>
       </c>
       <c r="B336" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>1535</v>
+        <v>1514</v>
       </c>
       <c r="B337" t="s">
-        <v>1536</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="B338" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>1777</v>
+        <v>1537</v>
       </c>
       <c r="B339" t="s">
-        <v>1778</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>1898</v>
+        <v>1777</v>
       </c>
       <c r="B340" t="s">
-        <v>1899</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="B341" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>1610</v>
+        <v>1900</v>
       </c>
       <c r="B342" t="s">
-        <v>1609</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="B343" t="s">
-        <v>1615</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>1618</v>
+        <v>1614</v>
       </c>
       <c r="B344" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>1616</v>
+        <v>1618</v>
       </c>
       <c r="B345" t="s">
-        <v>1617</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="B346" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>2001</v>
+        <v>1620</v>
       </c>
       <c r="B347" t="s">
-        <v>2002</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>2158</v>
+        <v>2001</v>
       </c>
       <c r="B348" t="s">
-        <v>2159</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>2172</v>
+        <v>2158</v>
       </c>
       <c r="B349" t="s">
-        <v>2173</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>2174</v>
+        <v>2172</v>
       </c>
       <c r="B350" t="s">
-        <v>2175</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>2176</v>
+        <v>2174</v>
       </c>
       <c r="B351" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>2184</v>
+        <v>2176</v>
       </c>
       <c r="B352" t="s">
-        <v>2185</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>2196</v>
+        <v>2184</v>
       </c>
       <c r="B353" t="s">
-        <v>2197</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>2204</v>
+        <v>2196</v>
       </c>
       <c r="B354" t="s">
-        <v>2205</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
       <c r="B355" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>2222</v>
+        <v>2206</v>
       </c>
       <c r="B356" t="s">
-        <v>2223</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="B357" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="B358" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="B359" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1514</v>
+        <v>2228</v>
       </c>
       <c r="B360" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>2231</v>
+        <v>1514</v>
       </c>
       <c r="B361" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>2234</v>
+        <v>2231</v>
       </c>
       <c r="B362" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>2242</v>
+        <v>2234</v>
       </c>
       <c r="B363" t="s">
-        <v>2243</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>2342</v>
+        <v>2242</v>
       </c>
       <c r="B364" t="s">
-        <v>2343</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="B365" t="s">
-        <v>2345</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>2346</v>
+        <v>2344</v>
       </c>
       <c r="B366" t="s">
-        <v>2347</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>2324</v>
+        <v>2346</v>
       </c>
       <c r="B367" t="s">
-        <v>2325</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="B368" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>2298</v>
+        <v>2326</v>
       </c>
       <c r="B369" t="s">
-        <v>2299</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="B370" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>2304</v>
+        <v>2300</v>
       </c>
       <c r="B371" t="s">
-        <v>2305</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
       <c r="B372" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
       <c r="B373" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>2312</v>
+        <v>2308</v>
       </c>
       <c r="B374" t="s">
-        <v>2313</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>2290</v>
+        <v>2312</v>
       </c>
       <c r="B375" t="s">
-        <v>2291</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>2350</v>
+        <v>2290</v>
       </c>
       <c r="B376" t="s">
-        <v>2351</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
       <c r="B377" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>2356</v>
+        <v>2352</v>
       </c>
       <c r="B378" t="s">
-        <v>2357</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>2360</v>
+        <v>2356</v>
       </c>
       <c r="B379" t="s">
-        <v>2361</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>2362</v>
+        <v>2360</v>
       </c>
       <c r="B380" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
       <c r="B381" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>2368</v>
+        <v>2364</v>
       </c>
       <c r="B382" t="s">
-        <v>2369</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>2370</v>
+        <v>2368</v>
       </c>
       <c r="B383" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
       <c r="B384" t="s">
-        <v>2377</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>2485</v>
+        <v>2376</v>
       </c>
       <c r="B385" t="s">
-        <v>2486</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>2489</v>
+        <v>2485</v>
       </c>
       <c r="B386" t="s">
-        <v>2490</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>2997</v>
+        <v>2489</v>
       </c>
       <c r="B387" t="s">
-        <v>2998</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>2491</v>
+        <v>2997</v>
       </c>
       <c r="B388" t="s">
-        <v>2492</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>2497</v>
+        <v>2491</v>
       </c>
       <c r="B389" t="s">
-        <v>2498</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>2501</v>
+        <v>2497</v>
       </c>
       <c r="B390" t="s">
-        <v>2502</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="B391" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
       <c r="B392" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="B393" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>2515</v>
+        <v>2507</v>
       </c>
       <c r="B394" t="s">
-        <v>2516</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="B395" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>2523</v>
+        <v>2517</v>
       </c>
       <c r="B396" t="s">
-        <v>2524</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="B397" t="s">
-        <v>2526</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>2529</v>
+        <v>2525</v>
       </c>
       <c r="B398" t="s">
-        <v>2530</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>2537</v>
+        <v>2529</v>
       </c>
       <c r="B399" t="s">
-        <v>2538</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="B400" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="B401" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>2563</v>
+        <v>2541</v>
       </c>
       <c r="B402" t="s">
-        <v>2561</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>2560</v>
+        <v>2563</v>
       </c>
       <c r="B403" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>2576</v>
+        <v>2560</v>
       </c>
       <c r="B404" t="s">
-        <v>2577</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="B405" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="B406" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>2594</v>
+        <v>2580</v>
       </c>
       <c r="B407" t="s">
-        <v>2595</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>2598</v>
+        <v>2594</v>
       </c>
       <c r="B408" t="s">
-        <v>2599</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>2651</v>
+        <v>2598</v>
       </c>
       <c r="B409" t="s">
-        <v>2650</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>1388</v>
+        <v>2651</v>
       </c>
       <c r="B410" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>2653</v>
+        <v>1388</v>
       </c>
       <c r="B411" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="B412" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>2660</v>
+        <v>2655</v>
       </c>
       <c r="B413" t="s">
-        <v>2659</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>2671</v>
+        <v>2660</v>
       </c>
       <c r="B414" t="s">
-        <v>2672</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
       <c r="B415" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>2678</v>
+        <v>2673</v>
       </c>
       <c r="B416" t="s">
-        <v>2677</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>2746</v>
+        <v>2678</v>
       </c>
       <c r="B417" t="s">
-        <v>2747</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>2771</v>
+        <v>2746</v>
       </c>
       <c r="B418" t="s">
-        <v>2772</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>2799</v>
+        <v>2771</v>
       </c>
       <c r="B419" t="s">
-        <v>2800</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>2802</v>
+        <v>2799</v>
       </c>
       <c r="B420" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>2814</v>
+        <v>2802</v>
       </c>
       <c r="B421" t="s">
-        <v>2815</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>2855</v>
+        <v>2814</v>
       </c>
       <c r="B422" t="s">
-        <v>2856</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="B423" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="B424" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>2863</v>
+        <v>2859</v>
       </c>
       <c r="B425" t="s">
-        <v>2864</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="B426" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>2870</v>
+        <v>2865</v>
       </c>
       <c r="B427" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>2901</v>
+        <v>2870</v>
       </c>
       <c r="B428" t="s">
-        <v>2902</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>2904</v>
+        <v>2901</v>
       </c>
       <c r="B429" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="B430" t="s">
-        <v>2906</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="B431" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="B432" t="s">
-        <v>2911</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="B433" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>2914</v>
+        <v>2910</v>
       </c>
       <c r="B434" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="B435" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>2919</v>
+        <v>2915</v>
       </c>
       <c r="B436" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>2918</v>
+        <v>2919</v>
       </c>
       <c r="B437" t="s">
-        <v>2922</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="B438" t="s">
-        <v>2920</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>1889</v>
+        <v>2921</v>
       </c>
       <c r="B439" t="s">
-        <v>2923</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>2925</v>
+        <v>1889</v>
       </c>
       <c r="B440" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="B441" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="B442" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
       <c r="B443" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="B444" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="B445" t="s">
-        <v>2935</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="B446" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>2939</v>
+        <v>2936</v>
       </c>
       <c r="B447" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="B448" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="B449" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="B450" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="B451" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="B452" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>2953</v>
+        <v>2949</v>
       </c>
       <c r="B453" t="s">
-        <v>2954</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="B454" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="B455" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>2019</v>
+        <v>2957</v>
       </c>
       <c r="B456" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>2036</v>
+        <v>2019</v>
       </c>
       <c r="B457" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>2970</v>
+        <v>2036</v>
       </c>
       <c r="B458" t="s">
-        <v>2971</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>2972</v>
+        <v>2970</v>
       </c>
       <c r="B459" t="s">
-        <v>2973</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>2975</v>
+        <v>2972</v>
       </c>
       <c r="B460" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>2983</v>
+        <v>2975</v>
       </c>
       <c r="B461" t="s">
-        <v>2984</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="B462" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>2999</v>
+        <v>2985</v>
       </c>
       <c r="B463" t="s">
-        <v>3000</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>3048</v>
+        <v>2999</v>
       </c>
       <c r="B464" t="s">
-        <v>3049</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>3140</v>
+        <v>3048</v>
       </c>
       <c r="B465" t="s">
-        <v>3139</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>3142</v>
+        <v>3140</v>
       </c>
       <c r="B466" t="s">
-        <v>3141</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>3144</v>
+        <v>3142</v>
       </c>
       <c r="B467" t="s">
-        <v>3143</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>3293</v>
+        <v>3144</v>
       </c>
       <c r="B468" t="s">
-        <v>3292</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>3295</v>
+        <v>3293</v>
       </c>
       <c r="B469" t="s">
-        <v>3294</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
       <c r="B470" t="s">
-        <v>3296</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B471" t="s">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
         <v>3299</v>
       </c>
-      <c r="B471" t="s">
+      <c r="B472" t="s">
         <v>3298</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A475" t="s">
-        <v>2447</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>2354</v>
-      </c>
-      <c r="B476" t="s">
-        <v>2355</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>2372</v>
+        <v>2354</v>
       </c>
       <c r="B477" t="s">
-        <v>2373</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>2994</v>
+        <v>2372</v>
       </c>
       <c r="B478" t="s">
-        <v>2993</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>2965</v>
+        <v>2994</v>
       </c>
       <c r="B479" t="s">
-        <v>2964</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>2978</v>
+        <v>2965</v>
       </c>
       <c r="B480" t="s">
-        <v>2979</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>3290</v>
+        <v>2978</v>
       </c>
       <c r="B481" t="s">
-        <v>3291</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B482" t="s">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
         <v>3317</v>
       </c>
-      <c r="B482" t="s">
+      <c r="B483" t="s">
         <v>3316</v>
-      </c>
-    </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A486" t="s">
-        <v>2809</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>2810</v>
-      </c>
-      <c r="B487" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B488" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
         <v>2812</v>
       </c>
-      <c r="B488" t="s">
+      <c r="B489" t="s">
         <v>2813</v>
-      </c>
-    </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A490" t="s">
-        <v>2867</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B491" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>2118</v>
+        <v>1982</v>
       </c>
       <c r="B492" t="s">
-        <v>2117</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>1543</v>
+        <v>2118</v>
       </c>
       <c r="B493" t="s">
-        <v>1544</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>1578</v>
+        <v>1543</v>
       </c>
       <c r="B494" t="s">
-        <v>2871</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>1972</v>
+        <v>1578</v>
       </c>
       <c r="B495" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>1936</v>
+        <v>1972</v>
       </c>
       <c r="B496" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>2875</v>
+        <v>1936</v>
       </c>
       <c r="B497" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="B498" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>1593</v>
+        <v>2877</v>
       </c>
       <c r="B499" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>2880</v>
+        <v>1593</v>
       </c>
       <c r="B500" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="B501" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1402</v>
+        <v>2882</v>
       </c>
       <c r="B502" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>2885</v>
+        <v>1402</v>
       </c>
       <c r="B503" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="B504" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="B505" t="s">
-        <v>2889</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>1460</v>
+        <v>2888</v>
       </c>
       <c r="B506" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>2028</v>
+        <v>1460</v>
       </c>
       <c r="B507" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>1299</v>
+        <v>2028</v>
       </c>
       <c r="B508" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>2893</v>
+        <v>1299</v>
       </c>
       <c r="B509" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>1965</v>
+        <v>2893</v>
       </c>
       <c r="B510" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>2896</v>
+        <v>1965</v>
       </c>
       <c r="B511" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>2545</v>
+        <v>2896</v>
       </c>
       <c r="B512" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>2899</v>
+        <v>2545</v>
       </c>
       <c r="B513" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>1597</v>
+        <v>2899</v>
       </c>
       <c r="B514" t="s">
-        <v>2471</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B515" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
         <v>2170</v>
       </c>
-      <c r="B515" t="s">
+      <c r="B516" t="s">
         <v>2171</v>
-      </c>
-    </row>
-    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A518" t="s">
-        <v>2389</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B519" t="s">
-        <v>1545</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1547</v>
+        <v>1455</v>
       </c>
       <c r="B520" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="B521" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="B522" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B523" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="B524" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1482</v>
+        <v>1555</v>
       </c>
       <c r="B525" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1558</v>
+        <v>1482</v>
       </c>
       <c r="B526" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1606</v>
+        <v>1558</v>
       </c>
       <c r="B527" t="s">
-        <v>1607</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1560</v>
+        <v>1606</v>
       </c>
       <c r="B528" t="s">
-        <v>1559</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="B529" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="B530" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="B531" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B532" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B533" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B534" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="B535" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="B536" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="B537" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1388</v>
+        <v>1578</v>
       </c>
       <c r="B538" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>1581</v>
+        <v>1388</v>
       </c>
       <c r="B539" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="B540" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="B541" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="B542" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="B543" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="B544" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="B545" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="B546" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="B547" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="B548" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="B549" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="B550" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
         <v>1603</v>
       </c>
-      <c r="B551" t="s">
+      <c r="B552" t="s">
         <v>1605</v>
-      </c>
-    </row>
-    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A554" t="s">
-        <v>2472</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>2473</v>
-      </c>
-      <c r="B555" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="B556" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="B557" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="B558" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B559" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
         <v>2481</v>
       </c>
-      <c r="B559" t="s">
+      <c r="B560" t="s">
         <v>2482</v>
-      </c>
-    </row>
-    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A562" t="s">
-        <v>2582</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B563" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>2584</v>
+        <v>1455</v>
       </c>
       <c r="B564" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>1589</v>
+        <v>2584</v>
       </c>
       <c r="B565" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>1566</v>
+        <v>1589</v>
       </c>
       <c r="B566" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>1602</v>
+        <v>1566</v>
       </c>
       <c r="B567" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1150</v>
+        <v>1602</v>
       </c>
       <c r="B568" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>1219</v>
+        <v>1150</v>
       </c>
       <c r="B569" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>1597</v>
+        <v>1219</v>
       </c>
       <c r="B570" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>2597</v>
+        <v>1597</v>
       </c>
       <c r="B571" t="s">
-        <v>2596</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>1593</v>
+        <v>2597</v>
       </c>
       <c r="B572" t="s">
-        <v>2600</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1560</v>
+        <v>1593</v>
       </c>
       <c r="B573" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1595</v>
+        <v>1560</v>
       </c>
       <c r="B574" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1549</v>
+        <v>1595</v>
       </c>
       <c r="B575" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B576" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
         <v>1388</v>
       </c>
-      <c r="B576" t="s">
+      <c r="B577" t="s">
         <v>2987</v>
-      </c>
-    </row>
-    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A580" t="s">
-        <v>2391</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B581" t="s">
-        <v>1636</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1388</v>
+        <v>1520</v>
       </c>
       <c r="B582" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1639</v>
+        <v>1388</v>
       </c>
       <c r="B583" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>1632</v>
+        <v>1639</v>
       </c>
       <c r="B584" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>1641</v>
+        <v>1632</v>
       </c>
       <c r="B585" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
       <c r="B586" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1451</v>
+        <v>1644</v>
       </c>
       <c r="B587" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1560</v>
+        <v>1451</v>
       </c>
       <c r="B588" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1648</v>
+        <v>1560</v>
       </c>
       <c r="B589" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B590" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="B591" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="B592" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="B593" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>2150</v>
+        <v>1655</v>
       </c>
       <c r="B594" t="s">
-        <v>2151</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>2591</v>
+        <v>2150</v>
       </c>
       <c r="B595" t="s">
-        <v>2590</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>3283</v>
+        <v>2591</v>
       </c>
       <c r="B596" t="s">
-        <v>3284</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>1683</v>
+        <v>3283</v>
       </c>
       <c r="B597" t="s">
-        <v>2621</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1593</v>
+        <v>1683</v>
       </c>
       <c r="B598" t="s">
-        <v>2662</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>2016</v>
+        <v>1593</v>
       </c>
       <c r="B599" t="s">
-        <v>3282</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B600" t="s">
+        <v>3282</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
         <v>3321</v>
       </c>
-      <c r="B600" t="s">
+      <c r="B601" t="s">
         <v>3320</v>
-      </c>
-    </row>
-    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B604" t="s">
-        <v>1657</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1447</v>
+        <v>1451</v>
       </c>
       <c r="B605" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1521</v>
+        <v>1447</v>
       </c>
       <c r="B606" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>1660</v>
+        <v>1521</v>
       </c>
       <c r="B607" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="B608" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>1639</v>
+        <v>1663</v>
       </c>
       <c r="B609" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>1651</v>
+        <v>1639</v>
       </c>
       <c r="B610" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>1641</v>
+        <v>1651</v>
       </c>
       <c r="B611" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>1667</v>
+        <v>1641</v>
       </c>
       <c r="B612" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>1160</v>
+        <v>1667</v>
       </c>
       <c r="B613" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>1459</v>
+        <v>1160</v>
       </c>
       <c r="B614" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>1388</v>
+        <v>1459</v>
       </c>
       <c r="B615" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1632</v>
+        <v>1388</v>
       </c>
       <c r="B616" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1520</v>
+        <v>1632</v>
       </c>
       <c r="B617" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1674</v>
+        <v>1520</v>
       </c>
       <c r="B618" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="B619" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="B620" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="B621" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1644</v>
+        <v>1681</v>
       </c>
       <c r="B622" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1683</v>
+        <v>1644</v>
       </c>
       <c r="B623" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1482</v>
+        <v>1683</v>
       </c>
       <c r="B624" t="s">
-        <v>1865</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>2152</v>
+        <v>1482</v>
       </c>
       <c r="B625" t="s">
-        <v>2153</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1699</v>
+        <v>2152</v>
       </c>
       <c r="B626" t="s">
-        <v>2641</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1712</v>
+        <v>1699</v>
       </c>
       <c r="B627" t="s">
-        <v>3149</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B628" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
         <v>3286</v>
       </c>
-      <c r="B628" t="s">
+      <c r="B629" t="s">
         <v>3285</v>
-      </c>
-    </row>
-    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A636" t="s">
-        <v>2393</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B637" t="s">
-        <v>1686</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>3309</v>
+        <v>1685</v>
       </c>
       <c r="B638" t="s">
-        <v>3308</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>1523</v>
+        <v>3309</v>
       </c>
       <c r="B639" t="s">
-        <v>1687</v>
+        <v>3308</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B640" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>1689</v>
+        <v>1524</v>
       </c>
       <c r="B641" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="B642" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="B643" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="B644" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B645" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
         <v>1459</v>
       </c>
-      <c r="B645" t="s">
+      <c r="B646" t="s">
         <v>1697</v>
-      </c>
-    </row>
-    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A647" t="s">
-        <v>2394</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B648" t="s">
-        <v>1729</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B649" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1483</v>
+        <v>1699</v>
       </c>
       <c r="B650" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1700</v>
+        <v>1483</v>
       </c>
       <c r="B651" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B652" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="B653" t="s">
-        <v>1702</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>1667</v>
+        <v>1703</v>
       </c>
       <c r="B654" t="s">
-        <v>1747</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1704</v>
+        <v>1667</v>
       </c>
       <c r="B655" t="s">
-        <v>1705</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="B656" t="s">
-        <v>1734</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B657" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B658" t="s">
-        <v>1709</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="B659" t="s">
-        <v>1736</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1459</v>
+        <v>1710</v>
       </c>
       <c r="B660" t="s">
-        <v>1711</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1689</v>
+        <v>1459</v>
       </c>
       <c r="B661" t="s">
-        <v>1737</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1712</v>
+        <v>1689</v>
       </c>
       <c r="B662" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1160</v>
+        <v>1712</v>
       </c>
       <c r="B663" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1714</v>
+        <v>1160</v>
       </c>
       <c r="B664" t="s">
-        <v>1713</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1696</v>
+        <v>1714</v>
       </c>
       <c r="B665" t="s">
-        <v>1740</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1715</v>
+        <v>1696</v>
       </c>
       <c r="B666" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="B667" t="s">
-        <v>1716</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1693</v>
+        <v>1717</v>
       </c>
       <c r="B668" t="s">
-        <v>1742</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1524</v>
+        <v>1693</v>
       </c>
       <c r="B669" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1718</v>
+        <v>1524</v>
       </c>
       <c r="B670" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="B671" t="s">
-        <v>1719</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B672" t="s">
-        <v>1745</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="B673" t="s">
-        <v>1722</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="B674" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B675" t="s">
-        <v>1746</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B676" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
         <v>1728</v>
       </c>
-      <c r="B676" t="s">
+      <c r="B677" t="s">
         <v>1727</v>
-      </c>
-    </row>
-    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A678" t="s">
-        <v>2395</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B679" t="s">
-        <v>1763</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="B680" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1689</v>
+        <v>1764</v>
       </c>
       <c r="B681" t="s">
-        <v>1870</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1872</v>
+        <v>1689</v>
       </c>
       <c r="B682" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>1533</v>
+        <v>1872</v>
       </c>
       <c r="B683" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1160</v>
+        <v>1533</v>
       </c>
       <c r="B684" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1875</v>
+        <v>1160</v>
       </c>
       <c r="B685" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B686" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>1880</v>
+        <v>1877</v>
       </c>
       <c r="B687" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B688" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>1718</v>
+        <v>1881</v>
       </c>
       <c r="B689" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1885</v>
+        <v>1718</v>
       </c>
       <c r="B690" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>1451</v>
+        <v>1885</v>
       </c>
       <c r="B691" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1887</v>
+        <v>1451</v>
       </c>
       <c r="B692" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="B693" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="B694" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B695" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
         <v>1893</v>
       </c>
-      <c r="B695" t="s">
+      <c r="B696" t="s">
         <v>1894</v>
-      </c>
-    </row>
-    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A697" t="s">
-        <v>2396</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B698" t="s">
-        <v>1904</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1906</v>
+        <v>1161</v>
       </c>
       <c r="B699" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1203</v>
+        <v>1906</v>
       </c>
       <c r="B700" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1236</v>
+        <v>1203</v>
       </c>
       <c r="B701" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1408</v>
+        <v>1236</v>
       </c>
       <c r="B702" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1230</v>
+        <v>1408</v>
       </c>
       <c r="B703" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>252</v>
+        <v>1230</v>
       </c>
       <c r="B704" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1187</v>
+        <v>252</v>
       </c>
       <c r="B705" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1238</v>
+        <v>1187</v>
       </c>
       <c r="B706" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B707" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
         <v>1181</v>
       </c>
-      <c r="B707" t="s">
+      <c r="B708" t="s">
         <v>1914</v>
-      </c>
-    </row>
-    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A709" t="s">
-        <v>2397</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B710" t="s">
-        <v>1916</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1756</v>
+        <v>1915</v>
       </c>
       <c r="B711" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1919</v>
+        <v>1756</v>
       </c>
       <c r="B712" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="B713" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B714" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="B715" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B716" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="B717" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1402</v>
+        <v>1929</v>
       </c>
       <c r="B718" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1934</v>
+        <v>1402</v>
       </c>
       <c r="B719" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="B720" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="B721" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1578</v>
+        <v>1936</v>
       </c>
       <c r="B722" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1939</v>
+        <v>1578</v>
       </c>
       <c r="B723" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="B724" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1299</v>
+        <v>1941</v>
       </c>
       <c r="B725" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1943</v>
+        <v>1299</v>
       </c>
       <c r="B726" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="B727" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="B728" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="B729" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="B730" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B731" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="B732" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="B733" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="B734" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1287</v>
+        <v>1960</v>
       </c>
       <c r="B735" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1963</v>
+        <v>1287</v>
       </c>
       <c r="B736" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1503</v>
+        <v>1963</v>
       </c>
       <c r="B737" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1965</v>
+        <v>1503</v>
       </c>
       <c r="B738" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="B739" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="B740" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="B741" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B742" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B743" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="B744" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="B745" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="B746" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B747" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
         <v>2962</v>
       </c>
-      <c r="B747" t="s">
+      <c r="B748" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chachi update for new year
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4098" uniqueCount="3324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="3334">
   <si>
     <t>Base Set</t>
   </si>
@@ -10005,6 +10005,36 @@
   </si>
   <si>
     <t>https://blowoutbuzz.files.wordpress.com/2016/12/2017-topps-pro-debut-moniak-auto.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-jeTScXLhNBE/WGkyY0JZ3mI/AAAAAAAAe24/dPKNVpHsd5opYzEIg1-_mqNOGRXiwUdtQCLcB/s1600/1967%2BTopps%2B%2523560%2BBunning.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-meu1Keyba7k/WGkyYxHHlvI/AAAAAAAAe28/by7E7RVUoKk15FsArlMH108aIv9Q_A1jwCLcB/s1600/1967%2BTopps%2B%2523595%2BRojas.jpg</t>
+  </si>
+  <si>
+    <t>Ozzie Virgil</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-jxjf7CvIeQA/WGHqfuRUWRI/AAAAAAABq3M/jEXUzUPgsyQ29OSZncHZs3dHy0nzQQQrgCLcB/s1600/Virgil%2B85T.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-6bRvw9eeEyY/WF7mdXfRLGI/AAAAAAAAgtY/RKDhzd3NME85FMII5tLLzjtLroC31hThgCLcB/s1600/pippen9697hoops.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scottie Pippen  1996-97 </t>
+  </si>
+  <si>
+    <t>Pete Rose 1985 Renata Galasso</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-JB8nIqBe16s/WGVV_aF8Q7I/AAAAAAAAcXU/5GEgYYG5uVgor_lK_jB2NN5a5r27_YBlwCLcB/s1600/Rose%2BRenata%2BGalasso%2BPete%2BRose%2BF.jpg</t>
+  </si>
+  <si>
+    <t>Steve Carlton Giants</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-3Bi43Defgv8/WGQlGlgxFsI/AAAAAAAAQ8c/KpoLGOJ6TIwNqZ9n9s8tcycA2G1g9hLqwCLcB/s1600/FREE%2BCARDS%2B009%2B3.jpg</t>
   </si>
 </sst>
 </file>
@@ -20422,10 +20452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B748"/>
+  <dimension ref="A1:B752"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="B324" sqref="B324"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="B473" sqref="B473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22958,6 +22988,14 @@
         <v>3302</v>
       </c>
     </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>3330</v>
+      </c>
+      <c r="B326" t="s">
+        <v>3331</v>
+      </c>
+    </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>2387</v>
@@ -24099,6 +24137,14 @@
         <v>3298</v>
       </c>
     </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>3332</v>
+      </c>
+      <c r="B473" t="s">
+        <v>3333</v>
+      </c>
+    </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>2447</v>
@@ -24160,6 +24206,14 @@
         <v>3316</v>
       </c>
     </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>3329</v>
+      </c>
+      <c r="B484" t="s">
+        <v>3328</v>
+      </c>
+    </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>2809</v>
@@ -24386,6 +24440,14 @@
         <v>2171</v>
       </c>
     </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>3326</v>
+      </c>
+      <c r="B517" t="s">
+        <v>3327</v>
+      </c>
+    </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>2389</v>
@@ -25642,397 +25704,413 @@
         <v>1894</v>
       </c>
     </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B697" t="s">
+        <v>3324</v>
+      </c>
+    </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A699" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B699" t="s">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A700" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B700" t="s">
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A701" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B701" t="s">
-        <v>1907</v>
+        <v>1524</v>
+      </c>
+      <c r="B698" t="s">
+        <v>3325</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B702" t="s">
-        <v>1908</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1408</v>
+        <v>1161</v>
       </c>
       <c r="B703" t="s">
-        <v>1909</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1230</v>
+        <v>1906</v>
       </c>
       <c r="B704" t="s">
-        <v>1910</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>252</v>
+        <v>1203</v>
       </c>
       <c r="B705" t="s">
-        <v>1911</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1187</v>
+        <v>1236</v>
       </c>
       <c r="B706" t="s">
-        <v>1912</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1238</v>
+        <v>1408</v>
       </c>
       <c r="B707" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>1181</v>
+        <v>1230</v>
       </c>
       <c r="B708" t="s">
-        <v>1914</v>
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" t="s">
+        <v>252</v>
+      </c>
+      <c r="B709" t="s">
+        <v>1911</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>2397</v>
+        <v>1187</v>
+      </c>
+      <c r="B710" t="s">
+        <v>1912</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1915</v>
+        <v>1238</v>
       </c>
       <c r="B711" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1756</v>
+        <v>1181</v>
       </c>
       <c r="B712" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" t="s">
-        <v>1919</v>
-      </c>
-      <c r="B713" t="s">
-        <v>1918</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1921</v>
-      </c>
-      <c r="B714" t="s">
-        <v>1920</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1923</v>
+        <v>1915</v>
       </c>
       <c r="B715" t="s">
-        <v>1922</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1925</v>
+        <v>1756</v>
       </c>
       <c r="B716" t="s">
-        <v>1924</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1926</v>
+        <v>1919</v>
       </c>
       <c r="B717" t="s">
-        <v>1927</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1929</v>
+        <v>1921</v>
       </c>
       <c r="B718" t="s">
-        <v>1928</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1402</v>
+        <v>1923</v>
       </c>
       <c r="B719" t="s">
-        <v>1930</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1934</v>
+        <v>1925</v>
       </c>
       <c r="B720" t="s">
-        <v>1931</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1933</v>
+        <v>1926</v>
       </c>
       <c r="B721" t="s">
-        <v>1932</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1936</v>
+        <v>1929</v>
       </c>
       <c r="B722" t="s">
-        <v>1935</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1578</v>
+        <v>1402</v>
       </c>
       <c r="B723" t="s">
-        <v>1937</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1939</v>
+        <v>1934</v>
       </c>
       <c r="B724" t="s">
-        <v>1938</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1941</v>
+        <v>1933</v>
       </c>
       <c r="B725" t="s">
-        <v>1940</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1299</v>
+        <v>1936</v>
       </c>
       <c r="B726" t="s">
-        <v>1942</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1943</v>
+        <v>1578</v>
       </c>
       <c r="B727" t="s">
-        <v>1944</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1946</v>
+        <v>1939</v>
       </c>
       <c r="B728" t="s">
-        <v>1945</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1948</v>
+        <v>1941</v>
       </c>
       <c r="B729" t="s">
-        <v>1947</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1950</v>
+        <v>1299</v>
       </c>
       <c r="B730" t="s">
-        <v>1949</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1952</v>
+        <v>1943</v>
       </c>
       <c r="B731" t="s">
-        <v>1951</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1953</v>
+        <v>1946</v>
       </c>
       <c r="B732" t="s">
-        <v>1954</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1956</v>
+        <v>1948</v>
       </c>
       <c r="B733" t="s">
-        <v>1955</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1958</v>
+        <v>1950</v>
       </c>
       <c r="B734" t="s">
-        <v>1957</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1960</v>
+        <v>1952</v>
       </c>
       <c r="B735" t="s">
-        <v>1959</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1287</v>
+        <v>1953</v>
       </c>
       <c r="B736" t="s">
-        <v>1961</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1963</v>
+        <v>1956</v>
       </c>
       <c r="B737" t="s">
-        <v>1962</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1503</v>
+        <v>1958</v>
       </c>
       <c r="B738" t="s">
-        <v>1964</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1965</v>
+        <v>1960</v>
       </c>
       <c r="B739" t="s">
-        <v>1966</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1968</v>
+        <v>1287</v>
       </c>
       <c r="B740" t="s">
-        <v>1967</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1970</v>
+        <v>1963</v>
       </c>
       <c r="B741" t="s">
-        <v>1969</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1972</v>
+        <v>1503</v>
       </c>
       <c r="B742" t="s">
-        <v>1971</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1973</v>
+        <v>1965</v>
       </c>
       <c r="B743" t="s">
-        <v>1974</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1976</v>
+        <v>1968</v>
       </c>
       <c r="B744" t="s">
-        <v>1975</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1978</v>
+        <v>1970</v>
       </c>
       <c r="B745" t="s">
-        <v>1977</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1980</v>
+        <v>1972</v>
       </c>
       <c r="B746" t="s">
-        <v>1979</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1982</v>
+        <v>1973</v>
       </c>
       <c r="B747" t="s">
-        <v>1981</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B748" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B749" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B750" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B751" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" t="s">
         <v>2962</v>
       </c>
-      <c r="B748" t="s">
+      <c r="B752" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sub app navbar component
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4122" uniqueCount="3344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4130" uniqueCount="3352">
   <si>
     <t>Base Set</t>
   </si>
@@ -10065,6 +10065,30 @@
   </si>
   <si>
     <t>https://3.bp.blogspot.com/-OFP-S6Qw7X8/WH29XbqG0YI/AAAAAAABrlI/Mf78RBmWXm4crAJQUZXKweQNsxgjn5T5QCLcB/s1600/mcgraw%2B71T.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-l6kL9a9YFsk/WG8GsdHdyOI/AAAAAAAAy30/aCFgVRuwvjsBPaXtUfeOxPdT4WPGYIQPgCLcB/s1600/PhotoScan.jpg</t>
+  </si>
+  <si>
+    <t>Lenny Dykstra 1996 UD Collectors Choice</t>
+  </si>
+  <si>
+    <t>Larry Bowa Kellogs</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-w28gn0QhqWw/WH6DS_qEcaI/AAAAAAABrlo/aQMFDw7momEbFXWaMjdCsF54IkSXKJSswCLcB/s1600/dimeboxes-4-4-4.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-uUj_ADdxtMs/WH6HIQnk7MI/AAAAAAABrl0/cPgsW9MjBuEzahD7XNa1173LncU-0W60gCLcB/s1600/dimeboxes-4.jpg</t>
+  </si>
+  <si>
+    <t>Tug McGraw Kelloggs</t>
+  </si>
+  <si>
+    <t>Ty Cobb</t>
+  </si>
+  <si>
+    <t>http://www.sportscollectorsdaily.com/wp-content/uploads/2017/01/1913-Ty-Cobb-photo-798x1024.jpg</t>
   </si>
 </sst>
 </file>
@@ -20490,10 +20514,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B752"/>
+  <dimension ref="A1:B757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A607" workbookViewId="0">
-      <selection activeCell="A630" sqref="A630"/>
+    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
+      <selection activeCell="B479" sqref="B479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22789,3406 +22813,3438 @@
         <v>3338</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>3011</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>1</v>
-      </c>
-      <c r="B295" t="s">
-        <v>3012</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>2042</v>
-      </c>
-      <c r="B296" t="s">
-        <v>3013</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>3015</v>
-      </c>
-      <c r="B297" t="s">
-        <v>3014</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>1442</v>
-      </c>
-      <c r="B298" t="s">
-        <v>3016</v>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B291" t="s">
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>3346</v>
+      </c>
+      <c r="B292" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>3349</v>
+      </c>
+      <c r="B293" t="s">
+        <v>3348</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>10</v>
-      </c>
-      <c r="B299" t="s">
-        <v>3017</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B300" t="s">
-        <v>3018</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>8</v>
+        <v>2042</v>
       </c>
       <c r="B301" t="s">
-        <v>3019</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>3021</v>
+        <v>3015</v>
       </c>
       <c r="B302" t="s">
-        <v>3020</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>3022</v>
+        <v>1442</v>
       </c>
       <c r="B303" t="s">
-        <v>3023</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>1859</v>
+        <v>10</v>
       </c>
       <c r="B304" t="s">
-        <v>3024</v>
+        <v>3017</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B305" t="s">
-        <v>3025</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B306" t="s">
-        <v>3026</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>3028</v>
+        <v>3021</v>
       </c>
       <c r="B307" t="s">
-        <v>3027</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>2567</v>
+        <v>3022</v>
       </c>
       <c r="B308" t="s">
-        <v>3029</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>1440</v>
+        <v>1859</v>
       </c>
       <c r="B309" t="s">
-        <v>3030</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>3031</v>
+        <v>14</v>
       </c>
       <c r="B310" t="s">
-        <v>3032</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>2462</v>
+        <v>15</v>
       </c>
       <c r="B311" t="s">
-        <v>2486</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>209</v>
+        <v>3028</v>
       </c>
       <c r="B312" t="s">
-        <v>3033</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>2065</v>
+        <v>2567</v>
       </c>
       <c r="B313" t="s">
-        <v>3034</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>143</v>
+        <v>1440</v>
       </c>
       <c r="B314" t="s">
-        <v>3035</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>3036</v>
+        <v>3031</v>
       </c>
       <c r="B315" t="s">
-        <v>1609</v>
+        <v>3032</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>2044</v>
+        <v>2462</v>
       </c>
       <c r="B316" t="s">
-        <v>3037</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>16</v>
+        <v>209</v>
       </c>
       <c r="B317" t="s">
-        <v>3038</v>
+        <v>3033</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>7</v>
+        <v>2065</v>
       </c>
       <c r="B318" t="s">
-        <v>3039</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>1170</v>
+        <v>143</v>
       </c>
       <c r="B319" t="s">
-        <v>3227</v>
+        <v>3035</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>2310</v>
+        <v>3036</v>
       </c>
       <c r="B320" t="s">
-        <v>3228</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>3271</v>
+        <v>2044</v>
       </c>
       <c r="B321" t="s">
-        <v>3270</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>3287</v>
+        <v>16</v>
       </c>
       <c r="B322" t="s">
-        <v>3286</v>
+        <v>3038</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>3318</v>
+        <v>7</v>
       </c>
       <c r="B323" t="s">
-        <v>3317</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>3321</v>
+        <v>1170</v>
       </c>
       <c r="B324" t="s">
-        <v>3322</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>3302</v>
+        <v>2310</v>
       </c>
       <c r="B325" t="s">
-        <v>3301</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>3329</v>
+        <v>3271</v>
       </c>
       <c r="B326" t="s">
-        <v>3330</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>3341</v>
+        <v>3287</v>
       </c>
       <c r="B327" t="s">
-        <v>3342</v>
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B328" t="s">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>3321</v>
+      </c>
+      <c r="B329" t="s">
+        <v>3322</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>2387</v>
+        <v>3302</v>
+      </c>
+      <c r="B330" t="s">
+        <v>3301</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>1518</v>
+        <v>3329</v>
       </c>
       <c r="B331" t="s">
-        <v>1903</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>1490</v>
+        <v>3341</v>
       </c>
       <c r="B332" t="s">
-        <v>1491</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
-        <v>259</v>
-      </c>
-      <c r="B333" t="s">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>1503</v>
-      </c>
-      <c r="B334" t="s">
-        <v>1504</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>1507</v>
-      </c>
-      <c r="B335" t="s">
-        <v>1505</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>1506</v>
+        <v>1518</v>
       </c>
       <c r="B336" t="s">
-        <v>1508</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>1514</v>
+        <v>1490</v>
       </c>
       <c r="B337" t="s">
-        <v>1513</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>1535</v>
+        <v>259</v>
       </c>
       <c r="B338" t="s">
-        <v>1536</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>1537</v>
+        <v>1503</v>
       </c>
       <c r="B339" t="s">
-        <v>1538</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>1777</v>
+        <v>1507</v>
       </c>
       <c r="B340" t="s">
-        <v>1778</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>1898</v>
+        <v>1506</v>
       </c>
       <c r="B341" t="s">
-        <v>1899</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>1900</v>
+        <v>1514</v>
       </c>
       <c r="B342" t="s">
-        <v>1901</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>1610</v>
+        <v>1535</v>
       </c>
       <c r="B343" t="s">
-        <v>1609</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>1614</v>
+        <v>1537</v>
       </c>
       <c r="B344" t="s">
-        <v>1615</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>1618</v>
+        <v>1777</v>
       </c>
       <c r="B345" t="s">
-        <v>1619</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>1616</v>
+        <v>1898</v>
       </c>
       <c r="B346" t="s">
-        <v>1617</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>1620</v>
+        <v>1900</v>
       </c>
       <c r="B347" t="s">
-        <v>1621</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>2001</v>
+        <v>1610</v>
       </c>
       <c r="B348" t="s">
-        <v>2002</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>2158</v>
+        <v>1614</v>
       </c>
       <c r="B349" t="s">
-        <v>2159</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>2172</v>
+        <v>1618</v>
       </c>
       <c r="B350" t="s">
-        <v>2173</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>2174</v>
+        <v>1616</v>
       </c>
       <c r="B351" t="s">
-        <v>2175</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>2176</v>
+        <v>1620</v>
       </c>
       <c r="B352" t="s">
-        <v>2177</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>2184</v>
+        <v>2001</v>
       </c>
       <c r="B353" t="s">
-        <v>2185</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>2196</v>
+        <v>2158</v>
       </c>
       <c r="B354" t="s">
-        <v>2197</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>2204</v>
+        <v>2172</v>
       </c>
       <c r="B355" t="s">
-        <v>2205</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>2206</v>
+        <v>2174</v>
       </c>
       <c r="B356" t="s">
-        <v>2207</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>2222</v>
+        <v>2176</v>
       </c>
       <c r="B357" t="s">
-        <v>2223</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>2224</v>
+        <v>2184</v>
       </c>
       <c r="B358" t="s">
-        <v>2225</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>2226</v>
+        <v>2196</v>
       </c>
       <c r="B359" t="s">
-        <v>2227</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>2228</v>
+        <v>2204</v>
       </c>
       <c r="B360" t="s">
-        <v>2229</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>1514</v>
+        <v>2206</v>
       </c>
       <c r="B361" t="s">
-        <v>2230</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>2231</v>
+        <v>2222</v>
       </c>
       <c r="B362" t="s">
-        <v>2232</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>2234</v>
+        <v>2224</v>
       </c>
       <c r="B363" t="s">
-        <v>2235</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>2242</v>
+        <v>2226</v>
       </c>
       <c r="B364" t="s">
-        <v>2243</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>2342</v>
+        <v>2228</v>
       </c>
       <c r="B365" t="s">
-        <v>2343</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>2344</v>
+        <v>1514</v>
       </c>
       <c r="B366" t="s">
-        <v>2345</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>2346</v>
+        <v>2231</v>
       </c>
       <c r="B367" t="s">
-        <v>2347</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>2324</v>
+        <v>2234</v>
       </c>
       <c r="B368" t="s">
-        <v>2325</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>2326</v>
+        <v>2242</v>
       </c>
       <c r="B369" t="s">
-        <v>2327</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>2298</v>
+        <v>2342</v>
       </c>
       <c r="B370" t="s">
-        <v>2299</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>2300</v>
+        <v>2344</v>
       </c>
       <c r="B371" t="s">
-        <v>2301</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>2304</v>
+        <v>2346</v>
       </c>
       <c r="B372" t="s">
-        <v>2305</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>2306</v>
+        <v>2324</v>
       </c>
       <c r="B373" t="s">
-        <v>2307</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>2308</v>
+        <v>2326</v>
       </c>
       <c r="B374" t="s">
-        <v>2309</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>2312</v>
+        <v>2298</v>
       </c>
       <c r="B375" t="s">
-        <v>2313</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>2290</v>
+        <v>2300</v>
       </c>
       <c r="B376" t="s">
-        <v>2291</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>2350</v>
+        <v>2304</v>
       </c>
       <c r="B377" t="s">
-        <v>2351</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>2352</v>
+        <v>2306</v>
       </c>
       <c r="B378" t="s">
-        <v>2353</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>2356</v>
+        <v>2308</v>
       </c>
       <c r="B379" t="s">
-        <v>2357</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>2360</v>
+        <v>2312</v>
       </c>
       <c r="B380" t="s">
-        <v>2361</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>2362</v>
+        <v>2290</v>
       </c>
       <c r="B381" t="s">
-        <v>2363</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>2364</v>
+        <v>2350</v>
       </c>
       <c r="B382" t="s">
-        <v>2365</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>2368</v>
+        <v>2352</v>
       </c>
       <c r="B383" t="s">
-        <v>2369</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>2370</v>
+        <v>2356</v>
       </c>
       <c r="B384" t="s">
-        <v>2371</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>2376</v>
+        <v>2360</v>
       </c>
       <c r="B385" t="s">
-        <v>2377</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>2485</v>
+        <v>2362</v>
       </c>
       <c r="B386" t="s">
-        <v>2486</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>2489</v>
+        <v>2364</v>
       </c>
       <c r="B387" t="s">
-        <v>2490</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>2997</v>
+        <v>2368</v>
       </c>
       <c r="B388" t="s">
-        <v>2998</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>2491</v>
+        <v>2370</v>
       </c>
       <c r="B389" t="s">
-        <v>2492</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>2497</v>
+        <v>2376</v>
       </c>
       <c r="B390" t="s">
-        <v>2498</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>2501</v>
+        <v>2485</v>
       </c>
       <c r="B391" t="s">
-        <v>2502</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>2503</v>
+        <v>2489</v>
       </c>
       <c r="B392" t="s">
-        <v>2504</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>2505</v>
+        <v>2997</v>
       </c>
       <c r="B393" t="s">
-        <v>2506</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>2507</v>
+        <v>2491</v>
       </c>
       <c r="B394" t="s">
-        <v>2508</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>2515</v>
+        <v>2497</v>
       </c>
       <c r="B395" t="s">
-        <v>2516</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>2517</v>
+        <v>2501</v>
       </c>
       <c r="B396" t="s">
-        <v>2518</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>2523</v>
+        <v>2503</v>
       </c>
       <c r="B397" t="s">
-        <v>2524</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>2525</v>
+        <v>2505</v>
       </c>
       <c r="B398" t="s">
-        <v>2526</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>2529</v>
+        <v>2507</v>
       </c>
       <c r="B399" t="s">
-        <v>2530</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>2537</v>
+        <v>2515</v>
       </c>
       <c r="B400" t="s">
-        <v>2538</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>2539</v>
+        <v>2517</v>
       </c>
       <c r="B401" t="s">
-        <v>2540</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>2541</v>
+        <v>2523</v>
       </c>
       <c r="B402" t="s">
-        <v>2542</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>2563</v>
+        <v>2525</v>
       </c>
       <c r="B403" t="s">
-        <v>2561</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>2560</v>
+        <v>2529</v>
       </c>
       <c r="B404" t="s">
-        <v>2562</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>2576</v>
+        <v>2537</v>
       </c>
       <c r="B405" t="s">
-        <v>2577</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>2578</v>
+        <v>2539</v>
       </c>
       <c r="B406" t="s">
-        <v>2579</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>2580</v>
+        <v>2541</v>
       </c>
       <c r="B407" t="s">
-        <v>2581</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>2594</v>
+        <v>2563</v>
       </c>
       <c r="B408" t="s">
-        <v>2595</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>2598</v>
+        <v>2560</v>
       </c>
       <c r="B409" t="s">
-        <v>2599</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>2651</v>
+        <v>2576</v>
       </c>
       <c r="B410" t="s">
-        <v>2650</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>1388</v>
+        <v>2578</v>
       </c>
       <c r="B411" t="s">
-        <v>2652</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>2653</v>
+        <v>2580</v>
       </c>
       <c r="B412" t="s">
-        <v>2654</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>2655</v>
+        <v>2594</v>
       </c>
       <c r="B413" t="s">
-        <v>2656</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>2660</v>
+        <v>2598</v>
       </c>
       <c r="B414" t="s">
-        <v>2659</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>2671</v>
+        <v>2651</v>
       </c>
       <c r="B415" t="s">
-        <v>2672</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>2673</v>
+        <v>1388</v>
       </c>
       <c r="B416" t="s">
-        <v>2674</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>2678</v>
+        <v>2653</v>
       </c>
       <c r="B417" t="s">
-        <v>2677</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>2746</v>
+        <v>2655</v>
       </c>
       <c r="B418" t="s">
-        <v>2747</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>2771</v>
+        <v>2660</v>
       </c>
       <c r="B419" t="s">
-        <v>2772</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>2799</v>
+        <v>2671</v>
       </c>
       <c r="B420" t="s">
-        <v>2800</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>2802</v>
+        <v>2673</v>
       </c>
       <c r="B421" t="s">
-        <v>2801</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>2814</v>
+        <v>2678</v>
       </c>
       <c r="B422" t="s">
-        <v>2815</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>2855</v>
+        <v>2746</v>
       </c>
       <c r="B423" t="s">
-        <v>2856</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>2858</v>
+        <v>2771</v>
       </c>
       <c r="B424" t="s">
-        <v>2857</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>2859</v>
+        <v>2799</v>
       </c>
       <c r="B425" t="s">
-        <v>2860</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>2863</v>
+        <v>2802</v>
       </c>
       <c r="B426" t="s">
-        <v>2864</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>2865</v>
+        <v>2814</v>
       </c>
       <c r="B427" t="s">
-        <v>2866</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>2870</v>
+        <v>2855</v>
       </c>
       <c r="B428" t="s">
-        <v>2869</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>2901</v>
+        <v>2858</v>
       </c>
       <c r="B429" t="s">
-        <v>2902</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>2904</v>
+        <v>2859</v>
       </c>
       <c r="B430" t="s">
-        <v>2903</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>2905</v>
+        <v>2863</v>
       </c>
       <c r="B431" t="s">
-        <v>2906</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>2907</v>
+        <v>2865</v>
       </c>
       <c r="B432" t="s">
-        <v>2908</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>2909</v>
+        <v>2870</v>
       </c>
       <c r="B433" t="s">
-        <v>2911</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>2910</v>
+        <v>2901</v>
       </c>
       <c r="B434" t="s">
-        <v>2912</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>2914</v>
+        <v>2904</v>
       </c>
       <c r="B435" t="s">
-        <v>2913</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>2915</v>
+        <v>2905</v>
       </c>
       <c r="B436" t="s">
-        <v>2916</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>2919</v>
+        <v>2907</v>
       </c>
       <c r="B437" t="s">
-        <v>2917</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>2918</v>
+        <v>2909</v>
       </c>
       <c r="B438" t="s">
-        <v>2922</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>2921</v>
+        <v>2910</v>
       </c>
       <c r="B439" t="s">
-        <v>2920</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>1889</v>
+        <v>2914</v>
       </c>
       <c r="B440" t="s">
-        <v>2923</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>2925</v>
+        <v>2915</v>
       </c>
       <c r="B441" t="s">
-        <v>2924</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>2927</v>
+        <v>2919</v>
       </c>
       <c r="B442" t="s">
-        <v>2926</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>2929</v>
+        <v>2918</v>
       </c>
       <c r="B443" t="s">
-        <v>2928</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>2931</v>
+        <v>2921</v>
       </c>
       <c r="B444" t="s">
-        <v>2930</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>2933</v>
+        <v>1889</v>
       </c>
       <c r="B445" t="s">
-        <v>2932</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>2934</v>
+        <v>2925</v>
       </c>
       <c r="B446" t="s">
-        <v>2935</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>2936</v>
+        <v>2927</v>
       </c>
       <c r="B447" t="s">
-        <v>2937</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>2939</v>
+        <v>2929</v>
       </c>
       <c r="B448" t="s">
-        <v>2938</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>2941</v>
+        <v>2931</v>
       </c>
       <c r="B449" t="s">
-        <v>2940</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>2943</v>
+        <v>2933</v>
       </c>
       <c r="B450" t="s">
-        <v>2942</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>2945</v>
+        <v>2934</v>
       </c>
       <c r="B451" t="s">
-        <v>2944</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>2947</v>
+        <v>2936</v>
       </c>
       <c r="B452" t="s">
-        <v>2946</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>2949</v>
+        <v>2939</v>
       </c>
       <c r="B453" t="s">
-        <v>2948</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>2953</v>
+        <v>2941</v>
       </c>
       <c r="B454" t="s">
-        <v>2954</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>2955</v>
+        <v>2943</v>
       </c>
       <c r="B455" t="s">
-        <v>2956</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>2957</v>
+        <v>2945</v>
       </c>
       <c r="B456" t="s">
-        <v>2958</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>2019</v>
+        <v>2947</v>
       </c>
       <c r="B457" t="s">
-        <v>2959</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>2036</v>
+        <v>2949</v>
       </c>
       <c r="B458" t="s">
-        <v>2960</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>2970</v>
+        <v>2953</v>
       </c>
       <c r="B459" t="s">
-        <v>2971</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>2972</v>
+        <v>2955</v>
       </c>
       <c r="B460" t="s">
-        <v>2973</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>2975</v>
+        <v>2957</v>
       </c>
       <c r="B461" t="s">
-        <v>2974</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>2983</v>
+        <v>2019</v>
       </c>
       <c r="B462" t="s">
-        <v>2984</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>2985</v>
+        <v>2036</v>
       </c>
       <c r="B463" t="s">
-        <v>2986</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>2999</v>
+        <v>2970</v>
       </c>
       <c r="B464" t="s">
-        <v>3000</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>3048</v>
+        <v>2972</v>
       </c>
       <c r="B465" t="s">
-        <v>3049</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>3139</v>
+        <v>2975</v>
       </c>
       <c r="B466" t="s">
-        <v>3138</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>3141</v>
+        <v>2983</v>
       </c>
       <c r="B467" t="s">
-        <v>3140</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>3143</v>
+        <v>2985</v>
       </c>
       <c r="B468" t="s">
-        <v>3142</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>3292</v>
+        <v>2999</v>
       </c>
       <c r="B469" t="s">
-        <v>3291</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>3294</v>
+        <v>3048</v>
       </c>
       <c r="B470" t="s">
-        <v>3293</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>3296</v>
+        <v>3139</v>
       </c>
       <c r="B471" t="s">
-        <v>3295</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>3298</v>
+        <v>3141</v>
       </c>
       <c r="B472" t="s">
-        <v>3297</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>3331</v>
+        <v>3143</v>
       </c>
       <c r="B473" t="s">
-        <v>3332</v>
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B474" t="s">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>3294</v>
+      </c>
+      <c r="B475" t="s">
+        <v>3293</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>2447</v>
+        <v>3296</v>
+      </c>
+      <c r="B476" t="s">
+        <v>3295</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>2354</v>
+        <v>3298</v>
       </c>
       <c r="B477" t="s">
-        <v>2355</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>2372</v>
+        <v>3331</v>
       </c>
       <c r="B478" t="s">
-        <v>2373</v>
+        <v>3332</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>2994</v>
+        <v>3350</v>
       </c>
       <c r="B479" t="s">
-        <v>2993</v>
-      </c>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A480" t="s">
-        <v>2965</v>
-      </c>
-      <c r="B480" t="s">
-        <v>2964</v>
+        <v>3351</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>2978</v>
-      </c>
-      <c r="B481" t="s">
-        <v>2979</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>3289</v>
+        <v>2354</v>
       </c>
       <c r="B482" t="s">
-        <v>3290</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>3316</v>
+        <v>2372</v>
       </c>
       <c r="B483" t="s">
-        <v>3315</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>3328</v>
+        <v>2994</v>
       </c>
       <c r="B484" t="s">
-        <v>3327</v>
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B485" t="s">
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>2978</v>
+      </c>
+      <c r="B486" t="s">
+        <v>2979</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>2809</v>
+        <v>3289</v>
+      </c>
+      <c r="B487" t="s">
+        <v>3290</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>2810</v>
+        <v>3316</v>
       </c>
       <c r="B488" t="s">
-        <v>2811</v>
+        <v>3315</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>2812</v>
+        <v>3328</v>
       </c>
       <c r="B489" t="s">
-        <v>2813</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A491" t="s">
-        <v>2867</v>
+        <v>3327</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B492" t="s">
-        <v>2868</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>2118</v>
+        <v>2810</v>
       </c>
       <c r="B493" t="s">
-        <v>2117</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>1543</v>
+        <v>2812</v>
       </c>
       <c r="B494" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
-        <v>1578</v>
-      </c>
-      <c r="B495" t="s">
-        <v>2871</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>1972</v>
-      </c>
-      <c r="B496" t="s">
-        <v>2872</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>1936</v>
+        <v>1982</v>
       </c>
       <c r="B497" t="s">
-        <v>2873</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>2875</v>
+        <v>2118</v>
       </c>
       <c r="B498" t="s">
-        <v>2874</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>2877</v>
+        <v>1543</v>
       </c>
       <c r="B499" t="s">
-        <v>2876</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>1593</v>
+        <v>1578</v>
       </c>
       <c r="B500" t="s">
-        <v>2878</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>2880</v>
+        <v>1972</v>
       </c>
       <c r="B501" t="s">
-        <v>2879</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>2882</v>
+        <v>1936</v>
       </c>
       <c r="B502" t="s">
-        <v>2881</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1402</v>
+        <v>2875</v>
       </c>
       <c r="B503" t="s">
-        <v>2883</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>2885</v>
+        <v>2877</v>
       </c>
       <c r="B504" t="s">
-        <v>2884</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>2887</v>
+        <v>1593</v>
       </c>
       <c r="B505" t="s">
-        <v>2886</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>2888</v>
+        <v>2880</v>
       </c>
       <c r="B506" t="s">
-        <v>2889</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>1460</v>
+        <v>2882</v>
       </c>
       <c r="B507" t="s">
-        <v>2890</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>2028</v>
+        <v>1402</v>
       </c>
       <c r="B508" t="s">
-        <v>2891</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>1299</v>
+        <v>2885</v>
       </c>
       <c r="B509" t="s">
-        <v>2892</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>2893</v>
+        <v>2887</v>
       </c>
       <c r="B510" t="s">
-        <v>2894</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1965</v>
+        <v>2888</v>
       </c>
       <c r="B511" t="s">
-        <v>2895</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>2896</v>
+        <v>1460</v>
       </c>
       <c r="B512" t="s">
-        <v>2897</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>2545</v>
+        <v>2028</v>
       </c>
       <c r="B513" t="s">
-        <v>2898</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>2899</v>
+        <v>1299</v>
       </c>
       <c r="B514" t="s">
-        <v>2900</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>1597</v>
+        <v>2893</v>
       </c>
       <c r="B515" t="s">
-        <v>2471</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>2170</v>
+        <v>1965</v>
       </c>
       <c r="B516" t="s">
-        <v>2171</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>3325</v>
+        <v>2896</v>
       </c>
       <c r="B517" t="s">
-        <v>3326</v>
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B518" t="s">
+        <v>2898</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>2389</v>
+        <v>2899</v>
+      </c>
+      <c r="B519" t="s">
+        <v>2900</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1455</v>
+        <v>1597</v>
       </c>
       <c r="B520" t="s">
-        <v>1545</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1547</v>
+        <v>2170</v>
       </c>
       <c r="B521" t="s">
-        <v>1546</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1549</v>
+        <v>3325</v>
       </c>
       <c r="B522" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A523" t="s">
-        <v>1551</v>
-      </c>
-      <c r="B523" t="s">
-        <v>1550</v>
+        <v>3326</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1553</v>
-      </c>
-      <c r="B524" t="s">
-        <v>1552</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1555</v>
+        <v>1455</v>
       </c>
       <c r="B525" t="s">
-        <v>1554</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1482</v>
+        <v>1547</v>
       </c>
       <c r="B526" t="s">
-        <v>1556</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1558</v>
+        <v>1549</v>
       </c>
       <c r="B527" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1606</v>
+        <v>1551</v>
       </c>
       <c r="B528" t="s">
-        <v>1607</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1560</v>
+        <v>1553</v>
       </c>
       <c r="B529" t="s">
-        <v>1559</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1562</v>
+        <v>1555</v>
       </c>
       <c r="B530" t="s">
-        <v>1561</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1564</v>
+        <v>1482</v>
       </c>
       <c r="B531" t="s">
-        <v>1563</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1566</v>
+        <v>1558</v>
       </c>
       <c r="B532" t="s">
-        <v>1565</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1567</v>
+        <v>1606</v>
       </c>
       <c r="B533" t="s">
-        <v>1568</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1570</v>
+        <v>1560</v>
       </c>
       <c r="B534" t="s">
-        <v>1569</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1571</v>
+        <v>1562</v>
       </c>
       <c r="B535" t="s">
-        <v>1572</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>1575</v>
+        <v>1564</v>
       </c>
       <c r="B536" t="s">
-        <v>1573</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1574</v>
+        <v>1566</v>
       </c>
       <c r="B537" t="s">
-        <v>1576</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1578</v>
+        <v>1567</v>
       </c>
       <c r="B538" t="s">
-        <v>1577</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>1388</v>
+        <v>1570</v>
       </c>
       <c r="B539" t="s">
-        <v>1579</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>1581</v>
+        <v>1571</v>
       </c>
       <c r="B540" t="s">
-        <v>1580</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>1583</v>
+        <v>1575</v>
       </c>
       <c r="B541" t="s">
-        <v>1582</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>1585</v>
+        <v>1574</v>
       </c>
       <c r="B542" t="s">
-        <v>1584</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>1587</v>
+        <v>1578</v>
       </c>
       <c r="B543" t="s">
-        <v>1586</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>1589</v>
+        <v>1388</v>
       </c>
       <c r="B544" t="s">
-        <v>1588</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1591</v>
+        <v>1581</v>
       </c>
       <c r="B545" t="s">
-        <v>1590</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1593</v>
+        <v>1583</v>
       </c>
       <c r="B546" t="s">
-        <v>1592</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1595</v>
+        <v>1585</v>
       </c>
       <c r="B547" t="s">
-        <v>1594</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>1597</v>
+        <v>1587</v>
       </c>
       <c r="B548" t="s">
-        <v>1596</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1600</v>
+        <v>1589</v>
       </c>
       <c r="B549" t="s">
-        <v>1598</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1599</v>
+        <v>1591</v>
       </c>
       <c r="B550" t="s">
-        <v>1601</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>1602</v>
+        <v>1593</v>
       </c>
       <c r="B551" t="s">
-        <v>1604</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>1603</v>
+        <v>1595</v>
       </c>
       <c r="B552" t="s">
-        <v>1605</v>
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B554" t="s">
+        <v>1598</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>2472</v>
+        <v>1599</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1601</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>2473</v>
+        <v>1602</v>
       </c>
       <c r="B556" t="s">
-        <v>2474</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>2475</v>
+        <v>1603</v>
       </c>
       <c r="B557" t="s">
-        <v>2476</v>
-      </c>
-    </row>
-    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A558" t="s">
-        <v>2477</v>
-      </c>
-      <c r="B558" t="s">
-        <v>2478</v>
-      </c>
-    </row>
-    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A559" t="s">
-        <v>2479</v>
-      </c>
-      <c r="B559" t="s">
-        <v>2480</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>2481</v>
-      </c>
-      <c r="B560" t="s">
-        <v>2482</v>
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>2473</v>
+      </c>
+      <c r="B561" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>2475</v>
+      </c>
+      <c r="B562" t="s">
+        <v>2476</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>2582</v>
+        <v>2477</v>
+      </c>
+      <c r="B563" t="s">
+        <v>2478</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>1455</v>
+        <v>2479</v>
       </c>
       <c r="B564" t="s">
-        <v>2583</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>2584</v>
+        <v>2481</v>
       </c>
       <c r="B565" t="s">
-        <v>2585</v>
-      </c>
-    </row>
-    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A566" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B566" t="s">
-        <v>2586</v>
-      </c>
-    </row>
-    <row r="567" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B567" t="s">
-        <v>2587</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1602</v>
-      </c>
-      <c r="B568" t="s">
-        <v>2588</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>1150</v>
+        <v>1455</v>
       </c>
       <c r="B569" t="s">
-        <v>2589</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>1219</v>
+        <v>2584</v>
       </c>
       <c r="B570" t="s">
-        <v>2592</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>1597</v>
+        <v>1589</v>
       </c>
       <c r="B571" t="s">
-        <v>2593</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>2597</v>
+        <v>1566</v>
       </c>
       <c r="B572" t="s">
-        <v>2596</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1593</v>
+        <v>1602</v>
       </c>
       <c r="B573" t="s">
-        <v>2600</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1560</v>
+        <v>1150</v>
       </c>
       <c r="B574" t="s">
-        <v>2601</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1595</v>
+        <v>1219</v>
       </c>
       <c r="B575" t="s">
-        <v>2602</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1549</v>
+        <v>1597</v>
       </c>
       <c r="B576" t="s">
-        <v>2603</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>1388</v>
+        <v>2597</v>
       </c>
       <c r="B577" t="s">
-        <v>2987</v>
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B578" t="s">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B579" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B580" t="s">
+        <v>2602</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>2391</v>
+        <v>1549</v>
+      </c>
+      <c r="B581" t="s">
+        <v>2603</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1520</v>
+        <v>1388</v>
       </c>
       <c r="B582" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A583" t="s">
-        <v>1388</v>
-      </c>
-      <c r="B583" t="s">
-        <v>1637</v>
-      </c>
-    </row>
-    <row r="584" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A584" t="s">
-        <v>1639</v>
-      </c>
-      <c r="B584" t="s">
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B585" t="s">
-        <v>1640</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B586" t="s">
-        <v>1642</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1644</v>
+        <v>1520</v>
       </c>
       <c r="B587" t="s">
-        <v>1643</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1451</v>
+        <v>1388</v>
       </c>
       <c r="B588" t="s">
-        <v>1645</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1560</v>
+        <v>1639</v>
       </c>
       <c r="B589" t="s">
-        <v>1646</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1648</v>
+        <v>1632</v>
       </c>
       <c r="B590" t="s">
-        <v>1647</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1649</v>
+        <v>1641</v>
       </c>
       <c r="B591" t="s">
-        <v>1650</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1651</v>
+        <v>1644</v>
       </c>
       <c r="B592" t="s">
-        <v>1652</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1653</v>
+        <v>1451</v>
       </c>
       <c r="B593" t="s">
-        <v>1654</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1655</v>
+        <v>1560</v>
       </c>
       <c r="B594" t="s">
-        <v>1656</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>2150</v>
+        <v>1648</v>
       </c>
       <c r="B595" t="s">
-        <v>2151</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>2591</v>
+        <v>1649</v>
       </c>
       <c r="B596" t="s">
-        <v>2590</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>3282</v>
+        <v>1651</v>
       </c>
       <c r="B597" t="s">
-        <v>3283</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1683</v>
+        <v>1653</v>
       </c>
       <c r="B598" t="s">
-        <v>2621</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="B599" t="s">
-        <v>2662</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>2016</v>
+        <v>2150</v>
       </c>
       <c r="B600" t="s">
-        <v>3281</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>3320</v>
+        <v>2591</v>
       </c>
       <c r="B601" t="s">
-        <v>3319</v>
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>3282</v>
+      </c>
+      <c r="B602" t="s">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B603" t="s">
+        <v>2621</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>2392</v>
+        <v>1593</v>
+      </c>
+      <c r="B604" t="s">
+        <v>2662</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1451</v>
+        <v>2016</v>
       </c>
       <c r="B605" t="s">
-        <v>1657</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1447</v>
+        <v>3320</v>
       </c>
       <c r="B606" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A607" t="s">
-        <v>1521</v>
-      </c>
-      <c r="B607" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A608" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B608" t="s">
-        <v>1661</v>
+        <v>3319</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>1663</v>
-      </c>
-      <c r="B609" t="s">
-        <v>1662</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>1639</v>
+        <v>1451</v>
       </c>
       <c r="B610" t="s">
-        <v>1664</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>1651</v>
+        <v>1447</v>
       </c>
       <c r="B611" t="s">
-        <v>1665</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>1641</v>
+        <v>1521</v>
       </c>
       <c r="B612" t="s">
-        <v>1666</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>1667</v>
+        <v>1660</v>
       </c>
       <c r="B613" t="s">
-        <v>1668</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>1160</v>
+        <v>1663</v>
       </c>
       <c r="B614" t="s">
-        <v>1669</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>1459</v>
+        <v>1639</v>
       </c>
       <c r="B615" t="s">
-        <v>1670</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1388</v>
+        <v>1651</v>
       </c>
       <c r="B616" t="s">
-        <v>1671</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1632</v>
+        <v>1641</v>
       </c>
       <c r="B617" t="s">
-        <v>1672</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1520</v>
+        <v>1667</v>
       </c>
       <c r="B618" t="s">
-        <v>1673</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1674</v>
+        <v>1160</v>
       </c>
       <c r="B619" t="s">
-        <v>1675</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1677</v>
+        <v>1459</v>
       </c>
       <c r="B620" t="s">
-        <v>1676</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>1679</v>
+        <v>1388</v>
       </c>
       <c r="B621" t="s">
-        <v>1678</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1681</v>
+        <v>1632</v>
       </c>
       <c r="B622" t="s">
-        <v>1680</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1644</v>
+        <v>1520</v>
       </c>
       <c r="B623" t="s">
-        <v>1682</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1683</v>
+        <v>1674</v>
       </c>
       <c r="B624" t="s">
-        <v>1684</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>1482</v>
+        <v>1677</v>
       </c>
       <c r="B625" t="s">
-        <v>1865</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>2152</v>
+        <v>1679</v>
       </c>
       <c r="B626" t="s">
-        <v>2153</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1699</v>
+        <v>1681</v>
       </c>
       <c r="B627" t="s">
-        <v>2641</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1712</v>
+        <v>1644</v>
       </c>
       <c r="B628" t="s">
-        <v>3148</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>3285</v>
+        <v>1683</v>
       </c>
       <c r="B629" t="s">
-        <v>3284</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>2016</v>
+        <v>1482</v>
       </c>
       <c r="B630" t="s">
-        <v>3340</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B631" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B632" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B633" t="s">
+        <v>3148</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>3285</v>
+      </c>
+      <c r="B634" t="s">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B635" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
         <v>1460</v>
       </c>
-      <c r="B631" t="s">
+      <c r="B636" t="s">
         <v>3343</v>
-      </c>
-    </row>
-    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A637" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A638" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B638" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A639" t="s">
-        <v>3308</v>
-      </c>
-      <c r="B639" t="s">
-        <v>3307</v>
-      </c>
-    </row>
-    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A640" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B640" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A641" t="s">
-        <v>1524</v>
-      </c>
-      <c r="B641" t="s">
-        <v>1688</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B642" t="s">
-        <v>1690</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1691</v>
+        <v>1685</v>
       </c>
       <c r="B643" t="s">
-        <v>1692</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1693</v>
+        <v>3308</v>
       </c>
       <c r="B644" t="s">
-        <v>1694</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1696</v>
+        <v>1523</v>
       </c>
       <c r="B645" t="s">
-        <v>1695</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1459</v>
+        <v>1524</v>
       </c>
       <c r="B646" t="s">
-        <v>1697</v>
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B647" t="s">
+        <v>1690</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>2394</v>
+        <v>1691</v>
+      </c>
+      <c r="B648" t="s">
+        <v>1692</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1698</v>
+        <v>1693</v>
       </c>
       <c r="B649" t="s">
-        <v>1729</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="B650" t="s">
-        <v>1730</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1483</v>
+        <v>1459</v>
       </c>
       <c r="B651" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A652" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B652" t="s">
-        <v>1732</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1701</v>
-      </c>
-      <c r="B653" t="s">
-        <v>1733</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>1703</v>
+        <v>1698</v>
       </c>
       <c r="B654" t="s">
-        <v>1702</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1667</v>
+        <v>1699</v>
       </c>
       <c r="B655" t="s">
-        <v>1747</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>1704</v>
+        <v>1483</v>
       </c>
       <c r="B656" t="s">
-        <v>1705</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>1706</v>
+        <v>1700</v>
       </c>
       <c r="B657" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>1707</v>
+        <v>1701</v>
       </c>
       <c r="B658" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1708</v>
+        <v>1703</v>
       </c>
       <c r="B659" t="s">
-        <v>1709</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1710</v>
+        <v>1667</v>
       </c>
       <c r="B660" t="s">
-        <v>1736</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1459</v>
+        <v>1704</v>
       </c>
       <c r="B661" t="s">
-        <v>1711</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1689</v>
+        <v>1706</v>
       </c>
       <c r="B662" t="s">
-        <v>1737</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1712</v>
+        <v>1707</v>
       </c>
       <c r="B663" t="s">
-        <v>1738</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1160</v>
+        <v>1708</v>
       </c>
       <c r="B664" t="s">
-        <v>1739</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1714</v>
+        <v>1710</v>
       </c>
       <c r="B665" t="s">
-        <v>1713</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1696</v>
+        <v>1459</v>
       </c>
       <c r="B666" t="s">
-        <v>1740</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1715</v>
+        <v>1689</v>
       </c>
       <c r="B667" t="s">
-        <v>1741</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
       <c r="B668" t="s">
-        <v>1716</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1693</v>
+        <v>1160</v>
       </c>
       <c r="B669" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1524</v>
+        <v>1714</v>
       </c>
       <c r="B670" t="s">
-        <v>1743</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1718</v>
+        <v>1696</v>
       </c>
       <c r="B671" t="s">
-        <v>1744</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1720</v>
+        <v>1715</v>
       </c>
       <c r="B672" t="s">
-        <v>1719</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1721</v>
+        <v>1717</v>
       </c>
       <c r="B673" t="s">
-        <v>1745</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1723</v>
+        <v>1693</v>
       </c>
       <c r="B674" t="s">
-        <v>1722</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1725</v>
+        <v>1524</v>
       </c>
       <c r="B675" t="s">
-        <v>1724</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1726</v>
+        <v>1718</v>
       </c>
       <c r="B676" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1728</v>
+        <v>1720</v>
       </c>
       <c r="B677" t="s">
-        <v>1727</v>
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B678" t="s">
+        <v>1745</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>2395</v>
+        <v>1723</v>
+      </c>
+      <c r="B679" t="s">
+        <v>1722</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1762</v>
+        <v>1725</v>
       </c>
       <c r="B680" t="s">
-        <v>1763</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1764</v>
+        <v>1726</v>
       </c>
       <c r="B681" t="s">
-        <v>1765</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1689</v>
+        <v>1728</v>
       </c>
       <c r="B682" t="s">
-        <v>1870</v>
-      </c>
-    </row>
-    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A683" t="s">
-        <v>1872</v>
-      </c>
-      <c r="B683" t="s">
-        <v>1871</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B684" t="s">
-        <v>1873</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1160</v>
+        <v>1762</v>
       </c>
       <c r="B685" t="s">
-        <v>1874</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>1875</v>
+        <v>1764</v>
       </c>
       <c r="B686" t="s">
-        <v>1876</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>1877</v>
+        <v>1689</v>
       </c>
       <c r="B687" t="s">
-        <v>1878</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>1880</v>
+        <v>1872</v>
       </c>
       <c r="B688" t="s">
-        <v>1879</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>1881</v>
+        <v>1533</v>
       </c>
       <c r="B689" t="s">
-        <v>1882</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1718</v>
+        <v>1160</v>
       </c>
       <c r="B690" t="s">
-        <v>1883</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>1885</v>
+        <v>1875</v>
       </c>
       <c r="B691" t="s">
-        <v>1884</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1451</v>
+        <v>1877</v>
       </c>
       <c r="B692" t="s">
-        <v>1886</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1887</v>
+        <v>1880</v>
       </c>
       <c r="B693" t="s">
-        <v>1888</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1889</v>
+        <v>1881</v>
       </c>
       <c r="B694" t="s">
-        <v>1890</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1891</v>
+        <v>1718</v>
       </c>
       <c r="B695" t="s">
-        <v>1892</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1893</v>
+        <v>1885</v>
       </c>
       <c r="B696" t="s">
-        <v>1894</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1699</v>
+        <v>1451</v>
       </c>
       <c r="B697" t="s">
-        <v>3323</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1524</v>
+        <v>1887</v>
       </c>
       <c r="B698" t="s">
-        <v>3324</v>
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B699" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B700" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B701" t="s">
+        <v>1894</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>2396</v>
+        <v>1699</v>
+      </c>
+      <c r="B702" t="s">
+        <v>3323</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1161</v>
+        <v>1524</v>
       </c>
       <c r="B703" t="s">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B704" t="s">
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A705" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B705" t="s">
-        <v>1907</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A706" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B706" t="s">
-        <v>1908</v>
+        <v>3324</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B707" t="s">
-        <v>1909</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>1230</v>
+        <v>1161</v>
       </c>
       <c r="B708" t="s">
-        <v>1910</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>252</v>
+        <v>1906</v>
       </c>
       <c r="B709" t="s">
-        <v>1911</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1187</v>
+        <v>1203</v>
       </c>
       <c r="B710" t="s">
-        <v>1912</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B711" t="s">
-        <v>1913</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1181</v>
+        <v>1408</v>
       </c>
       <c r="B712" t="s">
-        <v>1914</v>
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B713" t="s">
+        <v>1910</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>2397</v>
+        <v>252</v>
+      </c>
+      <c r="B714" t="s">
+        <v>1911</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1915</v>
+        <v>1187</v>
       </c>
       <c r="B715" t="s">
-        <v>1916</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1756</v>
+        <v>1238</v>
       </c>
       <c r="B716" t="s">
-        <v>1917</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1919</v>
+        <v>1181</v>
       </c>
       <c r="B717" t="s">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" t="s">
-        <v>1921</v>
-      </c>
-      <c r="B718" t="s">
-        <v>1920</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1923</v>
-      </c>
-      <c r="B719" t="s">
-        <v>1922</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1925</v>
+        <v>1915</v>
       </c>
       <c r="B720" t="s">
-        <v>1924</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1926</v>
+        <v>1756</v>
       </c>
       <c r="B721" t="s">
-        <v>1927</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1929</v>
+        <v>1919</v>
       </c>
       <c r="B722" t="s">
-        <v>1928</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1402</v>
+        <v>1921</v>
       </c>
       <c r="B723" t="s">
-        <v>1930</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1934</v>
+        <v>1923</v>
       </c>
       <c r="B724" t="s">
-        <v>1931</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1933</v>
+        <v>1925</v>
       </c>
       <c r="B725" t="s">
-        <v>1932</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1936</v>
+        <v>1926</v>
       </c>
       <c r="B726" t="s">
-        <v>1935</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1578</v>
+        <v>1929</v>
       </c>
       <c r="B727" t="s">
-        <v>1937</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1939</v>
+        <v>1402</v>
       </c>
       <c r="B728" t="s">
-        <v>1938</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1941</v>
+        <v>1934</v>
       </c>
       <c r="B729" t="s">
-        <v>1940</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1299</v>
+        <v>1933</v>
       </c>
       <c r="B730" t="s">
-        <v>1942</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1943</v>
+        <v>1936</v>
       </c>
       <c r="B731" t="s">
-        <v>1944</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1946</v>
+        <v>1578</v>
       </c>
       <c r="B732" t="s">
-        <v>1945</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1948</v>
+        <v>1939</v>
       </c>
       <c r="B733" t="s">
-        <v>1947</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1950</v>
+        <v>1941</v>
       </c>
       <c r="B734" t="s">
-        <v>1949</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1952</v>
+        <v>1299</v>
       </c>
       <c r="B735" t="s">
-        <v>1951</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1953</v>
+        <v>1943</v>
       </c>
       <c r="B736" t="s">
-        <v>1954</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1956</v>
+        <v>1946</v>
       </c>
       <c r="B737" t="s">
-        <v>1955</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1958</v>
+        <v>1948</v>
       </c>
       <c r="B738" t="s">
-        <v>1957</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1960</v>
+        <v>1950</v>
       </c>
       <c r="B739" t="s">
-        <v>1959</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1287</v>
+        <v>1952</v>
       </c>
       <c r="B740" t="s">
-        <v>1961</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1963</v>
+        <v>1953</v>
       </c>
       <c r="B741" t="s">
-        <v>1962</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1503</v>
+        <v>1956</v>
       </c>
       <c r="B742" t="s">
-        <v>1964</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1965</v>
+        <v>1958</v>
       </c>
       <c r="B743" t="s">
-        <v>1966</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1968</v>
+        <v>1960</v>
       </c>
       <c r="B744" t="s">
-        <v>1967</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1970</v>
+        <v>1287</v>
       </c>
       <c r="B745" t="s">
-        <v>1969</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1972</v>
+        <v>1963</v>
       </c>
       <c r="B746" t="s">
-        <v>1971</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1973</v>
+        <v>1503</v>
       </c>
       <c r="B747" t="s">
-        <v>1974</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>1976</v>
+        <v>1965</v>
       </c>
       <c r="B748" t="s">
-        <v>1975</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>1978</v>
+        <v>1968</v>
       </c>
       <c r="B749" t="s">
-        <v>1977</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="B750" t="s">
-        <v>1979</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>1982</v>
+        <v>1972</v>
       </c>
       <c r="B751" t="s">
-        <v>1981</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B752" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B753" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B754" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B755" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B756" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
         <v>2962</v>
       </c>
-      <c r="B752" t="s">
+      <c r="B757" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add app navbar and sidebar to bftree
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="21" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4130" uniqueCount="3352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4132" uniqueCount="3354">
   <si>
     <t>Base Set</t>
   </si>
@@ -10089,6 +10089,12 @@
   </si>
   <si>
     <t>http://www.sportscollectorsdaily.com/wp-content/uploads/2017/01/1913-Ty-Cobb-photo-798x1024.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/--WKJsAJJS_Q/WII3qWtH4lI/AAAAAAAAe6k/Be_vbWQf72MdRN8fJr-GPukHjSX34I1yACLcB/s1600/2017%2BChachi%2BNew%2BAdditions%2B%25237%2BSaunders.jpg</t>
+  </si>
+  <si>
+    <t>Michael Saunders</t>
   </si>
 </sst>
 </file>
@@ -10456,10 +10462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10626,199 +10632,199 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>3131</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>3133</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>2063</v>
       </c>
       <c r="B24" t="s">
-        <v>3134</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2063</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>3135</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>1859</v>
       </c>
       <c r="B26" t="s">
-        <v>3136</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1859</v>
+        <v>3152</v>
       </c>
       <c r="B27" t="s">
-        <v>3151</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3152</v>
+        <v>3154</v>
       </c>
       <c r="B28" t="s">
-        <v>3153</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3154</v>
+        <v>2610</v>
       </c>
       <c r="B29" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="B30" t="s">
-        <v>3156</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2612</v>
+        <v>3159</v>
       </c>
       <c r="B31" t="s">
-        <v>3157</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>3159</v>
+        <v>2836</v>
       </c>
       <c r="B32" t="s">
-        <v>3158</v>
+        <v>3160</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>2836</v>
+        <v>3161</v>
       </c>
       <c r="B33" t="s">
-        <v>3160</v>
+        <v>3162</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3161</v>
+        <v>3163</v>
       </c>
       <c r="B34" t="s">
-        <v>3162</v>
+        <v>3164</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>3163</v>
+        <v>3165</v>
       </c>
       <c r="B35" t="s">
-        <v>3164</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>3165</v>
+        <v>239</v>
       </c>
       <c r="B36" t="s">
-        <v>3166</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>3168</v>
       </c>
       <c r="B37" t="s">
-        <v>3167</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3168</v>
+        <v>3337</v>
       </c>
       <c r="B38" t="s">
-        <v>3169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>3337</v>
-      </c>
-      <c r="B39" t="s">
         <v>3336</v>
       </c>
     </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>3103</v>
+      </c>
+    </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3313</v>
+      </c>
       <c r="B41" t="s">
-        <v>3103</v>
+        <v>3305</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3313</v>
+        <v>3104</v>
       </c>
       <c r="B42" t="s">
-        <v>3305</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3104</v>
+        <v>3107</v>
       </c>
       <c r="B43" t="s">
-        <v>3105</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3107</v>
+        <v>3314</v>
       </c>
       <c r="B44" t="s">
-        <v>3106</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3314</v>
+        <v>3299</v>
       </c>
       <c r="B45" t="s">
-        <v>3288</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>3299</v>
+        <v>3310</v>
       </c>
       <c r="B46" t="s">
-        <v>3300</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3310</v>
+        <v>3353</v>
       </c>
       <c r="B47" t="s">
-        <v>3309</v>
+        <v>3352</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -10925,6 +10931,14 @@
       </c>
       <c r="B63" t="s">
         <v>3132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3131</v>
       </c>
     </row>
   </sheetData>
@@ -20516,7 +20530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
+    <sheetView topLeftCell="A451" workbookViewId="0">
       <selection activeCell="B479" sqref="B479"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Componentizing doc mgr - App broken
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="3359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4140" uniqueCount="3361">
   <si>
     <t>Base Set</t>
   </si>
@@ -10110,6 +10110,12 @@
   </si>
   <si>
     <t>https://1.bp.blogspot.com/-mb8d4RBzHtM/WIh3ve9mopI/AAAAAAAACzw/yskrRUYAeeQyoaKcccwpjIend8GTqffiQCLcB/s1600/topps1972-377F.jpg</t>
+  </si>
+  <si>
+    <t>Rick Wise four cards</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-gHwFpu8LpZk/WIkJAvGozGI/AAAAAAABr3U/kCL6Z-bpVY0uIWixiUwr9BohTm8jSbi7ACLcB/s1600/wise-2.jpg</t>
   </si>
 </sst>
 </file>
@@ -20543,10 +20549,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B760"/>
+  <dimension ref="A1:B761"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
-      <selection activeCell="B610" sqref="B610"/>
+      <selection activeCell="B602" sqref="B602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25145,1159 +25151,1167 @@
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>1655</v>
+        <v>3359</v>
       </c>
       <c r="B602" t="s">
-        <v>1656</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>2150</v>
+        <v>1655</v>
       </c>
       <c r="B603" t="s">
-        <v>2151</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>2591</v>
+        <v>2150</v>
       </c>
       <c r="B604" t="s">
-        <v>2590</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>3282</v>
+        <v>2591</v>
       </c>
       <c r="B605" t="s">
-        <v>3283</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1683</v>
+        <v>3282</v>
       </c>
       <c r="B606" t="s">
-        <v>2621</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>1593</v>
+        <v>1683</v>
       </c>
       <c r="B607" t="s">
-        <v>2662</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>2016</v>
+        <v>1593</v>
       </c>
       <c r="B608" t="s">
-        <v>3281</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>3320</v>
+        <v>2016</v>
       </c>
       <c r="B609" t="s">
-        <v>3319</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B610" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
         <v>1455</v>
       </c>
-      <c r="B610" t="s">
+      <c r="B611" t="s">
         <v>3358</v>
-      </c>
-    </row>
-    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A612" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B613" t="s">
-        <v>1657</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>1447</v>
+        <v>1451</v>
       </c>
       <c r="B614" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>1521</v>
+        <v>1447</v>
       </c>
       <c r="B615" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1660</v>
+        <v>1521</v>
       </c>
       <c r="B616" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="B617" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1639</v>
+        <v>1663</v>
       </c>
       <c r="B618" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1651</v>
+        <v>1639</v>
       </c>
       <c r="B619" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1641</v>
+        <v>1651</v>
       </c>
       <c r="B620" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>1667</v>
+        <v>1641</v>
       </c>
       <c r="B621" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1160</v>
+        <v>1667</v>
       </c>
       <c r="B622" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1459</v>
+        <v>1160</v>
       </c>
       <c r="B623" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1388</v>
+        <v>1459</v>
       </c>
       <c r="B624" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>1632</v>
+        <v>1388</v>
       </c>
       <c r="B625" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1520</v>
+        <v>1632</v>
       </c>
       <c r="B626" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1674</v>
+        <v>1520</v>
       </c>
       <c r="B627" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="B628" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="B629" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="B630" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>1644</v>
+        <v>1681</v>
       </c>
       <c r="B631" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>1683</v>
+        <v>1644</v>
       </c>
       <c r="B632" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>1482</v>
+        <v>1683</v>
       </c>
       <c r="B633" t="s">
-        <v>1865</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>2152</v>
+        <v>1482</v>
       </c>
       <c r="B634" t="s">
-        <v>2153</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>1699</v>
+        <v>2152</v>
       </c>
       <c r="B635" t="s">
-        <v>2641</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1712</v>
+        <v>1699</v>
       </c>
       <c r="B636" t="s">
-        <v>3148</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>3285</v>
+        <v>1712</v>
       </c>
       <c r="B637" t="s">
-        <v>3284</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>2016</v>
+        <v>3285</v>
       </c>
       <c r="B638" t="s">
-        <v>3340</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B639" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
         <v>1460</v>
       </c>
-      <c r="B639" t="s">
+      <c r="B640" t="s">
         <v>3343</v>
-      </c>
-    </row>
-    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A645" t="s">
-        <v>2393</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B646" t="s">
-        <v>1686</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>3308</v>
+        <v>1685</v>
       </c>
       <c r="B647" t="s">
-        <v>3307</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1523</v>
+        <v>3308</v>
       </c>
       <c r="B648" t="s">
-        <v>1687</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B649" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1689</v>
+        <v>1524</v>
       </c>
       <c r="B650" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="B651" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="B652" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="B653" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B654" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
         <v>1459</v>
       </c>
-      <c r="B654" t="s">
+      <c r="B655" t="s">
         <v>1697</v>
-      </c>
-    </row>
-    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A656" t="s">
-        <v>2394</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B657" t="s">
-        <v>1729</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B658" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1483</v>
+        <v>1699</v>
       </c>
       <c r="B659" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1700</v>
+        <v>1483</v>
       </c>
       <c r="B660" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B661" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="B662" t="s">
-        <v>1702</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1667</v>
+        <v>1703</v>
       </c>
       <c r="B663" t="s">
-        <v>1747</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1704</v>
+        <v>1667</v>
       </c>
       <c r="B664" t="s">
-        <v>1705</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="B665" t="s">
-        <v>1734</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B666" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B667" t="s">
-        <v>1709</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="B668" t="s">
-        <v>1736</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1459</v>
+        <v>1710</v>
       </c>
       <c r="B669" t="s">
-        <v>1711</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1689</v>
+        <v>1459</v>
       </c>
       <c r="B670" t="s">
-        <v>1737</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1712</v>
+        <v>1689</v>
       </c>
       <c r="B671" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1160</v>
+        <v>1712</v>
       </c>
       <c r="B672" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1714</v>
+        <v>1160</v>
       </c>
       <c r="B673" t="s">
-        <v>1713</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1696</v>
+        <v>1714</v>
       </c>
       <c r="B674" t="s">
-        <v>1740</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1715</v>
+        <v>1696</v>
       </c>
       <c r="B675" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="B676" t="s">
-        <v>1716</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1693</v>
+        <v>1717</v>
       </c>
       <c r="B677" t="s">
-        <v>1742</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>1524</v>
+        <v>1693</v>
       </c>
       <c r="B678" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1718</v>
+        <v>1524</v>
       </c>
       <c r="B679" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="B680" t="s">
-        <v>1719</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B681" t="s">
-        <v>1745</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="B682" t="s">
-        <v>1722</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="B683" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B684" t="s">
-        <v>1746</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B685" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
         <v>1728</v>
       </c>
-      <c r="B685" t="s">
+      <c r="B686" t="s">
         <v>1727</v>
-      </c>
-    </row>
-    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" t="s">
-        <v>2395</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B688" t="s">
-        <v>1763</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="B689" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1689</v>
+        <v>1764</v>
       </c>
       <c r="B690" t="s">
-        <v>1870</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>1872</v>
+        <v>1689</v>
       </c>
       <c r="B691" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1533</v>
+        <v>1872</v>
       </c>
       <c r="B692" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1160</v>
+        <v>1533</v>
       </c>
       <c r="B693" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1875</v>
+        <v>1160</v>
       </c>
       <c r="B694" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B695" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1880</v>
+        <v>1877</v>
       </c>
       <c r="B696" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B697" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1718</v>
+        <v>1881</v>
       </c>
       <c r="B698" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1885</v>
+        <v>1718</v>
       </c>
       <c r="B699" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1451</v>
+        <v>1885</v>
       </c>
       <c r="B700" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1887</v>
+        <v>1451</v>
       </c>
       <c r="B701" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="B702" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="B703" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B704" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1699</v>
+        <v>1893</v>
       </c>
       <c r="B705" t="s">
-        <v>3323</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B706" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
         <v>1524</v>
       </c>
-      <c r="B706" t="s">
+      <c r="B707" t="s">
         <v>3324</v>
-      </c>
-    </row>
-    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A710" t="s">
-        <v>2396</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B711" t="s">
-        <v>1904</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1906</v>
+        <v>1161</v>
       </c>
       <c r="B712" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1203</v>
+        <v>1906</v>
       </c>
       <c r="B713" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1236</v>
+        <v>1203</v>
       </c>
       <c r="B714" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1408</v>
+        <v>1236</v>
       </c>
       <c r="B715" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1230</v>
+        <v>1408</v>
       </c>
       <c r="B716" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>252</v>
+        <v>1230</v>
       </c>
       <c r="B717" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1187</v>
+        <v>252</v>
       </c>
       <c r="B718" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1238</v>
+        <v>1187</v>
       </c>
       <c r="B719" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B720" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
         <v>1181</v>
       </c>
-      <c r="B720" t="s">
+      <c r="B721" t="s">
         <v>1914</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A722" t="s">
-        <v>2397</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B723" t="s">
-        <v>1916</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1756</v>
+        <v>1915</v>
       </c>
       <c r="B724" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1919</v>
+        <v>1756</v>
       </c>
       <c r="B725" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="B726" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B727" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="B728" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B729" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="B730" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1402</v>
+        <v>1929</v>
       </c>
       <c r="B731" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1934</v>
+        <v>1402</v>
       </c>
       <c r="B732" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="B733" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="B734" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1578</v>
+        <v>1936</v>
       </c>
       <c r="B735" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1939</v>
+        <v>1578</v>
       </c>
       <c r="B736" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="B737" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1299</v>
+        <v>1941</v>
       </c>
       <c r="B738" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1943</v>
+        <v>1299</v>
       </c>
       <c r="B739" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="B740" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="B741" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="B742" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="B743" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B744" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="B745" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="B746" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="B747" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>1287</v>
+        <v>1960</v>
       </c>
       <c r="B748" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>1963</v>
+        <v>1287</v>
       </c>
       <c r="B749" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>1503</v>
+        <v>1963</v>
       </c>
       <c r="B750" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>1965</v>
+        <v>1503</v>
       </c>
       <c r="B751" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="B752" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="B753" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="B754" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B755" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B756" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="B757" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="B758" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="B759" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B760" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
         <v>2962</v>
       </c>
-      <c r="B760" t="s">
+      <c r="B761" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Unit test of libdoc
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4140" uniqueCount="3361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="3367">
   <si>
     <t>Base Set</t>
   </si>
@@ -10116,6 +10116,24 @@
   </si>
   <si>
     <t>https://3.bp.blogspot.com/-gHwFpu8LpZk/WIkJAvGozGI/AAAAAAABr3U/kCL6Z-bpVY0uIWixiUwr9BohTm8jSbi7ACLcB/s1600/wise-2.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-GDHmyDkvlmk/WIAUdWK5pPI/AAAAAAAAzAI/m2b6nOHzGnE6vfLXKO8vTWCGomgmzcJEACLcB/s1600/PhotoScan%2B%25282%2529.jpg</t>
+  </si>
+  <si>
+    <t>Darren Daulton 96 UD Collectors Choice</t>
+  </si>
+  <si>
+    <t>Yasiel Puig Heritage</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-PlJjpeV-jeM/WIuu_dm_EwI/AAAAAAABr7s/29D9dZUfkNgmy6RHmvrn8fdBYqs0jX31gCLcB/s1600/julie-4.jpg</t>
+  </si>
+  <si>
+    <t>http://www.sportscollectorsdaily.com/wp-content/uploads/2017/01/Joel-Embiid-National-Treasures-relic.jpg</t>
+  </si>
+  <si>
+    <t>Joel Embiid</t>
   </si>
 </sst>
 </file>
@@ -20549,10 +20567,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B761"/>
+  <dimension ref="A1:B762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
-      <selection activeCell="B602" sqref="B602"/>
+    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
+      <selection activeCell="G490" sqref="G490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20958,6 +20976,14 @@
         <v>3356</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3364</v>
+      </c>
+    </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>2386</v>
@@ -23157,6 +23183,14 @@
         <v>3342</v>
       </c>
     </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>3362</v>
+      </c>
+      <c r="B336" t="s">
+        <v>3361</v>
+      </c>
+    </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>2387</v>
@@ -24353,1965 +24387,1973 @@
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>2978</v>
+        <v>3366</v>
       </c>
       <c r="B489" t="s">
-        <v>2979</v>
+        <v>3365</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>3289</v>
+        <v>2978</v>
       </c>
       <c r="B490" t="s">
-        <v>3290</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>3316</v>
+        <v>3289</v>
       </c>
       <c r="B491" t="s">
-        <v>3315</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B492" t="s">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
         <v>3328</v>
       </c>
-      <c r="B492" t="s">
+      <c r="B493" t="s">
         <v>3327</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
-        <v>2809</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>2810</v>
-      </c>
-      <c r="B496" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B497" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
         <v>2812</v>
       </c>
-      <c r="B497" t="s">
+      <c r="B498" t="s">
         <v>2813</v>
-      </c>
-    </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A499" t="s">
-        <v>2867</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B500" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>2118</v>
+        <v>1982</v>
       </c>
       <c r="B501" t="s">
-        <v>2117</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1543</v>
+        <v>2118</v>
       </c>
       <c r="B502" t="s">
-        <v>1544</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1578</v>
+        <v>1543</v>
       </c>
       <c r="B503" t="s">
-        <v>2871</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>1972</v>
+        <v>1578</v>
       </c>
       <c r="B504" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>1936</v>
+        <v>1972</v>
       </c>
       <c r="B505" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>2875</v>
+        <v>1936</v>
       </c>
       <c r="B506" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="B507" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>1593</v>
+        <v>2877</v>
       </c>
       <c r="B508" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>2880</v>
+        <v>1593</v>
       </c>
       <c r="B509" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="B510" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1402</v>
+        <v>2882</v>
       </c>
       <c r="B511" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>2885</v>
+        <v>1402</v>
       </c>
       <c r="B512" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="B513" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="B514" t="s">
-        <v>2889</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>1460</v>
+        <v>2888</v>
       </c>
       <c r="B515" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>2028</v>
+        <v>1460</v>
       </c>
       <c r="B516" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>1299</v>
+        <v>2028</v>
       </c>
       <c r="B517" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>2893</v>
+        <v>1299</v>
       </c>
       <c r="B518" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1965</v>
+        <v>2893</v>
       </c>
       <c r="B519" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>2896</v>
+        <v>1965</v>
       </c>
       <c r="B520" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>2545</v>
+        <v>2896</v>
       </c>
       <c r="B521" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>2899</v>
+        <v>2545</v>
       </c>
       <c r="B522" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1597</v>
+        <v>2899</v>
       </c>
       <c r="B523" t="s">
-        <v>2471</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>2170</v>
+        <v>1597</v>
       </c>
       <c r="B524" t="s">
-        <v>2171</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B525" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
         <v>3325</v>
       </c>
-      <c r="B525" t="s">
+      <c r="B526" t="s">
         <v>3326</v>
-      </c>
-    </row>
-    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A527" t="s">
-        <v>2389</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B528" t="s">
-        <v>1545</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1547</v>
+        <v>1455</v>
       </c>
       <c r="B529" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="B530" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="B531" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B532" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="B533" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1482</v>
+        <v>1555</v>
       </c>
       <c r="B534" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1558</v>
+        <v>1482</v>
       </c>
       <c r="B535" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>1606</v>
+        <v>1558</v>
       </c>
       <c r="B536" t="s">
-        <v>1607</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1560</v>
+        <v>1606</v>
       </c>
       <c r="B537" t="s">
-        <v>1559</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="B538" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="B539" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="B540" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B541" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B542" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B543" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="B544" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="B545" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="B546" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1388</v>
+        <v>1578</v>
       </c>
       <c r="B547" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>1581</v>
+        <v>1388</v>
       </c>
       <c r="B548" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="B549" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="B550" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="B551" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="B552" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="B553" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="B554" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="B555" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="B556" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="B557" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="B558" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="B559" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B560" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
         <v>1603</v>
       </c>
-      <c r="B560" t="s">
+      <c r="B561" t="s">
         <v>1605</v>
-      </c>
-    </row>
-    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A563" t="s">
-        <v>2472</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>2473</v>
-      </c>
-      <c r="B564" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="B565" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="B566" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="B567" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B568" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
         <v>2481</v>
       </c>
-      <c r="B568" t="s">
+      <c r="B569" t="s">
         <v>2482</v>
-      </c>
-    </row>
-    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A571" t="s">
-        <v>2582</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B572" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>2584</v>
+        <v>1455</v>
       </c>
       <c r="B573" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1589</v>
+        <v>2584</v>
       </c>
       <c r="B574" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1566</v>
+        <v>1589</v>
       </c>
       <c r="B575" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1602</v>
+        <v>1566</v>
       </c>
       <c r="B576" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>1150</v>
+        <v>1602</v>
       </c>
       <c r="B577" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>1219</v>
+        <v>1150</v>
       </c>
       <c r="B578" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1597</v>
+        <v>1219</v>
       </c>
       <c r="B579" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>2597</v>
+        <v>1597</v>
       </c>
       <c r="B580" t="s">
-        <v>2596</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1593</v>
+        <v>2597</v>
       </c>
       <c r="B581" t="s">
-        <v>2600</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1560</v>
+        <v>1593</v>
       </c>
       <c r="B582" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1595</v>
+        <v>1560</v>
       </c>
       <c r="B583" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>1549</v>
+        <v>1595</v>
       </c>
       <c r="B584" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B585" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
         <v>1388</v>
       </c>
-      <c r="B585" t="s">
+      <c r="B586" t="s">
         <v>2987</v>
-      </c>
-    </row>
-    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
-        <v>2391</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B590" t="s">
-        <v>1636</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1388</v>
+        <v>1520</v>
       </c>
       <c r="B591" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1639</v>
+        <v>1388</v>
       </c>
       <c r="B592" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1632</v>
+        <v>1639</v>
       </c>
       <c r="B593" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1641</v>
+        <v>1632</v>
       </c>
       <c r="B594" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
       <c r="B595" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>1451</v>
+        <v>1644</v>
       </c>
       <c r="B596" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>1560</v>
+        <v>1451</v>
       </c>
       <c r="B597" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1648</v>
+        <v>1560</v>
       </c>
       <c r="B598" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B599" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="B600" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="B601" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>3359</v>
+        <v>1653</v>
       </c>
       <c r="B602" t="s">
-        <v>3360</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1655</v>
+        <v>3359</v>
       </c>
       <c r="B603" t="s">
-        <v>1656</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>2150</v>
+        <v>1655</v>
       </c>
       <c r="B604" t="s">
-        <v>2151</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>2591</v>
+        <v>2150</v>
       </c>
       <c r="B605" t="s">
-        <v>2590</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>3282</v>
+        <v>2591</v>
       </c>
       <c r="B606" t="s">
-        <v>3283</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>1683</v>
+        <v>3282</v>
       </c>
       <c r="B607" t="s">
-        <v>2621</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>1593</v>
+        <v>1683</v>
       </c>
       <c r="B608" t="s">
-        <v>2662</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>2016</v>
+        <v>1593</v>
       </c>
       <c r="B609" t="s">
-        <v>3281</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>3320</v>
+        <v>2016</v>
       </c>
       <c r="B610" t="s">
-        <v>3319</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B611" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
         <v>1455</v>
       </c>
-      <c r="B611" t="s">
+      <c r="B612" t="s">
         <v>3358</v>
-      </c>
-    </row>
-    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A613" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B614" t="s">
-        <v>1657</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>1447</v>
+        <v>1451</v>
       </c>
       <c r="B615" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1521</v>
+        <v>1447</v>
       </c>
       <c r="B616" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1660</v>
+        <v>1521</v>
       </c>
       <c r="B617" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="B618" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1639</v>
+        <v>1663</v>
       </c>
       <c r="B619" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1651</v>
+        <v>1639</v>
       </c>
       <c r="B620" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>1641</v>
+        <v>1651</v>
       </c>
       <c r="B621" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1667</v>
+        <v>1641</v>
       </c>
       <c r="B622" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1160</v>
+        <v>1667</v>
       </c>
       <c r="B623" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1459</v>
+        <v>1160</v>
       </c>
       <c r="B624" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>1388</v>
+        <v>1459</v>
       </c>
       <c r="B625" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1632</v>
+        <v>1388</v>
       </c>
       <c r="B626" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1520</v>
+        <v>1632</v>
       </c>
       <c r="B627" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1674</v>
+        <v>1520</v>
       </c>
       <c r="B628" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="B629" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="B630" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="B631" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>1644</v>
+        <v>1681</v>
       </c>
       <c r="B632" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>1683</v>
+        <v>1644</v>
       </c>
       <c r="B633" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>1482</v>
+        <v>1683</v>
       </c>
       <c r="B634" t="s">
-        <v>1865</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>2152</v>
+        <v>1482</v>
       </c>
       <c r="B635" t="s">
-        <v>2153</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1699</v>
+        <v>2152</v>
       </c>
       <c r="B636" t="s">
-        <v>2641</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1712</v>
+        <v>1699</v>
       </c>
       <c r="B637" t="s">
-        <v>3148</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>3285</v>
+        <v>1712</v>
       </c>
       <c r="B638" t="s">
-        <v>3284</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>2016</v>
+        <v>3285</v>
       </c>
       <c r="B639" t="s">
-        <v>3340</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B640" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
         <v>1460</v>
       </c>
-      <c r="B640" t="s">
+      <c r="B641" t="s">
         <v>3343</v>
-      </c>
-    </row>
-    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A646" t="s">
-        <v>2393</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B647" t="s">
-        <v>1686</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>3308</v>
+        <v>1685</v>
       </c>
       <c r="B648" t="s">
-        <v>3307</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1523</v>
+        <v>3308</v>
       </c>
       <c r="B649" t="s">
-        <v>1687</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B650" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1689</v>
+        <v>1524</v>
       </c>
       <c r="B651" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="B652" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="B653" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="B654" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B655" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" t="s">
         <v>1459</v>
       </c>
-      <c r="B655" t="s">
+      <c r="B656" t="s">
         <v>1697</v>
-      </c>
-    </row>
-    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A657" t="s">
-        <v>2394</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B658" t="s">
-        <v>1729</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B659" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1483</v>
+        <v>1699</v>
       </c>
       <c r="B660" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1700</v>
+        <v>1483</v>
       </c>
       <c r="B661" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B662" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="B663" t="s">
-        <v>1702</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1667</v>
+        <v>1703</v>
       </c>
       <c r="B664" t="s">
-        <v>1747</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1704</v>
+        <v>1667</v>
       </c>
       <c r="B665" t="s">
-        <v>1705</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="B666" t="s">
-        <v>1734</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B667" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B668" t="s">
-        <v>1709</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="B669" t="s">
-        <v>1736</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1459</v>
+        <v>1710</v>
       </c>
       <c r="B670" t="s">
-        <v>1711</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1689</v>
+        <v>1459</v>
       </c>
       <c r="B671" t="s">
-        <v>1737</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1712</v>
+        <v>1689</v>
       </c>
       <c r="B672" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1160</v>
+        <v>1712</v>
       </c>
       <c r="B673" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1714</v>
+        <v>1160</v>
       </c>
       <c r="B674" t="s">
-        <v>1713</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1696</v>
+        <v>1714</v>
       </c>
       <c r="B675" t="s">
-        <v>1740</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1715</v>
+        <v>1696</v>
       </c>
       <c r="B676" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="B677" t="s">
-        <v>1716</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>1693</v>
+        <v>1717</v>
       </c>
       <c r="B678" t="s">
-        <v>1742</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1524</v>
+        <v>1693</v>
       </c>
       <c r="B679" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1718</v>
+        <v>1524</v>
       </c>
       <c r="B680" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="B681" t="s">
-        <v>1719</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B682" t="s">
-        <v>1745</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="B683" t="s">
-        <v>1722</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="B684" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B685" t="s">
-        <v>1746</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B686" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" t="s">
         <v>1728</v>
       </c>
-      <c r="B686" t="s">
+      <c r="B687" t="s">
         <v>1727</v>
-      </c>
-    </row>
-    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A688" t="s">
-        <v>2395</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B689" t="s">
-        <v>1763</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="B690" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>1689</v>
+        <v>1764</v>
       </c>
       <c r="B691" t="s">
-        <v>1870</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1872</v>
+        <v>1689</v>
       </c>
       <c r="B692" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1533</v>
+        <v>1872</v>
       </c>
       <c r="B693" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1160</v>
+        <v>1533</v>
       </c>
       <c r="B694" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1875</v>
+        <v>1160</v>
       </c>
       <c r="B695" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B696" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1880</v>
+        <v>1877</v>
       </c>
       <c r="B697" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B698" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1718</v>
+        <v>1881</v>
       </c>
       <c r="B699" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1885</v>
+        <v>1718</v>
       </c>
       <c r="B700" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1451</v>
+        <v>1885</v>
       </c>
       <c r="B701" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1887</v>
+        <v>1451</v>
       </c>
       <c r="B702" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="B703" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="B704" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B705" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1699</v>
+        <v>1893</v>
       </c>
       <c r="B706" t="s">
-        <v>3323</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B707" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
         <v>1524</v>
       </c>
-      <c r="B707" t="s">
+      <c r="B708" t="s">
         <v>3324</v>
-      </c>
-    </row>
-    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A711" t="s">
-        <v>2396</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B712" t="s">
-        <v>1904</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1906</v>
+        <v>1161</v>
       </c>
       <c r="B713" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1203</v>
+        <v>1906</v>
       </c>
       <c r="B714" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1236</v>
+        <v>1203</v>
       </c>
       <c r="B715" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1408</v>
+        <v>1236</v>
       </c>
       <c r="B716" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1230</v>
+        <v>1408</v>
       </c>
       <c r="B717" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>252</v>
+        <v>1230</v>
       </c>
       <c r="B718" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1187</v>
+        <v>252</v>
       </c>
       <c r="B719" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1238</v>
+        <v>1187</v>
       </c>
       <c r="B720" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" t="s">
         <v>1181</v>
       </c>
-      <c r="B721" t="s">
+      <c r="B722" t="s">
         <v>1914</v>
-      </c>
-    </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" t="s">
-        <v>2397</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B724" t="s">
-        <v>1916</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1756</v>
+        <v>1915</v>
       </c>
       <c r="B725" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1919</v>
+        <v>1756</v>
       </c>
       <c r="B726" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="B727" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B728" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="B729" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B730" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="B731" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1402</v>
+        <v>1929</v>
       </c>
       <c r="B732" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1934</v>
+        <v>1402</v>
       </c>
       <c r="B733" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="B734" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="B735" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1578</v>
+        <v>1936</v>
       </c>
       <c r="B736" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1939</v>
+        <v>1578</v>
       </c>
       <c r="B737" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="B738" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1299</v>
+        <v>1941</v>
       </c>
       <c r="B739" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1943</v>
+        <v>1299</v>
       </c>
       <c r="B740" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="B741" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="B742" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="B743" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="B744" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B745" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="B746" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="B747" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="B748" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>1287</v>
+        <v>1960</v>
       </c>
       <c r="B749" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>1963</v>
+        <v>1287</v>
       </c>
       <c r="B750" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>1503</v>
+        <v>1963</v>
       </c>
       <c r="B751" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>1965</v>
+        <v>1503</v>
       </c>
       <c r="B752" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="B753" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="B754" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="B755" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B756" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B757" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="B758" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="B759" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="B760" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B761" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
         <v>2962</v>
       </c>
-      <c r="B761" t="s">
+      <c r="B762" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fool with charity bag
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="3417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4203" uniqueCount="3419">
   <si>
     <t>Base Set</t>
   </si>
@@ -10284,6 +10284,12 @@
   </si>
   <si>
     <t>Pat Corrales 11</t>
+  </si>
+  <si>
+    <t>Richie Ashburn 51 Bowman</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-hTHtjEAU8nQ/WKNitVNyu5I/AAAAAAAAloo/UPOPcU1ljSYj2Cst1MlV7DNc01ffvHaAgCLcB/s1600/imk323.jpg</t>
   </si>
 </sst>
 </file>
@@ -20732,8 +20738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A504" workbookViewId="0">
-      <selection activeCell="B503" sqref="B503"/>
+    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="B344" sqref="B344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23392,6 +23398,14 @@
       </c>
       <c r="B343" t="s">
         <v>3370</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>3417</v>
+      </c>
+      <c r="B344" t="s">
+        <v>3418</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-write of charity bag front end
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4203" uniqueCount="3419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4207" uniqueCount="3423">
   <si>
     <t>Base Set</t>
   </si>
@@ -10290,6 +10290,18 @@
   </si>
   <si>
     <t>https://4.bp.blogspot.com/-hTHtjEAU8nQ/WKNitVNyu5I/AAAAAAAAloo/UPOPcU1ljSYj2Cst1MlV7DNc01ffvHaAgCLcB/s1600/imk323.jpg</t>
+  </si>
+  <si>
+    <t>Wes Chamberlain 94 Collectors Choice</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-SVKziKS8ia8/WKXgxjFfztI/AAAAAAAAh2M/D6JDKwPYnAgkjvn6GCrSzdLNNPAV9LP-wCLcB/s1600/wes.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-PU0c1hjB6Jk/WKXgvuhyJiI/AAAAAAAAh14/W6dj7hRi4l0zgLMiFd2ppbpluAmCuyL2gCEw/s1600/76.jpg</t>
+  </si>
+  <si>
+    <t>Wes Chamberlain 94 Collectors Choice Back</t>
   </si>
 </sst>
 </file>
@@ -20739,7 +20751,7 @@
   <dimension ref="A1:B806"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="B344" sqref="B344"/>
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23406,6 +23418,22 @@
       </c>
       <c r="B344" t="s">
         <v>3418</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>3419</v>
+      </c>
+      <c r="B345" t="s">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>3422</v>
+      </c>
+      <c r="B346" t="s">
+        <v>3421</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More charity, bunt, chachi
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4207" uniqueCount="3423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4209" uniqueCount="3425">
   <si>
     <t>Base Set</t>
   </si>
@@ -10302,6 +10302,12 @@
   </si>
   <si>
     <t>Wes Chamberlain 94 Collectors Choice Back</t>
+  </si>
+  <si>
+    <t>Mickey Moniak 2017 Topps Heritage</t>
+  </si>
+  <si>
+    <t>https://www.topps.com/wp/wp-content/uploads/2017/02/Mickey-Moniak.png</t>
   </si>
 </sst>
 </file>
@@ -20748,10 +20754,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B806"/>
+  <dimension ref="A1:B807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="C333" sqref="C333"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="B339" sqref="B339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23374,3400 +23380,3408 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>3302</v>
+        <v>3423</v>
       </c>
       <c r="B339" t="s">
-        <v>3301</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>3329</v>
+        <v>3302</v>
       </c>
       <c r="B340" t="s">
-        <v>3330</v>
+        <v>3301</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>3341</v>
+        <v>3329</v>
       </c>
       <c r="B341" t="s">
-        <v>3342</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>3362</v>
+        <v>3341</v>
       </c>
       <c r="B342" t="s">
-        <v>3361</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>3369</v>
+        <v>3362</v>
       </c>
       <c r="B343" t="s">
-        <v>3370</v>
+        <v>3361</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>3417</v>
+        <v>3369</v>
       </c>
       <c r="B344" t="s">
-        <v>3418</v>
+        <v>3370</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>3419</v>
+        <v>3417</v>
       </c>
       <c r="B345" t="s">
-        <v>3420</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
+        <v>3419</v>
+      </c>
+      <c r="B346" t="s">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
         <v>3422</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B347" t="s">
         <v>3421</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
-        <v>2387</v>
-      </c>
-    </row>
+    <row r="349" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>1518</v>
-      </c>
-      <c r="B350" t="s">
-        <v>1903</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>1490</v>
+        <v>1518</v>
       </c>
       <c r="B351" t="s">
-        <v>1491</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>259</v>
+        <v>1490</v>
       </c>
       <c r="B352" t="s">
-        <v>1500</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>1503</v>
+        <v>259</v>
       </c>
       <c r="B353" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>1507</v>
+        <v>1503</v>
       </c>
       <c r="B354" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="B355" t="s">
-        <v>1508</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>1514</v>
+        <v>1506</v>
       </c>
       <c r="B356" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>1535</v>
+        <v>1514</v>
       </c>
       <c r="B357" t="s">
-        <v>1536</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="B358" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>1777</v>
+        <v>1537</v>
       </c>
       <c r="B359" t="s">
-        <v>1778</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1898</v>
+        <v>1777</v>
       </c>
       <c r="B360" t="s">
-        <v>1899</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="B361" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>1610</v>
+        <v>1900</v>
       </c>
       <c r="B362" t="s">
-        <v>1609</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="B363" t="s">
-        <v>1615</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>1618</v>
+        <v>1614</v>
       </c>
       <c r="B364" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>1616</v>
+        <v>1618</v>
       </c>
       <c r="B365" t="s">
-        <v>1617</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="B366" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>2001</v>
+        <v>1620</v>
       </c>
       <c r="B367" t="s">
-        <v>2002</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>2158</v>
+        <v>2001</v>
       </c>
       <c r="B368" t="s">
-        <v>2159</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>2172</v>
+        <v>2158</v>
       </c>
       <c r="B369" t="s">
-        <v>2173</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>2174</v>
+        <v>2172</v>
       </c>
       <c r="B370" t="s">
-        <v>2175</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>2176</v>
+        <v>2174</v>
       </c>
       <c r="B371" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>2184</v>
+        <v>2176</v>
       </c>
       <c r="B372" t="s">
-        <v>2185</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>2196</v>
+        <v>2184</v>
       </c>
       <c r="B373" t="s">
-        <v>2197</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>2204</v>
+        <v>2196</v>
       </c>
       <c r="B374" t="s">
-        <v>2205</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
       <c r="B375" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>2222</v>
+        <v>2206</v>
       </c>
       <c r="B376" t="s">
-        <v>2223</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="B377" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="B378" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="B379" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>1514</v>
+        <v>2228</v>
       </c>
       <c r="B380" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>2231</v>
+        <v>1514</v>
       </c>
       <c r="B381" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>2234</v>
+        <v>2231</v>
       </c>
       <c r="B382" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>2242</v>
+        <v>2234</v>
       </c>
       <c r="B383" t="s">
-        <v>2243</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>2342</v>
+        <v>2242</v>
       </c>
       <c r="B384" t="s">
-        <v>2343</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="B385" t="s">
-        <v>2345</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>2346</v>
+        <v>2344</v>
       </c>
       <c r="B386" t="s">
-        <v>2347</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>2324</v>
+        <v>2346</v>
       </c>
       <c r="B387" t="s">
-        <v>2325</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="B388" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>2298</v>
+        <v>2326</v>
       </c>
       <c r="B389" t="s">
-        <v>2299</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="B390" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>2304</v>
+        <v>2300</v>
       </c>
       <c r="B391" t="s">
-        <v>2305</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
       <c r="B392" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
       <c r="B393" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>2312</v>
+        <v>2308</v>
       </c>
       <c r="B394" t="s">
-        <v>2313</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>2290</v>
+        <v>2312</v>
       </c>
       <c r="B395" t="s">
-        <v>2291</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>2350</v>
+        <v>2290</v>
       </c>
       <c r="B396" t="s">
-        <v>2351</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
       <c r="B397" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>2356</v>
+        <v>2352</v>
       </c>
       <c r="B398" t="s">
-        <v>2357</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>2360</v>
+        <v>2356</v>
       </c>
       <c r="B399" t="s">
-        <v>2361</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>2362</v>
+        <v>2360</v>
       </c>
       <c r="B400" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
       <c r="B401" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>2368</v>
+        <v>2364</v>
       </c>
       <c r="B402" t="s">
-        <v>2369</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>2370</v>
+        <v>2368</v>
       </c>
       <c r="B403" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
       <c r="B404" t="s">
-        <v>2377</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>2485</v>
+        <v>2376</v>
       </c>
       <c r="B405" t="s">
-        <v>2486</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>2489</v>
+        <v>2485</v>
       </c>
       <c r="B406" t="s">
-        <v>2490</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>2997</v>
+        <v>2489</v>
       </c>
       <c r="B407" t="s">
-        <v>2998</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>2491</v>
+        <v>2997</v>
       </c>
       <c r="B408" t="s">
-        <v>2492</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>2497</v>
+        <v>2491</v>
       </c>
       <c r="B409" t="s">
-        <v>2498</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>2501</v>
+        <v>2497</v>
       </c>
       <c r="B410" t="s">
-        <v>2502</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="B411" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
       <c r="B412" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="B413" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>2515</v>
+        <v>2507</v>
       </c>
       <c r="B414" t="s">
-        <v>2516</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="B415" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>2523</v>
+        <v>2517</v>
       </c>
       <c r="B416" t="s">
-        <v>2524</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="B417" t="s">
-        <v>2526</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>2529</v>
+        <v>2525</v>
       </c>
       <c r="B418" t="s">
-        <v>2530</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>2537</v>
+        <v>2529</v>
       </c>
       <c r="B419" t="s">
-        <v>2538</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="B420" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="B421" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>2563</v>
+        <v>2541</v>
       </c>
       <c r="B422" t="s">
-        <v>2561</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>2560</v>
+        <v>2563</v>
       </c>
       <c r="B423" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>2576</v>
+        <v>2560</v>
       </c>
       <c r="B424" t="s">
-        <v>2577</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="B425" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="B426" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>2594</v>
+        <v>2580</v>
       </c>
       <c r="B427" t="s">
-        <v>2595</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>2598</v>
+        <v>2594</v>
       </c>
       <c r="B428" t="s">
-        <v>2599</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>2651</v>
+        <v>2598</v>
       </c>
       <c r="B429" t="s">
-        <v>2650</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>1388</v>
+        <v>2651</v>
       </c>
       <c r="B430" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>2653</v>
+        <v>1388</v>
       </c>
       <c r="B431" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="B432" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>2660</v>
+        <v>2655</v>
       </c>
       <c r="B433" t="s">
-        <v>2659</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>2671</v>
+        <v>2660</v>
       </c>
       <c r="B434" t="s">
-        <v>2672</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
       <c r="B435" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>2678</v>
+        <v>2673</v>
       </c>
       <c r="B436" t="s">
-        <v>2677</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>2746</v>
+        <v>2678</v>
       </c>
       <c r="B437" t="s">
-        <v>2747</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>2771</v>
+        <v>2746</v>
       </c>
       <c r="B438" t="s">
-        <v>2772</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>2799</v>
+        <v>2771</v>
       </c>
       <c r="B439" t="s">
-        <v>2800</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>2802</v>
+        <v>2799</v>
       </c>
       <c r="B440" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>2814</v>
+        <v>2802</v>
       </c>
       <c r="B441" t="s">
-        <v>2815</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>2855</v>
+        <v>2814</v>
       </c>
       <c r="B442" t="s">
-        <v>2856</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="B443" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="B444" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>2863</v>
+        <v>2859</v>
       </c>
       <c r="B445" t="s">
-        <v>2864</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="B446" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>2870</v>
+        <v>2865</v>
       </c>
       <c r="B447" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>2901</v>
+        <v>2870</v>
       </c>
       <c r="B448" t="s">
-        <v>2902</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>2904</v>
+        <v>2901</v>
       </c>
       <c r="B449" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="B450" t="s">
-        <v>2906</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="B451" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="B452" t="s">
-        <v>2911</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="B453" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>2914</v>
+        <v>2910</v>
       </c>
       <c r="B454" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="B455" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>2919</v>
+        <v>2915</v>
       </c>
       <c r="B456" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>2918</v>
+        <v>2919</v>
       </c>
       <c r="B457" t="s">
-        <v>2922</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="B458" t="s">
-        <v>2920</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>1889</v>
+        <v>2921</v>
       </c>
       <c r="B459" t="s">
-        <v>2923</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>2925</v>
+        <v>1889</v>
       </c>
       <c r="B460" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="B461" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="B462" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
       <c r="B463" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="B464" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="B465" t="s">
-        <v>2935</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="B466" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>2939</v>
+        <v>2936</v>
       </c>
       <c r="B467" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="B468" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="B469" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="B470" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="B471" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="B472" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>2953</v>
+        <v>2949</v>
       </c>
       <c r="B473" t="s">
-        <v>2954</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="B474" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="B475" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>2019</v>
+        <v>2957</v>
       </c>
       <c r="B476" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>2036</v>
+        <v>2019</v>
       </c>
       <c r="B477" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>2970</v>
+        <v>2036</v>
       </c>
       <c r="B478" t="s">
-        <v>2971</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>2972</v>
+        <v>2970</v>
       </c>
       <c r="B479" t="s">
-        <v>2973</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>2975</v>
+        <v>2972</v>
       </c>
       <c r="B480" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>2983</v>
+        <v>2975</v>
       </c>
       <c r="B481" t="s">
-        <v>2984</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="B482" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>2999</v>
+        <v>2985</v>
       </c>
       <c r="B483" t="s">
-        <v>3000</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>3048</v>
+        <v>2999</v>
       </c>
       <c r="B484" t="s">
-        <v>3049</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>3139</v>
+        <v>3048</v>
       </c>
       <c r="B485" t="s">
-        <v>3138</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>3141</v>
+        <v>3139</v>
       </c>
       <c r="B486" t="s">
-        <v>3140</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>3143</v>
+        <v>3141</v>
       </c>
       <c r="B487" t="s">
-        <v>3142</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>3292</v>
+        <v>3143</v>
       </c>
       <c r="B488" t="s">
-        <v>3291</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>3294</v>
+        <v>3292</v>
       </c>
       <c r="B489" t="s">
-        <v>3293</v>
+        <v>3291</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>3296</v>
+        <v>3294</v>
       </c>
       <c r="B490" t="s">
-        <v>3295</v>
+        <v>3293</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
       <c r="B491" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>3331</v>
+        <v>3298</v>
       </c>
       <c r="B492" t="s">
-        <v>3332</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>3350</v>
+        <v>3331</v>
       </c>
       <c r="B493" t="s">
-        <v>3351</v>
+        <v>3332</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>3367</v>
+        <v>3350</v>
       </c>
       <c r="B494" t="s">
-        <v>3368</v>
+        <v>3351</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>3378</v>
+        <v>3367</v>
       </c>
       <c r="B495" t="s">
-        <v>3379</v>
+        <v>3368</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>3380</v>
+        <v>3378</v>
       </c>
       <c r="B496" t="s">
-        <v>3381</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>3382</v>
+        <v>3380</v>
       </c>
       <c r="B497" t="s">
-        <v>3383</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>3385</v>
+        <v>3382</v>
       </c>
       <c r="B498" t="s">
-        <v>3384</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>3387</v>
+        <v>3385</v>
       </c>
       <c r="B499" t="s">
-        <v>3386</v>
+        <v>3384</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
+        <v>3387</v>
+      </c>
+      <c r="B500" t="s">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
         <v>3388</v>
       </c>
-      <c r="B500" t="s">
+      <c r="B501" t="s">
         <v>3389</v>
-      </c>
-    </row>
-    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A502" t="s">
-        <v>3391</v>
-      </c>
-      <c r="B502" t="s">
-        <v>3392</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>3406</v>
+        <v>3391</v>
       </c>
       <c r="B503" t="s">
-        <v>3393</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>3407</v>
+        <v>3406</v>
       </c>
       <c r="B504" t="s">
-        <v>3394</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>3408</v>
+        <v>3407</v>
       </c>
       <c r="B505" t="s">
-        <v>3395</v>
+        <v>3394</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>3409</v>
+        <v>3408</v>
       </c>
       <c r="B506" t="s">
-        <v>3396</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>3410</v>
+        <v>3409</v>
       </c>
       <c r="B507" t="s">
-        <v>3397</v>
+        <v>3396</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>3411</v>
+        <v>3410</v>
       </c>
       <c r="B508" t="s">
-        <v>3398</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>3412</v>
+        <v>3411</v>
       </c>
       <c r="B509" t="s">
-        <v>3399</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="B510" t="s">
-        <v>3400</v>
+        <v>3399</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>3414</v>
+        <v>3413</v>
       </c>
       <c r="B511" t="s">
-        <v>3401</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>3415</v>
+        <v>3414</v>
       </c>
       <c r="B512" t="s">
-        <v>3402</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>3416</v>
+        <v>3415</v>
       </c>
       <c r="B513" t="s">
-        <v>3403</v>
+        <v>3402</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
+        <v>3416</v>
+      </c>
+      <c r="B514" t="s">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
         <v>3405</v>
       </c>
-      <c r="B514" t="s">
+      <c r="B515" t="s">
         <v>3404</v>
-      </c>
-    </row>
-    <row r="528" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A528" t="s">
-        <v>2447</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>2354</v>
-      </c>
-      <c r="B529" t="s">
-        <v>2355</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>2372</v>
+        <v>2354</v>
       </c>
       <c r="B530" t="s">
-        <v>2373</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>2994</v>
+        <v>2372</v>
       </c>
       <c r="B531" t="s">
-        <v>2993</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>2965</v>
+        <v>2994</v>
       </c>
       <c r="B532" t="s">
-        <v>2964</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>3366</v>
+        <v>2965</v>
       </c>
       <c r="B533" t="s">
-        <v>3365</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>2978</v>
+        <v>3366</v>
       </c>
       <c r="B534" t="s">
-        <v>2979</v>
+        <v>3365</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>3289</v>
+        <v>2978</v>
       </c>
       <c r="B535" t="s">
-        <v>3290</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>3316</v>
+        <v>3289</v>
       </c>
       <c r="B536" t="s">
-        <v>3315</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>3328</v>
+        <v>3316</v>
       </c>
       <c r="B537" t="s">
-        <v>3327</v>
+        <v>3315</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
+        <v>3328</v>
+      </c>
+      <c r="B538" t="s">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
         <v>3371</v>
       </c>
-      <c r="B538" t="s">
+      <c r="B539" t="s">
         <v>3372</v>
-      </c>
-    </row>
-    <row r="540" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A540" t="s">
-        <v>2809</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>2810</v>
-      </c>
-      <c r="B541" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B542" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
         <v>2812</v>
       </c>
-      <c r="B542" t="s">
+      <c r="B543" t="s">
         <v>2813</v>
-      </c>
-    </row>
-    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A544" t="s">
-        <v>2867</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B545" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>2118</v>
+        <v>1982</v>
       </c>
       <c r="B546" t="s">
-        <v>2117</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1543</v>
+        <v>2118</v>
       </c>
       <c r="B547" t="s">
-        <v>1544</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>1578</v>
+        <v>1543</v>
       </c>
       <c r="B548" t="s">
-        <v>2871</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1972</v>
+        <v>1578</v>
       </c>
       <c r="B549" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1936</v>
+        <v>1972</v>
       </c>
       <c r="B550" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>2875</v>
+        <v>1936</v>
       </c>
       <c r="B551" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="B552" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>1593</v>
+        <v>2877</v>
       </c>
       <c r="B553" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>2880</v>
+        <v>1593</v>
       </c>
       <c r="B554" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="B555" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>1402</v>
+        <v>2882</v>
       </c>
       <c r="B556" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>2885</v>
+        <v>1402</v>
       </c>
       <c r="B557" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="B558" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="B559" t="s">
-        <v>2889</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>1460</v>
+        <v>2888</v>
       </c>
       <c r="B560" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>2028</v>
+        <v>1460</v>
       </c>
       <c r="B561" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>1299</v>
+        <v>2028</v>
       </c>
       <c r="B562" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>2893</v>
+        <v>1299</v>
       </c>
       <c r="B563" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>1965</v>
+        <v>2893</v>
       </c>
       <c r="B564" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>2896</v>
+        <v>1965</v>
       </c>
       <c r="B565" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>2545</v>
+        <v>2896</v>
       </c>
       <c r="B566" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>2899</v>
+        <v>2545</v>
       </c>
       <c r="B567" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1597</v>
+        <v>2899</v>
       </c>
       <c r="B568" t="s">
-        <v>2471</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>2170</v>
+        <v>1597</v>
       </c>
       <c r="B569" t="s">
-        <v>2171</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B570" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
         <v>3325</v>
       </c>
-      <c r="B570" t="s">
+      <c r="B571" t="s">
         <v>3326</v>
-      </c>
-    </row>
-    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A572" t="s">
-        <v>2389</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B573" t="s">
-        <v>1545</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1547</v>
+        <v>1455</v>
       </c>
       <c r="B574" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="B575" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="B576" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B577" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="B578" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1482</v>
+        <v>1555</v>
       </c>
       <c r="B579" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>1558</v>
+        <v>1482</v>
       </c>
       <c r="B580" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1606</v>
+        <v>1558</v>
       </c>
       <c r="B581" t="s">
-        <v>1607</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1560</v>
+        <v>1606</v>
       </c>
       <c r="B582" t="s">
-        <v>1559</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="B583" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="B584" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="B585" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B586" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B587" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B588" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="B589" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="B590" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="B591" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1388</v>
+        <v>1578</v>
       </c>
       <c r="B592" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1581</v>
+        <v>1388</v>
       </c>
       <c r="B593" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="B594" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="B595" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="B596" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="B597" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="B598" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="B599" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="B600" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="B601" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="B602" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="B603" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="B604" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B605" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
         <v>1603</v>
       </c>
-      <c r="B605" t="s">
+      <c r="B606" t="s">
         <v>1605</v>
-      </c>
-    </row>
-    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A608" t="s">
-        <v>2472</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>2473</v>
-      </c>
-      <c r="B609" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="B610" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="B611" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="B612" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B613" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
         <v>2481</v>
       </c>
-      <c r="B613" t="s">
+      <c r="B614" t="s">
         <v>2482</v>
-      </c>
-    </row>
-    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A616" t="s">
-        <v>2582</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B617" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>2584</v>
+        <v>1455</v>
       </c>
       <c r="B618" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>1589</v>
+        <v>2584</v>
       </c>
       <c r="B619" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1566</v>
+        <v>1589</v>
       </c>
       <c r="B620" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>1602</v>
+        <v>1566</v>
       </c>
       <c r="B621" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1150</v>
+        <v>1602</v>
       </c>
       <c r="B622" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>1219</v>
+        <v>1150</v>
       </c>
       <c r="B623" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1597</v>
+        <v>1219</v>
       </c>
       <c r="B624" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>2597</v>
+        <v>1597</v>
       </c>
       <c r="B625" t="s">
-        <v>2596</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1593</v>
+        <v>2597</v>
       </c>
       <c r="B626" t="s">
-        <v>2600</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1560</v>
+        <v>1593</v>
       </c>
       <c r="B627" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1595</v>
+        <v>1560</v>
       </c>
       <c r="B628" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>1549</v>
+        <v>1595</v>
       </c>
       <c r="B629" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B630" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
         <v>1388</v>
       </c>
-      <c r="B630" t="s">
+      <c r="B631" t="s">
         <v>2987</v>
-      </c>
-    </row>
-    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A634" t="s">
-        <v>2391</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B635" t="s">
-        <v>1636</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1388</v>
+        <v>1520</v>
       </c>
       <c r="B636" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1639</v>
+        <v>1388</v>
       </c>
       <c r="B637" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>1632</v>
+        <v>1639</v>
       </c>
       <c r="B638" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>1641</v>
+        <v>1632</v>
       </c>
       <c r="B639" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
       <c r="B640" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>1451</v>
+        <v>1644</v>
       </c>
       <c r="B641" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1560</v>
+        <v>1451</v>
       </c>
       <c r="B642" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1648</v>
+        <v>1560</v>
       </c>
       <c r="B643" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B644" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="B645" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="B646" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>3359</v>
+        <v>1653</v>
       </c>
       <c r="B647" t="s">
-        <v>3360</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1655</v>
+        <v>3359</v>
       </c>
       <c r="B648" t="s">
-        <v>1656</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>2150</v>
+        <v>1655</v>
       </c>
       <c r="B649" t="s">
-        <v>2151</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>2591</v>
+        <v>2150</v>
       </c>
       <c r="B650" t="s">
-        <v>2590</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>3282</v>
+        <v>2591</v>
       </c>
       <c r="B651" t="s">
-        <v>3283</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1683</v>
+        <v>3282</v>
       </c>
       <c r="B652" t="s">
-        <v>2621</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1593</v>
+        <v>1683</v>
       </c>
       <c r="B653" t="s">
-        <v>2662</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>2016</v>
+        <v>1593</v>
       </c>
       <c r="B654" t="s">
-        <v>3281</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>3320</v>
+        <v>2016</v>
       </c>
       <c r="B655" t="s">
-        <v>3319</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B656" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
         <v>1455</v>
       </c>
-      <c r="B656" t="s">
+      <c r="B657" t="s">
         <v>3358</v>
-      </c>
-    </row>
-    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A658" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B659" t="s">
-        <v>1657</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1447</v>
+        <v>1451</v>
       </c>
       <c r="B660" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>1521</v>
+        <v>1447</v>
       </c>
       <c r="B661" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>1660</v>
+        <v>1521</v>
       </c>
       <c r="B662" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="B663" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>1639</v>
+        <v>1663</v>
       </c>
       <c r="B664" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1651</v>
+        <v>1639</v>
       </c>
       <c r="B665" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1641</v>
+        <v>1651</v>
       </c>
       <c r="B666" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1667</v>
+        <v>1641</v>
       </c>
       <c r="B667" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1160</v>
+        <v>1667</v>
       </c>
       <c r="B668" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1459</v>
+        <v>1160</v>
       </c>
       <c r="B669" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1388</v>
+        <v>1459</v>
       </c>
       <c r="B670" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1632</v>
+        <v>1388</v>
       </c>
       <c r="B671" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1520</v>
+        <v>1632</v>
       </c>
       <c r="B672" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1674</v>
+        <v>1520</v>
       </c>
       <c r="B673" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="B674" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="B675" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="B676" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1644</v>
+        <v>1681</v>
       </c>
       <c r="B677" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>1683</v>
+        <v>1644</v>
       </c>
       <c r="B678" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1482</v>
+        <v>1683</v>
       </c>
       <c r="B679" t="s">
-        <v>1865</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>2152</v>
+        <v>1482</v>
       </c>
       <c r="B680" t="s">
-        <v>2153</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1699</v>
+        <v>2152</v>
       </c>
       <c r="B681" t="s">
-        <v>2641</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1712</v>
+        <v>1699</v>
       </c>
       <c r="B682" t="s">
-        <v>3148</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>3285</v>
+        <v>1712</v>
       </c>
       <c r="B683" t="s">
-        <v>3284</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>2016</v>
+        <v>3285</v>
       </c>
       <c r="B684" t="s">
-        <v>3340</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B685" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
         <v>1460</v>
       </c>
-      <c r="B685" t="s">
+      <c r="B686" t="s">
         <v>3343</v>
-      </c>
-    </row>
-    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A691" t="s">
-        <v>2393</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B692" t="s">
-        <v>1686</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>3308</v>
+        <v>1685</v>
       </c>
       <c r="B693" t="s">
-        <v>3307</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1523</v>
+        <v>3308</v>
       </c>
       <c r="B694" t="s">
-        <v>1687</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B695" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1689</v>
+        <v>1524</v>
       </c>
       <c r="B696" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="B697" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="B698" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="B699" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B700" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
         <v>1459</v>
       </c>
-      <c r="B700" t="s">
+      <c r="B701" t="s">
         <v>1697</v>
-      </c>
-    </row>
-    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A702" t="s">
-        <v>2394</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B703" t="s">
-        <v>1729</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B704" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1483</v>
+        <v>1699</v>
       </c>
       <c r="B705" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1700</v>
+        <v>1483</v>
       </c>
       <c r="B706" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B707" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="B708" t="s">
-        <v>1702</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>1667</v>
+        <v>1703</v>
       </c>
       <c r="B709" t="s">
-        <v>1747</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1704</v>
+        <v>1667</v>
       </c>
       <c r="B710" t="s">
-        <v>1705</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="B711" t="s">
-        <v>1734</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B712" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B713" t="s">
-        <v>1709</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="B714" t="s">
-        <v>1736</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1459</v>
+        <v>1710</v>
       </c>
       <c r="B715" t="s">
-        <v>1711</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1689</v>
+        <v>1459</v>
       </c>
       <c r="B716" t="s">
-        <v>1737</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1712</v>
+        <v>1689</v>
       </c>
       <c r="B717" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1160</v>
+        <v>1712</v>
       </c>
       <c r="B718" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1714</v>
+        <v>1160</v>
       </c>
       <c r="B719" t="s">
-        <v>1713</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1696</v>
+        <v>1714</v>
       </c>
       <c r="B720" t="s">
-        <v>1740</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1715</v>
+        <v>1696</v>
       </c>
       <c r="B721" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="B722" t="s">
-        <v>1716</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1693</v>
+        <v>1717</v>
       </c>
       <c r="B723" t="s">
-        <v>1742</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1524</v>
+        <v>1693</v>
       </c>
       <c r="B724" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1718</v>
+        <v>1524</v>
       </c>
       <c r="B725" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="B726" t="s">
-        <v>1719</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B727" t="s">
-        <v>1745</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="B728" t="s">
-        <v>1722</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="B729" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B730" t="s">
-        <v>1746</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B731" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" t="s">
         <v>1728</v>
       </c>
-      <c r="B731" t="s">
+      <c r="B732" t="s">
         <v>1727</v>
-      </c>
-    </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A733" t="s">
-        <v>2395</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B734" t="s">
-        <v>1763</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="B735" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1689</v>
+        <v>1764</v>
       </c>
       <c r="B736" t="s">
-        <v>1870</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1872</v>
+        <v>1689</v>
       </c>
       <c r="B737" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1533</v>
+        <v>1872</v>
       </c>
       <c r="B738" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1160</v>
+        <v>1533</v>
       </c>
       <c r="B739" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1875</v>
+        <v>1160</v>
       </c>
       <c r="B740" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B741" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1880</v>
+        <v>1877</v>
       </c>
       <c r="B742" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B743" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1718</v>
+        <v>1881</v>
       </c>
       <c r="B744" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1885</v>
+        <v>1718</v>
       </c>
       <c r="B745" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1451</v>
+        <v>1885</v>
       </c>
       <c r="B746" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1887</v>
+        <v>1451</v>
       </c>
       <c r="B747" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="B748" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="B749" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B750" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>1699</v>
+        <v>1893</v>
       </c>
       <c r="B751" t="s">
-        <v>3323</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B752" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
         <v>1524</v>
       </c>
-      <c r="B752" t="s">
+      <c r="B753" t="s">
         <v>3324</v>
-      </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A756" t="s">
-        <v>2396</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B757" t="s">
-        <v>1904</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>1906</v>
+        <v>1161</v>
       </c>
       <c r="B758" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>1203</v>
+        <v>1906</v>
       </c>
       <c r="B759" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>1236</v>
+        <v>1203</v>
       </c>
       <c r="B760" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>1408</v>
+        <v>1236</v>
       </c>
       <c r="B761" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>1230</v>
+        <v>1408</v>
       </c>
       <c r="B762" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>252</v>
+        <v>1230</v>
       </c>
       <c r="B763" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>1187</v>
+        <v>252</v>
       </c>
       <c r="B764" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>1238</v>
+        <v>1187</v>
       </c>
       <c r="B765" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B766" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A767" t="s">
         <v>1181</v>
       </c>
-      <c r="B766" t="s">
+      <c r="B767" t="s">
         <v>1914</v>
-      </c>
-    </row>
-    <row r="768" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A768" t="s">
-        <v>2397</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B769" t="s">
-        <v>1916</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>1756</v>
+        <v>1915</v>
       </c>
       <c r="B770" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>1919</v>
+        <v>1756</v>
       </c>
       <c r="B771" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="B772" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B773" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="B774" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B775" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="B776" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>1402</v>
+        <v>1929</v>
       </c>
       <c r="B777" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>1934</v>
+        <v>1402</v>
       </c>
       <c r="B778" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="B779" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="B780" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>1578</v>
+        <v>1936</v>
       </c>
       <c r="B781" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>1939</v>
+        <v>1578</v>
       </c>
       <c r="B782" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="B783" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>1299</v>
+        <v>1941</v>
       </c>
       <c r="B784" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>1943</v>
+        <v>1299</v>
       </c>
       <c r="B785" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="B786" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="B787" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="B788" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="B789" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B790" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="B791" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="B792" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="B793" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>1287</v>
+        <v>1960</v>
       </c>
       <c r="B794" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>1963</v>
+        <v>1287</v>
       </c>
       <c r="B795" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>1503</v>
+        <v>1963</v>
       </c>
       <c r="B796" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>1965</v>
+        <v>1503</v>
       </c>
       <c r="B797" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="B798" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="B799" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="B800" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B801" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B802" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="B803" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="B804" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="B805" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B806" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A807" t="s">
         <v>2962</v>
       </c>
-      <c r="B806" t="s">
+      <c r="B807" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working loadstage and library
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23460" windowHeight="10695"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="21" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4209" uniqueCount="3425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4213" uniqueCount="3425">
   <si>
     <t>Base Set</t>
   </si>
@@ -9428,9 +9428,6 @@
     <t>https://4.bp.blogspot.com/-AcYeDOHUAqQ/V_AGDTyAapI/AAAAAAAAeSc/W01x_DTccMcttca9NOYzOsdL5QwiSTVLwCLcB/s1600/Gomez.jpg</t>
   </si>
   <si>
-    <t>https://3.bp.blogspot.com/-LSb8b0_zsU8/V_AGDsaWmlI/AAAAAAAAeSg/uKtR7xOr-Zk8bhxf70HMjeikcuFYmZe4gCLcB/s1600/Gonzalez.jpg</t>
-  </si>
-  <si>
     <t>https://4.bp.blogspot.com/-xtmOQplwPb0/V_AGELIjHDI/AAAAAAAAeS4/Tq0VBQ4P5_kOZ0CU4SS_4Q0jt4uZ7vrZgCLcB/s1600/Mariot.jpg</t>
   </si>
   <si>
@@ -9899,9 +9896,6 @@
     <t>Mickey Moniak 2016 Bowman Draft</t>
   </si>
   <si>
-    <t>https://2.bp.blogspot.com/-64_8tpE_rSI/WEIkYUdUIbI/AAAAAAAAevs/2TvfaTzd-JoUKsDu3PN4-LDX96N5NMsfQCLcB/s1600/2017%2BChachi%2BNew%2BAdditions%2B%25233%2BRollins.jpg</t>
-  </si>
-  <si>
     <t>Bobby Jones</t>
   </si>
   <si>
@@ -9950,9 +9944,6 @@
     <t>https://2.bp.blogspot.com/-qCurIO8WHZU/WEoG8mwpePI/AAAAAAAAey8/o6xHdlRJ8cUf_iEjhhBZyK-4kJMbnLzOACLcB/s1600/2017%2BChachi%2BDepartures%2B%25236%2BEllis.jpg</t>
   </si>
   <si>
-    <t>https://3.bp.blogspot.com/-LwkH03CowBs/WFHzQhcq4mI/AAAAAAAAe00/NtFk4CEaX6crqefRIBBK1VJYbdZa4mZ5QCLcB/s1600/2017%2BChachi%2BNew%2BAdditions%2B%25235%2BShaffer.jpg</t>
-  </si>
-  <si>
     <t>https://4.bp.blogspot.com/-a45GEDuG_yg/WFHzQkK2nkI/AAAAAAAAe0w/d6M2jXq9cEY1BeONFP3ed_bul2l3tBGkwCLcB/s1600/2017%2BChachi%2BDepartures%2B%25237%2BBurriss.jpg</t>
   </si>
   <si>
@@ -9974,12 +9965,6 @@
     <t>https://1.bp.blogspot.com/--GFH4Qt3ulk/WFnR8yuqD7I/AAAAAAAAe1c/-5tQ1czFc-Ajm9z_lT7T0_QddPhgURrHQCLcB/s1600/2017%2BChachi%2BDepartures%2B%25239%2BKlein.jpg</t>
   </si>
   <si>
-    <t>x-Richie Shaffer</t>
-  </si>
-  <si>
-    <t>x-David Rollins</t>
-  </si>
-  <si>
     <t>https://3.bp.blogspot.com/-tqtawj7nwuI/WFnjH-qE0RI/AAAAAAAACkc/TYeyQ2l-W5UfmFQ1FGVlxpC_ykTURrZBgCLcB/s1600/1992-93%2BUpper%2BDeck%2Bbasketball_0003.jpg</t>
   </si>
   <si>
@@ -10308,6 +10293,21 @@
   </si>
   <si>
     <t>https://www.topps.com/wp/wp-content/uploads/2017/02/Mickey-Moniak.png</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-zCFk6YVs_rc/WKyaP9DPt3I/AAAAAAAAfDE/9CFV4cUNuc04D8dLxYRjFljLo4wP-KFiQCLcB/s1600/2017%2BChachi%2BDepartures%2B%252310%2BParedes.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-mxDJTw3WTeU/WKyaPzdID2I/AAAAAAAAfDA/yN66fmMogIk9A1wxAUpMRshhbigicZmNwCLcB/s1600/2017%2BChachi%2BDepartures%2B%252312%2BGonzalez.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-GtYo14-6nvk/WKyaP2QcFLI/AAAAAAAAfC8/D_q1KD6ZB2IdDdJVyUkzH52sW20HoeCXgCLcB/s1600/2017%2BChachi%2BDepartures%2B%252313%2BBourjos.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-JnLP7Xsy67M/WKyaQJVlx_I/AAAAAAAAfDI/bYrpJK4nuREpmkeLVWk4yI-EoLddsEH-ACLcB/s1600/2017%2BChachi%2BDepartures%2B%252314%2BRussell.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-wY32bdaCn5I/WKyaQGj06rI/AAAAAAAAfDM/sMF1uzy32wIa1wDB8vxl8MpwjcCw2567ACLcB/s1600/2017%2BChachi%2BDepartures%2B%252315%2BHernandez%2BD.jpg</t>
   </si>
 </sst>
 </file>
@@ -10675,10 +10675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10696,7 +10696,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10848,7 +10848,7 @@
         <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>3133</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -10856,7 +10856,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>3134</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -10864,7 +10864,7 @@
         <v>2063</v>
       </c>
       <c r="B24" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -10872,7 +10872,7 @@
         <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -10880,23 +10880,23 @@
         <v>1859</v>
       </c>
       <c r="B26" t="s">
-        <v>3151</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B27" t="s">
         <v>3152</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3153</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>3153</v>
+      </c>
+      <c r="B28" t="s">
         <v>3154</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3155</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -10904,7 +10904,7 @@
         <v>2610</v>
       </c>
       <c r="B29" t="s">
-        <v>3156</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -10912,15 +10912,15 @@
         <v>2612</v>
       </c>
       <c r="B30" t="s">
-        <v>3157</v>
+        <v>3156</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3159</v>
+        <v>3158</v>
       </c>
       <c r="B31" t="s">
-        <v>3158</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -10928,31 +10928,31 @@
         <v>2836</v>
       </c>
       <c r="B32" t="s">
-        <v>3160</v>
+        <v>3159</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B33" t="s">
         <v>3161</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3162</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B34" t="s">
         <v>3163</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3164</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>3164</v>
+      </c>
+      <c r="B35" t="s">
         <v>3165</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3166</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -10960,23 +10960,23 @@
         <v>239</v>
       </c>
       <c r="B36" t="s">
-        <v>3167</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>3167</v>
+      </c>
+      <c r="B37" t="s">
         <v>3168</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3169</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3337</v>
+        <v>3332</v>
       </c>
       <c r="B38" t="s">
-        <v>3336</v>
+        <v>3331</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -10986,108 +10986,108 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>3313</v>
+        <v>3104</v>
       </c>
       <c r="B41" t="s">
-        <v>3305</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3104</v>
+        <v>3107</v>
       </c>
       <c r="B42" t="s">
-        <v>3105</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3107</v>
+        <v>3297</v>
       </c>
       <c r="B43" t="s">
-        <v>3106</v>
+        <v>3298</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3314</v>
+        <v>3307</v>
       </c>
       <c r="B44" t="s">
-        <v>3288</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3299</v>
+        <v>3348</v>
       </c>
       <c r="B45" t="s">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>3310</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3309</v>
+        <v>3347</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>3353</v>
-      </c>
       <c r="B47" t="s">
-        <v>3352</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3108</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>3108</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>2627</v>
       </c>
       <c r="B51" t="s">
-        <v>3109</v>
+        <v>3146</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="B52" t="s">
-        <v>3146</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>2627</v>
+        <v>2837</v>
       </c>
       <c r="B53" t="s">
-        <v>3147</v>
+        <v>3301</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>2567</v>
       </c>
       <c r="B54" t="s">
-        <v>3150</v>
+        <v>3302</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>2837</v>
+        <v>3015</v>
       </c>
       <c r="B55" t="s">
         <v>3303</v>
@@ -11095,76 +11095,92 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>2567</v>
+        <v>140</v>
       </c>
       <c r="B56" t="s">
-        <v>3304</v>
+        <v>3308</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>3015</v>
+        <v>2462</v>
       </c>
       <c r="B57" t="s">
-        <v>3306</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>3311</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2462</v>
+        <v>2046</v>
       </c>
       <c r="B59" t="s">
-        <v>3312</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B60" t="s">
-        <v>3335</v>
+        <v>3421</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3422</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
       <c r="B62" t="s">
-        <v>3149</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>3148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>2460</v>
       </c>
-      <c r="B63" t="s">
-        <v>3132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>143</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>3131</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>1757</v>
       </c>
-      <c r="B67" t="s">
-        <v>3390</v>
+      <c r="B70" t="s">
+        <v>3385</v>
       </c>
     </row>
   </sheetData>
@@ -13698,7 +13714,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>3206</v>
+        <v>3205</v>
       </c>
     </row>
   </sheetData>
@@ -17749,15 +17765,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>3170</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3171</v>
+        <v>3170</v>
       </c>
       <c r="B50" t="s">
-        <v>3179</v>
+        <v>3178</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -17765,23 +17781,23 @@
         <v>270</v>
       </c>
       <c r="B51" t="s">
-        <v>3180</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
       <c r="B52" t="s">
-        <v>3181</v>
+        <v>3180</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3173</v>
+        <v>3172</v>
       </c>
       <c r="B53" t="s">
-        <v>3182</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -17789,79 +17805,79 @@
         <v>267</v>
       </c>
       <c r="B54" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>3174</v>
+        <v>3173</v>
       </c>
       <c r="B55" t="s">
-        <v>3184</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>3175</v>
+        <v>3174</v>
       </c>
       <c r="B56" t="s">
-        <v>3185</v>
+        <v>3184</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>3176</v>
+        <v>3175</v>
       </c>
       <c r="B57" t="s">
-        <v>3186</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>3177</v>
+        <v>3176</v>
       </c>
       <c r="B58" t="s">
-        <v>3187</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>3178</v>
+        <v>3177</v>
       </c>
       <c r="B59" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>3189</v>
+        <v>3188</v>
       </c>
       <c r="B60" t="s">
-        <v>3196</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>3190</v>
+        <v>3189</v>
       </c>
       <c r="B61" t="s">
-        <v>3197</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="B62" t="s">
-        <v>3198</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>3192</v>
+        <v>3191</v>
       </c>
       <c r="B63" t="s">
-        <v>3199</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -17869,7 +17885,7 @@
         <v>271</v>
       </c>
       <c r="B64" t="s">
-        <v>3200</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -17877,7 +17893,7 @@
         <v>268</v>
       </c>
       <c r="B65" t="s">
-        <v>3201</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -17885,60 +17901,60 @@
         <v>269</v>
       </c>
       <c r="B66" t="s">
-        <v>3202</v>
+        <v>3201</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>3193</v>
+        <v>3192</v>
       </c>
       <c r="B67" t="s">
-        <v>3203</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="B68" t="s">
-        <v>3204</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>3195</v>
+        <v>3194</v>
       </c>
       <c r="B69" t="s">
-        <v>3205</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>3207</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="B72" t="s">
-        <v>3216</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>3209</v>
+        <v>3208</v>
       </c>
       <c r="B73" t="s">
-        <v>3217</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>3210</v>
+        <v>3209</v>
       </c>
       <c r="B74" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -17946,15 +17962,15 @@
         <v>1490</v>
       </c>
       <c r="B75" t="s">
-        <v>3219</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="B76" t="s">
-        <v>3220</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -17962,15 +17978,15 @@
         <v>1925</v>
       </c>
       <c r="B77" t="s">
-        <v>3221</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="B78" t="s">
-        <v>3222</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -17978,60 +17994,60 @@
         <v>1933</v>
       </c>
       <c r="B79" t="s">
-        <v>3223</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>3213</v>
+        <v>3212</v>
       </c>
       <c r="B80" t="s">
-        <v>3224</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
       <c r="B81" t="s">
-        <v>3225</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>3215</v>
+        <v>3214</v>
       </c>
       <c r="B82" t="s">
-        <v>3226</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>3230</v>
+        <v>3229</v>
       </c>
       <c r="B85" t="s">
-        <v>3237</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>3231</v>
+        <v>3230</v>
       </c>
       <c r="B86" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>3175</v>
+        <v>3174</v>
       </c>
       <c r="B87" t="s">
-        <v>3239</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -18039,7 +18055,7 @@
         <v>265</v>
       </c>
       <c r="B88" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -18047,7 +18063,7 @@
         <v>1933</v>
       </c>
       <c r="B89" t="s">
-        <v>3241</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -18055,31 +18071,31 @@
         <v>1939</v>
       </c>
       <c r="B90" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>3232</v>
+        <v>3231</v>
       </c>
       <c r="B91" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
       <c r="B92" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>3233</v>
+        <v>3232</v>
       </c>
       <c r="B93" t="s">
-        <v>3245</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -18087,23 +18103,23 @@
         <v>1926</v>
       </c>
       <c r="B94" t="s">
-        <v>3246</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>3234</v>
+        <v>3233</v>
       </c>
       <c r="B95" t="s">
-        <v>3247</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>3235</v>
+        <v>3234</v>
       </c>
       <c r="B96" t="s">
-        <v>3248</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -18111,7 +18127,7 @@
         <v>1923</v>
       </c>
       <c r="B97" t="s">
-        <v>3249</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -18119,15 +18135,15 @@
         <v>1963</v>
       </c>
       <c r="B98" t="s">
-        <v>3250</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>3236</v>
+        <v>3235</v>
       </c>
       <c r="B99" t="s">
-        <v>3251</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -18135,20 +18151,20 @@
         <v>1968</v>
       </c>
       <c r="B100" t="s">
-        <v>3252</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>3231</v>
+        <v>3230</v>
       </c>
       <c r="B103" t="s">
-        <v>3269</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -18156,23 +18172,23 @@
         <v>1946</v>
       </c>
       <c r="B104" t="s">
-        <v>3268</v>
+        <v>3267</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>3254</v>
+        <v>3253</v>
       </c>
       <c r="B105" t="s">
-        <v>3267</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="B106" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -18180,31 +18196,31 @@
         <v>1970</v>
       </c>
       <c r="B107" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="B108" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>3257</v>
+        <v>3256</v>
       </c>
       <c r="B109" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>3258</v>
+        <v>3257</v>
       </c>
       <c r="B110" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -18212,20 +18228,20 @@
         <v>1968</v>
       </c>
       <c r="B111" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>3258</v>
+      </c>
+      <c r="B112" t="s">
         <v>3259</v>
-      </c>
-      <c r="B112" t="s">
-        <v>3260</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>3272</v>
+        <v>3271</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -18233,7 +18249,7 @@
         <v>1960</v>
       </c>
       <c r="B115" t="s">
-        <v>3273</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -18241,7 +18257,7 @@
         <v>2875</v>
       </c>
       <c r="B116" t="s">
-        <v>3274</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -18249,7 +18265,7 @@
         <v>2882</v>
       </c>
       <c r="B117" t="s">
-        <v>3275</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -18257,7 +18273,7 @@
         <v>2028</v>
       </c>
       <c r="B118" t="s">
-        <v>3276</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -18265,7 +18281,7 @@
         <v>1978</v>
       </c>
       <c r="B119" t="s">
-        <v>3277</v>
+        <v>3276</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -18273,7 +18289,7 @@
         <v>1970</v>
       </c>
       <c r="B120" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -18281,7 +18297,7 @@
         <v>1929</v>
       </c>
       <c r="B121" t="s">
-        <v>3279</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -18289,7 +18305,7 @@
         <v>1972</v>
       </c>
       <c r="B122" t="s">
-        <v>3280</v>
+        <v>3279</v>
       </c>
     </row>
   </sheetData>
@@ -20756,7 +20772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+    <sheetView topLeftCell="A321" workbookViewId="0">
       <selection activeCell="B339" sqref="B339"/>
     </sheetView>
   </sheetViews>
@@ -21133,50 +21149,50 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3145</v>
+        <v>3144</v>
       </c>
       <c r="B47" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3333</v>
+        <v>3328</v>
       </c>
       <c r="B48" t="s">
-        <v>3334</v>
+        <v>3329</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3354</v>
+        <v>3349</v>
       </c>
       <c r="B49" t="s">
-        <v>3355</v>
+        <v>3350</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3357</v>
+        <v>3352</v>
       </c>
       <c r="B50" t="s">
-        <v>3356</v>
+        <v>3351</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>3363</v>
+        <v>3358</v>
       </c>
       <c r="B51" t="s">
-        <v>3364</v>
+        <v>3359</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>3353</v>
+        <v>3348</v>
       </c>
       <c r="B52" t="s">
-        <v>3373</v>
+        <v>3368</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -21184,15 +21200,15 @@
         <v>3104</v>
       </c>
       <c r="B53" t="s">
-        <v>3374</v>
+        <v>3369</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>3375</v>
+        <v>3370</v>
       </c>
       <c r="B54" t="s">
-        <v>3376</v>
+        <v>3371</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -21200,7 +21216,7 @@
         <v>3107</v>
       </c>
       <c r="B55" t="s">
-        <v>3377</v>
+        <v>3372</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -23103,34 +23119,34 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>3339</v>
+        <v>3334</v>
       </c>
       <c r="B299" t="s">
-        <v>3338</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>3345</v>
+        <v>3340</v>
       </c>
       <c r="B300" t="s">
-        <v>3344</v>
+        <v>3339</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>3346</v>
+        <v>3341</v>
       </c>
       <c r="B301" t="s">
-        <v>3347</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>3349</v>
+        <v>3344</v>
       </c>
       <c r="B302" t="s">
-        <v>3348</v>
+        <v>3343</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -23335,7 +23351,7 @@
         <v>1170</v>
       </c>
       <c r="B333" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -23343,111 +23359,111 @@
         <v>2310</v>
       </c>
       <c r="B334" t="s">
-        <v>3228</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>3271</v>
+        <v>3270</v>
       </c>
       <c r="B335" t="s">
-        <v>3270</v>
+        <v>3269</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>3287</v>
+        <v>3286</v>
       </c>
       <c r="B336" t="s">
-        <v>3286</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>3318</v>
+        <v>3313</v>
       </c>
       <c r="B337" t="s">
-        <v>3317</v>
+        <v>3312</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>3321</v>
+        <v>3316</v>
       </c>
       <c r="B338" t="s">
-        <v>3322</v>
+        <v>3317</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>3423</v>
+        <v>3418</v>
       </c>
       <c r="B339" t="s">
-        <v>3424</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>3302</v>
+        <v>3300</v>
       </c>
       <c r="B340" t="s">
-        <v>3301</v>
+        <v>3299</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>3329</v>
+        <v>3324</v>
       </c>
       <c r="B341" t="s">
-        <v>3330</v>
+        <v>3325</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>3341</v>
+        <v>3336</v>
       </c>
       <c r="B342" t="s">
-        <v>3342</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>3362</v>
+        <v>3357</v>
       </c>
       <c r="B343" t="s">
-        <v>3361</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>3369</v>
+        <v>3364</v>
       </c>
       <c r="B344" t="s">
-        <v>3370</v>
+        <v>3365</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="B345" t="s">
-        <v>3418</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>3419</v>
+        <v>3414</v>
       </c>
       <c r="B346" t="s">
-        <v>3420</v>
+        <v>3415</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>3422</v>
+        <v>3417</v>
       </c>
       <c r="B347" t="s">
-        <v>3421</v>
+        <v>3416</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24538,234 +24554,234 @@
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>3139</v>
+        <v>3138</v>
       </c>
       <c r="B486" t="s">
-        <v>3138</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>3141</v>
+        <v>3140</v>
       </c>
       <c r="B487" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>3143</v>
+        <v>3142</v>
       </c>
       <c r="B488" t="s">
-        <v>3142</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>3292</v>
+        <v>3290</v>
       </c>
       <c r="B489" t="s">
-        <v>3291</v>
+        <v>3289</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>3294</v>
+        <v>3292</v>
       </c>
       <c r="B490" t="s">
-        <v>3293</v>
+        <v>3291</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>3296</v>
+        <v>3294</v>
       </c>
       <c r="B491" t="s">
-        <v>3295</v>
+        <v>3293</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
       <c r="B492" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>3331</v>
+        <v>3326</v>
       </c>
       <c r="B493" t="s">
-        <v>3332</v>
+        <v>3327</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>3350</v>
+        <v>3345</v>
       </c>
       <c r="B494" t="s">
-        <v>3351</v>
+        <v>3346</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>3367</v>
+        <v>3362</v>
       </c>
       <c r="B495" t="s">
-        <v>3368</v>
+        <v>3363</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>3378</v>
+        <v>3373</v>
       </c>
       <c r="B496" t="s">
-        <v>3379</v>
+        <v>3374</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>3380</v>
+        <v>3375</v>
       </c>
       <c r="B497" t="s">
-        <v>3381</v>
+        <v>3376</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>3382</v>
+        <v>3377</v>
       </c>
       <c r="B498" t="s">
-        <v>3383</v>
+        <v>3378</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>3385</v>
+        <v>3380</v>
       </c>
       <c r="B499" t="s">
-        <v>3384</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>3387</v>
+        <v>3382</v>
       </c>
       <c r="B500" t="s">
-        <v>3386</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>3388</v>
+        <v>3383</v>
       </c>
       <c r="B501" t="s">
-        <v>3389</v>
+        <v>3384</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>3391</v>
+        <v>3386</v>
       </c>
       <c r="B503" t="s">
-        <v>3392</v>
+        <v>3387</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>3406</v>
+        <v>3401</v>
       </c>
       <c r="B504" t="s">
-        <v>3393</v>
+        <v>3388</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>3407</v>
+        <v>3402</v>
       </c>
       <c r="B505" t="s">
-        <v>3394</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>3408</v>
+        <v>3403</v>
       </c>
       <c r="B506" t="s">
-        <v>3395</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>3409</v>
+        <v>3404</v>
       </c>
       <c r="B507" t="s">
-        <v>3396</v>
+        <v>3391</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>3410</v>
+        <v>3405</v>
       </c>
       <c r="B508" t="s">
-        <v>3397</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>3411</v>
+        <v>3406</v>
       </c>
       <c r="B509" t="s">
-        <v>3398</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>3412</v>
+        <v>3407</v>
       </c>
       <c r="B510" t="s">
-        <v>3399</v>
+        <v>3394</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>3413</v>
+        <v>3408</v>
       </c>
       <c r="B511" t="s">
-        <v>3400</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>3414</v>
+        <v>3409</v>
       </c>
       <c r="B512" t="s">
-        <v>3401</v>
+        <v>3396</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>3415</v>
+        <v>3410</v>
       </c>
       <c r="B513" t="s">
-        <v>3402</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>3416</v>
+        <v>3411</v>
       </c>
       <c r="B514" t="s">
-        <v>3403</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>3405</v>
+        <v>3400</v>
       </c>
       <c r="B515" t="s">
-        <v>3404</v>
+        <v>3399</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
@@ -24807,10 +24823,10 @@
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>3366</v>
+        <v>3361</v>
       </c>
       <c r="B534" t="s">
-        <v>3365</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
@@ -24823,34 +24839,34 @@
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>3289</v>
+        <v>3287</v>
       </c>
       <c r="B536" t="s">
-        <v>3290</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>3316</v>
+        <v>3311</v>
       </c>
       <c r="B537" t="s">
-        <v>3315</v>
+        <v>3310</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>3328</v>
+        <v>3323</v>
       </c>
       <c r="B538" t="s">
-        <v>3327</v>
+        <v>3322</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>3371</v>
+        <v>3366</v>
       </c>
       <c r="B539" t="s">
-        <v>3372</v>
+        <v>3367</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
@@ -25081,10 +25097,10 @@
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>3325</v>
+        <v>3320</v>
       </c>
       <c r="B571" t="s">
-        <v>3326</v>
+        <v>3321</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
@@ -25621,10 +25637,10 @@
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>3359</v>
+        <v>3354</v>
       </c>
       <c r="B648" t="s">
-        <v>3360</v>
+        <v>3355</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
@@ -25653,10 +25669,10 @@
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B652" t="s">
         <v>3282</v>
-      </c>
-      <c r="B652" t="s">
-        <v>3283</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
@@ -25680,15 +25696,15 @@
         <v>2016</v>
       </c>
       <c r="B655" t="s">
-        <v>3281</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>3320</v>
+        <v>3315</v>
       </c>
       <c r="B656" t="s">
-        <v>3319</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
@@ -25696,7 +25712,7 @@
         <v>1455</v>
       </c>
       <c r="B657" t="s">
-        <v>3358</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
@@ -25893,15 +25909,15 @@
         <v>1712</v>
       </c>
       <c r="B683" t="s">
-        <v>3148</v>
+        <v>3147</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>3285</v>
+        <v>3284</v>
       </c>
       <c r="B684" t="s">
-        <v>3284</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
@@ -25909,7 +25925,7 @@
         <v>2016</v>
       </c>
       <c r="B685" t="s">
-        <v>3340</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
@@ -25917,7 +25933,7 @@
         <v>1460</v>
       </c>
       <c r="B686" t="s">
-        <v>3343</v>
+        <v>3338</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
@@ -25935,10 +25951,10 @@
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>3308</v>
+        <v>3305</v>
       </c>
       <c r="B694" t="s">
-        <v>3307</v>
+        <v>3304</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
@@ -26380,7 +26396,7 @@
         <v>1699</v>
       </c>
       <c r="B752" t="s">
-        <v>3323</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
@@ -26388,7 +26404,7 @@
         <v>1524</v>
       </c>
       <c r="B753" t="s">
-        <v>3324</v>
+        <v>3319</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sub nav menues, chachis
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="3434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4242" uniqueCount="3452">
   <si>
     <t>Base Set</t>
   </si>
@@ -10335,6 +10335,60 @@
   </si>
   <si>
     <t>https://3.bp.blogspot.com/-EgIu-yRnLCk/WK4D9PikivI/AAAAAAABsy4/FR4IrGPDQRcVZY-SucYy7RPA7WgFyXUkQCLcB/s1600/buffet-1-1-1.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-zcxiTYB58Po/V_jW-2UvmKI/AAAAAAAAKdI/SxrWNuTGMEEM_n2vKBEgxFfH3Z372MzDQCLcB/s1600/1973-DEDICATED-BOB-BOONE.jpg</t>
+  </si>
+  <si>
+    <t>Bob Boone CTNW</t>
+  </si>
+  <si>
+    <t>Larry Bowa CTNW</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-YglNKn6J670/V-j94OHxZzI/AAAAAAAAKYQ/vHrNibNLsaAx5dISzR79tVqCEDSObmtCgCLcB/s1600/1970-DEDICATED-ROOKIE-BOWA.jpg</t>
+  </si>
+  <si>
+    <t>Cookie Rojas Now and Then CTNW</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-wLPwj5_LlUg/V-Or6aJoFWI/AAAAAAAAKWM/Q9RJWSU4UcokRjjKaa0sFCKtRiOwg3NZACLcB/s1600/1977-ROJAS-THEN-AND-NOW%25281%2529.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-dci8okE6Fgs/V-EMpzpuUDI/AAAAAAAAKVQ/V9eefFGjGeUrCUkMgLM1jrFNPh6qi3ImwCLcB/s1600/1973-MISSING-BATEMAN%25281%2529.jpg</t>
+  </si>
+  <si>
+    <t>John Bateman CTNW</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-Tcm2_fixJvM/V0LelXg04JI/AAAAAAAAJog/RkRsgpyZHK0ImNDysLq7E5ze-r95YAXjACLcB/s1600/1971-MISSING-HUTTO.jpg</t>
+  </si>
+  <si>
+    <t>Jim Hutto CTNW</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-RNsrwjCoD1o/VssC9Wb_EcI/AAAAAAAAJAI/_5d-hhiYAtU/s1600/1970-MISSING-RAFFO.jpg</t>
+  </si>
+  <si>
+    <t>Al Raffo CTNW</t>
+  </si>
+  <si>
+    <t>Jerry Martin 1976 CTNW</t>
+  </si>
+  <si>
+    <t>http://3.bp.blogspot.com/-T-5rB00s1r0/VizYyIwZCBI/AAAAAAAAIJg/ZnbFYO5x8pQ/s1600/1976%2BPROJECT%2BJERRY%2BMARTIN%2BFOR%2BBLOG.jpg</t>
+  </si>
+  <si>
+    <t>Joe Hoerner 1976 CTNW</t>
+  </si>
+  <si>
+    <t>http://2.bp.blogspot.com/-tS8v7BODeLw/VflnKQujmXI/AAAAAAAAH5g/5jdi1TmY0Nk/s1600/1976-PROJECT-JOE-HOERNER-FOR-BLOG.jpg</t>
+  </si>
+  <si>
+    <t>http://4.bp.blogspot.com/-2NOeGlrxshw/VSJJQb1STBI/AAAAAAAAF-I/9VAFh6NhQiE/s1600/1971-DEDICATED-ROOKIE-LUZINSKI.jpg</t>
+  </si>
+  <si>
+    <t>Greg Luzinski CTNY</t>
   </si>
 </sst>
 </file>
@@ -20011,10 +20065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20281,512 +20335,528 @@
         <v>2703</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3436</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3437</v>
+      </c>
+    </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3445</v>
+      </c>
       <c r="B35" t="s">
+        <v>3444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>1446</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>1558</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>2019</v>
-      </c>
-      <c r="B37" t="s">
-        <v>2020</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1161</v>
+        <v>1558</v>
       </c>
       <c r="B38" t="s">
-        <v>2021</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="B39" t="s">
-        <v>2023</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2024</v>
+        <v>1161</v>
       </c>
       <c r="B40" t="s">
-        <v>2025</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2026</v>
+        <v>2022</v>
       </c>
       <c r="B41" t="s">
-        <v>2027</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1448</v>
+        <v>2024</v>
       </c>
       <c r="B42" t="s">
-        <v>1450</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1452</v>
+        <v>2026</v>
       </c>
       <c r="B43" t="s">
-        <v>1454</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1456</v>
+        <v>1448</v>
       </c>
       <c r="B44" t="s">
-        <v>1457</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1460</v>
+        <v>1452</v>
       </c>
       <c r="B45" t="s">
-        <v>1462</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1463</v>
+        <v>1456</v>
       </c>
       <c r="B46" t="s">
-        <v>1466</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1483</v>
+        <v>1460</v>
       </c>
       <c r="B47" t="s">
-        <v>1484</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1522</v>
+        <v>1463</v>
       </c>
       <c r="B48" t="s">
-        <v>1525</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1523</v>
+        <v>1483</v>
       </c>
       <c r="B49" t="s">
-        <v>1526</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="B50" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1533</v>
+        <v>1523</v>
       </c>
       <c r="B51" t="s">
-        <v>1534</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1771</v>
+        <v>1524</v>
       </c>
       <c r="B52" t="s">
-        <v>1773</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1772</v>
+        <v>1533</v>
       </c>
       <c r="B53" t="s">
-        <v>1774</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1714</v>
+        <v>1771</v>
       </c>
       <c r="B54" t="s">
-        <v>1848</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1845</v>
+        <v>1772</v>
       </c>
       <c r="B55" t="s">
-        <v>1849</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1846</v>
+        <v>1714</v>
       </c>
       <c r="B56" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="B57" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>2010</v>
+        <v>1846</v>
       </c>
       <c r="B58" t="s">
-        <v>2011</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2012</v>
+        <v>1847</v>
       </c>
       <c r="B59" t="s">
-        <v>2013</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="B60" t="s">
-        <v>2015</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2028</v>
+        <v>2012</v>
       </c>
       <c r="B61" t="s">
-        <v>2029</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>2030</v>
+        <v>2014</v>
       </c>
       <c r="B62" t="s">
-        <v>2031</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2032</v>
+        <v>2028</v>
       </c>
       <c r="B63" t="s">
-        <v>2033</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>2034</v>
+        <v>2030</v>
       </c>
       <c r="B64" t="s">
-        <v>2035</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>2036</v>
+        <v>2032</v>
       </c>
       <c r="B65" t="s">
-        <v>2037</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>2038</v>
+        <v>2034</v>
       </c>
       <c r="B66" t="s">
-        <v>2039</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>2040</v>
+        <v>2036</v>
       </c>
       <c r="B67" t="s">
-        <v>2041</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1725</v>
+        <v>2038</v>
       </c>
       <c r="B68" t="s">
-        <v>2448</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>2449</v>
+        <v>2040</v>
       </c>
       <c r="B69" t="s">
-        <v>2450</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2451</v>
+        <v>1725</v>
       </c>
       <c r="B70" t="s">
-        <v>2452</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1581</v>
+        <v>2449</v>
       </c>
       <c r="B71" t="s">
-        <v>2455</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1593</v>
+        <v>2451</v>
       </c>
       <c r="B72" t="s">
-        <v>2543</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>2545</v>
+        <v>1581</v>
       </c>
       <c r="B73" t="s">
-        <v>2546</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>2564</v>
+        <v>1593</v>
       </c>
       <c r="B74" t="s">
-        <v>2565</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>1718</v>
+        <v>2545</v>
       </c>
       <c r="B75" t="s">
-        <v>2623</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>2632</v>
+        <v>2564</v>
       </c>
       <c r="B76" t="s">
-        <v>2633</v>
+        <v>2565</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>2642</v>
+        <v>1718</v>
       </c>
       <c r="B77" t="s">
-        <v>2643</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>2685</v>
+        <v>2632</v>
       </c>
       <c r="B78" t="s">
-        <v>2686</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>2688</v>
+        <v>2642</v>
       </c>
       <c r="B79" t="s">
-        <v>2689</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>2690</v>
+        <v>2685</v>
       </c>
       <c r="B80" t="s">
-        <v>2691</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>2693</v>
+        <v>2688</v>
       </c>
       <c r="B81" t="s">
-        <v>2692</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>1595</v>
+        <v>2690</v>
       </c>
       <c r="B82" t="s">
-        <v>2694</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>2597</v>
+        <v>2693</v>
       </c>
       <c r="B83" t="s">
-        <v>2695</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>2697</v>
+        <v>1595</v>
       </c>
       <c r="B84" t="s">
-        <v>2696</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>2698</v>
+        <v>2597</v>
       </c>
       <c r="B85" t="s">
-        <v>2699</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>2705</v>
+        <v>2697</v>
       </c>
       <c r="B86" t="s">
-        <v>2704</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>1620</v>
+        <v>2698</v>
       </c>
       <c r="B87" t="s">
-        <v>2706</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>2743</v>
+        <v>2705</v>
       </c>
       <c r="B88" t="s">
-        <v>2742</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1571</v>
+        <v>1620</v>
       </c>
       <c r="B89" t="s">
-        <v>2773</v>
+        <v>2706</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>2775</v>
+        <v>2743</v>
       </c>
       <c r="B90" t="s">
-        <v>2774</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>2777</v>
+        <v>1571</v>
       </c>
       <c r="B91" t="s">
-        <v>2776</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1585</v>
+        <v>2775</v>
       </c>
       <c r="B92" t="s">
-        <v>2778</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>2779</v>
+        <v>2777</v>
       </c>
       <c r="B93" t="s">
-        <v>2780</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>2781</v>
+        <v>1585</v>
       </c>
       <c r="B94" t="s">
-        <v>2782</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>2783</v>
+        <v>2779</v>
       </c>
       <c r="B95" t="s">
-        <v>2784</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1696</v>
+        <v>2781</v>
       </c>
       <c r="B96" t="s">
-        <v>2785</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>2786</v>
+        <v>2783</v>
       </c>
       <c r="B97" t="s">
-        <v>2787</v>
+        <v>2784</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>2788</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>2789</v>
       </c>
     </row>
@@ -20797,10 +20867,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B813"/>
+  <dimension ref="A1:B821"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A618" workbookViewId="0">
-      <selection activeCell="A639" sqref="A639"/>
+    <sheetView tabSelected="1" topLeftCell="A679" workbookViewId="0">
+      <selection activeCell="A702" sqref="A702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25162,1709 +25232,1770 @@
         <v>3321</v>
       </c>
     </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>3438</v>
+      </c>
+      <c r="B578" t="s">
+        <v>3439</v>
+      </c>
+    </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>2389</v>
+        <v>3446</v>
+      </c>
+      <c r="B579" t="s">
+        <v>3447</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>1455</v>
+        <v>3448</v>
       </c>
       <c r="B580" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A581" t="s">
-        <v>1547</v>
-      </c>
-      <c r="B581" t="s">
-        <v>1546</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B582" t="s">
-        <v>1548</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1551</v>
+        <v>3435</v>
       </c>
       <c r="B583" t="s">
-        <v>1550</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>1553</v>
+        <v>3441</v>
       </c>
       <c r="B584" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B585" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="586" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A586" t="s">
-        <v>1482</v>
-      </c>
-      <c r="B586" t="s">
-        <v>1556</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1558</v>
-      </c>
-      <c r="B587" t="s">
-        <v>1557</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1606</v>
+        <v>1455</v>
       </c>
       <c r="B588" t="s">
-        <v>1607</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1560</v>
+        <v>1547</v>
       </c>
       <c r="B589" t="s">
-        <v>1559</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1562</v>
+        <v>1549</v>
       </c>
       <c r="B590" t="s">
-        <v>1561</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1564</v>
+        <v>1551</v>
       </c>
       <c r="B591" t="s">
-        <v>1563</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1566</v>
+        <v>1553</v>
       </c>
       <c r="B592" t="s">
-        <v>1565</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1567</v>
+        <v>1555</v>
       </c>
       <c r="B593" t="s">
-        <v>1568</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1570</v>
+        <v>1482</v>
       </c>
       <c r="B594" t="s">
-        <v>1569</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1571</v>
+        <v>1558</v>
       </c>
       <c r="B595" t="s">
-        <v>1572</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>1575</v>
+        <v>1606</v>
       </c>
       <c r="B596" t="s">
-        <v>1573</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>1574</v>
+        <v>1560</v>
       </c>
       <c r="B597" t="s">
-        <v>1576</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>1578</v>
+        <v>1562</v>
       </c>
       <c r="B598" t="s">
-        <v>1577</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1388</v>
+        <v>1564</v>
       </c>
       <c r="B599" t="s">
-        <v>1579</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>1581</v>
+        <v>1566</v>
       </c>
       <c r="B600" t="s">
-        <v>1580</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>1583</v>
+        <v>1567</v>
       </c>
       <c r="B601" t="s">
-        <v>1582</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>1585</v>
+        <v>1570</v>
       </c>
       <c r="B602" t="s">
-        <v>1584</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1587</v>
+        <v>1571</v>
       </c>
       <c r="B603" t="s">
-        <v>1586</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1589</v>
+        <v>1575</v>
       </c>
       <c r="B604" t="s">
-        <v>1588</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1591</v>
+        <v>1574</v>
       </c>
       <c r="B605" t="s">
-        <v>1590</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>1593</v>
+        <v>1578</v>
       </c>
       <c r="B606" t="s">
-        <v>1592</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>1595</v>
+        <v>1388</v>
       </c>
       <c r="B607" t="s">
-        <v>1594</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>1597</v>
+        <v>1581</v>
       </c>
       <c r="B608" t="s">
-        <v>1596</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>1600</v>
+        <v>1583</v>
       </c>
       <c r="B609" t="s">
-        <v>1598</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>1599</v>
+        <v>1585</v>
       </c>
       <c r="B610" t="s">
-        <v>1601</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>1602</v>
+        <v>1587</v>
       </c>
       <c r="B611" t="s">
-        <v>1604</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>1603</v>
+        <v>1589</v>
       </c>
       <c r="B612" t="s">
-        <v>1605</v>
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B613" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B614" t="s">
+        <v>1592</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>2472</v>
+        <v>1595</v>
+      </c>
+      <c r="B615" t="s">
+        <v>1594</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>2473</v>
+        <v>1597</v>
       </c>
       <c r="B616" t="s">
-        <v>2474</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>2475</v>
+        <v>1600</v>
       </c>
       <c r="B617" t="s">
-        <v>2476</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>2477</v>
+        <v>1599</v>
       </c>
       <c r="B618" t="s">
-        <v>2478</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>2479</v>
+        <v>1602</v>
       </c>
       <c r="B619" t="s">
-        <v>2480</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>2481</v>
+        <v>1603</v>
       </c>
       <c r="B620" t="s">
-        <v>2482</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>2582</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1455</v>
+        <v>2473</v>
       </c>
       <c r="B624" t="s">
-        <v>2583</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>2584</v>
+        <v>2475</v>
       </c>
       <c r="B625" t="s">
-        <v>2585</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1589</v>
+        <v>2477</v>
       </c>
       <c r="B626" t="s">
-        <v>2586</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1566</v>
+        <v>2479</v>
       </c>
       <c r="B627" t="s">
-        <v>2587</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1602</v>
+        <v>2481</v>
       </c>
       <c r="B628" t="s">
-        <v>2588</v>
-      </c>
-    </row>
-    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A629" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B629" t="s">
-        <v>2589</v>
-      </c>
-    </row>
-    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A630" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B630" t="s">
-        <v>2592</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>1597</v>
-      </c>
-      <c r="B631" t="s">
-        <v>2593</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>2597</v>
+        <v>1455</v>
       </c>
       <c r="B632" t="s">
-        <v>2596</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>1593</v>
+        <v>2584</v>
       </c>
       <c r="B633" t="s">
-        <v>2600</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>1560</v>
+        <v>1589</v>
       </c>
       <c r="B634" t="s">
-        <v>2601</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>1595</v>
+        <v>1566</v>
       </c>
       <c r="B635" t="s">
-        <v>2602</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>1549</v>
+        <v>1602</v>
       </c>
       <c r="B636" t="s">
-        <v>2603</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1388</v>
+        <v>1150</v>
       </c>
       <c r="B637" t="s">
-        <v>2987</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>1583</v>
+        <v>1219</v>
       </c>
       <c r="B638" t="s">
-        <v>3433</v>
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B639" t="s">
+        <v>2593</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>2597</v>
+      </c>
+      <c r="B640" t="s">
+        <v>2596</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>2391</v>
+        <v>1593</v>
+      </c>
+      <c r="B641" t="s">
+        <v>2600</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1520</v>
+        <v>1560</v>
       </c>
       <c r="B642" t="s">
-        <v>1636</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1388</v>
+        <v>1595</v>
       </c>
       <c r="B643" t="s">
-        <v>1637</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1639</v>
+        <v>1549</v>
       </c>
       <c r="B644" t="s">
-        <v>1638</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1632</v>
+        <v>1388</v>
       </c>
       <c r="B645" t="s">
-        <v>1640</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1641</v>
+        <v>1583</v>
       </c>
       <c r="B646" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A647" t="s">
-        <v>1644</v>
-      </c>
-      <c r="B647" t="s">
-        <v>1643</v>
-      </c>
-    </row>
-    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A648" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B648" t="s">
-        <v>1645</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B649" t="s">
-        <v>1646</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1648</v>
+        <v>1520</v>
       </c>
       <c r="B650" t="s">
-        <v>1647</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1649</v>
+        <v>1388</v>
       </c>
       <c r="B651" t="s">
-        <v>1650</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1651</v>
+        <v>1639</v>
       </c>
       <c r="B652" t="s">
-        <v>1652</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1653</v>
+        <v>1632</v>
       </c>
       <c r="B653" t="s">
-        <v>1654</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>3354</v>
+        <v>1641</v>
       </c>
       <c r="B654" t="s">
-        <v>3355</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1655</v>
+        <v>1644</v>
       </c>
       <c r="B655" t="s">
-        <v>1656</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>2150</v>
+        <v>1451</v>
       </c>
       <c r="B656" t="s">
-        <v>2151</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>2591</v>
+        <v>1560</v>
       </c>
       <c r="B657" t="s">
-        <v>2590</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>3281</v>
+        <v>1648</v>
       </c>
       <c r="B658" t="s">
-        <v>3282</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1683</v>
+        <v>1649</v>
       </c>
       <c r="B659" t="s">
-        <v>2621</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>1593</v>
+        <v>1651</v>
       </c>
       <c r="B660" t="s">
-        <v>2662</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>2016</v>
+        <v>1653</v>
       </c>
       <c r="B661" t="s">
-        <v>3280</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>3315</v>
+        <v>3354</v>
       </c>
       <c r="B662" t="s">
-        <v>3314</v>
+        <v>3355</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>1455</v>
+        <v>1655</v>
       </c>
       <c r="B663" t="s">
-        <v>3353</v>
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B664" t="s">
+        <v>2151</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>2392</v>
+        <v>2591</v>
+      </c>
+      <c r="B665" t="s">
+        <v>2590</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1451</v>
+        <v>3281</v>
       </c>
       <c r="B666" t="s">
-        <v>1657</v>
+        <v>3282</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1447</v>
+        <v>1683</v>
       </c>
       <c r="B667" t="s">
-        <v>1658</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1521</v>
+        <v>1593</v>
       </c>
       <c r="B668" t="s">
-        <v>1659</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1660</v>
+        <v>2016</v>
       </c>
       <c r="B669" t="s">
-        <v>1661</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>1663</v>
+        <v>3315</v>
       </c>
       <c r="B670" t="s">
-        <v>1662</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1639</v>
+        <v>1455</v>
       </c>
       <c r="B671" t="s">
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A672" t="s">
-        <v>1651</v>
-      </c>
-      <c r="B672" t="s">
-        <v>1665</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B673" t="s">
-        <v>1666</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1667</v>
+        <v>1451</v>
       </c>
       <c r="B674" t="s">
-        <v>1668</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1160</v>
+        <v>1447</v>
       </c>
       <c r="B675" t="s">
-        <v>1669</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1459</v>
+        <v>1521</v>
       </c>
       <c r="B676" t="s">
-        <v>1670</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1388</v>
+        <v>1660</v>
       </c>
       <c r="B677" t="s">
-        <v>1671</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>1632</v>
+        <v>1663</v>
       </c>
       <c r="B678" t="s">
-        <v>1672</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>1520</v>
+        <v>1639</v>
       </c>
       <c r="B679" t="s">
-        <v>1673</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>1674</v>
+        <v>1651</v>
       </c>
       <c r="B680" t="s">
-        <v>1675</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>1677</v>
+        <v>1641</v>
       </c>
       <c r="B681" t="s">
-        <v>1676</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>1679</v>
+        <v>1667</v>
       </c>
       <c r="B682" t="s">
-        <v>1678</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>1681</v>
+        <v>1160</v>
       </c>
       <c r="B683" t="s">
-        <v>1680</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1644</v>
+        <v>1459</v>
       </c>
       <c r="B684" t="s">
-        <v>1682</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1683</v>
+        <v>1388</v>
       </c>
       <c r="B685" t="s">
-        <v>1684</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>1482</v>
+        <v>1632</v>
       </c>
       <c r="B686" t="s">
-        <v>1865</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>2152</v>
+        <v>1520</v>
       </c>
       <c r="B687" t="s">
-        <v>2153</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>1699</v>
+        <v>1674</v>
       </c>
       <c r="B688" t="s">
-        <v>2641</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>1712</v>
+        <v>1677</v>
       </c>
       <c r="B689" t="s">
-        <v>3147</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>3284</v>
+        <v>1679</v>
       </c>
       <c r="B690" t="s">
-        <v>3283</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>2016</v>
+        <v>1681</v>
       </c>
       <c r="B691" t="s">
-        <v>3335</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1460</v>
+        <v>1644</v>
       </c>
       <c r="B692" t="s">
-        <v>3338</v>
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B693" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B694" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B695" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B696" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B697" t="s">
+        <v>3147</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>2393</v>
+        <v>3284</v>
+      </c>
+      <c r="B698" t="s">
+        <v>3283</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1685</v>
+        <v>2016</v>
       </c>
       <c r="B699" t="s">
-        <v>1686</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>3305</v>
+        <v>1460</v>
       </c>
       <c r="B700" t="s">
-        <v>3304</v>
+        <v>3338</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1523</v>
+        <v>3443</v>
       </c>
       <c r="B701" t="s">
-        <v>1687</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1524</v>
+        <v>3451</v>
       </c>
       <c r="B702" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B703" t="s">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B704" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A705" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B705" t="s">
-        <v>1694</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1696</v>
-      </c>
-      <c r="B706" t="s">
-        <v>1695</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1459</v>
+        <v>1685</v>
       </c>
       <c r="B707" t="s">
-        <v>1697</v>
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B708" t="s">
+        <v>3304</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>2394</v>
+        <v>1523</v>
+      </c>
+      <c r="B709" t="s">
+        <v>1687</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1698</v>
+        <v>1524</v>
       </c>
       <c r="B710" t="s">
-        <v>1729</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1699</v>
+        <v>1689</v>
       </c>
       <c r="B711" t="s">
-        <v>1730</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1483</v>
+        <v>1691</v>
       </c>
       <c r="B712" t="s">
-        <v>1731</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1700</v>
+        <v>1693</v>
       </c>
       <c r="B713" t="s">
-        <v>1732</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1701</v>
+        <v>1696</v>
       </c>
       <c r="B714" t="s">
-        <v>1733</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1703</v>
+        <v>1459</v>
       </c>
       <c r="B715" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A716" t="s">
-        <v>1667</v>
-      </c>
-      <c r="B716" t="s">
-        <v>1747</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1704</v>
-      </c>
-      <c r="B717" t="s">
-        <v>1705</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1706</v>
+        <v>1698</v>
       </c>
       <c r="B718" t="s">
-        <v>1734</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1707</v>
+        <v>1699</v>
       </c>
       <c r="B719" t="s">
-        <v>1735</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1708</v>
+        <v>1483</v>
       </c>
       <c r="B720" t="s">
-        <v>1709</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1710</v>
+        <v>1700</v>
       </c>
       <c r="B721" t="s">
-        <v>1736</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1459</v>
+        <v>1701</v>
       </c>
       <c r="B722" t="s">
-        <v>1711</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1689</v>
+        <v>1703</v>
       </c>
       <c r="B723" t="s">
-        <v>1737</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1712</v>
+        <v>1667</v>
       </c>
       <c r="B724" t="s">
-        <v>1738</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1160</v>
+        <v>1704</v>
       </c>
       <c r="B725" t="s">
-        <v>1739</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1714</v>
+        <v>1706</v>
       </c>
       <c r="B726" t="s">
-        <v>1713</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1696</v>
+        <v>1707</v>
       </c>
       <c r="B727" t="s">
-        <v>1740</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1715</v>
+        <v>1708</v>
       </c>
       <c r="B728" t="s">
-        <v>1741</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1717</v>
+        <v>1710</v>
       </c>
       <c r="B729" t="s">
-        <v>1716</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1693</v>
+        <v>1459</v>
       </c>
       <c r="B730" t="s">
-        <v>1742</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1524</v>
+        <v>1689</v>
       </c>
       <c r="B731" t="s">
-        <v>1743</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1718</v>
+        <v>1712</v>
       </c>
       <c r="B732" t="s">
-        <v>1744</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1720</v>
+        <v>1160</v>
       </c>
       <c r="B733" t="s">
-        <v>1719</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1721</v>
+        <v>1714</v>
       </c>
       <c r="B734" t="s">
-        <v>1745</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1723</v>
+        <v>1696</v>
       </c>
       <c r="B735" t="s">
-        <v>1722</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1725</v>
+        <v>1715</v>
       </c>
       <c r="B736" t="s">
-        <v>1724</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1726</v>
+        <v>1717</v>
       </c>
       <c r="B737" t="s">
-        <v>1746</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1728</v>
+        <v>1693</v>
       </c>
       <c r="B738" t="s">
-        <v>1727</v>
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B739" t="s">
+        <v>1743</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>2395</v>
+        <v>1718</v>
+      </c>
+      <c r="B740" t="s">
+        <v>1744</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1762</v>
+        <v>1720</v>
       </c>
       <c r="B741" t="s">
-        <v>1763</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1764</v>
+        <v>1721</v>
       </c>
       <c r="B742" t="s">
-        <v>1765</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1689</v>
+        <v>1723</v>
       </c>
       <c r="B743" t="s">
-        <v>1870</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1872</v>
+        <v>1725</v>
       </c>
       <c r="B744" t="s">
-        <v>1871</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1533</v>
+        <v>1726</v>
       </c>
       <c r="B745" t="s">
-        <v>1873</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1160</v>
+        <v>1728</v>
       </c>
       <c r="B746" t="s">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A747" t="s">
-        <v>1875</v>
-      </c>
-      <c r="B747" t="s">
-        <v>1876</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>1877</v>
-      </c>
-      <c r="B748" t="s">
-        <v>1878</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>1880</v>
+        <v>1762</v>
       </c>
       <c r="B749" t="s">
-        <v>1879</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>1881</v>
+        <v>1764</v>
       </c>
       <c r="B750" t="s">
-        <v>1882</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>1718</v>
+        <v>1689</v>
       </c>
       <c r="B751" t="s">
-        <v>1883</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>1885</v>
+        <v>1872</v>
       </c>
       <c r="B752" t="s">
-        <v>1884</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>1451</v>
+        <v>1533</v>
       </c>
       <c r="B753" t="s">
-        <v>1886</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>1887</v>
+        <v>1160</v>
       </c>
       <c r="B754" t="s">
-        <v>1888</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>1889</v>
+        <v>1875</v>
       </c>
       <c r="B755" t="s">
-        <v>1890</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>1891</v>
+        <v>1877</v>
       </c>
       <c r="B756" t="s">
-        <v>1892</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>1893</v>
+        <v>1880</v>
       </c>
       <c r="B757" t="s">
-        <v>1894</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>1699</v>
+        <v>1881</v>
       </c>
       <c r="B758" t="s">
-        <v>3318</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>1524</v>
+        <v>1718</v>
       </c>
       <c r="B759" t="s">
-        <v>3319</v>
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A760" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B760" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B761" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B762" t="s">
+        <v>1888</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>2396</v>
+        <v>1889</v>
+      </c>
+      <c r="B763" t="s">
+        <v>1890</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>1161</v>
+        <v>1891</v>
       </c>
       <c r="B764" t="s">
-        <v>1904</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>1906</v>
+        <v>1893</v>
       </c>
       <c r="B765" t="s">
-        <v>1905</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>1203</v>
+        <v>1699</v>
       </c>
       <c r="B766" t="s">
-        <v>1907</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>1236</v>
+        <v>1524</v>
       </c>
       <c r="B767" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="768" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A768" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B768" t="s">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="769" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A769" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B769" t="s">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="770" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A770" t="s">
-        <v>252</v>
-      </c>
-      <c r="B770" t="s">
-        <v>1911</v>
+        <v>3319</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B771" t="s">
-        <v>1912</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>1238</v>
+        <v>1161</v>
       </c>
       <c r="B772" t="s">
-        <v>1913</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>1181</v>
+        <v>1906</v>
       </c>
       <c r="B773" t="s">
-        <v>1914</v>
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B774" t="s">
+        <v>1907</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>2397</v>
+        <v>1236</v>
+      </c>
+      <c r="B775" t="s">
+        <v>1908</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>1915</v>
+        <v>1408</v>
       </c>
       <c r="B776" t="s">
-        <v>1916</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>1756</v>
+        <v>1230</v>
       </c>
       <c r="B777" t="s">
-        <v>1917</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>1919</v>
+        <v>252</v>
       </c>
       <c r="B778" t="s">
-        <v>1918</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>1921</v>
+        <v>1187</v>
       </c>
       <c r="B779" t="s">
-        <v>1920</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>1923</v>
+        <v>1238</v>
       </c>
       <c r="B780" t="s">
-        <v>1922</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>1925</v>
+        <v>1181</v>
       </c>
       <c r="B781" t="s">
-        <v>1924</v>
-      </c>
-    </row>
-    <row r="782" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A782" t="s">
-        <v>1926</v>
-      </c>
-      <c r="B782" t="s">
-        <v>1927</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>1929</v>
-      </c>
-      <c r="B783" t="s">
-        <v>1928</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>1402</v>
+        <v>1915</v>
       </c>
       <c r="B784" t="s">
-        <v>1930</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>1934</v>
+        <v>1756</v>
       </c>
       <c r="B785" t="s">
-        <v>1931</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>1933</v>
+        <v>1919</v>
       </c>
       <c r="B786" t="s">
-        <v>1932</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>1936</v>
+        <v>1921</v>
       </c>
       <c r="B787" t="s">
-        <v>1935</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>1578</v>
+        <v>1923</v>
       </c>
       <c r="B788" t="s">
-        <v>1937</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>1939</v>
+        <v>1925</v>
       </c>
       <c r="B789" t="s">
-        <v>1938</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>1941</v>
+        <v>1926</v>
       </c>
       <c r="B790" t="s">
-        <v>1940</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>1299</v>
+        <v>1929</v>
       </c>
       <c r="B791" t="s">
-        <v>1942</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>1943</v>
+        <v>1402</v>
       </c>
       <c r="B792" t="s">
-        <v>1944</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>1946</v>
+        <v>1934</v>
       </c>
       <c r="B793" t="s">
-        <v>1945</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>1948</v>
+        <v>1933</v>
       </c>
       <c r="B794" t="s">
-        <v>1947</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>1950</v>
+        <v>1936</v>
       </c>
       <c r="B795" t="s">
-        <v>1949</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>1952</v>
+        <v>1578</v>
       </c>
       <c r="B796" t="s">
-        <v>1951</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>1953</v>
+        <v>1939</v>
       </c>
       <c r="B797" t="s">
-        <v>1954</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>1956</v>
+        <v>1941</v>
       </c>
       <c r="B798" t="s">
-        <v>1955</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>1958</v>
+        <v>1299</v>
       </c>
       <c r="B799" t="s">
-        <v>1957</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>1960</v>
+        <v>1943</v>
       </c>
       <c r="B800" t="s">
-        <v>1959</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>1287</v>
+        <v>1946</v>
       </c>
       <c r="B801" t="s">
-        <v>1961</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>1963</v>
+        <v>1948</v>
       </c>
       <c r="B802" t="s">
-        <v>1962</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>1503</v>
+        <v>1950</v>
       </c>
       <c r="B803" t="s">
-        <v>1964</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>1965</v>
+        <v>1952</v>
       </c>
       <c r="B804" t="s">
-        <v>1966</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>1968</v>
+        <v>1953</v>
       </c>
       <c r="B805" t="s">
-        <v>1967</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>1970</v>
+        <v>1956</v>
       </c>
       <c r="B806" t="s">
-        <v>1969</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>1972</v>
+        <v>1958</v>
       </c>
       <c r="B807" t="s">
-        <v>1971</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>1973</v>
+        <v>1960</v>
       </c>
       <c r="B808" t="s">
-        <v>1974</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>1976</v>
+        <v>1287</v>
       </c>
       <c r="B809" t="s">
-        <v>1975</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
-        <v>1978</v>
+        <v>1963</v>
       </c>
       <c r="B810" t="s">
-        <v>1977</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>1980</v>
+        <v>1503</v>
       </c>
       <c r="B811" t="s">
-        <v>1979</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>1982</v>
+        <v>1965</v>
       </c>
       <c r="B812" t="s">
-        <v>1981</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B813" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A814" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B814" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A815" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B815" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B816" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B817" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B818" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B820" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
         <v>2962</v>
       </c>
-      <c r="B813" t="s">
+      <c r="B821" t="s">
         <v>2961</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial CPCR Tier Stuff
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="19416" windowHeight="10632" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="19416" windowHeight="10572" firstSheet="14" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="21" r:id="rId1"/>
@@ -34,8 +34,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Heaney, Daniel H CIV NSWCDD, W42</author>
+  </authors>
+  <commentList>
+    <comment ref="B428" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Heaney, Daniel H CIV NSWCDD, W42:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5532" uniqueCount="4341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5599" uniqueCount="4391">
   <si>
     <t>Base Set</t>
   </si>
@@ -13058,13 +13092,163 @@
   </si>
   <si>
     <t>2016 Topps Phillies</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-hZoZYafGDCU/WZJaqoZfc-I/AAAAAAAAhCc/XCh7jh6ldjIZQz1m_iz99spUrzQz_1K9QCLcBGAs/s1600/2005%2BPhillies%2BTeam%2BIssue%2B%252333%2BOfferman.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-T4uD0unZZcs/WZJarMATYwI/AAAAAAAAhC0/QnZQ6dJEADY5WPPH5vTpqJLYCsukLnwQACLcBGAs/s1600/2008%2BPhillies%2BTeam%2BIssue%2B%252357%2BSeanez.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-fel44rxFYFA/WZJarPw1QkI/AAAAAAAAhCs/3sfnSPvYgm8fCuIxxz5incdYrwp7wGo8ACLcBGAs/s1600/2009%2BPhillies%2BTeam%2BIssue%2BUpdate%2B%252323%2BBako.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-AUAJJIU_XFM/WZJaqvp2LgI/AAAAAAAAhCk/XvmbOC-zziUvZRLhZ0GIZ4GV3JiVAvDogCLcBGAs/s1600/2005%2BTopps%2BUpdate%2B%2523UH4%2BTucker.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-wyqvYhl17y8/WZJaqgBROGI/AAAAAAAAhCg/YHkQx_NIIHkXVViCu1hf3vAjw1162mSLQCLcBGAs/s1600/2005%2BTopps%2BUpdate%2B%2523UH80%2BUrbina.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-c4I7HUO93mg/WZJaq7shDgI/AAAAAAAAhCo/Wr28EhITSrIgvhDfxbAVsCxmNKx-G0fogCLcBGAs/s1600/2006%2BTopps%2BPhillies%2BFan%2BAppreciation%2BDay%2B%252312%2BWhite.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-d2HaTSL071g/WZJarFI7XAI/AAAAAAAAhCw/d6483mp_RpEJMab0MyAYHWZgB4UZ3gboACLcBGAs/s1600/2010%2BUpper%2BDeck%2B%2523381%2BTaschner.jpg</t>
+  </si>
+  <si>
+    <t>Rhys Hoskins in Action</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-_QALQTrRx6o/WZOQQkdMxKI/AAAAAAAAhDE/nlbIb1qSLyMx_8pz6Pya-VZ2gFZwXG4IACLcBGAs/s1600/2017%2BChachi%2BIn%2BAction%2B%25237%2BHoskins.jpg</t>
+  </si>
+  <si>
+    <t>Missing Links of the 2000s</t>
+  </si>
+  <si>
+    <t>Kirk Bullinger</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-qfpwmMlGffU/WZOTA8IkKOI/AAAAAAAAhDc/9E06xoaU5ZgFVmB4QSablzi5ap5lJd2CwCLcBGAs/s1600/2017%2BChachi%2BPhillies%2BMissing%2BLinks%2Bof%2Bthe%2B2000s%2B%25231%2BBullinger.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-B9oG8vilHCw/WZYVia2KALI/AAAAAAAAhEg/91FOrLnLSikR95yDjz-VWkoaIulZCRxNgCLcBGAs/s1600/1982%2BTopps%2B%252320%2BMaddox.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-94w1fqQwETU/WZYViR1a3-I/AAAAAAAAhEc/nmnGlmnypWoEM5PjhieZSJaDcC4GW0B7ACLcBGAs/s1600/1982%2BTopps%2B%2523722%2BMartin.jpg</t>
+  </si>
+  <si>
+    <t>Pedro Florimon</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-gUJK8blwWow/WZY1FJH7P3I/AAAAAAAAhFE/HD3kGDEoCksEajxnYIqzxYMausWEtarAACLcBGAs/s1600/2017%2BChachi%2B%252354%2BFlorimon.jpg</t>
+  </si>
+  <si>
+    <t>Pedro Florimon in Action</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-hjWEAHs4ywE/WZorUkzJFqI/AAAAAAAAhIc/H4j1VqGf7KweO0oNL9AzzJqIoMzI7ibigCLcBGAs/s1600/2017%2BChachi%2BIn%2BAction%2B%25238%2BFlorimon.jpg</t>
+  </si>
+  <si>
+    <t>Manny Trillo</t>
+  </si>
+  <si>
+    <t>Louis Aguayo</t>
+  </si>
+  <si>
+    <t>Ramon Aviles</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-tBmTTVnHDjA/WZmyz9bx-TI/AAAAAAAAhHg/oTCv95lknLkQ7pDbrsE2Y-TLfV9geSGQwCLcBGAs/s1600/1982%2BTopps%2B%2523152%2BAviles.jpg</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-P8r8h9RCXqM/WZmyz5m8K-I/AAAAAAAAhHY/gdgFEWyToZ4SKNhvELTYqZDsc8uX2JGfgCLcBGAs/s1600/1982%2BTopps%2B%2523220%2BTrillo.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-oXLH1f3Kr_8/WZmyz84bruI/AAAAAAAAhHc/uXs3E9ApIpwN0ThmuA68qb7NtHOFAi60gCLcBGAs/s1600/1982%2BTopps%2B%2523449%2BAguayo.jpg</t>
+  </si>
+  <si>
+    <t>Chris Pritchett</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-FaCeFi4hjPo/WZoVIryCYTI/AAAAAAAAhHw/cyy7mO6Ruysq93ppcH3YDxhzz7-MpkDZwCLcBGAs/s1600/2017%2BChachi%2BPhillies%2BMissing%2BLinks%2Bof%2Bthe%2B2000s%2B%25232%2BPritchett.jpg</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-2jNyL689TtI/WZosXv12jbI/AAAAAAAAhIk/zkf4iaFoHQQCAiG6bvvDID1L2PL96XcvgCLcBGAs/s1600/2017%2BChachi%2BPhillies%2BMissing%2BLinks%2Bof%2Bthe%2B2000s%2B%25233%2BB.%2BWard.jpg</t>
+  </si>
+  <si>
+    <t>Bryan Ward</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-pr4uYv0nuz4/WZ62dkCXroI/AAAAAAAAMgQ/qEva-qPmuJkuDrosNmn93_kniGpQCVv0ACLcBGAs/s1600/1974-NOT-REALLY-LARRY-COX.jpg</t>
+  </si>
+  <si>
+    <t>Ivan DeJesus</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-4FKsHC_vS24/WZ-L-16PaqI/AAAAAAAAhKU/AnXQ15JRkqws55bXNy3nz9TzUNxybfyiwCLcBGAs/s1600/1982%2BTopps%2B%2523484%2BDeJesus.jpg</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-DbX1-JRh47c/WZ-L-xRNS_I/AAAAAAAAhKc/q3En1aNkPks7fdiUuWvuSTDg2tfuv4mfwCLcBGAs/s1600/1982%2BTopps%2BTraded%2B%252310T%2BBowa.jpg</t>
+  </si>
+  <si>
+    <t>Ivan DeJusus</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-DsyMyxAS_oM/WZ-L-9C1mKI/AAAAAAAAhKY/tkwkbLZvfJIVhuHtJJhhJ_oRopco7OEXgCLcBGAs/s1600/1982%2BTopps%2B%2523515%2BBowa.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-yV6B4qQeJWQ/WZ-L_EBsuLI/AAAAAAAAhKg/VDB_0rUWvfgnrbvlmugcblPZh8RhVa6DgCLcBGAs/s1600/1982%2BTopps%2BTraded%2B%252327T%2BDeJesus.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-itETFYA8CJY/WaHHNzNSFeI/AAAAAAAAhLk/ad3gOnz0uc0iKYc4tt6G9JQ6oCJtGYFYACLcBGAs/s1600/2017%2BChachi%2B%252356%2BHoskins%2BHL.jpg</t>
+  </si>
+  <si>
+    <t>Highlights: Rhys Hoskins</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-WVyM5vF-KKc/WZ-HZgWe4zI/AAAAAAAAhKI/Ol3pBjbFuz4wjyH7KsQ9a2x6n22g9WiPgCLcBGAs/s1600/2017%2BChachi%2B%252355%2BRios.jpg</t>
+  </si>
+  <si>
+    <t>Yacksel Rios</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-5lorDZwT058/WaNj3-GgLII/AAAAAAAAhMo/gU92dK10CVsTL2C8saS0h-Rtpl62BU6KACLcBGAs/s1600/2017%2BChachi%2B%252357%2BHoskins%2BHL.jpg</t>
+  </si>
+  <si>
+    <t>Highlights: Rhys Hoskins Triple Play</t>
+  </si>
+  <si>
+    <t>https://d8bixwancjkpp.cloudfront.net/wp-content/uploads/2017/08/Rhys.jpg</t>
+  </si>
+  <si>
+    <t>https://click.linksynergy.com/deeplink?id=HBIziMwGv6o&amp;mid=39268&amp;murl=https%3A%2F%2Fwww.topps.com%2Fcollectibles%2Ftrading-cards%2Ftopps-now.html%2F</t>
+  </si>
+  <si>
+    <t>Rhys Hoskins Topps NOW</t>
+  </si>
+  <si>
+    <t>Rhys Hoskins 2016 Panini Elite Extra</t>
+  </si>
+  <si>
+    <t>Steve Carlton In Action</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-bWQBDf70cPs/WaScpG2IQqI/AAAAAAAAhNE/v3dWHaS9ymkvAhl8bD1UyahqPNQBCc8FQCLcBGAs/s1600/1982%2BTopps%2B%25231%2BCarlton%2BHL.jpg</t>
+  </si>
+  <si>
+    <t>Mark Holzmer</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-2_W1mxPLZig/WaHH5jj4a5I/AAAAAAAAhLs/uDwC0h6YFTYXUEGVcQg1T7q-rsUxgfo3gCLcBGAs/s1600/2017%2BChachi%2BPhillies%2BMissing%2BLinks%2Bof%2Bthe%2B2000s%2B%25234%2BHolzemer.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-qgZkP0VA-aw/WZh7sLctRyI/AAAAAAAAqgE/4XsjBt8VJGY09HH-PwODdQ0oxJOUvpXhQCLcBGAs/s1600/Topps%2B1969%2B073%2BBriggs.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13094,6 +13278,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -13423,10 +13620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13753,653 +13950,701 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>3732</v>
+        <v>4377</v>
       </c>
       <c r="B42" t="s">
-        <v>3733</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>3785</v>
+        <v>4381</v>
       </c>
       <c r="B43" t="s">
-        <v>3786</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>3817</v>
+        <v>3732</v>
       </c>
       <c r="B44" t="s">
-        <v>3816</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>4019</v>
+        <v>3785</v>
       </c>
       <c r="B45" t="s">
-        <v>4020</v>
+        <v>3786</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4116</v>
+        <v>3817</v>
       </c>
       <c r="B46" t="s">
-        <v>4115</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>4122</v>
+        <v>4019</v>
       </c>
       <c r="B47" t="s">
-        <v>4121</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>4138</v>
+        <v>4116</v>
       </c>
       <c r="B48" t="s">
-        <v>4139</v>
+        <v>4115</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1389</v>
+        <v>4122</v>
       </c>
       <c r="B49" t="s">
-        <v>3815</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1231</v>
+        <v>4348</v>
       </c>
       <c r="B50" t="s">
-        <v>3819</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1388</v>
+        <v>4357</v>
       </c>
       <c r="B51" t="s">
-        <v>3822</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1401</v>
+        <v>4138</v>
       </c>
       <c r="B52" t="s">
-        <v>3856</v>
+        <v>4139</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1402</v>
+        <v>1389</v>
       </c>
       <c r="B53" t="s">
-        <v>3858</v>
+        <v>3815</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1750</v>
+        <v>1231</v>
       </c>
       <c r="B54" t="s">
-        <v>3859</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>3874</v>
+        <v>1388</v>
       </c>
       <c r="B55" t="s">
-        <v>3873</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>2032</v>
+        <v>1401</v>
       </c>
       <c r="B56" t="s">
-        <v>3910</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>4182</v>
+        <v>1402</v>
       </c>
       <c r="B57" t="s">
-        <v>4183</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>4184</v>
+        <v>1750</v>
       </c>
       <c r="B58" t="s">
-        <v>4185</v>
+        <v>3859</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>3027</v>
+        <v>3874</v>
       </c>
       <c r="B59" t="s">
-        <v>4280</v>
+        <v>3873</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>138</v>
+        <v>2032</v>
       </c>
       <c r="B60" t="s">
-        <v>2999</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>4174</v>
+        <v>4182</v>
       </c>
       <c r="B61" t="s">
-        <v>4247</v>
+        <v>4183</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>4305</v>
+        <v>4184</v>
       </c>
       <c r="B62" t="s">
-        <v>4306</v>
+        <v>4185</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>3027</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4280</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>2537</v>
+        <v>138</v>
       </c>
       <c r="B64" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>2501</v>
+        <v>4174</v>
       </c>
       <c r="B65" t="s">
-        <v>3025</v>
+        <v>4247</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>2721</v>
+        <v>4305</v>
       </c>
       <c r="B66" t="s">
-        <v>3028</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>3029</v>
+        <v>4355</v>
       </c>
       <c r="B67" t="s">
-        <v>3030</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>3033</v>
+        <v>4379</v>
       </c>
       <c r="B68" t="s">
-        <v>3034</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>3024</v>
-      </c>
-      <c r="B69" t="s">
-        <v>4026</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>3861</v>
+        <v>2537</v>
       </c>
       <c r="B70" t="s">
-        <v>3860</v>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>2501</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3025</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>2721</v>
+      </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>132</v>
+        <v>3029</v>
       </c>
       <c r="B73" t="s">
-        <v>2984</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>3033</v>
       </c>
       <c r="B74" t="s">
-        <v>3018</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>2518</v>
+        <v>3024</v>
       </c>
       <c r="B75" t="s">
-        <v>3019</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>209</v>
+        <v>3861</v>
       </c>
       <c r="B76" t="s">
-        <v>3021</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>2722</v>
-      </c>
-      <c r="B77" t="s">
-        <v>3165</v>
+        <v>3860</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>2458</v>
-      </c>
       <c r="B78" t="s">
-        <v>3166</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>2897</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>3167</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="B80" t="s">
-        <v>3171</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>2364</v>
+        <v>2518</v>
       </c>
       <c r="B81" t="s">
-        <v>3172</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>2036</v>
+        <v>209</v>
       </c>
       <c r="B82" t="s">
-        <v>3280</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>2722</v>
       </c>
       <c r="B83" t="s">
-        <v>3281</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>2</v>
+        <v>2458</v>
       </c>
       <c r="B84" t="s">
-        <v>3282</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>22</v>
+        <v>2897</v>
       </c>
       <c r="B85" t="s">
-        <v>3283</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="B86" t="s">
-        <v>3284</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>2364</v>
       </c>
       <c r="B87" t="s">
-        <v>3576</v>
+        <v>3172</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>2036</v>
       </c>
       <c r="B88" t="s">
-        <v>3596</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>2441</v>
+        <v>143</v>
       </c>
       <c r="B89" t="s">
-        <v>4028</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>4029</v>
+        <v>3282</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B91" t="s">
-        <v>4099</v>
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3596</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>2441</v>
+      </c>
       <c r="B95" t="s">
-        <v>26</v>
+        <v>4028</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>2362</v>
+        <v>14</v>
       </c>
       <c r="B96" t="s">
-        <v>3004</v>
+        <v>4029</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>3556</v>
+        <v>13</v>
       </c>
       <c r="B97" t="s">
-        <v>3557</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>3230</v>
-      </c>
-      <c r="B98" t="s">
-        <v>3563</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>3562</v>
-      </c>
-      <c r="B99" t="s">
-        <v>3564</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>2616</v>
-      </c>
-      <c r="B100" t="s">
-        <v>3577</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>12</v>
-      </c>
       <c r="B101" t="s">
-        <v>4024</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>2362</v>
       </c>
       <c r="B102" t="s">
-        <v>4025</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>2055</v>
+        <v>3556</v>
       </c>
       <c r="B103" t="s">
-        <v>4027</v>
+        <v>3557</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>3230</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3563</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>3562</v>
+      </c>
       <c r="B105" t="s">
-        <v>85</v>
+        <v>3564</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>1751</v>
+        <v>2616</v>
       </c>
       <c r="B106" t="s">
-        <v>3245</v>
+        <v>3577</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>2034</v>
+        <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>2368</v>
+        <v>4024</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="B108" t="s">
-        <v>2675</v>
+        <v>4025</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>3464</v>
+        <v>2055</v>
       </c>
       <c r="B109" t="s">
-        <v>3463</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>2983</v>
-      </c>
-      <c r="B110" t="s">
-        <v>3567</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>3579</v>
-      </c>
       <c r="B111" t="s">
-        <v>3580</v>
+        <v>85</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>3209</v>
+        <v>1751</v>
       </c>
       <c r="B112" t="s">
-        <v>3566</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>3163</v>
+        <v>2034</v>
       </c>
       <c r="B113" t="s">
-        <v>3568</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>3644</v>
+        <v>8</v>
       </c>
       <c r="B114" t="s">
-        <v>3643</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>2982</v>
+        <v>3464</v>
       </c>
       <c r="B115" t="s">
-        <v>3569</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>3876</v>
+        <v>2983</v>
       </c>
       <c r="B116" t="s">
-        <v>3877</v>
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>3579</v>
+      </c>
+      <c r="B117" t="s">
+        <v>3580</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>3209</v>
+      </c>
       <c r="B118" t="s">
-        <v>2701</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>247</v>
+        <v>3163</v>
       </c>
       <c r="B119" t="s">
-        <v>3314</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>3644</v>
       </c>
       <c r="B120" t="s">
-        <v>3315</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>2982</v>
       </c>
       <c r="B121" t="s">
-        <v>3316</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>142</v>
+        <v>3876</v>
       </c>
       <c r="B122" t="s">
-        <v>3317</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>252</v>
-      </c>
-      <c r="B123" t="s">
-        <v>3318</v>
+        <v>3877</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>191</v>
-      </c>
       <c r="B124" t="s">
-        <v>3319</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>192</v>
+        <v>247</v>
       </c>
       <c r="B125" t="s">
-        <v>3320</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>194</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>3321</v>
+        <v>3315</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>3323</v>
+        <v>3316</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>1238</v>
+        <v>142</v>
       </c>
       <c r="B128" t="s">
-        <v>3324</v>
+        <v>3317</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>1277</v>
+        <v>252</v>
       </c>
       <c r="B129" t="s">
-        <v>3465</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>3322</v>
+        <v>191</v>
       </c>
       <c r="B130" t="s">
-        <v>3325</v>
+        <v>3319</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>192</v>
+      </c>
+      <c r="B131" t="s">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>194</v>
+      </c>
+      <c r="B132" t="s">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>130</v>
+      </c>
+      <c r="B133" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B134" t="s">
+        <v>3324</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B135" t="s">
+        <v>3465</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>13</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B137" t="s">
         <v>4100</v>
       </c>
     </row>
@@ -22655,10 +22900,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B162"/>
+  <dimension ref="A1:B179"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161:B161"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23020,321 +23265,281 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>3035</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>3036</v>
+        <v>4351</v>
       </c>
       <c r="B50" t="s">
-        <v>3044</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>270</v>
+        <v>4365</v>
       </c>
       <c r="B51" t="s">
-        <v>3045</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>3037</v>
+        <v>4368</v>
       </c>
       <c r="B52" t="s">
-        <v>3046</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>3038</v>
+        <v>4388</v>
       </c>
       <c r="B53" t="s">
-        <v>3047</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>267</v>
-      </c>
-      <c r="B54" t="s">
-        <v>3048</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>3039</v>
-      </c>
-      <c r="B55" t="s">
-        <v>3049</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>3040</v>
-      </c>
-      <c r="B56" t="s">
-        <v>3050</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>3041</v>
-      </c>
-      <c r="B57" t="s">
-        <v>3051</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>3042</v>
-      </c>
-      <c r="B58" t="s">
-        <v>3052</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>3043</v>
-      </c>
-      <c r="B59" t="s">
-        <v>3053</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>3054</v>
-      </c>
       <c r="B60" t="s">
-        <v>3061</v>
+        <v>3035</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>3055</v>
+        <v>3036</v>
       </c>
       <c r="B61" t="s">
-        <v>3062</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>3056</v>
+        <v>270</v>
       </c>
       <c r="B62" t="s">
-        <v>3063</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>3057</v>
+        <v>3037</v>
       </c>
       <c r="B63" t="s">
-        <v>3064</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>271</v>
+        <v>3038</v>
       </c>
       <c r="B64" t="s">
-        <v>3065</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B65" t="s">
-        <v>3066</v>
+        <v>3048</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>269</v>
+        <v>3039</v>
       </c>
       <c r="B66" t="s">
-        <v>3067</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>3058</v>
+        <v>3040</v>
       </c>
       <c r="B67" t="s">
-        <v>3068</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>3059</v>
+        <v>3041</v>
       </c>
       <c r="B68" t="s">
-        <v>3069</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>3060</v>
+        <v>3042</v>
       </c>
       <c r="B69" t="s">
-        <v>3070</v>
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3053</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>3054</v>
+      </c>
       <c r="B71" t="s">
-        <v>3072</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>3073</v>
+        <v>3055</v>
       </c>
       <c r="B72" t="s">
-        <v>3081</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>3074</v>
+        <v>3056</v>
       </c>
       <c r="B73" t="s">
-        <v>3082</v>
+        <v>3063</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>3075</v>
+        <v>3057</v>
       </c>
       <c r="B74" t="s">
-        <v>3083</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>1490</v>
+        <v>271</v>
       </c>
       <c r="B75" t="s">
-        <v>3084</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>3076</v>
+        <v>268</v>
       </c>
       <c r="B76" t="s">
-        <v>3085</v>
+        <v>3066</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1915</v>
+        <v>269</v>
       </c>
       <c r="B77" t="s">
-        <v>3086</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>3077</v>
+        <v>3058</v>
       </c>
       <c r="B78" t="s">
-        <v>3087</v>
+        <v>3068</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1923</v>
+        <v>3059</v>
       </c>
       <c r="B79" t="s">
-        <v>3088</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>3078</v>
+        <v>3060</v>
       </c>
       <c r="B80" t="s">
-        <v>3089</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>3079</v>
-      </c>
-      <c r="B81" t="s">
-        <v>3090</v>
+        <v>3070</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>3080</v>
-      </c>
       <c r="B82" t="s">
-        <v>3091</v>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>3073</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3081</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>3074</v>
+      </c>
       <c r="B84" t="s">
-        <v>3094</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>3095</v>
+        <v>3075</v>
       </c>
       <c r="B85" t="s">
-        <v>3102</v>
+        <v>3083</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>3096</v>
+        <v>1490</v>
       </c>
       <c r="B86" t="s">
-        <v>3103</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>3040</v>
+        <v>3076</v>
       </c>
       <c r="B87" t="s">
-        <v>3104</v>
+        <v>3085</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>265</v>
+        <v>1915</v>
       </c>
       <c r="B88" t="s">
-        <v>3105</v>
+        <v>3086</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1923</v>
+        <v>3077</v>
       </c>
       <c r="B89" t="s">
-        <v>3106</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1929</v>
+        <v>1923</v>
       </c>
       <c r="B90" t="s">
-        <v>3107</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>3097</v>
+        <v>3078</v>
       </c>
       <c r="B91" t="s">
-        <v>3108</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -23342,140 +23547,140 @@
         <v>3079</v>
       </c>
       <c r="B92" t="s">
-        <v>3109</v>
+        <v>3090</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>3098</v>
+        <v>3080</v>
       </c>
       <c r="B93" t="s">
-        <v>3110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>1916</v>
-      </c>
-      <c r="B94" t="s">
-        <v>3111</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>3099</v>
-      </c>
       <c r="B95" t="s">
-        <v>3112</v>
+        <v>3094</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>3100</v>
+        <v>3095</v>
       </c>
       <c r="B96" t="s">
-        <v>3113</v>
+        <v>3102</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1913</v>
+        <v>3096</v>
       </c>
       <c r="B97" t="s">
-        <v>3114</v>
+        <v>3103</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1953</v>
+        <v>3040</v>
       </c>
       <c r="B98" t="s">
-        <v>3115</v>
+        <v>3104</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>3101</v>
+        <v>265</v>
       </c>
       <c r="B99" t="s">
-        <v>3116</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>1958</v>
+        <v>1923</v>
       </c>
       <c r="B100" t="s">
-        <v>3117</v>
+        <v>3106</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3107</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>3097</v>
+      </c>
       <c r="B102" t="s">
-        <v>3118</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>3096</v>
+        <v>3079</v>
       </c>
       <c r="B103" t="s">
-        <v>3134</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>1936</v>
+        <v>3098</v>
       </c>
       <c r="B104" t="s">
-        <v>3133</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>3119</v>
+        <v>1916</v>
       </c>
       <c r="B105" t="s">
-        <v>3132</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>3120</v>
+        <v>3099</v>
       </c>
       <c r="B106" t="s">
-        <v>3131</v>
+        <v>3112</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>1960</v>
+        <v>3100</v>
       </c>
       <c r="B107" t="s">
-        <v>3129</v>
+        <v>3113</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>3121</v>
+        <v>1913</v>
       </c>
       <c r="B108" t="s">
-        <v>3130</v>
+        <v>3114</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>3122</v>
+        <v>1953</v>
       </c>
       <c r="B109" t="s">
-        <v>3128</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>3123</v>
+        <v>3101</v>
       </c>
       <c r="B110" t="s">
-        <v>3127</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -23483,385 +23688,518 @@
         <v>1958</v>
       </c>
       <c r="B111" t="s">
-        <v>3126</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>3124</v>
-      </c>
-      <c r="B112" t="s">
-        <v>3125</v>
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>3118</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>3096</v>
+      </c>
       <c r="B114" t="s">
-        <v>3137</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>1950</v>
+        <v>1936</v>
       </c>
       <c r="B115" t="s">
-        <v>3138</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>2760</v>
+        <v>3119</v>
       </c>
       <c r="B116" t="s">
-        <v>3139</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>2767</v>
+        <v>3120</v>
       </c>
       <c r="B117" t="s">
-        <v>3140</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>2018</v>
+        <v>1960</v>
       </c>
       <c r="B118" t="s">
-        <v>3141</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>1968</v>
+        <v>3121</v>
       </c>
       <c r="B119" t="s">
-        <v>3142</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>1960</v>
+        <v>3122</v>
       </c>
       <c r="B120" t="s">
-        <v>3143</v>
+        <v>3128</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>1919</v>
+        <v>3123</v>
       </c>
       <c r="B121" t="s">
-        <v>3144</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>1962</v>
+        <v>1958</v>
       </c>
       <c r="B122" t="s">
-        <v>3145</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>2069</v>
-      </c>
-      <c r="B124" t="s">
-        <v>3813</v>
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B123" t="s">
+        <v>3125</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>2075</v>
-      </c>
       <c r="B125" t="s">
-        <v>3814</v>
+        <v>3137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B126" t="s">
+        <v>3138</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>4188</v>
+        <v>2760</v>
+      </c>
+      <c r="B127" t="s">
+        <v>3139</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>4189</v>
+        <v>2767</v>
       </c>
       <c r="B128" t="s">
-        <v>4201</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>4190</v>
+        <v>2018</v>
       </c>
       <c r="B129" t="s">
-        <v>4207</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>4191</v>
+        <v>1968</v>
       </c>
       <c r="B130" t="s">
-        <v>4205</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>4192</v>
+        <v>1960</v>
       </c>
       <c r="B131" t="s">
-        <v>4202</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>4193</v>
+        <v>1919</v>
       </c>
       <c r="B132" t="s">
-        <v>4204</v>
+        <v>3144</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>4194</v>
+        <v>1962</v>
       </c>
       <c r="B133" t="s">
-        <v>4206</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>4195</v>
+        <v>2069</v>
       </c>
       <c r="B134" t="s">
-        <v>4208</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>4196</v>
+        <v>2075</v>
       </c>
       <c r="B135" t="s">
-        <v>4203</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>4197</v>
-      </c>
-      <c r="B136" t="s">
-        <v>4211</v>
+        <v>3814</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>4198</v>
-      </c>
-      <c r="B137" t="s">
-        <v>4212</v>
+        <v>4188</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>4199</v>
+        <v>4189</v>
       </c>
       <c r="B138" t="s">
-        <v>4210</v>
+        <v>4201</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>4200</v>
+        <v>4190</v>
       </c>
       <c r="B139" t="s">
-        <v>4209</v>
+        <v>4207</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>4217</v>
+        <v>4191</v>
       </c>
       <c r="B140" t="s">
-        <v>4222</v>
+        <v>4205</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>4218</v>
+        <v>4192</v>
       </c>
       <c r="B141" t="s">
-        <v>4224</v>
+        <v>4202</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>4219</v>
+        <v>4193</v>
       </c>
       <c r="B142" t="s">
-        <v>4237</v>
+        <v>4204</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>4220</v>
+        <v>4194</v>
       </c>
       <c r="B143" t="s">
-        <v>4223</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>4221</v>
+        <v>4195</v>
       </c>
       <c r="B144" t="s">
-        <v>4236</v>
+        <v>4208</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>4228</v>
+        <v>4196</v>
       </c>
       <c r="B145" t="s">
-        <v>4225</v>
+        <v>4203</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>4229</v>
+        <v>4197</v>
       </c>
       <c r="B146" t="s">
-        <v>4226</v>
+        <v>4211</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>4227</v>
+        <v>4198</v>
       </c>
       <c r="B147" t="s">
-        <v>4238</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>4230</v>
+        <v>4199</v>
       </c>
       <c r="B148" t="s">
-        <v>4235</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>4231</v>
+        <v>4200</v>
       </c>
       <c r="B149" t="s">
-        <v>4241</v>
+        <v>4209</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>4232</v>
+        <v>4217</v>
       </c>
       <c r="B150" t="s">
-        <v>4239</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>4233</v>
+        <v>4218</v>
       </c>
       <c r="B151" t="s">
-        <v>4242</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>4234</v>
+        <v>4219</v>
       </c>
       <c r="B152" t="s">
-        <v>4240</v>
+        <v>4237</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>4315</v>
+        <v>4220</v>
       </c>
       <c r="B153" t="s">
-        <v>4332</v>
+        <v>4223</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>4316</v>
+        <v>4221</v>
       </c>
       <c r="B154" t="s">
-        <v>4328</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>4317</v>
+        <v>4228</v>
       </c>
       <c r="B155" t="s">
-        <v>4333</v>
+        <v>4225</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>4318</v>
+        <v>4229</v>
       </c>
       <c r="B156" t="s">
-        <v>4334</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>4319</v>
+        <v>4227</v>
       </c>
       <c r="B157" t="s">
-        <v>4320</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>4322</v>
+        <v>4230</v>
       </c>
       <c r="B158" t="s">
-        <v>4321</v>
+        <v>4235</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>4323</v>
+        <v>4231</v>
       </c>
       <c r="B159" t="s">
-        <v>4327</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>4324</v>
+        <v>4232</v>
       </c>
       <c r="B160" t="s">
-        <v>4329</v>
+        <v>4239</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>4325</v>
+        <v>4233</v>
       </c>
       <c r="B161" t="s">
-        <v>4330</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>4234</v>
+      </c>
+      <c r="B162" t="s">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>4315</v>
+      </c>
+      <c r="B163" t="s">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>4316</v>
+      </c>
+      <c r="B164" t="s">
+        <v>4328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>4317</v>
+      </c>
+      <c r="B165" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>4318</v>
+      </c>
+      <c r="B166" t="s">
+        <v>4334</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>4319</v>
+      </c>
+      <c r="B167" t="s">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>4322</v>
+      </c>
+      <c r="B168" t="s">
+        <v>4321</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>4323</v>
+      </c>
+      <c r="B169" t="s">
+        <v>4327</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>4324</v>
+      </c>
+      <c r="B170" t="s">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>4325</v>
+      </c>
+      <c r="B171" t="s">
+        <v>4330</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
         <v>4326</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B172" t="s">
         <v>4331</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B173" t="s">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B174" t="s">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B175" t="s">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B177" t="s">
+        <v>4342</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B179" t="s">
+        <v>4347</v>
       </c>
     </row>
   </sheetData>
@@ -24356,10 +24694,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24524,6 +24862,14 @@
         <v>1629</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>3546</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4369</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24531,10 +24877,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24648,6 +24994,14 @@
         <v>2139</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4390</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24655,10 +25009,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24903,388 +25257,468 @@
         <v>4313</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>4359</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4363</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4360</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4364</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4361</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4362</v>
+      </c>
+    </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>3586</v>
+        <v>1388</v>
       </c>
       <c r="B35" t="s">
-        <v>3588</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1685</v>
+        <v>4373</v>
       </c>
       <c r="B36" t="s">
-        <v>3597</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>3613</v>
+        <v>4386</v>
       </c>
       <c r="B37" t="s">
-        <v>3614</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>3652</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3653</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3696</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3699</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>3697</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3700</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>3698</v>
+        <v>3586</v>
       </c>
       <c r="B41" t="s">
-        <v>3701</v>
+        <v>3588</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>3712</v>
+        <v>1685</v>
       </c>
       <c r="B42" t="s">
-        <v>3836</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>3713</v>
+        <v>3613</v>
       </c>
       <c r="B43" t="s">
-        <v>3719</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>3714</v>
+        <v>3652</v>
       </c>
       <c r="B44" t="s">
-        <v>3718</v>
+        <v>3653</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1968</v>
+        <v>3696</v>
       </c>
       <c r="B45" t="s">
-        <v>3725</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>3697</v>
       </c>
       <c r="B46" t="s">
-        <v>3730</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>3726</v>
+        <v>3698</v>
       </c>
       <c r="B47" t="s">
-        <v>3729</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>2018</v>
+        <v>3712</v>
       </c>
       <c r="B48" t="s">
-        <v>3728</v>
+        <v>3836</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>3101</v>
+        <v>3713</v>
       </c>
       <c r="B49" t="s">
-        <v>3727</v>
+        <v>3719</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>261</v>
+        <v>3714</v>
       </c>
       <c r="B50" t="s">
-        <v>3745</v>
+        <v>3718</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>262</v>
+        <v>1968</v>
       </c>
       <c r="B51" t="s">
-        <v>3746</v>
+        <v>3725</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>2018</v>
+        <v>259</v>
       </c>
       <c r="B52" t="s">
-        <v>3747</v>
+        <v>3730</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>2004</v>
+        <v>3726</v>
       </c>
       <c r="B53" t="s">
-        <v>3748</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1490</v>
+        <v>2018</v>
       </c>
       <c r="B54" t="s">
-        <v>3752</v>
+        <v>3728</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>3751</v>
+        <v>3101</v>
       </c>
       <c r="B55" t="s">
-        <v>3753</v>
+        <v>3727</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1555</v>
+        <v>261</v>
       </c>
       <c r="B56" t="s">
-        <v>3754</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1931</v>
+        <v>262</v>
       </c>
       <c r="B57" t="s">
-        <v>3755</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>3042</v>
+        <v>2018</v>
       </c>
       <c r="B58" t="s">
-        <v>3789</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>2773</v>
+        <v>2004</v>
       </c>
       <c r="B59" t="s">
-        <v>3811</v>
+        <v>3748</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>2666</v>
+        <v>1490</v>
       </c>
       <c r="B60" t="s">
-        <v>3812</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>3824</v>
+        <v>3751</v>
       </c>
       <c r="B61" t="s">
-        <v>3825</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>2009</v>
+        <v>1555</v>
       </c>
       <c r="B62" t="s">
-        <v>3853</v>
+        <v>3754</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>2664</v>
+        <v>1931</v>
       </c>
       <c r="B63" t="s">
-        <v>3862</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>2772</v>
+        <v>3042</v>
       </c>
       <c r="B64" t="s">
-        <v>3863</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>3871</v>
+        <v>2773</v>
       </c>
       <c r="B65" t="s">
-        <v>3872</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>3915</v>
+        <v>2666</v>
       </c>
       <c r="B66" t="s">
-        <v>3916</v>
+        <v>3812</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>2760</v>
+        <v>3824</v>
       </c>
       <c r="B67" t="s">
-        <v>4093</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4091</v>
+        <v>2009</v>
       </c>
       <c r="B68" t="s">
-        <v>4092</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1580</v>
+        <v>2664</v>
       </c>
       <c r="B69" t="s">
-        <v>4107</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>4108</v>
+        <v>2772</v>
       </c>
       <c r="B70" t="s">
-        <v>4109</v>
+        <v>3863</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>3097</v>
+        <v>3871</v>
       </c>
       <c r="B71" t="s">
-        <v>4117</v>
+        <v>3872</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>2006</v>
+        <v>3915</v>
       </c>
       <c r="B72" t="s">
-        <v>4140</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1639</v>
+        <v>2760</v>
       </c>
       <c r="B73" t="s">
-        <v>4141</v>
+        <v>4093</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>3098</v>
+        <v>4091</v>
       </c>
       <c r="B74" t="s">
-        <v>4156</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>1401</v>
+        <v>1580</v>
       </c>
       <c r="B75" t="s">
-        <v>4157</v>
+        <v>4107</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>4162</v>
+        <v>4108</v>
       </c>
       <c r="B76" t="s">
-        <v>4163</v>
+        <v>4109</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>4164</v>
+        <v>3097</v>
       </c>
       <c r="B77" t="s">
-        <v>4166</v>
+        <v>4117</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>4165</v>
+        <v>2006</v>
       </c>
       <c r="B78" t="s">
-        <v>4167</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1584</v>
+        <v>1639</v>
       </c>
       <c r="B79" t="s">
-        <v>4181</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>4277</v>
+        <v>3098</v>
       </c>
       <c r="B80" t="s">
-        <v>4278</v>
+        <v>4156</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1938</v>
+        <v>1401</v>
       </c>
       <c r="B81" t="s">
-        <v>4279</v>
+        <v>4157</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>4162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>4164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>4165</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>4277</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4278</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B87" t="s">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>1706</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B88" t="s">
         <v>4314</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>3936</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4354</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>4370</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4372</v>
       </c>
     </row>
   </sheetData>
@@ -25293,11 +25727,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C684"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
-      <selection activeCell="A409" sqref="A409:XFD409"/>
+    <sheetView topLeftCell="A410" workbookViewId="0">
+      <selection activeCell="A429" sqref="A429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29122,8 +29556,22 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>4385</v>
+      </c>
+      <c r="B428" t="s">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>4384</v>
+      </c>
+      <c r="B429" t="s">
+        <v>4383</v>
+      </c>
+    </row>
     <row r="430" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="431" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="432" spans="1:2" x14ac:dyDescent="0.3">
@@ -31053,15 +31501,16 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B660"/>
+  <dimension ref="A1:B662"/>
   <sheetViews>
-    <sheetView topLeftCell="A635" workbookViewId="0">
-      <selection activeCell="A648" sqref="A648:XFD648"/>
+    <sheetView topLeftCell="A572" workbookViewId="0">
+      <selection activeCell="B579" sqref="B579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35131,429 +35580,445 @@
         <v>2679</v>
       </c>
     </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A587" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B587" t="s">
+        <v>4344</v>
+      </c>
+    </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
-        <v>4295</v>
-      </c>
-    </row>
-    <row r="589" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A589" t="s">
-        <v>20</v>
-      </c>
-      <c r="B589" t="s">
-        <v>2446</v>
+        <v>1121</v>
+      </c>
+      <c r="B588" t="s">
+        <v>4345</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
+        <v>4295</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A591" t="s">
+        <v>20</v>
+      </c>
+      <c r="B591" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A592" t="s">
         <v>4339</v>
       </c>
-      <c r="B590" t="s">
+      <c r="B592" t="s">
         <v>3164</v>
-      </c>
-    </row>
-    <row r="594" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A594" t="s">
-        <v>2328</v>
-      </c>
-    </row>
-    <row r="595" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A595" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B595" t="s">
-        <v>1894</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
-        <v>1896</v>
-      </c>
-      <c r="B596" t="s">
-        <v>1895</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
-        <v>1203</v>
+        <v>1161</v>
       </c>
       <c r="B597" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
-        <v>1236</v>
+        <v>1896</v>
       </c>
       <c r="B598" t="s">
-        <v>1898</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
-        <v>1408</v>
+        <v>1203</v>
       </c>
       <c r="B599" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
       <c r="B600" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
-        <v>252</v>
+        <v>1408</v>
       </c>
       <c r="B601" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
-        <v>1187</v>
+        <v>1230</v>
       </c>
       <c r="B602" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
-        <v>1238</v>
+        <v>252</v>
       </c>
       <c r="B603" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
-        <v>1181</v>
+        <v>1187</v>
       </c>
       <c r="B604" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B605" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A606" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B606" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A607" t="s">
         <v>20</v>
       </c>
-      <c r="B605" t="s">
+      <c r="B607" t="s">
         <v>2447</v>
-      </c>
-    </row>
-    <row r="609" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A609" t="s">
-        <v>4296</v>
-      </c>
-    </row>
-    <row r="610" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A610" t="s">
-        <v>20</v>
-      </c>
-      <c r="B610" t="s">
-        <v>2448</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
-        <v>1232</v>
-      </c>
-      <c r="B611" t="s">
-        <v>2430</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
-        <v>1228</v>
+        <v>20</v>
       </c>
       <c r="B612" t="s">
-        <v>2346</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B613" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A614" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B614" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A615" t="s">
         <v>2234</v>
       </c>
-      <c r="B613" t="s">
+      <c r="B615" t="s">
         <v>2348</v>
-      </c>
-    </row>
-    <row r="616" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A616" t="s">
-        <v>3843</v>
-      </c>
-    </row>
-    <row r="617" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A617" t="s">
-        <v>1800</v>
-      </c>
-      <c r="B617" t="s">
-        <v>1799</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
-        <v>2943</v>
-      </c>
-      <c r="B618" t="s">
-        <v>2942</v>
+        <v>3843</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
-        <v>2951</v>
+        <v>1800</v>
       </c>
       <c r="B619" t="s">
-        <v>2950</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
-        <v>2969</v>
+        <v>2943</v>
       </c>
       <c r="B620" t="s">
-        <v>2968</v>
+        <v>2942</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A621" t="s">
+        <v>2951</v>
+      </c>
+      <c r="B621" t="s">
+        <v>2950</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
-        <v>3845</v>
-      </c>
-    </row>
-    <row r="623" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A623" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B623" t="s">
-        <v>1829</v>
+        <v>2969</v>
+      </c>
+      <c r="B622" t="s">
+        <v>2968</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B624" t="s">
-        <v>1830</v>
+        <v>3845</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
-        <v>1283</v>
+        <v>1353</v>
       </c>
       <c r="B625" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
-        <v>1832</v>
+        <v>1354</v>
       </c>
       <c r="B626" t="s">
-        <v>1833</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
-        <v>1981</v>
+        <v>1283</v>
       </c>
       <c r="B627" t="s">
-        <v>1982</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
-        <v>2187</v>
+        <v>1832</v>
       </c>
       <c r="B628" t="s">
-        <v>2188</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B629" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A630" t="s">
+        <v>2187</v>
+      </c>
+      <c r="B630" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A631" t="s">
         <v>2458</v>
       </c>
-      <c r="B629" t="s">
+      <c r="B631" t="s">
         <v>2887</v>
       </c>
     </row>
-    <row r="632" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A632" t="s">
+    <row r="634" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A634" t="s">
         <v>3844</v>
       </c>
     </row>
-    <row r="633" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A633" t="s">
+    <row r="635" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A635" t="s">
         <v>1809</v>
       </c>
-      <c r="B633" t="s">
+      <c r="B635" t="s">
         <v>1810</v>
-      </c>
-    </row>
-    <row r="636" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A636" t="s">
-        <v>3840</v>
-      </c>
-    </row>
-    <row r="637" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A637" t="s">
-        <v>3593</v>
-      </c>
-      <c r="B637" t="s">
-        <v>3592</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
-        <v>1790</v>
-      </c>
-      <c r="B638" t="s">
-        <v>1791</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
-        <v>2171</v>
+        <v>3593</v>
       </c>
       <c r="B639" t="s">
-        <v>2172</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
-        <v>3830</v>
+        <v>1790</v>
       </c>
       <c r="B640" t="s">
-        <v>3831</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
-        <v>209</v>
+        <v>2171</v>
       </c>
       <c r="B641" t="s">
-        <v>2915</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
-        <v>143</v>
+        <v>3830</v>
       </c>
       <c r="B642" t="s">
-        <v>2917</v>
+        <v>3831</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A643" t="s">
+        <v>209</v>
+      </c>
+      <c r="B643" t="s">
+        <v>2915</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
-        <v>4340</v>
-      </c>
-    </row>
-    <row r="645" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A645" t="s">
-        <v>15</v>
-      </c>
-      <c r="B645" t="s">
-        <v>2570</v>
+        <v>143</v>
+      </c>
+      <c r="B644" t="s">
+        <v>2917</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
-        <v>2508</v>
-      </c>
-      <c r="B646" t="s">
-        <v>2509</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
+        <v>15</v>
+      </c>
+      <c r="B647" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A648" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B648" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A649" t="s">
         <v>4298</v>
       </c>
-      <c r="B647" t="s">
+      <c r="B649" t="s">
         <v>2920</v>
       </c>
     </row>
-    <row r="648" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A648" t="s">
+    <row r="650" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A650" t="s">
         <v>7</v>
       </c>
-      <c r="B648" t="s">
+      <c r="B650" t="s">
         <v>2921</v>
       </c>
     </row>
-    <row r="650" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A650" t="s">
+    <row r="652" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A652" t="s">
         <v>3841</v>
-      </c>
-    </row>
-    <row r="651" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A651" t="s">
-        <v>3537</v>
-      </c>
-      <c r="B651" t="s">
-        <v>3536</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
-        <v>3839</v>
-      </c>
-    </row>
-    <row r="654" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A654" t="s">
-        <v>3821</v>
-      </c>
-      <c r="B654" t="s">
-        <v>3820</v>
+        <v>3537</v>
+      </c>
+      <c r="B653" t="s">
+        <v>3536</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
-        <v>1780</v>
-      </c>
-      <c r="B655" t="s">
-        <v>1781</v>
+        <v>3839</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
-        <v>1813</v>
+        <v>3821</v>
       </c>
       <c r="B656" t="s">
-        <v>1814</v>
+        <v>3820</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
-        <v>1821</v>
+        <v>1780</v>
       </c>
       <c r="B657" t="s">
-        <v>1822</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
-        <v>1845</v>
+        <v>1813</v>
       </c>
       <c r="B658" t="s">
-        <v>1846</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
-        <v>3359</v>
+        <v>1821</v>
       </c>
       <c r="B659" t="s">
-        <v>3360</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B660" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A661" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B661" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A662" t="s">
         <v>3462</v>
       </c>
-      <c r="B660" t="s">
+      <c r="B662" t="s">
         <v>3461</v>
       </c>
     </row>

</xml_diff>

<commit_message>
doit directive to execute office files on server
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="17964" windowHeight="6060" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="17964" windowHeight="6060" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="25" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="4782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6120" uniqueCount="4789">
   <si>
     <t>Base Set</t>
   </si>
@@ -14414,6 +14414,27 @@
   </si>
   <si>
     <t>Katie Uhlaender</t>
+  </si>
+  <si>
+    <t>https://4.bp.blogspot.com/-3K6W41kS9cQ/WnIu7NZd3oI/AAAAAAAB1Tk/lOeKnNEK1EQFCvYJCypjNno_HppASzHewCLcBGAs/s1600/gamble2-2.jpg</t>
+  </si>
+  <si>
+    <t>Jose Altuve</t>
+  </si>
+  <si>
+    <t>https://shlabotnikreport.files.wordpress.com/2018/01/2018-tsrchives-jose-altuve-astros-180116.jpg</t>
+  </si>
+  <si>
+    <t>https://shlabotnikreport.files.wordpress.com/2018/01/2018-tsrchives-giancarlo-stanton-yankees-180106.jpg</t>
+  </si>
+  <si>
+    <t>Giancarlo Stanton</t>
+  </si>
+  <si>
+    <t>https://3.bp.blogspot.com/-VJ0zpjhIHaY/Wm8ApDJQbsI/AAAAAAAANcQ/sAQP5nessq8Ikt2Vp8exi2ZSpFpW7r0swCLcBGAs/s1600/1977-NOT-REALLY-FRED-ANDREWS.jpg</t>
+  </si>
+  <si>
+    <t>Fred Andrews</t>
   </si>
 </sst>
 </file>
@@ -20344,7 +20365,7 @@
         <v>} , { "name" : "Chad Qualls", "link" : "https://lh3.googleusercontent.com/wnBtJWdXCvLMobsNBKGP62e871VvDIyqt0dZCcJzYmc=w225-h321-p-no""</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>3068</v>
       </c>
@@ -28127,8 +28148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A741" workbookViewId="0">
-      <selection activeCell="A759" sqref="A759"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28212,6 +28233,22 @@
       </c>
       <c r="B10" t="s">
         <v>4397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4783</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4786</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4785</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -34606,10 +34643,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B811"/>
   <sheetViews>
-    <sheetView topLeftCell="A474" workbookViewId="0">
-      <pane ySplit="3168" topLeftCell="A732"/>
-      <selection activeCell="A481" sqref="A481"/>
-      <selection pane="bottomLeft" activeCell="A733" sqref="A733"/>
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
+      <pane ySplit="3168" topLeftCell="A732" activePane="bottomLeft"/>
+      <selection activeCell="A459" sqref="A459"/>
+      <selection pane="bottomLeft" activeCell="F734" sqref="F734:G734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37065,6 +37102,14 @@
         <v>4364</v>
       </c>
     </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B329" t="s">
+        <v>4782</v>
+      </c>
+    </row>
     <row r="333" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>2320</v>
@@ -38027,6 +38072,14 @@
       </c>
       <c r="B457" t="s">
         <v>3957</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>4788</v>
+      </c>
+      <c r="B458" t="s">
+        <v>4787</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Script to copy saved tiddly back on original
</commit_message>
<xml_diff>
--- a/chachis.xlsx
+++ b/chachis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4608" windowWidth="17304" windowHeight="2532" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="5040" windowWidth="17304" windowHeight="2532" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="25" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <author>Heaney, Daniel H CIV NSWCDD, W42</author>
   </authors>
   <commentList>
-    <comment ref="B468" authorId="0" shapeId="0">
+    <comment ref="B469" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6716" uniqueCount="5170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6724" uniqueCount="5178">
   <si>
     <t>Base Set</t>
   </si>
@@ -15584,6 +15584,30 @@
   </si>
   <si>
     <t>https://2.bp.blogspot.com/-d2iFLZW8-OM/W1pJEpwvUhI/AAAAAAAApBg/kcm1LQ-gj6ou5v46NUBszeRwoxmxYFJfACLcBGAs/s1600/Frankenset_008.JPG</t>
+  </si>
+  <si>
+    <t>Mike Schmidt Fleer Tribute</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/--WcOkQl_wmI/W2MuMpuVusI/AAAAAAABSyg/XBRIWSWkw3U-orHSSRNM5-d-PXXNZbwMwCLcBGAs/s1600/ScanImage215%2B%25284%2529.jpg</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-7swba-47Zk0/W3bpHyKR6ZI/AAAAAAAAk3w/F4WcP4Ua8oQp7m4NhD3Gv4Zs0nu9G7t7QCLcBGAs/s1600/2018%2BChachi%2B%252349%2BLoup.jpg</t>
+  </si>
+  <si>
+    <t>Aaron Loup</t>
+  </si>
+  <si>
+    <t>https://2.bp.blogspot.com/-9JY29W4VrfQ/W3C8c5cdn5I/AAAAAAAAk0I/kziYFSoO6okoD_TGg5u87CHtQfEnVpYqQCLcBGAs/s1600/2018%2BChachi%2B%252350%2BBour.jpg</t>
+  </si>
+  <si>
+    <t>Justin Bour</t>
+  </si>
+  <si>
+    <t>Wilson Ramos</t>
+  </si>
+  <si>
+    <t>https://1.bp.blogspot.com/-T3b64kZU8_U/W3b0K4oQCHI/AAAAAAAAk4c/1BZL-xLejDUQCex2wRiOt_gQcifSyASHACLcBGAs/s1600/2018%2BChachi%2B%252351%2BRamos.jpg</t>
   </si>
 </sst>
 </file>
@@ -15967,8 +15991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16435,6 +16459,30 @@
       </c>
       <c r="B59" t="s">
         <v>5124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>5173</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>5175</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>5176</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5177</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -31696,10 +31744,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C807"/>
+  <dimension ref="A1:C808"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
-      <selection activeCell="B400" sqref="B400"/>
+    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="B435" sqref="B435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35655,634 +35703,634 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
-        <v>2877</v>
+        <v>5170</v>
       </c>
       <c r="B435" t="s">
-        <v>2876</v>
+        <v>5171</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
-        <v>3770</v>
+        <v>2877</v>
       </c>
       <c r="B436" t="s">
-        <v>3771</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
-        <v>2501</v>
+        <v>3770</v>
       </c>
       <c r="B437" t="s">
-        <v>2504</v>
+        <v>3771</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
-        <v>2537</v>
+        <v>2501</v>
       </c>
       <c r="B438" t="s">
-        <v>2538</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
-        <v>3480</v>
+        <v>2537</v>
       </c>
       <c r="B439" t="s">
-        <v>3483</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
-        <v>2238</v>
+        <v>3480</v>
       </c>
       <c r="B440" t="s">
-        <v>2239</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
-        <v>2869</v>
+        <v>2238</v>
       </c>
       <c r="B441" t="s">
-        <v>2870</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
-        <v>2144</v>
+        <v>2869</v>
       </c>
       <c r="B442" t="s">
-        <v>2145</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
-        <v>2922</v>
+        <v>2144</v>
       </c>
       <c r="B443" t="s">
-        <v>2923</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
-        <v>5139</v>
+        <v>2922</v>
       </c>
       <c r="B444" t="s">
-        <v>5140</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
-        <v>3621</v>
+        <v>5139</v>
       </c>
       <c r="B445" t="s">
-        <v>3620</v>
+        <v>5140</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
-        <v>2202</v>
+        <v>3621</v>
       </c>
       <c r="B446" t="s">
-        <v>2203</v>
+        <v>3620</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
-        <v>2386</v>
+        <v>2202</v>
       </c>
       <c r="B447" t="s">
-        <v>2387</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
-        <v>2231</v>
+        <v>2386</v>
       </c>
       <c r="B448" t="s">
-        <v>2344</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
-        <v>5156</v>
+        <v>2231</v>
       </c>
       <c r="B449" t="s">
-        <v>5155</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
-        <v>1792</v>
+        <v>5156</v>
       </c>
       <c r="B450" t="s">
-        <v>1793</v>
+        <v>5155</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
-        <v>3334</v>
+        <v>1792</v>
       </c>
       <c r="B451" t="s">
-        <v>3335</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
-        <v>2600</v>
+        <v>3334</v>
       </c>
       <c r="B452" t="s">
-        <v>2601</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
-        <v>2674</v>
+        <v>2600</v>
       </c>
       <c r="B453" t="s">
-        <v>2675</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
-        <v>3184</v>
+        <v>2674</v>
       </c>
       <c r="B454" t="s">
-        <v>3185</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
-        <v>4635</v>
+        <v>3184</v>
       </c>
       <c r="B455" t="s">
-        <v>4636</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
-        <v>2174</v>
+        <v>4635</v>
       </c>
       <c r="B456" t="s">
-        <v>2175</v>
+        <v>4636</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
-        <v>2947</v>
+        <v>2174</v>
       </c>
       <c r="B457" t="s">
-        <v>2946</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
-        <v>1788</v>
+        <v>2947</v>
       </c>
       <c r="B458" t="s">
-        <v>1789</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
-        <v>2224</v>
+        <v>1788</v>
       </c>
       <c r="B459" t="s">
-        <v>2225</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
-        <v>2410</v>
+        <v>2224</v>
       </c>
       <c r="B460" t="s">
-        <v>2411</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
-        <v>2945</v>
+        <v>2410</v>
       </c>
       <c r="B461" t="s">
-        <v>2944</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
-        <v>2408</v>
+        <v>2945</v>
       </c>
       <c r="B462" t="s">
-        <v>2409</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>2154</v>
+        <v>2408</v>
       </c>
       <c r="B463" t="s">
-        <v>2155</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>2156</v>
+        <v>2154</v>
       </c>
       <c r="B464" t="s">
-        <v>2157</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>2938</v>
+        <v>2156</v>
       </c>
       <c r="B465" t="s">
-        <v>2937</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>4239</v>
+        <v>2938</v>
       </c>
       <c r="B466" t="s">
-        <v>4238</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
-        <v>4302</v>
+        <v>4239</v>
       </c>
       <c r="B467" t="s">
-        <v>4303</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
-        <v>4380</v>
+        <v>4302</v>
       </c>
       <c r="B468" t="s">
-        <v>4377</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
-        <v>4299</v>
+        <v>4380</v>
       </c>
       <c r="B469" t="s">
-        <v>4298</v>
+        <v>4377</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
-        <v>4688</v>
+        <v>4299</v>
       </c>
       <c r="B470" t="s">
-        <v>4687</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
-        <v>4379</v>
+        <v>4688</v>
       </c>
       <c r="B471" t="s">
-        <v>4378</v>
+        <v>4687</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
-        <v>4599</v>
+        <v>4379</v>
       </c>
       <c r="B472" t="s">
-        <v>4600</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
-        <v>4885</v>
+        <v>4599</v>
       </c>
       <c r="B473" t="s">
-        <v>4884</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
-        <v>5118</v>
+        <v>4885</v>
       </c>
       <c r="B474" t="s">
-        <v>5115</v>
+        <v>4884</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
-        <v>2886</v>
+        <v>5118</v>
       </c>
       <c r="B475" t="s">
-        <v>2887</v>
+        <v>5115</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
-        <v>2961</v>
+        <v>2886</v>
       </c>
       <c r="B476" t="s">
-        <v>2960</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
-        <v>3269</v>
+        <v>2961</v>
       </c>
       <c r="B477" t="s">
-        <v>3270</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
-        <v>1783</v>
+        <v>3269</v>
       </c>
       <c r="B478" t="s">
-        <v>1782</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
-        <v>4025</v>
+        <v>1783</v>
       </c>
       <c r="B479" t="s">
-        <v>4026</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
-        <v>2236</v>
+        <v>4025</v>
       </c>
       <c r="B480" t="s">
-        <v>2237</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
-        <v>2943</v>
+        <v>2236</v>
       </c>
       <c r="B481" t="s">
-        <v>2942</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
-        <v>4306</v>
+        <v>2943</v>
       </c>
       <c r="B482" t="s">
-        <v>4307</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
-        <v>2518</v>
+        <v>4306</v>
       </c>
       <c r="B483" t="s">
-        <v>2519</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
-        <v>3747</v>
+        <v>2518</v>
       </c>
       <c r="B484" t="s">
-        <v>3746</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
-        <v>3801</v>
+        <v>3747</v>
       </c>
       <c r="B485" t="s">
-        <v>3800</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
-        <v>2526</v>
+        <v>3801</v>
       </c>
       <c r="B486" t="s">
-        <v>2527</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B487" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
         <v>4690</v>
       </c>
-      <c r="B487" t="s">
+      <c r="B488" t="s">
         <v>4689</v>
-      </c>
-    </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A489" t="s">
-        <v>2933</v>
-      </c>
-      <c r="B489" t="s">
-        <v>2932</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
-        <v>1773</v>
+        <v>2933</v>
       </c>
       <c r="B490" t="s">
-        <v>1774</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
-        <v>2645</v>
+        <v>1773</v>
       </c>
       <c r="B491" t="s">
-        <v>2646</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>2293</v>
+        <v>2645</v>
       </c>
       <c r="B492" t="s">
-        <v>2294</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
-        <v>2546</v>
+        <v>2293</v>
       </c>
       <c r="B493" t="s">
-        <v>2547</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
-        <v>2166</v>
+        <v>2546</v>
       </c>
       <c r="B494" t="s">
-        <v>2167</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
-        <v>2176</v>
+        <v>2166</v>
       </c>
       <c r="B495" t="s">
-        <v>2177</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
-        <v>2168</v>
+        <v>2176</v>
       </c>
       <c r="B496" t="s">
-        <v>2169</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
-        <v>2447</v>
+        <v>2168</v>
       </c>
       <c r="B497" t="s">
-        <v>2448</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
-        <v>3336</v>
+        <v>2447</v>
       </c>
       <c r="B498" t="s">
-        <v>3337</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
-        <v>3832</v>
+        <v>3336</v>
       </c>
       <c r="B499" t="s">
-        <v>3831</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
-        <v>4798</v>
+        <v>3832</v>
       </c>
       <c r="B500" t="s">
-        <v>4797</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
-        <v>4943</v>
+        <v>4798</v>
       </c>
       <c r="B501" t="s">
-        <v>3324</v>
+        <v>4797</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
-        <v>3309</v>
+        <v>4943</v>
       </c>
       <c r="B502" t="s">
-        <v>4942</v>
+        <v>3324</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
-        <v>1170</v>
+        <v>3309</v>
       </c>
       <c r="B503" t="s">
-        <v>3089</v>
+        <v>4942</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
-        <v>3527</v>
+        <v>1170</v>
       </c>
       <c r="B504" t="s">
-        <v>3528</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
-        <v>1136</v>
+        <v>3527</v>
       </c>
       <c r="B505" t="s">
-        <v>2962</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
-        <v>4240</v>
+        <v>1136</v>
       </c>
       <c r="B506" t="s">
-        <v>4241</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
-        <v>2596</v>
+        <v>4240</v>
       </c>
       <c r="B507" t="s">
-        <v>2597</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
+        <v>2596</v>
+      </c>
+      <c r="B508" t="s">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A509" t="s">
         <v>3285</v>
       </c>
-      <c r="B508" t="s">
+      <c r="B509" t="s">
         <v>3284</v>
-      </c>
-    </row>
-    <row r="509" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A509" t="s">
-        <v>1588</v>
-      </c>
-      <c r="B509" t="s">
-        <v>2221</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
-        <v>1834</v>
+        <v>1588</v>
       </c>
       <c r="B510" t="s">
-        <v>1835</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
-        <v>3463</v>
+        <v>1834</v>
       </c>
       <c r="B511" t="s">
-        <v>3464</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
-        <v>1836</v>
+        <v>3463</v>
       </c>
       <c r="B512" t="s">
-        <v>1837</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
-        <v>1962</v>
+        <v>1836</v>
       </c>
       <c r="B513" t="s">
-        <v>4280</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
-        <v>2254</v>
+        <v>1962</v>
       </c>
       <c r="B514" t="s">
-        <v>2255</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -36290,183 +36338,183 @@
         <v>2254</v>
       </c>
       <c r="B515" t="s">
-        <v>3090</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
-        <v>3529</v>
+        <v>2254</v>
       </c>
       <c r="B516" t="s">
-        <v>3530</v>
+        <v>3090</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
-        <v>1485</v>
+        <v>3529</v>
       </c>
       <c r="B517" t="s">
-        <v>1486</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
-        <v>1989</v>
+        <v>1485</v>
       </c>
       <c r="B518" t="s">
-        <v>1988</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
-        <v>1982</v>
+        <v>1989</v>
       </c>
       <c r="B519" t="s">
-        <v>1983</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="B520" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="B521" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
-        <v>2033</v>
+        <v>1987</v>
       </c>
       <c r="B522" t="s">
-        <v>2917</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
-        <v>2188</v>
+        <v>2033</v>
       </c>
       <c r="B523" t="s">
-        <v>2189</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
-        <v>2206</v>
+        <v>2188</v>
       </c>
       <c r="B524" t="s">
-        <v>2207</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B525" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A526" t="s">
         <v>2442</v>
       </c>
-      <c r="B525" t="s">
+      <c r="B526" t="s">
         <v>2443</v>
-      </c>
-    </row>
-    <row r="526" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A526" t="s">
-        <v>3203</v>
-      </c>
-      <c r="B526" t="s">
-        <v>3202</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
-        <v>3518</v>
+        <v>3203</v>
       </c>
       <c r="B527" t="s">
-        <v>3519</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
-        <v>3829</v>
+        <v>3518</v>
       </c>
       <c r="B528" t="s">
-        <v>3830</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
-        <v>3524</v>
+        <v>3829</v>
       </c>
       <c r="B529" t="s">
-        <v>3523</v>
+        <v>3830</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
-        <v>4983</v>
+        <v>3524</v>
       </c>
       <c r="B530" t="s">
-        <v>4984</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
-        <v>3647</v>
+        <v>4983</v>
       </c>
       <c r="B531" t="s">
-        <v>3648</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
+        <v>3647</v>
+      </c>
+      <c r="B532" t="s">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A533" t="s">
         <v>5108</v>
       </c>
-      <c r="B532" t="s">
+      <c r="B533" t="s">
         <v>5107</v>
-      </c>
-    </row>
-    <row r="533" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A533" t="s">
-        <v>2598</v>
-      </c>
-      <c r="B533" t="s">
-        <v>2599</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
-        <v>2964</v>
+        <v>2598</v>
       </c>
       <c r="B534" t="s">
-        <v>2963</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
-        <v>3271</v>
+        <v>2964</v>
       </c>
       <c r="B535" t="s">
-        <v>3272</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
-        <v>3274</v>
+        <v>3271</v>
       </c>
       <c r="B536" t="s">
-        <v>3273</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
-        <v>1850</v>
+        <v>3274</v>
       </c>
       <c r="B537" t="s">
-        <v>1851</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -36474,998 +36522,998 @@
         <v>1850</v>
       </c>
       <c r="B538" t="s">
-        <v>1979</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A540" t="s">
         <v>1192</v>
       </c>
-      <c r="B539" t="s">
+      <c r="B540" t="s">
         <v>1823</v>
       </c>
     </row>
-    <row r="540" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="541" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A542" t="s">
-        <v>2318</v>
-      </c>
-    </row>
+    <row r="542" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="543" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
-        <v>2864</v>
-      </c>
-      <c r="B543" t="s">
-        <v>2865</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
-        <v>1505</v>
+        <v>2864</v>
       </c>
       <c r="B544" t="s">
-        <v>1503</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="B545" t="s">
-        <v>1506</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
-        <v>2212</v>
+        <v>1504</v>
       </c>
       <c r="B546" t="s">
-        <v>2213</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
-        <v>2297</v>
+        <v>2212</v>
       </c>
       <c r="B547" t="s">
-        <v>2298</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
-        <v>2295</v>
+        <v>2297</v>
       </c>
       <c r="B548" t="s">
-        <v>2296</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
-        <v>4083</v>
+        <v>2295</v>
       </c>
       <c r="B549" t="s">
-        <v>2813</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
-        <v>2456</v>
+        <v>4083</v>
       </c>
       <c r="B550" t="s">
-        <v>2909</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
-        <v>3234</v>
+        <v>2456</v>
       </c>
       <c r="B551" t="s">
-        <v>3235</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
-        <v>2449</v>
+        <v>3234</v>
       </c>
       <c r="B552" t="s">
-        <v>2451</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
-        <v>2452</v>
+        <v>2449</v>
       </c>
       <c r="B553" t="s">
-        <v>2450</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
-        <v>3220</v>
+        <v>2452</v>
       </c>
       <c r="B554" t="s">
-        <v>3221</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
-        <v>1</v>
+        <v>3220</v>
       </c>
       <c r="B555" t="s">
-        <v>2892</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
-        <v>1442</v>
+        <v>1</v>
       </c>
       <c r="B556" t="s">
-        <v>2896</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
-        <v>3010</v>
+        <v>1442</v>
       </c>
       <c r="B557" t="s">
-        <v>3009</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
-        <v>2398</v>
+        <v>3010</v>
       </c>
       <c r="B558" t="s">
-        <v>2399</v>
+        <v>3009</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="B559" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="B560" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="B561" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
-        <v>2192</v>
+        <v>2404</v>
       </c>
       <c r="B562" t="s">
-        <v>2193</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
-        <v>2242</v>
+        <v>2192</v>
       </c>
       <c r="B563" t="s">
-        <v>2243</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
-        <v>2390</v>
+        <v>2242</v>
       </c>
       <c r="B564" t="s">
-        <v>2391</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
-        <v>3239</v>
+        <v>2390</v>
       </c>
       <c r="B565" t="s">
-        <v>3238</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
-        <v>2270</v>
+        <v>3239</v>
       </c>
       <c r="B566" t="s">
-        <v>2271</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
-        <v>1530</v>
+        <v>2270</v>
       </c>
       <c r="B567" t="s">
-        <v>1531</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
-        <v>2146</v>
+        <v>1530</v>
       </c>
       <c r="B568" t="s">
-        <v>2147</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
-        <v>3240</v>
+        <v>2146</v>
       </c>
       <c r="B569" t="s">
-        <v>3241</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
-        <v>1880</v>
+        <v>3240</v>
       </c>
       <c r="B570" t="s">
-        <v>2806</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
-        <v>2866</v>
+        <v>1880</v>
       </c>
       <c r="B571" t="s">
-        <v>2867</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
-        <v>2911</v>
+        <v>2866</v>
       </c>
       <c r="B572" t="s">
-        <v>2912</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
-        <v>2214</v>
+        <v>2911</v>
       </c>
       <c r="B573" t="s">
-        <v>2215</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
-        <v>2804</v>
+        <v>2214</v>
       </c>
       <c r="B574" t="s">
-        <v>2803</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
-        <v>2184</v>
+        <v>2804</v>
       </c>
       <c r="B575" t="s">
-        <v>2185</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
-        <v>2654</v>
+        <v>2184</v>
       </c>
       <c r="B576" t="s">
-        <v>2655</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
-        <v>1613</v>
+        <v>2654</v>
       </c>
       <c r="B577" t="s">
-        <v>1614</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
-        <v>1609</v>
+        <v>1613</v>
       </c>
       <c r="B578" t="s">
-        <v>1610</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="B579" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
-        <v>14</v>
+        <v>1611</v>
       </c>
       <c r="B580" t="s">
-        <v>2905</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B581" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
-        <v>3632</v>
+        <v>15</v>
       </c>
       <c r="B582" t="s">
-        <v>3633</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
-        <v>2465</v>
+        <v>3632</v>
       </c>
       <c r="B583" t="s">
-        <v>2466</v>
+        <v>3633</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
-        <v>1513</v>
+        <v>2465</v>
       </c>
       <c r="B584" t="s">
-        <v>1893</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
-        <v>2697</v>
+        <v>1513</v>
       </c>
       <c r="B585" t="s">
-        <v>2698</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
-        <v>2291</v>
+        <v>2697</v>
       </c>
       <c r="B586" t="s">
-        <v>2292</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
-        <v>2544</v>
+        <v>2291</v>
       </c>
       <c r="B587" t="s">
-        <v>2545</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
-        <v>10</v>
+        <v>2544</v>
       </c>
       <c r="B588" t="s">
-        <v>2897</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
-        <v>1440</v>
+        <v>10</v>
       </c>
       <c r="B589" t="s">
-        <v>2910</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
-        <v>3602</v>
+        <v>1440</v>
       </c>
       <c r="B590" t="s">
-        <v>3601</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
-        <v>2433</v>
+        <v>3602</v>
       </c>
       <c r="B591" t="s">
-        <v>2434</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
-        <v>2793</v>
+        <v>2433</v>
       </c>
       <c r="B592" t="s">
-        <v>2795</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
-        <v>2792</v>
+        <v>2793</v>
       </c>
       <c r="B593" t="s">
-        <v>2794</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
-        <v>2816</v>
+        <v>2792</v>
       </c>
       <c r="B594" t="s">
-        <v>2817</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
-        <v>2227</v>
+        <v>2816</v>
       </c>
       <c r="B595" t="s">
-        <v>2228</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
-        <v>4079</v>
+        <v>2227</v>
       </c>
       <c r="B596" t="s">
-        <v>2283</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
-        <v>2234</v>
+        <v>4079</v>
       </c>
       <c r="B597" t="s">
-        <v>2235</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
-        <v>2542</v>
+        <v>2234</v>
       </c>
       <c r="B598" t="s">
-        <v>2543</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
-        <v>2895</v>
+        <v>2542</v>
       </c>
       <c r="B599" t="s">
-        <v>2894</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
-        <v>2856</v>
+        <v>2895</v>
       </c>
       <c r="B600" t="s">
-        <v>2855</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
-        <v>2753</v>
+        <v>2856</v>
       </c>
       <c r="B601" t="s">
-        <v>2752</v>
+        <v>2855</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
-        <v>2901</v>
+        <v>2753</v>
       </c>
       <c r="B602" t="s">
-        <v>2900</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
-        <v>3358</v>
+        <v>2901</v>
       </c>
       <c r="B603" t="s">
-        <v>3359</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
-        <v>2790</v>
+        <v>3358</v>
       </c>
       <c r="B604" t="s">
-        <v>2791</v>
+        <v>3359</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
-        <v>2487</v>
+        <v>2790</v>
       </c>
       <c r="B605" t="s">
-        <v>2488</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
-        <v>4938</v>
+        <v>2487</v>
       </c>
       <c r="B606" t="s">
-        <v>4937</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
-        <v>2810</v>
+        <v>4938</v>
       </c>
       <c r="B607" t="s">
-        <v>2809</v>
+        <v>4937</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
-        <v>3616</v>
+        <v>2810</v>
       </c>
       <c r="B608" t="s">
-        <v>3617</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
-        <v>2808</v>
+        <v>3616</v>
       </c>
       <c r="B609" t="s">
-        <v>2807</v>
+        <v>3617</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
-        <v>3348</v>
+        <v>2808</v>
       </c>
       <c r="B610" t="s">
-        <v>3349</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
-        <v>22</v>
+        <v>3348</v>
       </c>
       <c r="B611" t="s">
-        <v>2898</v>
+        <v>3349</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
-        <v>4171</v>
+        <v>22</v>
       </c>
       <c r="B612" t="s">
-        <v>4172</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
-        <v>2210</v>
+        <v>4171</v>
       </c>
       <c r="B613" t="s">
-        <v>2211</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
-        <v>2311</v>
+        <v>2210</v>
       </c>
       <c r="B614" t="s">
-        <v>2312</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
-        <v>8</v>
+        <v>2311</v>
       </c>
       <c r="B615" t="s">
-        <v>2899</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
-        <v>2549</v>
+        <v>8</v>
       </c>
       <c r="B616" t="s">
-        <v>2548</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
-        <v>1852</v>
+        <v>2549</v>
       </c>
       <c r="B617" t="s">
-        <v>2904</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
-        <v>2162</v>
+        <v>1852</v>
       </c>
       <c r="B618" t="s">
-        <v>2163</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
-        <v>4080</v>
+        <v>2162</v>
       </c>
       <c r="B619" t="s">
-        <v>2282</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
-        <v>2784</v>
+        <v>4080</v>
       </c>
       <c r="B620" t="s">
-        <v>2785</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
-        <v>2412</v>
+        <v>2784</v>
       </c>
       <c r="B621" t="s">
-        <v>2413</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
-        <v>2008</v>
+        <v>2412</v>
       </c>
       <c r="B622" t="s">
-        <v>2840</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
-        <v>2164</v>
+        <v>2008</v>
       </c>
       <c r="B623" t="s">
-        <v>2165</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
-        <v>2483</v>
+        <v>2164</v>
       </c>
       <c r="B624" t="s">
-        <v>2484</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
-        <v>2797</v>
+        <v>2483</v>
       </c>
       <c r="B625" t="s">
-        <v>2796</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
-        <v>3626</v>
+        <v>2797</v>
       </c>
       <c r="B626" t="s">
-        <v>3627</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
-        <v>2560</v>
+        <v>3626</v>
       </c>
       <c r="B627" t="s">
-        <v>2561</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
-        <v>4459</v>
+        <v>2560</v>
       </c>
       <c r="B628" t="s">
-        <v>4458</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
-        <v>2908</v>
+        <v>4459</v>
       </c>
       <c r="B629" t="s">
-        <v>2907</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A630" t="s">
-        <v>3630</v>
+        <v>2908</v>
       </c>
       <c r="B630" t="s">
-        <v>3631</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
-        <v>2419</v>
+        <v>3630</v>
       </c>
       <c r="B631" t="s">
-        <v>2420</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
-        <v>2928</v>
+        <v>2419</v>
       </c>
       <c r="B632" t="s">
-        <v>2929</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
-        <v>2880</v>
+        <v>2928</v>
       </c>
       <c r="B633" t="s">
-        <v>2881</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
-        <v>3232</v>
+        <v>2880</v>
       </c>
       <c r="B634" t="s">
-        <v>3233</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
-        <v>2812</v>
+        <v>3232</v>
       </c>
       <c r="B635" t="s">
-        <v>2811</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
-        <v>2031</v>
+        <v>2812</v>
       </c>
       <c r="B636" t="s">
-        <v>2893</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
-        <v>2831</v>
+        <v>2031</v>
       </c>
       <c r="B637" t="s">
-        <v>2830</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
-        <v>4903</v>
+        <v>2831</v>
       </c>
       <c r="B638" t="s">
-        <v>4902</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
-        <v>2540</v>
+        <v>4903</v>
       </c>
       <c r="B639" t="s">
-        <v>2539</v>
+        <v>4902</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
-        <v>4927</v>
+        <v>2540</v>
       </c>
       <c r="B640" t="s">
-        <v>4926</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
-        <v>2748</v>
+        <v>4927</v>
       </c>
       <c r="B641" t="s">
-        <v>2749</v>
+        <v>4926</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
-        <v>3157</v>
+        <v>2748</v>
       </c>
       <c r="B642" t="s">
-        <v>3156</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
-        <v>3155</v>
+        <v>3157</v>
       </c>
       <c r="B643" t="s">
-        <v>3154</v>
+        <v>3156</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
-        <v>3159</v>
+        <v>3155</v>
       </c>
       <c r="B644" t="s">
-        <v>3158</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
-        <v>3153</v>
+        <v>3159</v>
       </c>
       <c r="B645" t="s">
-        <v>3152</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
-        <v>3778</v>
+        <v>3153</v>
       </c>
       <c r="B646" t="s">
-        <v>3779</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
-        <v>1771</v>
+        <v>3778</v>
       </c>
       <c r="B647" t="s">
-        <v>1772</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
-        <v>2287</v>
+        <v>1771</v>
       </c>
       <c r="B648" t="s">
-        <v>2288</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
-        <v>1388</v>
+        <v>2287</v>
       </c>
       <c r="B649" t="s">
-        <v>2541</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
-        <v>3478</v>
+        <v>1388</v>
       </c>
       <c r="B650" t="s">
-        <v>3479</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
-        <v>1501</v>
+        <v>3478</v>
       </c>
       <c r="B651" t="s">
-        <v>1502</v>
+        <v>3479</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
-        <v>2829</v>
+        <v>1501</v>
       </c>
       <c r="B652" t="s">
-        <v>2828</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
-        <v>2303</v>
+        <v>2829</v>
       </c>
       <c r="B653" t="s">
-        <v>2304</v>
+        <v>2828</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
-        <v>2299</v>
+        <v>2303</v>
       </c>
       <c r="B654" t="s">
-        <v>2300</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
-        <v>2305</v>
+        <v>2299</v>
       </c>
       <c r="B655" t="s">
-        <v>2306</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
-        <v>2798</v>
+        <v>2305</v>
       </c>
       <c r="B656" t="s">
-        <v>2799</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
-        <v>3781</v>
+        <v>2798</v>
       </c>
       <c r="B657" t="s">
-        <v>3780</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
-        <v>2567</v>
+        <v>3781</v>
       </c>
       <c r="B658" t="s">
-        <v>2566</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
-        <v>1990</v>
+        <v>2567</v>
       </c>
       <c r="B659" t="s">
-        <v>1991</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
-        <v>1532</v>
+        <v>1990</v>
       </c>
       <c r="B660" t="s">
-        <v>1533</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
-        <v>3788</v>
+        <v>1532</v>
       </c>
       <c r="B661" t="s">
-        <v>3789</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
-        <v>2788</v>
+        <v>3788</v>
       </c>
       <c r="B662" t="s">
-        <v>2789</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
-        <v>1490</v>
+        <v>2788</v>
       </c>
       <c r="B663" t="s">
-        <v>1491</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A664" t="s">
-        <v>1509</v>
+        <v>1490</v>
       </c>
       <c r="B664" t="s">
-        <v>1508</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.3">
@@ -37473,276 +37521,276 @@
         <v>1509</v>
       </c>
       <c r="B665" t="s">
-        <v>2218</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A666" t="s">
-        <v>2422</v>
+        <v>1509</v>
       </c>
       <c r="B666" t="s">
-        <v>2423</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
-        <v>2194</v>
+        <v>2422</v>
       </c>
       <c r="B667" t="s">
-        <v>2195</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
-        <v>2222</v>
+        <v>2194</v>
       </c>
       <c r="B668" t="s">
-        <v>2223</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
-        <v>3258</v>
+        <v>2222</v>
       </c>
       <c r="B669" t="s">
-        <v>3245</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
-        <v>3267</v>
+        <v>3258</v>
       </c>
       <c r="B670" t="s">
-        <v>3254</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A671" t="s">
-        <v>3268</v>
+        <v>3267</v>
       </c>
       <c r="B671" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A672" t="s">
-        <v>3259</v>
+        <v>3268</v>
       </c>
       <c r="B672" t="s">
-        <v>3246</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
-        <v>3260</v>
+        <v>3259</v>
       </c>
       <c r="B673" t="s">
-        <v>3247</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A674" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="B674" t="s">
-        <v>3248</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
       <c r="B675" t="s">
-        <v>3249</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
       <c r="B676" t="s">
-        <v>3250</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
       <c r="B677" t="s">
-        <v>3251</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
       <c r="B678" t="s">
-        <v>3252</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
       <c r="B679" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" t="s">
-        <v>3257</v>
+        <v>3266</v>
       </c>
       <c r="B680" t="s">
-        <v>3256</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
-        <v>3243</v>
+        <v>3257</v>
       </c>
       <c r="B681" t="s">
-        <v>3244</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" t="s">
-        <v>3008</v>
+        <v>3243</v>
       </c>
       <c r="B682" t="s">
-        <v>3007</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
-        <v>2248</v>
+        <v>3008</v>
       </c>
       <c r="B683" t="s">
-        <v>2249</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
       <c r="B684" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
-        <v>2388</v>
+        <v>2250</v>
       </c>
       <c r="B685" t="s">
-        <v>2389</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="B686" t="s">
-        <v>2253</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" t="s">
-        <v>2878</v>
+        <v>2252</v>
       </c>
       <c r="B687" t="s">
-        <v>2879</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" t="s">
-        <v>3758</v>
+        <v>2878</v>
       </c>
       <c r="B688" t="s">
-        <v>3764</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" t="s">
-        <v>3759</v>
+        <v>3758</v>
       </c>
       <c r="B689" t="s">
-        <v>3765</v>
+        <v>3764</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" t="s">
-        <v>3760</v>
+        <v>3759</v>
       </c>
       <c r="B690" t="s">
-        <v>3766</v>
+        <v>3765</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" t="s">
-        <v>3761</v>
+        <v>3760</v>
       </c>
       <c r="B691" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" t="s">
-        <v>3762</v>
+        <v>3761</v>
       </c>
       <c r="B692" t="s">
-        <v>3768</v>
+        <v>3767</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" t="s">
-        <v>3763</v>
+        <v>3762</v>
       </c>
       <c r="B693" t="s">
-        <v>3769</v>
+        <v>3768</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
-        <v>2818</v>
+        <v>3763</v>
       </c>
       <c r="B694" t="s">
-        <v>2819</v>
+        <v>3769</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A695" t="s">
-        <v>3288</v>
+        <v>2818</v>
       </c>
       <c r="B695" t="s">
-        <v>3289</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" t="s">
-        <v>2256</v>
+        <v>3288</v>
       </c>
       <c r="B696" t="s">
-        <v>2257</v>
+        <v>3289</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
-        <v>2902</v>
+        <v>2256</v>
       </c>
       <c r="B697" t="s">
-        <v>2903</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
-        <v>2363</v>
+        <v>2902</v>
       </c>
       <c r="B698" t="s">
-        <v>2385</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
-        <v>2384</v>
+        <v>2363</v>
       </c>
       <c r="B699" t="s">
         <v>2385</v>
@@ -37750,623 +37798,623 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
-        <v>2742</v>
+        <v>2384</v>
       </c>
       <c r="B700" t="s">
-        <v>2743</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A701" t="s">
-        <v>2562</v>
+        <v>2742</v>
       </c>
       <c r="B701" t="s">
-        <v>2563</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702" t="s">
-        <v>1615</v>
+        <v>2562</v>
       </c>
       <c r="B702" t="s">
-        <v>1616</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" t="s">
-        <v>2417</v>
+        <v>1615</v>
       </c>
       <c r="B703" t="s">
-        <v>2418</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" t="s">
-        <v>3707</v>
+        <v>2417</v>
       </c>
       <c r="B704" t="s">
-        <v>3708</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" t="s">
-        <v>2851</v>
+        <v>3707</v>
       </c>
       <c r="B705" t="s">
-        <v>2852</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706" t="s">
-        <v>3824</v>
+        <v>2851</v>
       </c>
       <c r="B706" t="s">
-        <v>3823</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
-        <v>1888</v>
+        <v>3824</v>
       </c>
       <c r="B707" t="s">
-        <v>1889</v>
+        <v>3823</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
-        <v>2738</v>
+        <v>1888</v>
       </c>
       <c r="B708" t="s">
-        <v>2739</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
-        <v>2801</v>
+        <v>2738</v>
       </c>
       <c r="B709" t="s">
-        <v>2805</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
-        <v>3330</v>
+        <v>2801</v>
       </c>
       <c r="B710" t="s">
-        <v>3331</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711" t="s">
-        <v>1890</v>
+        <v>3330</v>
       </c>
       <c r="B711" t="s">
-        <v>1891</v>
+        <v>3331</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712" t="s">
-        <v>4633</v>
+        <v>1890</v>
       </c>
       <c r="B712" t="s">
-        <v>4634</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713" t="s">
-        <v>3643</v>
+        <v>4633</v>
       </c>
       <c r="B713" t="s">
-        <v>3644</v>
+        <v>4634</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A714" t="s">
-        <v>2431</v>
+        <v>3643</v>
       </c>
       <c r="B714" t="s">
-        <v>2432</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715" t="s">
-        <v>2886</v>
+        <v>2431</v>
       </c>
       <c r="B715" t="s">
-        <v>3477</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
-        <v>2741</v>
+        <v>2886</v>
       </c>
       <c r="B716" t="s">
-        <v>2740</v>
+        <v>3477</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717" t="s">
-        <v>2219</v>
+        <v>2741</v>
       </c>
       <c r="B717" t="s">
-        <v>2220</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718" t="s">
-        <v>4941</v>
+        <v>2219</v>
       </c>
       <c r="B718" t="s">
-        <v>4940</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A719" t="s">
-        <v>2838</v>
+        <v>4941</v>
       </c>
       <c r="B719" t="s">
-        <v>2839</v>
+        <v>4940</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A720" t="s">
-        <v>2160</v>
+        <v>2838</v>
       </c>
       <c r="B720" t="s">
-        <v>2161</v>
+        <v>2839</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
-        <v>2802</v>
+        <v>2160</v>
       </c>
       <c r="B721" t="s">
-        <v>2800</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A722" t="s">
-        <v>2834</v>
+        <v>2802</v>
       </c>
       <c r="B722" t="s">
-        <v>2835</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A723" t="s">
-        <v>2244</v>
+        <v>2834</v>
       </c>
       <c r="B723" t="s">
-        <v>2245</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
-        <v>2825</v>
+        <v>2244</v>
       </c>
       <c r="B724" t="s">
-        <v>2824</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A725" t="s">
-        <v>2268</v>
+        <v>2825</v>
       </c>
       <c r="B725" t="s">
-        <v>2269</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726" t="s">
-        <v>2216</v>
+        <v>2268</v>
       </c>
       <c r="B726" t="s">
-        <v>2217</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A727" t="s">
-        <v>3825</v>
+        <v>2216</v>
       </c>
       <c r="B727" t="s">
-        <v>3826</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728" t="s">
-        <v>2172</v>
+        <v>3825</v>
       </c>
       <c r="B728" t="s">
-        <v>2173</v>
+        <v>3826</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729" t="s">
-        <v>4081</v>
+        <v>2172</v>
       </c>
       <c r="B729" t="s">
-        <v>2284</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A730" t="s">
-        <v>2414</v>
+        <v>4081</v>
       </c>
       <c r="B730" t="s">
-        <v>2415</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A731" t="s">
-        <v>2394</v>
+        <v>2414</v>
       </c>
       <c r="B731" t="s">
-        <v>2395</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A732" t="s">
-        <v>2821</v>
+        <v>2394</v>
       </c>
       <c r="B732" t="s">
-        <v>2820</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A733" t="s">
-        <v>259</v>
+        <v>2821</v>
       </c>
       <c r="B733" t="s">
-        <v>1498</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A734" t="s">
-        <v>3918</v>
+        <v>259</v>
       </c>
       <c r="B734" t="s">
-        <v>3917</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A735" t="s">
-        <v>2746</v>
+        <v>3918</v>
       </c>
       <c r="B735" t="s">
-        <v>2747</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A736" t="s">
-        <v>2815</v>
+        <v>2746</v>
       </c>
       <c r="B736" t="s">
-        <v>2814</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A737" t="s">
-        <v>3186</v>
+        <v>2815</v>
       </c>
       <c r="B737" t="s">
-        <v>3187</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738" t="s">
-        <v>4595</v>
+        <v>3186</v>
       </c>
       <c r="B738" t="s">
-        <v>4596</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A739" t="s">
-        <v>3012</v>
+        <v>4595</v>
       </c>
       <c r="B739" t="s">
-        <v>3011</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A740" t="s">
-        <v>2054</v>
+        <v>3012</v>
       </c>
       <c r="B740" t="s">
-        <v>2914</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A741" t="s">
-        <v>2467</v>
+        <v>2054</v>
       </c>
       <c r="B741" t="s">
-        <v>2468</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A742" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
       <c r="B742" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A743" t="s">
-        <v>2836</v>
+        <v>2469</v>
       </c>
       <c r="B743" t="s">
-        <v>2837</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744" t="s">
-        <v>3645</v>
+        <v>2836</v>
       </c>
       <c r="B744" t="s">
-        <v>3646</v>
+        <v>2837</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745" t="s">
-        <v>4092</v>
+        <v>3645</v>
       </c>
       <c r="B745" t="s">
-        <v>4091</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746" t="s">
-        <v>3860</v>
+        <v>4092</v>
       </c>
       <c r="B746" t="s">
-        <v>3861</v>
+        <v>4091</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747" t="s">
-        <v>2823</v>
+        <v>3860</v>
       </c>
       <c r="B747" t="s">
-        <v>2822</v>
+        <v>3861</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" t="s">
-        <v>2827</v>
+        <v>2823</v>
       </c>
       <c r="B748" t="s">
-        <v>2826</v>
+        <v>2822</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749" t="s">
-        <v>2285</v>
+        <v>2827</v>
       </c>
       <c r="B749" t="s">
-        <v>2286</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A750" t="s">
-        <v>3607</v>
+        <v>2285</v>
       </c>
       <c r="B750" t="s">
-        <v>3606</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751" t="s">
-        <v>4082</v>
+        <v>3607</v>
       </c>
       <c r="B751" t="s">
-        <v>2632</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A752" t="s">
-        <v>2787</v>
+        <v>4082</v>
       </c>
       <c r="B752" t="s">
-        <v>2786</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A753" t="s">
-        <v>4089</v>
+        <v>2787</v>
       </c>
       <c r="B753" t="s">
-        <v>4090</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A754" t="s">
-        <v>4144</v>
+        <v>4089</v>
       </c>
       <c r="B754" t="s">
-        <v>4143</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A755" t="s">
-        <v>3204</v>
+        <v>4144</v>
       </c>
       <c r="B755" t="s">
-        <v>3205</v>
+        <v>4143</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A756" t="s">
-        <v>3657</v>
+        <v>3204</v>
       </c>
       <c r="B756" t="s">
-        <v>3658</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A757" t="s">
-        <v>2685</v>
+        <v>3657</v>
       </c>
       <c r="B757" t="s">
-        <v>2684</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A758" t="s">
-        <v>2682</v>
+        <v>2685</v>
       </c>
       <c r="B758" t="s">
-        <v>2683</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759" t="s">
-        <v>1605</v>
+        <v>2682</v>
       </c>
       <c r="B759" t="s">
-        <v>1604</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A760" t="s">
-        <v>3237</v>
+        <v>1605</v>
       </c>
       <c r="B760" t="s">
-        <v>3236</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A761" t="s">
-        <v>2853</v>
+        <v>3237</v>
       </c>
       <c r="B761" t="s">
-        <v>2854</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A762" t="s">
-        <v>2429</v>
+        <v>2853</v>
       </c>
       <c r="B762" t="s">
-        <v>2430</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A763" t="s">
-        <v>2025</v>
+        <v>2429</v>
       </c>
       <c r="B763" t="s">
-        <v>2841</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A764" t="s">
+        <v>2025</v>
+      </c>
+      <c r="B764" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A765" t="s">
         <v>3230</v>
       </c>
-      <c r="B764" t="s">
+      <c r="B765" t="s">
         <v>3231</v>
-      </c>
-    </row>
-    <row r="769" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A769" t="s">
-        <v>2348</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A770" t="s">
-        <v>2289</v>
-      </c>
-      <c r="B770" t="s">
-        <v>2290</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A771" t="s">
-        <v>2307</v>
+        <v>2289</v>
       </c>
       <c r="B771" t="s">
-        <v>2308</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A772" t="s">
-        <v>2875</v>
+        <v>2307</v>
       </c>
       <c r="B772" t="s">
-        <v>2874</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A773" t="s">
-        <v>2846</v>
+        <v>2875</v>
       </c>
       <c r="B773" t="s">
-        <v>2845</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A774" t="s">
-        <v>3219</v>
+        <v>2846</v>
       </c>
       <c r="B774" t="s">
-        <v>3218</v>
+        <v>2845</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A775" t="s">
-        <v>2859</v>
+        <v>3219</v>
       </c>
       <c r="B775" t="s">
-        <v>2860</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A776" t="s">
-        <v>3150</v>
+        <v>2859</v>
       </c>
       <c r="B776" t="s">
-        <v>3151</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A777" t="s">
-        <v>3171</v>
+        <v>3150</v>
       </c>
       <c r="B777" t="s">
-        <v>3170</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A778" t="s">
-        <v>3908</v>
+        <v>3171</v>
       </c>
       <c r="B778" t="s">
-        <v>3907</v>
+        <v>3170</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A779" t="s">
-        <v>3183</v>
+        <v>3908</v>
       </c>
       <c r="B779" t="s">
-        <v>3182</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A780" t="s">
-        <v>3223</v>
+        <v>3183</v>
       </c>
       <c r="B780" t="s">
-        <v>3224</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A781" t="s">
-        <v>4528</v>
+        <v>3223</v>
       </c>
       <c r="B781" t="s">
-        <v>3921</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.3">
@@ -38374,173 +38422,181 @@
         <v>4528</v>
       </c>
       <c r="B782" t="s">
-        <v>4527</v>
+        <v>3921</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A783" t="s">
-        <v>3923</v>
+        <v>4528</v>
       </c>
       <c r="B783" t="s">
-        <v>3922</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A784" t="s">
-        <v>4416</v>
+        <v>3923</v>
       </c>
       <c r="B784" t="s">
-        <v>4417</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
+        <v>4416</v>
+      </c>
+      <c r="B785" t="s">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A786" t="s">
         <v>4586</v>
       </c>
-      <c r="B785" t="s">
+      <c r="B786" t="s">
         <v>4585</v>
-      </c>
-    </row>
-    <row r="787" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A787" t="s">
-        <v>2692</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A788" t="s">
-        <v>2693</v>
-      </c>
-      <c r="B788" t="s">
-        <v>2694</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A789" t="s">
-        <v>2695</v>
+        <v>2693</v>
       </c>
       <c r="B789" t="s">
-        <v>2696</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A790" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B790" t="s">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A791" t="s">
         <v>3910</v>
       </c>
-      <c r="B790" t="s">
+      <c r="B791" t="s">
         <v>3909</v>
-      </c>
-    </row>
-    <row r="792" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A792" t="s">
-        <v>4773</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
-        <v>2372</v>
-      </c>
-      <c r="B793" t="s">
-        <v>2373</v>
+        <v>4773</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="B794" t="s">
-        <v>2375</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
-        <v>2376</v>
+        <v>2374</v>
       </c>
       <c r="B795" t="s">
-        <v>2377</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A796" t="s">
-        <v>2378</v>
+        <v>2376</v>
       </c>
       <c r="B796" t="s">
-        <v>2379</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A797" t="s">
-        <v>2380</v>
+        <v>2378</v>
       </c>
       <c r="B797" t="s">
-        <v>2381</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A798" t="s">
-        <v>4777</v>
+        <v>2380</v>
       </c>
       <c r="B798" t="s">
-        <v>4776</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A799" t="s">
-        <v>4779</v>
+        <v>4777</v>
       </c>
       <c r="B799" t="s">
-        <v>4778</v>
+        <v>4776</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A800" t="s">
-        <v>4774</v>
+        <v>4779</v>
       </c>
       <c r="B800" t="s">
-        <v>4775</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A801" t="s">
+        <v>4774</v>
+      </c>
+      <c r="B801" t="s">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A802" t="s">
         <v>4781</v>
       </c>
-      <c r="B801" t="s">
+      <c r="B802" t="s">
         <v>4780</v>
-      </c>
-    </row>
-    <row r="803" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A803" t="s">
-        <v>3757</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
-        <v>3756</v>
-      </c>
-      <c r="B804" t="s">
-        <v>3755</v>
+        <v>3757</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
-        <v>4451</v>
+        <v>3756</v>
       </c>
       <c r="B805" t="s">
-        <v>4452</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
-        <v>4453</v>
+        <v>4451</v>
       </c>
       <c r="B806" t="s">
-        <v>4454</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
+        <v>4453</v>
+      </c>
+      <c r="B807" t="s">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A808" t="s">
         <v>4455</v>
       </c>
-      <c r="B807" t="s">
+      <c r="B808" t="s">
         <v>4456</v>
       </c>
     </row>

</xml_diff>